<commit_message>
commit before I revert
</commit_message>
<xml_diff>
--- a/CharCreator.xlsx
+++ b/CharCreator.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -93,18 +93,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -116,7 +110,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -140,12 +134,6 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -165,19 +153,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Lit" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Lit1" xfId="21" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <font>
+        <sz val="10"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
     </dxf>
   </dxfs>
 </styleSheet>
@@ -188,10 +179,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V1067"/>
+  <dimension ref="A1:AD1067"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1028" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1059" activeCellId="0" sqref="L1059"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A337" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V364" activeCellId="0" sqref="V364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -205,8 +196,10 @@
     <col collapsed="false" hidden="false" max="14" min="14" style="1" width="6.57142857142857"/>
     <col collapsed="false" hidden="false" max="16" min="15" style="1" width="9.14285714285714"/>
     <col collapsed="false" hidden="false" max="21" min="17" style="1" width="6.57142857142857"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="84.280612244898"/>
-    <col collapsed="false" hidden="false" max="256" min="23" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="21.015306122449"/>
+    <col collapsed="false" hidden="false" max="27" min="23" style="1" width="4.53571428571429"/>
+    <col collapsed="false" hidden="false" max="29" min="28" style="1" width="2.56632653061224"/>
+    <col collapsed="false" hidden="false" max="256" min="30" style="1" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
@@ -268,6 +261,38 @@
         <f aca="false">CONCATENATE("    ",Q1,", ",R1,", ",S1,", ",T1,", ",U1,", /* ASCII ",N1," (",O1,"), character: ",P1," */")</f>
         <v>    0x00, 0x00, 0x00, 0x00, 0x00, /* ASCII 32 (0x20), character: ' ' */</v>
       </c>
+      <c r="W1" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q1,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X1" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R1,2))</f>
+        <v>0</v>
+      </c>
+      <c r="Y1" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S1,2))</f>
+        <v>0</v>
+      </c>
+      <c r="Z1" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T1,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AA1" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U1,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB1" s="1" t="n">
+        <f aca="false">IF(W1=0,IF(X1=0,IF(Y1=0,IF(Z1=0,IF(AA1=0,1,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC1" s="1" t="n">
+        <f aca="false">IF(AA1=0,IF(Z1=0,IF(Y1=0,IF(X1=0,IF(W1=0,3,1),2),3),4),5)</f>
+        <v>3</v>
+      </c>
+      <c r="AD1" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC1*16)+AB1,2),",")</f>
+        <v>0x31,</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
@@ -322,15 +347,15 @@
       </c>
       <c r="R2" s="2" t="str">
         <f aca="false">INDEX(F:F,$M2+8,1)</f>
-        <v>0xFB</v>
+        <v>0x60</v>
       </c>
       <c r="S2" s="2" t="str">
         <f aca="false">INDEX(G:G,$M2+8,1)</f>
-        <v>0xFB</v>
+        <v>0xFA</v>
       </c>
       <c r="T2" s="2" t="str">
         <f aca="false">INDEX(H:H,$M2+8,1)</f>
-        <v>0x00</v>
+        <v>0x60</v>
       </c>
       <c r="U2" s="2" t="str">
         <f aca="false">INDEX(I:I,$M2+8,1)</f>
@@ -338,7 +363,39 @@
       </c>
       <c r="V2" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q2,", ",R2,", ",S2,", ",T2,", ",U2,", /* ASCII ",N2," (",O2,"), character: ",P2," */")</f>
-        <v>    0x00, 0xFB, 0xFB, 0x00, 0x00, /* ASCII 33 (0x21), character: '!' */</v>
+        <v>    0x00, 0x60, 0xFA, 0x60, 0x00, /* ASCII 33 (0x21), character: '!' */</v>
+      </c>
+      <c r="W2" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q2,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X2" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R2,2))</f>
+        <v>96</v>
+      </c>
+      <c r="Y2" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S2,2))</f>
+        <v>250</v>
+      </c>
+      <c r="Z2" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T2,2))</f>
+        <v>96</v>
+      </c>
+      <c r="AA2" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U2,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB2" s="1" t="n">
+        <f aca="false">IF(W2=0,IF(X2=0,IF(Y2=0,IF(Z2=0,IF(AA2=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC2" s="1" t="n">
+        <f aca="false">IF(AA2=0,IF(Z2=0,IF(Y2=0,IF(X2=0,IF(W2=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD2" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC2*16)+AB2,2),",")</f>
+        <v>0x41,</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -413,6 +470,38 @@
         <f aca="false">CONCATENATE("    ",Q3,", ",R3,", ",S3,", ",T3,", ",U3,", /* ASCII ",N3," (",O3,"), character: ",P3," */")</f>
         <v>    0x20, 0xC0, 0x00, 0x20, 0xC0, /* ASCII 34 (0x22), character: '"' */</v>
       </c>
+      <c r="W3" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q3,2))</f>
+        <v>32</v>
+      </c>
+      <c r="X3" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R3,2))</f>
+        <v>192</v>
+      </c>
+      <c r="Y3" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S3,2))</f>
+        <v>0</v>
+      </c>
+      <c r="Z3" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T3,2))</f>
+        <v>32</v>
+      </c>
+      <c r="AA3" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U3,2))</f>
+        <v>192</v>
+      </c>
+      <c r="AB3" s="1" t="n">
+        <f aca="false">IF(W3=0,IF(X3=0,IF(Y3=0,IF(Z3=0,IF(AA3=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC3" s="1" t="n">
+        <f aca="false">IF(AA3=0,IF(Z3=0,IF(Y3=0,IF(X3=0,IF(W3=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD3" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC3*16)+AB3,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
@@ -472,6 +561,38 @@
         <f aca="false">CONCATENATE("    ",Q4,", ",R4,", ",S4,", ",T4,", ",U4,", /* ASCII ",N4," (",O4,"), character: ",P4," */")</f>
         <v>    0x28, 0x7C, 0x28, 0x7C, 0x28, /* ASCII 35 (0x23), character: '#' */</v>
       </c>
+      <c r="W4" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q4,2))</f>
+        <v>40</v>
+      </c>
+      <c r="X4" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R4,2))</f>
+        <v>124</v>
+      </c>
+      <c r="Y4" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S4,2))</f>
+        <v>40</v>
+      </c>
+      <c r="Z4" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T4,2))</f>
+        <v>124</v>
+      </c>
+      <c r="AA4" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U4,2))</f>
+        <v>40</v>
+      </c>
+      <c r="AB4" s="1" t="n">
+        <f aca="false">IF(W4=0,IF(X4=0,IF(Y4=0,IF(Z4=0,IF(AA4=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC4" s="1" t="n">
+        <f aca="false">IF(AA4=0,IF(Z4=0,IF(Y4=0,IF(X4=0,IF(W4=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD4" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC4*16)+AB4,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0"/>
@@ -531,6 +652,38 @@
         <f aca="false">CONCATENATE("    ",Q5,", ",R5,", ",S5,", ",T5,", ",U5,", /* ASCII ",N5," (",O5,"), character: ",P5," */")</f>
         <v>    0x24, 0x54, 0xFE, 0x54, 0x48, /* ASCII 36 (0x24), character: '$' */</v>
       </c>
+      <c r="W5" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q5,2))</f>
+        <v>36</v>
+      </c>
+      <c r="X5" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R5,2))</f>
+        <v>84</v>
+      </c>
+      <c r="Y5" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S5,2))</f>
+        <v>254</v>
+      </c>
+      <c r="Z5" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T5,2))</f>
+        <v>84</v>
+      </c>
+      <c r="AA5" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U5,2))</f>
+        <v>72</v>
+      </c>
+      <c r="AB5" s="1" t="n">
+        <f aca="false">IF(W5=0,IF(X5=0,IF(Y5=0,IF(Z5=0,IF(AA5=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC5" s="1" t="n">
+        <f aca="false">IF(AA5=0,IF(Z5=0,IF(Y5=0,IF(X5=0,IF(W5=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD5" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC5*16)+AB5,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0"/>
@@ -590,6 +743,38 @@
         <f aca="false">CONCATENATE("    ",Q6,", ",R6,", ",S6,", ",T6,", ",U6,", /* ASCII ",N6," (",O6,"), character: ",P6," */")</f>
         <v>    0x64, 0x68, 0x10, 0x2C, 0x4C, /* ASCII 37 (0x25), character: '%' */</v>
       </c>
+      <c r="W6" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q6,2))</f>
+        <v>100</v>
+      </c>
+      <c r="X6" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R6,2))</f>
+        <v>104</v>
+      </c>
+      <c r="Y6" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S6,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Z6" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T6,2))</f>
+        <v>44</v>
+      </c>
+      <c r="AA6" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U6,2))</f>
+        <v>76</v>
+      </c>
+      <c r="AB6" s="1" t="n">
+        <f aca="false">IF(W6=0,IF(X6=0,IF(Y6=0,IF(Z6=0,IF(AA6=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC6" s="1" t="n">
+        <f aca="false">IF(AA6=0,IF(Z6=0,IF(Y6=0,IF(X6=0,IF(W6=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD6" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC6*16)+AB6,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0"/>
@@ -648,6 +833,38 @@
       <c r="V7" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q7,", ",R7,", ",S7,", ",T7,", ",U7,", /* ASCII ",N7," (",O7,"), character: ",P7," */")</f>
         <v>    0x34, 0x4A, 0x4A, 0x24, 0x0A, /* ASCII 38 (0x26), character: '&amp;' */</v>
+      </c>
+      <c r="W7" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q7,2))</f>
+        <v>52</v>
+      </c>
+      <c r="X7" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R7,2))</f>
+        <v>74</v>
+      </c>
+      <c r="Y7" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S7,2))</f>
+        <v>74</v>
+      </c>
+      <c r="Z7" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T7,2))</f>
+        <v>36</v>
+      </c>
+      <c r="AA7" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U7,2))</f>
+        <v>10</v>
+      </c>
+      <c r="AB7" s="1" t="n">
+        <f aca="false">IF(W7=0,IF(X7=0,IF(Y7=0,IF(Z7=0,IF(AA7=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC7" s="1" t="n">
+        <f aca="false">IF(AA7=0,IF(Z7=0,IF(Y7=0,IF(X7=0,IF(W7=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD7" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC7*16)+AB7,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -705,6 +922,38 @@
         <f aca="false">CONCATENATE("    ",Q8,", ",R8,", ",S8,", ",T8,", ",U8,", /* ASCII ",N8," (",O8,"), character: ",P8," */")</f>
         <v>    0x20, 0xC0, 0x00, 0x00, 0x00, /* ASCII 39 (0x27), character: ''' */</v>
       </c>
+      <c r="W8" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q8,2))</f>
+        <v>32</v>
+      </c>
+      <c r="X8" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R8,2))</f>
+        <v>192</v>
+      </c>
+      <c r="Y8" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S8,2))</f>
+        <v>0</v>
+      </c>
+      <c r="Z8" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T8,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AA8" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U8,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB8" s="1" t="n">
+        <f aca="false">IF(W8=0,IF(X8=0,IF(Y8=0,IF(Z8=0,IF(AA8=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC8" s="1" t="n">
+        <f aca="false">IF(AA8=0,IF(Z8=0,IF(Y8=0,IF(X8=0,IF(W8=0,5,1),2),3),4),5)</f>
+        <v>2</v>
+      </c>
+      <c r="AD8" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC8*16)+AB8,2),",")</f>
+        <v>0x20,</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0"/>
@@ -761,6 +1010,38 @@
         <f aca="false">CONCATENATE("    ",Q9,", ",R9,", ",S9,", ",T9,", ",U9,", /* ASCII ",N9," (",O9,"), character: ",P9," */")</f>
         <v>    0x00, 0x38, 0x44, 0x82, 0x00, /* ASCII 40 (0x28), character: '(' */</v>
       </c>
+      <c r="W9" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q9,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X9" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R9,2))</f>
+        <v>56</v>
+      </c>
+      <c r="Y9" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S9,2))</f>
+        <v>68</v>
+      </c>
+      <c r="Z9" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T9,2))</f>
+        <v>130</v>
+      </c>
+      <c r="AA9" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U9,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB9" s="1" t="n">
+        <f aca="false">IF(W9=0,IF(X9=0,IF(Y9=0,IF(Z9=0,IF(AA9=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC9" s="1" t="n">
+        <f aca="false">IF(AA9=0,IF(Z9=0,IF(Y9=0,IF(X9=0,IF(W9=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD9" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC9*16)+AB9,2),",")</f>
+        <v>0x41,</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0"/>
@@ -816,6 +1097,38 @@
         <f aca="false">CONCATENATE("    ",Q10,", ",R10,", ",S10,", ",T10,", ",U10,", /* ASCII ",N10," (",O10,"), character: ",P10," */")</f>
         <v>    0x00, 0x82, 0x44, 0x38, 0x00, /* ASCII 41 (0x29), character: ')' */</v>
       </c>
+      <c r="W10" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q10,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X10" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R10,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Y10" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S10,2))</f>
+        <v>68</v>
+      </c>
+      <c r="Z10" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T10,2))</f>
+        <v>56</v>
+      </c>
+      <c r="AA10" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U10,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB10" s="1" t="n">
+        <f aca="false">IF(W10=0,IF(X10=0,IF(Y10=0,IF(Z10=0,IF(AA10=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC10" s="1" t="n">
+        <f aca="false">IF(AA10=0,IF(Z10=0,IF(Y10=0,IF(X10=0,IF(W10=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD10" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC10*16)+AB10,2),",")</f>
+        <v>0x41,</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0"/>
@@ -883,6 +1196,38 @@
       <c r="V11" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q11,", ",R11,", ",S11,", ",T11,", ",U11,", /* ASCII ",N11," (",O11,"), character: ",P11," */")</f>
         <v>    0x28, 0x10, 0x7C, 0x10, 0x28, /* ASCII 42 (0x2A), character: '*' */</v>
+      </c>
+      <c r="W11" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q11,2))</f>
+        <v>40</v>
+      </c>
+      <c r="X11" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R11,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Y11" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S11,2))</f>
+        <v>124</v>
+      </c>
+      <c r="Z11" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T11,2))</f>
+        <v>16</v>
+      </c>
+      <c r="AA11" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U11,2))</f>
+        <v>40</v>
+      </c>
+      <c r="AB11" s="1" t="n">
+        <f aca="false">IF(W11=0,IF(X11=0,IF(Y11=0,IF(Z11=0,IF(AA11=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC11" s="1" t="n">
+        <f aca="false">IF(AA11=0,IF(Z11=0,IF(Y11=0,IF(X11=0,IF(W11=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD11" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC11*16)+AB11,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -937,6 +1282,38 @@
         <f aca="false">CONCATENATE("    ",Q12,", ",R12,", ",S12,", ",T12,", ",U12,", /* ASCII ",N12," (",O12,"), character: ",P12," */")</f>
         <v>    0x10, 0x10, 0x7C, 0x10, 0x10, /* ASCII 43 (0x2B), character: '+' */</v>
       </c>
+      <c r="W12" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q12,2))</f>
+        <v>16</v>
+      </c>
+      <c r="X12" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R12,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Y12" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S12,2))</f>
+        <v>124</v>
+      </c>
+      <c r="Z12" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T12,2))</f>
+        <v>16</v>
+      </c>
+      <c r="AA12" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U12,2))</f>
+        <v>16</v>
+      </c>
+      <c r="AB12" s="1" t="n">
+        <f aca="false">IF(W12=0,IF(X12=0,IF(Y12=0,IF(Z12=0,IF(AA12=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC12" s="1" t="n">
+        <f aca="false">IF(AA12=0,IF(Z12=0,IF(Y12=0,IF(X12=0,IF(W12=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD12" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC12*16)+AB12,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0"/>
@@ -1004,6 +1381,38 @@
         <f aca="false">CONCATENATE("    ",Q13,", ",R13,", ",S13,", ",T13,", ",U13,", /* ASCII ",N13," (",O13,"), character: ",P13," */")</f>
         <v>    0x00, 0x0D, 0x0E, 0x00, 0x00, /* ASCII 44 (0x2C), character: ',' */</v>
       </c>
+      <c r="W13" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q13,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X13" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R13,2))</f>
+        <v>13</v>
+      </c>
+      <c r="Y13" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S13,2))</f>
+        <v>14</v>
+      </c>
+      <c r="Z13" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T13,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AA13" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U13,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB13" s="1" t="n">
+        <f aca="false">IF(W13=0,IF(X13=0,IF(Y13=0,IF(Z13=0,IF(AA13=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC13" s="1" t="n">
+        <f aca="false">IF(AA13=0,IF(Z13=0,IF(Y13=0,IF(X13=0,IF(W13=0,5,1),2),3),4),5)</f>
+        <v>3</v>
+      </c>
+      <c r="AD13" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC13*16)+AB13,2),",")</f>
+        <v>0x31,</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
@@ -1023,9 +1432,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="0"/>
-      <c r="F14" s="0" t="n">
-        <v>1</v>
-      </c>
+      <c r="F14" s="0"/>
       <c r="G14" s="2" t="n">
         <v>1</v>
       </c>
@@ -1075,6 +1482,38 @@
       <c r="V14" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q14,", ",R14,", ",S14,", ",T14,", ",U14,", /* ASCII ",N14," (",O14,"), character: ",P14," */")</f>
         <v>    0x10, 0x10, 0x10, 0x10, 0x00, /* ASCII 45 (0x2D), character: '-' */</v>
+      </c>
+      <c r="W14" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q14,2))</f>
+        <v>16</v>
+      </c>
+      <c r="X14" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R14,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Y14" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S14,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Z14" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T14,2))</f>
+        <v>16</v>
+      </c>
+      <c r="AA14" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U14,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB14" s="1" t="n">
+        <f aca="false">IF(W14=0,IF(X14=0,IF(Y14=0,IF(Z14=0,IF(AA14=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC14" s="1" t="n">
+        <f aca="false">IF(AA14=0,IF(Z14=0,IF(Y14=0,IF(X14=0,IF(W14=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD14" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC14*16)+AB14,2),",")</f>
+        <v>0x40,</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1092,11 +1531,13 @@
       <c r="G15" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H15" s="0"/>
+      <c r="H15" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="I15" s="0"/>
       <c r="J15" s="2" t="str">
         <f aca="false">F22</f>
-        <v>0xFB</v>
+        <v>0x60</v>
       </c>
       <c r="L15" s="0"/>
       <c r="M15" s="2" t="n">
@@ -1138,6 +1579,38 @@
       <c r="V15" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q15,", ",R15,", ",S15,", ",T15,", ",U15,", /* ASCII ",N15," (",O15,"), character: ",P15," */")</f>
         <v>    0x00, 0x06, 0x06, 0x00, 0x00, /* ASCII 46 (0x2E), character: '.' */</v>
+      </c>
+      <c r="W15" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q15,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X15" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R15,2))</f>
+        <v>6</v>
+      </c>
+      <c r="Y15" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S15,2))</f>
+        <v>6</v>
+      </c>
+      <c r="Z15" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T15,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AA15" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U15,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB15" s="1" t="n">
+        <f aca="false">IF(W15=0,IF(X15=0,IF(Y15=0,IF(Z15=0,IF(AA15=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC15" s="1" t="n">
+        <f aca="false">IF(AA15=0,IF(Z15=0,IF(Y15=0,IF(X15=0,IF(W15=0,5,1),2),3),4),5)</f>
+        <v>3</v>
+      </c>
+      <c r="AD15" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC15*16)+AB15,2),",")</f>
+        <v>0x31,</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1155,11 +1628,13 @@
       <c r="G16" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H16" s="0"/>
+      <c r="H16" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="I16" s="0"/>
       <c r="J16" s="2" t="str">
         <f aca="false">G22</f>
-        <v>0xFB</v>
+        <v>0xFA</v>
       </c>
       <c r="L16" s="0"/>
       <c r="M16" s="2" t="n">
@@ -1201,6 +1676,38 @@
       <c r="V16" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q16,", ",R16,", ",S16,", ",T16,", ",U16,", /* ASCII ",N16," (",O16,"), character: ",P16," */")</f>
         <v>    0x03, 0x0C, 0x30, 0xC0, 0x00, /* ASCII 47 (0x2F), character: '/' */</v>
+      </c>
+      <c r="W16" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q16,2))</f>
+        <v>3</v>
+      </c>
+      <c r="X16" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R16,2))</f>
+        <v>12</v>
+      </c>
+      <c r="Y16" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S16,2))</f>
+        <v>48</v>
+      </c>
+      <c r="Z16" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T16,2))</f>
+        <v>192</v>
+      </c>
+      <c r="AA16" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U16,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB16" s="1" t="n">
+        <f aca="false">IF(W16=0,IF(X16=0,IF(Y16=0,IF(Z16=0,IF(AA16=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC16" s="1" t="n">
+        <f aca="false">IF(AA16=0,IF(Z16=0,IF(Y16=0,IF(X16=0,IF(W16=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD16" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC16*16)+AB16,2),",")</f>
+        <v>0x40,</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1212,9 +1719,7 @@
         <v>4</v>
       </c>
       <c r="E17" s="0"/>
-      <c r="F17" s="0" t="n">
-        <v>1</v>
-      </c>
+      <c r="F17" s="0"/>
       <c r="G17" s="2" t="n">
         <v>1</v>
       </c>
@@ -1222,7 +1727,7 @@
       <c r="I17" s="0"/>
       <c r="J17" s="2" t="str">
         <f aca="false">H22</f>
-        <v>0x00</v>
+        <v>0x60</v>
       </c>
       <c r="L17" s="0"/>
       <c r="M17" s="2" t="n">
@@ -1264,6 +1769,38 @@
       <c r="V17" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q17,", ",R17,", ",S17,", ",T17,", ",U17,", /* ASCII ",N17," (",O17,"), character: ",P17," */")</f>
         <v>    0x7C, 0x8A, 0x92, 0xA2, 0x7C, /* ASCII 48 (0x30), character: '0' */</v>
+      </c>
+      <c r="W17" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q17,2))</f>
+        <v>124</v>
+      </c>
+      <c r="X17" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R17,2))</f>
+        <v>138</v>
+      </c>
+      <c r="Y17" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S17,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Z17" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T17,2))</f>
+        <v>162</v>
+      </c>
+      <c r="AA17" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U17,2))</f>
+        <v>124</v>
+      </c>
+      <c r="AB17" s="1" t="n">
+        <f aca="false">IF(W17=0,IF(X17=0,IF(Y17=0,IF(Z17=0,IF(AA17=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC17" s="1" t="n">
+        <f aca="false">IF(AA17=0,IF(Z17=0,IF(Y17=0,IF(X17=0,IF(W17=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD17" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC17*16)+AB17,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1275,9 +1812,7 @@
         <v>3</v>
       </c>
       <c r="E18" s="0"/>
-      <c r="F18" s="0" t="n">
-        <v>1</v>
-      </c>
+      <c r="F18" s="0"/>
       <c r="G18" s="2" t="n">
         <v>1</v>
       </c>
@@ -1327,6 +1862,38 @@
       <c r="V18" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q18,", ",R18,", ",S18,", ",T18,", ",U18,", /* ASCII ",N18," (",O18,"), character: ",P18," */")</f>
         <v>    0x00, 0x42, 0xFE, 0x02, 0x00, /* ASCII 49 (0x31), character: '1' */</v>
+      </c>
+      <c r="W18" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q18,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X18" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R18,2))</f>
+        <v>66</v>
+      </c>
+      <c r="Y18" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S18,2))</f>
+        <v>254</v>
+      </c>
+      <c r="Z18" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T18,2))</f>
+        <v>2</v>
+      </c>
+      <c r="AA18" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U18,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB18" s="1" t="n">
+        <f aca="false">IF(W18=0,IF(X18=0,IF(Y18=0,IF(Z18=0,IF(AA18=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC18" s="1" t="n">
+        <f aca="false">IF(AA18=0,IF(Z18=0,IF(Y18=0,IF(X18=0,IF(W18=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD18" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC18*16)+AB18,2),",")</f>
+        <v>0x41,</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1384,6 +1951,38 @@
         <f aca="false">CONCATENATE("    ",Q19,", ",R19,", ",S19,", ",T19,", ",U19,", /* ASCII ",N19," (",O19,"), character: ",P19," */")</f>
         <v>    0x46, 0x8A, 0x92, 0x92, 0x62, /* ASCII 50 (0x32), character: '2' */</v>
       </c>
+      <c r="W19" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q19,2))</f>
+        <v>70</v>
+      </c>
+      <c r="X19" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R19,2))</f>
+        <v>138</v>
+      </c>
+      <c r="Y19" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S19,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Z19" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T19,2))</f>
+        <v>146</v>
+      </c>
+      <c r="AA19" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U19,2))</f>
+        <v>98</v>
+      </c>
+      <c r="AB19" s="1" t="n">
+        <f aca="false">IF(W19=0,IF(X19=0,IF(Y19=0,IF(Z19=0,IF(AA19=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC19" s="1" t="n">
+        <f aca="false">IF(AA19=0,IF(Z19=0,IF(Y19=0,IF(X19=0,IF(W19=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD19" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC19*16)+AB19,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0"/>
@@ -1394,9 +1993,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="0"/>
-      <c r="F20" s="0" t="n">
-        <v>1</v>
-      </c>
+      <c r="F20" s="0"/>
       <c r="G20" s="2" t="n">
         <v>1</v>
       </c>
@@ -1444,8 +2041,40 @@
         <f aca="false">CONCATENATE("    ",Q20,", ",R20,", ",S20,", ",T20,", ",U20,", /* ASCII ",N20," (",O20,"), character: ",P20," */")</f>
         <v>    0x44, 0x92, 0x92, 0x92, 0x6C, /* ASCII 51 (0x33), character: '3' */</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="W20" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q20,2))</f>
+        <v>68</v>
+      </c>
+      <c r="X20" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R20,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Y20" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S20,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Z20" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T20,2))</f>
+        <v>146</v>
+      </c>
+      <c r="AA20" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U20,2))</f>
+        <v>108</v>
+      </c>
+      <c r="AB20" s="1" t="n">
+        <f aca="false">IF(W20=0,IF(X20=0,IF(Y20=0,IF(Z20=0,IF(AA20=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC20" s="1" t="n">
+        <f aca="false">IF(AA20=0,IF(Z20=0,IF(Y20=0,IF(X20=0,IF(W20=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD20" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC20*16)+AB20,2),",")</f>
+        <v>0x50,</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0"/>
       <c r="B21" s="0"/>
       <c r="C21" s="0"/>
@@ -1454,12 +2083,8 @@
         <v>0</v>
       </c>
       <c r="E21" s="0"/>
-      <c r="F21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G21" s="0" t="n">
-        <v>1</v>
-      </c>
+      <c r="F21" s="0"/>
+      <c r="G21" s="0"/>
       <c r="H21" s="0"/>
       <c r="I21" s="0"/>
       <c r="J21" s="0"/>
@@ -1503,6 +2128,38 @@
       <c r="V21" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q21,", ",R21,", ",S21,", ",T21,", ",U21,", /* ASCII ",N21," (",O21,"), character: ",P21," */")</f>
         <v>    0x38, 0xE8, 0xC8, 0xFE, 0x08, /* ASCII 52 (0x34), character: '4' */</v>
+      </c>
+      <c r="W21" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q21,2))</f>
+        <v>56</v>
+      </c>
+      <c r="X21" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R21,2))</f>
+        <v>232</v>
+      </c>
+      <c r="Y21" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S21,2))</f>
+        <v>200</v>
+      </c>
+      <c r="Z21" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T21,2))</f>
+        <v>254</v>
+      </c>
+      <c r="AA21" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U21,2))</f>
+        <v>8</v>
+      </c>
+      <c r="AB21" s="1" t="n">
+        <f aca="false">IF(W21=0,IF(X21=0,IF(Y21=0,IF(Z21=0,IF(AA21=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC21" s="1" t="n">
+        <f aca="false">IF(AA21=0,IF(Z21=0,IF(Y21=0,IF(X21=0,IF(W21=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD21" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC21*16)+AB21,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1516,15 +2173,15 @@
       </c>
       <c r="F22" s="2" t="str">
         <f aca="false">CONCATENATE("0x",DEC2HEX(SUM(IF(F21=1,2^$D21,0),IF(F20=1,2^$D20,0),IF(F19=1,2^$D19,0),IF(F18=1,2^$D18,0),IF(F17=1,2^$D17,0),IF(F16=1,2^$D16,0),IF(F15=1,2^$D15,0),IF(F14=1,2^$D14,0)),2))</f>
-        <v>0xFB</v>
+        <v>0x60</v>
       </c>
       <c r="G22" s="2" t="str">
         <f aca="false">CONCATENATE("0x",DEC2HEX(SUM(IF(G21=1,2^$D21,0),IF(G20=1,2^$D20,0),IF(G19=1,2^$D19,0),IF(G18=1,2^$D18,0),IF(G17=1,2^$D17,0),IF(G16=1,2^$D16,0),IF(G15=1,2^$D15,0),IF(G14=1,2^$D14,0)),2))</f>
-        <v>0xFB</v>
+        <v>0xFA</v>
       </c>
       <c r="H22" s="2" t="str">
         <f aca="false">CONCATENATE("0x",DEC2HEX(SUM(IF(H21=1,2^$D21,0),IF(H20=1,2^$D20,0),IF(H19=1,2^$D19,0),IF(H18=1,2^$D18,0),IF(H17=1,2^$D17,0),IF(H16=1,2^$D16,0),IF(H15=1,2^$D15,0),IF(H14=1,2^$D14,0)),2))</f>
-        <v>0x00</v>
+        <v>0x60</v>
       </c>
       <c r="I22" s="2" t="str">
         <f aca="false">CONCATENATE("0x",DEC2HEX(SUM(IF(I21=1,2^$D21,0),IF(I20=1,2^$D20,0),IF(I19=1,2^$D19,0),IF(I18=1,2^$D18,0),IF(I17=1,2^$D17,0),IF(I16=1,2^$D16,0),IF(I15=1,2^$D15,0),IF(I14=1,2^$D14,0)),2))</f>
@@ -1571,6 +2228,38 @@
       <c r="V22" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q22,", ",R22,", ",S22,", ",T22,", ",U22,", /* ASCII ",N22," (",O22,"), character: ",P22," */")</f>
         <v>    0xF4, 0x92, 0x92, 0x92, 0x8C, /* ASCII 53 (0x35), character: '5' */</v>
+      </c>
+      <c r="W22" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q22,2))</f>
+        <v>244</v>
+      </c>
+      <c r="X22" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R22,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Y22" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S22,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Z22" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T22,2))</f>
+        <v>146</v>
+      </c>
+      <c r="AA22" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U22,2))</f>
+        <v>140</v>
+      </c>
+      <c r="AB22" s="1" t="n">
+        <f aca="false">IF(W22=0,IF(X22=0,IF(Y22=0,IF(Z22=0,IF(AA22=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC22" s="1" t="n">
+        <f aca="false">IF(AA22=0,IF(Z22=0,IF(Y22=0,IF(X22=0,IF(W22=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD22" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC22*16)+AB22,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1625,6 +2314,38 @@
         <f aca="false">CONCATENATE("    ",Q23,", ",R23,", ",S23,", ",T23,", ",U23,", /* ASCII ",N23," (",O23,"), character: ",P23," */")</f>
         <v>    0x7C, 0x92, 0x92, 0x92, 0x4C, /* ASCII 54 (0x36), character: '6' */</v>
       </c>
+      <c r="W23" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q23,2))</f>
+        <v>124</v>
+      </c>
+      <c r="X23" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R23,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Y23" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S23,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Z23" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T23,2))</f>
+        <v>146</v>
+      </c>
+      <c r="AA23" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U23,2))</f>
+        <v>76</v>
+      </c>
+      <c r="AB23" s="1" t="n">
+        <f aca="false">IF(W23=0,IF(X23=0,IF(Y23=0,IF(Z23=0,IF(AA23=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC23" s="1" t="n">
+        <f aca="false">IF(AA23=0,IF(Z23=0,IF(Y23=0,IF(X23=0,IF(W23=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD23" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC23*16)+AB23,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0"/>
@@ -1692,6 +2413,38 @@
         <f aca="false">CONCATENATE("    ",Q24,", ",R24,", ",S24,", ",T24,", ",U24,", /* ASCII ",N24," (",O24,"), character: ",P24," */")</f>
         <v>    0x80, 0x88, 0x9E, 0xA8, 0xC0, /* ASCII 55 (0x37), character: '7' */</v>
       </c>
+      <c r="W24" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q24,2))</f>
+        <v>128</v>
+      </c>
+      <c r="X24" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R24,2))</f>
+        <v>136</v>
+      </c>
+      <c r="Y24" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S24,2))</f>
+        <v>158</v>
+      </c>
+      <c r="Z24" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T24,2))</f>
+        <v>168</v>
+      </c>
+      <c r="AA24" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U24,2))</f>
+        <v>192</v>
+      </c>
+      <c r="AB24" s="1" t="n">
+        <f aca="false">IF(W24=0,IF(X24=0,IF(Y24=0,IF(Z24=0,IF(AA24=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC24" s="1" t="n">
+        <f aca="false">IF(AA24=0,IF(Z24=0,IF(Y24=0,IF(X24=0,IF(W24=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD24" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC24*16)+AB24,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
@@ -1763,6 +2516,38 @@
       <c r="V25" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q25,", ",R25,", ",S25,", ",T25,", ",U25,", /* ASCII ",N25," (",O25,"), character: ",P25," */")</f>
         <v>    0x6C, 0x92, 0x92, 0x92, 0x6C, /* ASCII 56 (0x38), character: '8' */</v>
+      </c>
+      <c r="W25" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q25,2))</f>
+        <v>108</v>
+      </c>
+      <c r="X25" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R25,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Y25" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S25,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Z25" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T25,2))</f>
+        <v>146</v>
+      </c>
+      <c r="AA25" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U25,2))</f>
+        <v>108</v>
+      </c>
+      <c r="AB25" s="1" t="n">
+        <f aca="false">IF(W25=0,IF(X25=0,IF(Y25=0,IF(Z25=0,IF(AA25=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC25" s="1" t="n">
+        <f aca="false">IF(AA25=0,IF(Z25=0,IF(Y25=0,IF(X25=0,IF(W25=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD25" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC25*16)+AB25,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1827,6 +2612,38 @@
         <f aca="false">CONCATENATE("    ",Q26,", ",R26,", ",S26,", ",T26,", ",U26,", /* ASCII ",N26," (",O26,"), character: ",P26," */")</f>
         <v>    0x64, 0x92, 0x92, 0x92, 0x7C, /* ASCII 57 (0x39), character: '9' */</v>
       </c>
+      <c r="W26" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q26,2))</f>
+        <v>100</v>
+      </c>
+      <c r="X26" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R26,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Y26" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S26,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Z26" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T26,2))</f>
+        <v>146</v>
+      </c>
+      <c r="AA26" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U26,2))</f>
+        <v>124</v>
+      </c>
+      <c r="AB26" s="1" t="n">
+        <f aca="false">IF(W26=0,IF(X26=0,IF(Y26=0,IF(Z26=0,IF(AA26=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC26" s="1" t="n">
+        <f aca="false">IF(AA26=0,IF(Z26=0,IF(Y26=0,IF(X26=0,IF(W26=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD26" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC26*16)+AB26,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0"/>
@@ -1889,6 +2706,38 @@
       <c r="V27" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q27,", ",R27,", ",S27,", ",T27,", ",U27,", /* ASCII ",N27," (",O27,"), character: ",P27," */")</f>
         <v>    0x00, 0x6C, 0x6C, 0x00, 0x00, /* ASCII 58 (0x3A), character: ':' */</v>
+      </c>
+      <c r="W27" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q27,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X27" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R27,2))</f>
+        <v>108</v>
+      </c>
+      <c r="Y27" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S27,2))</f>
+        <v>108</v>
+      </c>
+      <c r="Z27" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T27,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AA27" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U27,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB27" s="1" t="n">
+        <f aca="false">IF(W27=0,IF(X27=0,IF(Y27=0,IF(Z27=0,IF(AA27=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC27" s="1" t="n">
+        <f aca="false">IF(AA27=0,IF(Z27=0,IF(Y27=0,IF(X27=0,IF(W27=0,5,1),2),3),4),5)</f>
+        <v>3</v>
+      </c>
+      <c r="AD27" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC27*16)+AB27,2),",")</f>
+        <v>0x31,</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1949,6 +2798,38 @@
         <f aca="false">CONCATENATE("    ",Q28,", ",R28,", ",S28,", ",T28,", ",U28,", /* ASCII ",N28," (",O28,"), character: ",P28," */")</f>
         <v>    0x00, 0x6D, 0x6E, 0x00, 0x00, /* ASCII 59 (0x3B), character: ';' */</v>
       </c>
+      <c r="W28" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q28,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X28" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R28,2))</f>
+        <v>109</v>
+      </c>
+      <c r="Y28" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S28,2))</f>
+        <v>110</v>
+      </c>
+      <c r="Z28" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T28,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AA28" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U28,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB28" s="1" t="n">
+        <f aca="false">IF(W28=0,IF(X28=0,IF(Y28=0,IF(Z28=0,IF(AA28=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC28" s="1" t="n">
+        <f aca="false">IF(AA28=0,IF(Z28=0,IF(Y28=0,IF(X28=0,IF(W28=0,5,1),2),3),4),5)</f>
+        <v>3</v>
+      </c>
+      <c r="AD28" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC28*16)+AB28,2),",")</f>
+        <v>0x31,</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0"/>
@@ -2007,6 +2888,38 @@
       <c r="V29" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q29,", ",R29,", ",S29,", ",T29,", ",U29,", /* ASCII ",N29," (",O29,"), character: ",P29," */")</f>
         <v>    0x00, 0x10, 0x28, 0x44, 0x82, /* ASCII 60 (0x3C), character: '&lt;' */</v>
+      </c>
+      <c r="W29" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q29,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X29" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R29,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Y29" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S29,2))</f>
+        <v>40</v>
+      </c>
+      <c r="Z29" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T29,2))</f>
+        <v>68</v>
+      </c>
+      <c r="AA29" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U29,2))</f>
+        <v>130</v>
+      </c>
+      <c r="AB29" s="1" t="n">
+        <f aca="false">IF(W29=0,IF(X29=0,IF(Y29=0,IF(Z29=0,IF(AA29=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC29" s="1" t="n">
+        <f aca="false">IF(AA29=0,IF(Z29=0,IF(Y29=0,IF(X29=0,IF(W29=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD29" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC29*16)+AB29,2),",")</f>
+        <v>0x51,</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2064,6 +2977,38 @@
         <f aca="false">CONCATENATE("    ",Q30,", ",R30,", ",S30,", ",T30,", ",U30,", /* ASCII ",N30," (",O30,"), character: ",P30," */")</f>
         <v>    0x28, 0x28, 0x28, 0x28, 0x28, /* ASCII 61 (0x3D), character: '=' */</v>
       </c>
+      <c r="W30" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q30,2))</f>
+        <v>40</v>
+      </c>
+      <c r="X30" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R30,2))</f>
+        <v>40</v>
+      </c>
+      <c r="Y30" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S30,2))</f>
+        <v>40</v>
+      </c>
+      <c r="Z30" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T30,2))</f>
+        <v>40</v>
+      </c>
+      <c r="AA30" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U30,2))</f>
+        <v>40</v>
+      </c>
+      <c r="AB30" s="1" t="n">
+        <f aca="false">IF(W30=0,IF(X30=0,IF(Y30=0,IF(Z30=0,IF(AA30=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC30" s="1" t="n">
+        <f aca="false">IF(AA30=0,IF(Z30=0,IF(Y30=0,IF(X30=0,IF(W30=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD30" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC30*16)+AB30,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0"/>
@@ -2120,6 +3065,38 @@
         <f aca="false">CONCATENATE("    ",Q31,", ",R31,", ",S31,", ",T31,", ",U31,", /* ASCII ",N31," (",O31,"), character: ",P31," */")</f>
         <v>    0x82, 0x44, 0x28, 0x10, 0x00, /* ASCII 62 (0x3E), character: '&gt;' */</v>
       </c>
+      <c r="W31" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q31,2))</f>
+        <v>130</v>
+      </c>
+      <c r="X31" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R31,2))</f>
+        <v>68</v>
+      </c>
+      <c r="Y31" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S31,2))</f>
+        <v>40</v>
+      </c>
+      <c r="Z31" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T31,2))</f>
+        <v>16</v>
+      </c>
+      <c r="AA31" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U31,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB31" s="1" t="n">
+        <f aca="false">IF(W31=0,IF(X31=0,IF(Y31=0,IF(Z31=0,IF(AA31=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC31" s="1" t="n">
+        <f aca="false">IF(AA31=0,IF(Z31=0,IF(Y31=0,IF(X31=0,IF(W31=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD31" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC31*16)+AB31,2),",")</f>
+        <v>0x40,</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0"/>
@@ -2176,6 +3153,38 @@
         <f aca="false">CONCATENATE("    ",Q32,", ",R32,", ",S32,", ",T32,", ",U32,", /* ASCII ",N32," (",O32,"), character: ",P32," */")</f>
         <v>    0x40, 0x80, 0x9A, 0xA0, 0x40, /* ASCII 63 (0x3F), character: '?' */</v>
       </c>
+      <c r="W32" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q32,2))</f>
+        <v>64</v>
+      </c>
+      <c r="X32" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R32,2))</f>
+        <v>128</v>
+      </c>
+      <c r="Y32" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S32,2))</f>
+        <v>154</v>
+      </c>
+      <c r="Z32" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T32,2))</f>
+        <v>160</v>
+      </c>
+      <c r="AA32" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U32,2))</f>
+        <v>64</v>
+      </c>
+      <c r="AB32" s="1" t="n">
+        <f aca="false">IF(W32=0,IF(X32=0,IF(Y32=0,IF(Z32=0,IF(AA32=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC32" s="1" t="n">
+        <f aca="false">IF(AA32=0,IF(Z32=0,IF(Y32=0,IF(X32=0,IF(W32=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD32" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC32*16)+AB32,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
@@ -2222,7 +3231,7 @@
       </c>
       <c r="Q33" s="2" t="str">
         <f aca="false">INDEX(E:E,$M33+8,1)</f>
-        <v>0xFE</v>
+        <v>0x7C</v>
       </c>
       <c r="R33" s="2" t="str">
         <f aca="false">INDEX(F:F,$M33+8,1)</f>
@@ -2238,11 +3247,43 @@
       </c>
       <c r="U33" s="2" t="str">
         <f aca="false">INDEX(I:I,$M33+8,1)</f>
-        <v>0xFA</v>
+        <v>0x7A</v>
       </c>
       <c r="V33" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q33,", ",R33,", ",S33,", ",T33,", ",U33,", /* ASCII ",N33," (",O33,"), character: ",P33," */")</f>
-        <v>    0xFE, 0x82, 0xBA, 0xAA, 0xFA, /* ASCII 64 (0x40), character: '@' */</v>
+        <v>    0x7C, 0x82, 0xBA, 0xAA, 0x7A, /* ASCII 64 (0x40), character: '@' */</v>
+      </c>
+      <c r="W33" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q33,2))</f>
+        <v>124</v>
+      </c>
+      <c r="X33" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R33,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Y33" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S33,2))</f>
+        <v>186</v>
+      </c>
+      <c r="Z33" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T33,2))</f>
+        <v>170</v>
+      </c>
+      <c r="AA33" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U33,2))</f>
+        <v>122</v>
+      </c>
+      <c r="AB33" s="1" t="n">
+        <f aca="false">IF(W33=0,IF(X33=0,IF(Y33=0,IF(Z33=0,IF(AA33=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC33" s="1" t="n">
+        <f aca="false">IF(AA33=0,IF(Z33=0,IF(Y33=0,IF(X33=0,IF(W33=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD33" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC33*16)+AB33,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2297,6 +3338,38 @@
         <f aca="false">CONCATENATE("    ",Q34,", ",R34,", ",S34,", ",T34,", ",U34,", /* ASCII ",N34," (",O34,"), character: ",P34," */")</f>
         <v>    0x3E, 0x48, 0x88, 0x48, 0x3E, /* ASCII 65 (0x41), character: 'A' */</v>
       </c>
+      <c r="W34" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q34,2))</f>
+        <v>62</v>
+      </c>
+      <c r="X34" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R34,2))</f>
+        <v>72</v>
+      </c>
+      <c r="Y34" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S34,2))</f>
+        <v>136</v>
+      </c>
+      <c r="Z34" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T34,2))</f>
+        <v>72</v>
+      </c>
+      <c r="AA34" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U34,2))</f>
+        <v>62</v>
+      </c>
+      <c r="AB34" s="1" t="n">
+        <f aca="false">IF(W34=0,IF(X34=0,IF(Y34=0,IF(Z34=0,IF(AA34=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC34" s="1" t="n">
+        <f aca="false">IF(AA34=0,IF(Z34=0,IF(Y34=0,IF(X34=0,IF(W34=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD34" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC34*16)+AB34,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0"/>
@@ -2363,6 +3436,38 @@
       <c r="V35" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q35,", ",R35,", ",S35,", ",T35,", ",U35,", /* ASCII ",N35," (",O35,"), character: ",P35," */")</f>
         <v>    0xFE, 0x92, 0x92, 0x92, 0x6C, /* ASCII 66 (0x42), character: 'B' */</v>
+      </c>
+      <c r="W35" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q35,2))</f>
+        <v>254</v>
+      </c>
+      <c r="X35" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R35,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Y35" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S35,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Z35" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T35,2))</f>
+        <v>146</v>
+      </c>
+      <c r="AA35" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U35,2))</f>
+        <v>108</v>
+      </c>
+      <c r="AB35" s="1" t="n">
+        <f aca="false">IF(W35=0,IF(X35=0,IF(Y35=0,IF(Z35=0,IF(AA35=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC35" s="1" t="n">
+        <f aca="false">IF(AA35=0,IF(Z35=0,IF(Y35=0,IF(X35=0,IF(W35=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD35" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC35*16)+AB35,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2432,6 +3537,38 @@
         <f aca="false">CONCATENATE("    ",Q36,", ",R36,", ",S36,", ",T36,", ",U36,", /* ASCII ",N36," (",O36,"), character: ",P36," */")</f>
         <v>    0x7C, 0x82, 0x82, 0x82, 0x44, /* ASCII 67 (0x43), character: 'C' */</v>
       </c>
+      <c r="W36" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q36,2))</f>
+        <v>124</v>
+      </c>
+      <c r="X36" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R36,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Y36" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S36,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Z36" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T36,2))</f>
+        <v>130</v>
+      </c>
+      <c r="AA36" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U36,2))</f>
+        <v>68</v>
+      </c>
+      <c r="AB36" s="1" t="n">
+        <f aca="false">IF(W36=0,IF(X36=0,IF(Y36=0,IF(Z36=0,IF(AA36=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC36" s="1" t="n">
+        <f aca="false">IF(AA36=0,IF(Z36=0,IF(Y36=0,IF(X36=0,IF(W36=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD36" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC36*16)+AB36,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0"/>
@@ -2495,6 +3632,38 @@
         <f aca="false">CONCATENATE("    ",Q37,", ",R37,", ",S37,", ",T37,", ",U37,", /* ASCII ",N37," (",O37,"), character: ",P37," */")</f>
         <v>    0xFE, 0x82, 0x82, 0x82, 0x7C, /* ASCII 68 (0x44), character: 'D' */</v>
       </c>
+      <c r="W37" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q37,2))</f>
+        <v>254</v>
+      </c>
+      <c r="X37" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R37,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Y37" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S37,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Z37" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T37,2))</f>
+        <v>130</v>
+      </c>
+      <c r="AA37" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U37,2))</f>
+        <v>124</v>
+      </c>
+      <c r="AB37" s="1" t="n">
+        <f aca="false">IF(W37=0,IF(X37=0,IF(Y37=0,IF(Z37=0,IF(AA37=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC37" s="1" t="n">
+        <f aca="false">IF(AA37=0,IF(Z37=0,IF(Y37=0,IF(X37=0,IF(W37=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD37" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC37*16)+AB37,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0"/>
@@ -2564,6 +3733,38 @@
         <f aca="false">CONCATENATE("    ",Q38,", ",R38,", ",S38,", ",T38,", ",U38,", /* ASCII ",N38," (",O38,"), character: ",P38," */")</f>
         <v>    0xFE, 0x92, 0x92, 0x92, 0x82, /* ASCII 69 (0x45), character: 'E' */</v>
       </c>
+      <c r="W38" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q38,2))</f>
+        <v>254</v>
+      </c>
+      <c r="X38" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R38,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Y38" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S38,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Z38" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T38,2))</f>
+        <v>146</v>
+      </c>
+      <c r="AA38" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U38,2))</f>
+        <v>130</v>
+      </c>
+      <c r="AB38" s="1" t="n">
+        <f aca="false">IF(W38=0,IF(X38=0,IF(Y38=0,IF(Z38=0,IF(AA38=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC38" s="1" t="n">
+        <f aca="false">IF(AA38=0,IF(Z38=0,IF(Y38=0,IF(X38=0,IF(W38=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD38" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC38*16)+AB38,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0"/>
@@ -2627,6 +3828,38 @@
         <f aca="false">CONCATENATE("    ",Q39,", ",R39,", ",S39,", ",T39,", ",U39,", /* ASCII ",N39," (",O39,"), character: ",P39," */")</f>
         <v>    0xFE, 0x90, 0x90, 0x90, 0x80, /* ASCII 70 (0x46), character: 'F' */</v>
       </c>
+      <c r="W39" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q39,2))</f>
+        <v>254</v>
+      </c>
+      <c r="X39" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R39,2))</f>
+        <v>144</v>
+      </c>
+      <c r="Y39" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S39,2))</f>
+        <v>144</v>
+      </c>
+      <c r="Z39" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T39,2))</f>
+        <v>144</v>
+      </c>
+      <c r="AA39" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U39,2))</f>
+        <v>128</v>
+      </c>
+      <c r="AB39" s="1" t="n">
+        <f aca="false">IF(W39=0,IF(X39=0,IF(Y39=0,IF(Z39=0,IF(AA39=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC39" s="1" t="n">
+        <f aca="false">IF(AA39=0,IF(Z39=0,IF(Y39=0,IF(X39=0,IF(W39=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD39" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC39*16)+AB39,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0"/>
@@ -2695,6 +3928,38 @@
       <c r="V40" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q40,", ",R40,", ",S40,", ",T40,", ",U40,", /* ASCII ",N40," (",O40,"), character: ",P40," */")</f>
         <v>    0x7C, 0x82, 0x8A, 0x8A, 0x4C, /* ASCII 71 (0x47), character: 'G' */</v>
+      </c>
+      <c r="W40" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q40,2))</f>
+        <v>124</v>
+      </c>
+      <c r="X40" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R40,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Y40" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S40,2))</f>
+        <v>138</v>
+      </c>
+      <c r="Z40" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T40,2))</f>
+        <v>138</v>
+      </c>
+      <c r="AA40" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U40,2))</f>
+        <v>76</v>
+      </c>
+      <c r="AB40" s="1" t="n">
+        <f aca="false">IF(W40=0,IF(X40=0,IF(Y40=0,IF(Z40=0,IF(AA40=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC40" s="1" t="n">
+        <f aca="false">IF(AA40=0,IF(Z40=0,IF(Y40=0,IF(X40=0,IF(W40=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD40" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC40*16)+AB40,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2755,6 +4020,38 @@
       <c r="V41" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q41,", ",R41,", ",S41,", ",T41,", ",U41,", /* ASCII ",N41," (",O41,"), character: ",P41," */")</f>
         <v>    0xFE, 0x10, 0x10, 0x10, 0xFE, /* ASCII 72 (0x48), character: 'H' */</v>
+      </c>
+      <c r="W41" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q41,2))</f>
+        <v>254</v>
+      </c>
+      <c r="X41" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R41,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Y41" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S41,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Z41" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T41,2))</f>
+        <v>16</v>
+      </c>
+      <c r="AA41" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U41,2))</f>
+        <v>254</v>
+      </c>
+      <c r="AB41" s="1" t="n">
+        <f aca="false">IF(W41=0,IF(X41=0,IF(Y41=0,IF(Z41=0,IF(AA41=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC41" s="1" t="n">
+        <f aca="false">IF(AA41=0,IF(Z41=0,IF(Y41=0,IF(X41=0,IF(W41=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD41" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC41*16)+AB41,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2812,6 +4109,38 @@
         <f aca="false">CONCATENATE("    ",Q42,", ",R42,", ",S42,", ",T42,", ",U42,", /* ASCII ",N42," (",O42,"), character: ",P42," */")</f>
         <v>    0x00, 0x82, 0xFE, 0x82, 0x00, /* ASCII 73 (0x49), character: 'I' */</v>
       </c>
+      <c r="W42" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q42,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X42" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R42,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Y42" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S42,2))</f>
+        <v>254</v>
+      </c>
+      <c r="Z42" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T42,2))</f>
+        <v>130</v>
+      </c>
+      <c r="AA42" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U42,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB42" s="1" t="n">
+        <f aca="false">IF(W42=0,IF(X42=0,IF(Y42=0,IF(Z42=0,IF(AA42=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC42" s="1" t="n">
+        <f aca="false">IF(AA42=0,IF(Z42=0,IF(Y42=0,IF(X42=0,IF(W42=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD42" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC42*16)+AB42,2),",")</f>
+        <v>0x41,</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0"/>
@@ -2868,6 +4197,38 @@
         <f aca="false">CONCATENATE("    ",Q43,", ",R43,", ",S43,", ",T43,", ",U43,", /* ASCII ",N43," (",O43,"), character: ",P43," */")</f>
         <v>    0x0C, 0x02, 0x82, 0xFC, 0x80, /* ASCII 74 (0x4A), character: 'J' */</v>
       </c>
+      <c r="W43" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q43,2))</f>
+        <v>12</v>
+      </c>
+      <c r="X43" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R43,2))</f>
+        <v>2</v>
+      </c>
+      <c r="Y43" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S43,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Z43" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T43,2))</f>
+        <v>252</v>
+      </c>
+      <c r="AA43" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U43,2))</f>
+        <v>128</v>
+      </c>
+      <c r="AB43" s="1" t="n">
+        <f aca="false">IF(W43=0,IF(X43=0,IF(Y43=0,IF(Z43=0,IF(AA43=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC43" s="1" t="n">
+        <f aca="false">IF(AA43=0,IF(Z43=0,IF(Y43=0,IF(X43=0,IF(W43=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD43" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC43*16)+AB43,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0"/>
@@ -2935,6 +4296,38 @@
       <c r="V44" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q44,", ",R44,", ",S44,", ",T44,", ",U44,", /* ASCII ",N44," (",O44,"), character: ",P44," */")</f>
         <v>    0xFE, 0x10, 0x28, 0x44, 0x82, /* ASCII 75 (0x4B), character: 'K' */</v>
+      </c>
+      <c r="W44" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q44,2))</f>
+        <v>254</v>
+      </c>
+      <c r="X44" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R44,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Y44" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S44,2))</f>
+        <v>40</v>
+      </c>
+      <c r="Z44" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T44,2))</f>
+        <v>68</v>
+      </c>
+      <c r="AA44" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U44,2))</f>
+        <v>130</v>
+      </c>
+      <c r="AB44" s="1" t="n">
+        <f aca="false">IF(W44=0,IF(X44=0,IF(Y44=0,IF(Z44=0,IF(AA44=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC44" s="1" t="n">
+        <f aca="false">IF(AA44=0,IF(Z44=0,IF(Y44=0,IF(X44=0,IF(W44=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD44" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC44*16)+AB44,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2989,6 +4382,38 @@
         <f aca="false">CONCATENATE("    ",Q45,", ",R45,", ",S45,", ",T45,", ",U45,", /* ASCII ",N45," (",O45,"), character: ",P45," */")</f>
         <v>    0xFE, 0x02, 0x02, 0x02, 0x02, /* ASCII 76 (0x4C), character: 'L' */</v>
       </c>
+      <c r="W45" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q45,2))</f>
+        <v>254</v>
+      </c>
+      <c r="X45" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R45,2))</f>
+        <v>2</v>
+      </c>
+      <c r="Y45" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S45,2))</f>
+        <v>2</v>
+      </c>
+      <c r="Z45" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T45,2))</f>
+        <v>2</v>
+      </c>
+      <c r="AA45" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U45,2))</f>
+        <v>2</v>
+      </c>
+      <c r="AB45" s="1" t="n">
+        <f aca="false">IF(W45=0,IF(X45=0,IF(Y45=0,IF(Z45=0,IF(AA45=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC45" s="1" t="n">
+        <f aca="false">IF(AA45=0,IF(Z45=0,IF(Y45=0,IF(X45=0,IF(W45=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD45" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC45*16)+AB45,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0"/>
@@ -3056,6 +4481,38 @@
         <f aca="false">CONCATENATE("    ",Q46,", ",R46,", ",S46,", ",T46,", ",U46,", /* ASCII ",N46," (",O46,"), character: ",P46," */")</f>
         <v>    0xFE, 0x40, 0x20, 0x40, 0xFE, /* ASCII 77 (0x4D), character: 'M' */</v>
       </c>
+      <c r="W46" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q46,2))</f>
+        <v>254</v>
+      </c>
+      <c r="X46" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R46,2))</f>
+        <v>64</v>
+      </c>
+      <c r="Y46" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S46,2))</f>
+        <v>32</v>
+      </c>
+      <c r="Z46" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T46,2))</f>
+        <v>64</v>
+      </c>
+      <c r="AA46" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U46,2))</f>
+        <v>254</v>
+      </c>
+      <c r="AB46" s="1" t="n">
+        <f aca="false">IF(W46=0,IF(X46=0,IF(Y46=0,IF(Z46=0,IF(AA46=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC46" s="1" t="n">
+        <f aca="false">IF(AA46=0,IF(Z46=0,IF(Y46=0,IF(X46=0,IF(W46=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD46" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC46*16)+AB46,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="n">
@@ -3125,6 +4582,38 @@
       <c r="V47" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q47,", ",R47,", ",S47,", ",T47,", ",U47,", /* ASCII ",N47," (",O47,"), character: ",P47," */")</f>
         <v>    0xFE, 0x20, 0x10, 0x08, 0xFE, /* ASCII 78 (0x4E), character: 'N' */</v>
+      </c>
+      <c r="W47" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q47,2))</f>
+        <v>254</v>
+      </c>
+      <c r="X47" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R47,2))</f>
+        <v>32</v>
+      </c>
+      <c r="Y47" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S47,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Z47" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T47,2))</f>
+        <v>8</v>
+      </c>
+      <c r="AA47" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U47,2))</f>
+        <v>254</v>
+      </c>
+      <c r="AB47" s="1" t="n">
+        <f aca="false">IF(W47=0,IF(X47=0,IF(Y47=0,IF(Z47=0,IF(AA47=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC47" s="1" t="n">
+        <f aca="false">IF(AA47=0,IF(Z47=0,IF(Y47=0,IF(X47=0,IF(W47=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD47" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC47*16)+AB47,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3193,6 +4682,38 @@
         <f aca="false">CONCATENATE("    ",Q48,", ",R48,", ",S48,", ",T48,", ",U48,", /* ASCII ",N48," (",O48,"), character: ",P48," */")</f>
         <v>    0x7C, 0x82, 0x82, 0x82, 0x7C, /* ASCII 79 (0x4F), character: 'O' */</v>
       </c>
+      <c r="W48" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q48,2))</f>
+        <v>124</v>
+      </c>
+      <c r="X48" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R48,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Y48" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S48,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Z48" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T48,2))</f>
+        <v>130</v>
+      </c>
+      <c r="AA48" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U48,2))</f>
+        <v>124</v>
+      </c>
+      <c r="AB48" s="1" t="n">
+        <f aca="false">IF(W48=0,IF(X48=0,IF(Y48=0,IF(Z48=0,IF(AA48=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC48" s="1" t="n">
+        <f aca="false">IF(AA48=0,IF(Z48=0,IF(Y48=0,IF(X48=0,IF(W48=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD48" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC48*16)+AB48,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0"/>
@@ -3256,6 +4777,38 @@
         <f aca="false">CONCATENATE("    ",Q49,", ",R49,", ",S49,", ",T49,", ",U49,", /* ASCII ",N49," (",O49,"), character: ",P49," */")</f>
         <v>    0xFE, 0x90, 0x90, 0x90, 0x60, /* ASCII 80 (0x50), character: 'P' */</v>
       </c>
+      <c r="W49" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q49,2))</f>
+        <v>254</v>
+      </c>
+      <c r="X49" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R49,2))</f>
+        <v>144</v>
+      </c>
+      <c r="Y49" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S49,2))</f>
+        <v>144</v>
+      </c>
+      <c r="Z49" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T49,2))</f>
+        <v>144</v>
+      </c>
+      <c r="AA49" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U49,2))</f>
+        <v>96</v>
+      </c>
+      <c r="AB49" s="1" t="n">
+        <f aca="false">IF(W49=0,IF(X49=0,IF(Y49=0,IF(Z49=0,IF(AA49=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC49" s="1" t="n">
+        <f aca="false">IF(AA49=0,IF(Z49=0,IF(Y49=0,IF(X49=0,IF(W49=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD49" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC49*16)+AB49,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0"/>
@@ -3321,6 +4874,38 @@
         <f aca="false">CONCATENATE("    ",Q50,", ",R50,", ",S50,", ",T50,", ",U50,", /* ASCII ",N50," (",O50,"), character: ",P50," */")</f>
         <v>    0x7C, 0x82, 0x86, 0x82, 0x7D, /* ASCII 81 (0x51), character: 'Q' */</v>
       </c>
+      <c r="W50" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q50,2))</f>
+        <v>124</v>
+      </c>
+      <c r="X50" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R50,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Y50" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S50,2))</f>
+        <v>134</v>
+      </c>
+      <c r="Z50" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T50,2))</f>
+        <v>130</v>
+      </c>
+      <c r="AA50" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U50,2))</f>
+        <v>125</v>
+      </c>
+      <c r="AB50" s="1" t="n">
+        <f aca="false">IF(W50=0,IF(X50=0,IF(Y50=0,IF(Z50=0,IF(AA50=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC50" s="1" t="n">
+        <f aca="false">IF(AA50=0,IF(Z50=0,IF(Y50=0,IF(X50=0,IF(W50=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD50" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC50*16)+AB50,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0"/>
@@ -3383,6 +4968,38 @@
       <c r="V51" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q51,", ",R51,", ",S51,", ",T51,", ",U51,", /* ASCII ",N51," (",O51,"), character: ",P51," */")</f>
         <v>    0xFE, 0x90, 0x90, 0x90, 0x6E, /* ASCII 82 (0x52), character: 'R' */</v>
+      </c>
+      <c r="W51" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q51,2))</f>
+        <v>254</v>
+      </c>
+      <c r="X51" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R51,2))</f>
+        <v>144</v>
+      </c>
+      <c r="Y51" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S51,2))</f>
+        <v>144</v>
+      </c>
+      <c r="Z51" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T51,2))</f>
+        <v>144</v>
+      </c>
+      <c r="AA51" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U51,2))</f>
+        <v>110</v>
+      </c>
+      <c r="AB51" s="1" t="n">
+        <f aca="false">IF(W51=0,IF(X51=0,IF(Y51=0,IF(Z51=0,IF(AA51=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC51" s="1" t="n">
+        <f aca="false">IF(AA51=0,IF(Z51=0,IF(Y51=0,IF(X51=0,IF(W51=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD51" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC51*16)+AB51,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3448,6 +5065,38 @@
         <f aca="false">CONCATENATE("    ",Q52,", ",R52,", ",S52,", ",T52,", ",U52,", /* ASCII ",N52," (",O52,"), character: ",P52," */")</f>
         <v>    0x62, 0x92, 0x92, 0x92, 0x8C, /* ASCII 83 (0x53), character: 'S' */</v>
       </c>
+      <c r="W52" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q52,2))</f>
+        <v>98</v>
+      </c>
+      <c r="X52" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R52,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Y52" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S52,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Z52" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T52,2))</f>
+        <v>146</v>
+      </c>
+      <c r="AA52" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U52,2))</f>
+        <v>140</v>
+      </c>
+      <c r="AB52" s="1" t="n">
+        <f aca="false">IF(W52=0,IF(X52=0,IF(Y52=0,IF(Z52=0,IF(AA52=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC52" s="1" t="n">
+        <f aca="false">IF(AA52=0,IF(Z52=0,IF(Y52=0,IF(X52=0,IF(W52=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD52" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC52*16)+AB52,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0"/>
@@ -3505,6 +5154,38 @@
       <c r="V53" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q53,", ",R53,", ",S53,", ",T53,", ",U53,", /* ASCII ",N53," (",O53,"), character: ",P53," */")</f>
         <v>    0x80, 0x80, 0xFE, 0x80, 0x80, /* ASCII 84 (0x54), character: 'T' */</v>
+      </c>
+      <c r="W53" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q53,2))</f>
+        <v>128</v>
+      </c>
+      <c r="X53" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R53,2))</f>
+        <v>128</v>
+      </c>
+      <c r="Y53" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S53,2))</f>
+        <v>254</v>
+      </c>
+      <c r="Z53" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T53,2))</f>
+        <v>128</v>
+      </c>
+      <c r="AA53" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U53,2))</f>
+        <v>128</v>
+      </c>
+      <c r="AB53" s="1" t="n">
+        <f aca="false">IF(W53=0,IF(X53=0,IF(Y53=0,IF(Z53=0,IF(AA53=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC53" s="1" t="n">
+        <f aca="false">IF(AA53=0,IF(Z53=0,IF(Y53=0,IF(X53=0,IF(W53=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD53" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC53*16)+AB53,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3562,6 +5243,38 @@
         <f aca="false">CONCATENATE("    ",Q54,", ",R54,", ",S54,", ",T54,", ",U54,", /* ASCII ",N54," (",O54,"), character: ",P54," */")</f>
         <v>    0xFC, 0x02, 0x02, 0x02, 0xFC, /* ASCII 85 (0x55), character: 'U' */</v>
       </c>
+      <c r="W54" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q54,2))</f>
+        <v>252</v>
+      </c>
+      <c r="X54" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R54,2))</f>
+        <v>2</v>
+      </c>
+      <c r="Y54" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S54,2))</f>
+        <v>2</v>
+      </c>
+      <c r="Z54" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T54,2))</f>
+        <v>2</v>
+      </c>
+      <c r="AA54" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U54,2))</f>
+        <v>252</v>
+      </c>
+      <c r="AB54" s="1" t="n">
+        <f aca="false">IF(W54=0,IF(X54=0,IF(Y54=0,IF(Z54=0,IF(AA54=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC54" s="1" t="n">
+        <f aca="false">IF(AA54=0,IF(Z54=0,IF(Y54=0,IF(X54=0,IF(W54=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD54" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC54*16)+AB54,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0"/>
@@ -3629,6 +5342,38 @@
       <c r="V55" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q55,", ",R55,", ",S55,", ",T55,", ",U55,", /* ASCII ",N55," (",O55,"), character: ",P55," */")</f>
         <v>    0xE0, 0x38, 0x0E, 0x38, 0xE0, /* ASCII 86 (0x56), character: 'V' */</v>
+      </c>
+      <c r="W55" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q55,2))</f>
+        <v>224</v>
+      </c>
+      <c r="X55" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R55,2))</f>
+        <v>56</v>
+      </c>
+      <c r="Y55" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S55,2))</f>
+        <v>14</v>
+      </c>
+      <c r="Z55" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T55,2))</f>
+        <v>56</v>
+      </c>
+      <c r="AA55" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U55,2))</f>
+        <v>224</v>
+      </c>
+      <c r="AB55" s="1" t="n">
+        <f aca="false">IF(W55=0,IF(X55=0,IF(Y55=0,IF(Z55=0,IF(AA55=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC55" s="1" t="n">
+        <f aca="false">IF(AA55=0,IF(Z55=0,IF(Y55=0,IF(X55=0,IF(W55=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD55" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC55*16)+AB55,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3683,6 +5428,38 @@
         <f aca="false">CONCATENATE("    ",Q56,", ",R56,", ",S56,", ",T56,", ",U56,", /* ASCII ",N56," (",O56,"), character: ",P56," */")</f>
         <v>    0xFC, 0x02, 0x0C, 0x02, 0xFC, /* ASCII 87 (0x57), character: 'W' */</v>
       </c>
+      <c r="W56" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q56,2))</f>
+        <v>252</v>
+      </c>
+      <c r="X56" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R56,2))</f>
+        <v>2</v>
+      </c>
+      <c r="Y56" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S56,2))</f>
+        <v>12</v>
+      </c>
+      <c r="Z56" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T56,2))</f>
+        <v>2</v>
+      </c>
+      <c r="AA56" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U56,2))</f>
+        <v>252</v>
+      </c>
+      <c r="AB56" s="1" t="n">
+        <f aca="false">IF(W56=0,IF(X56=0,IF(Y56=0,IF(Z56=0,IF(AA56=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC56" s="1" t="n">
+        <f aca="false">IF(AA56=0,IF(Z56=0,IF(Y56=0,IF(X56=0,IF(W56=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD56" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC56*16)+AB56,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0"/>
@@ -3749,6 +5526,38 @@
       <c r="V57" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q57,", ",R57,", ",S57,", ",T57,", ",U57,", /* ASCII ",N57," (",O57,"), character: ",P57," */")</f>
         <v>    0xC6, 0x28, 0x10, 0x28, 0xC6, /* ASCII 88 (0x58), character: 'X' */</v>
+      </c>
+      <c r="W57" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q57,2))</f>
+        <v>198</v>
+      </c>
+      <c r="X57" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R57,2))</f>
+        <v>40</v>
+      </c>
+      <c r="Y57" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S57,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Z57" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T57,2))</f>
+        <v>40</v>
+      </c>
+      <c r="AA57" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U57,2))</f>
+        <v>198</v>
+      </c>
+      <c r="AB57" s="1" t="n">
+        <f aca="false">IF(W57=0,IF(X57=0,IF(Y57=0,IF(Z57=0,IF(AA57=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC57" s="1" t="n">
+        <f aca="false">IF(AA57=0,IF(Z57=0,IF(Y57=0,IF(X57=0,IF(W57=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD57" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC57*16)+AB57,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3818,6 +5627,38 @@
         <f aca="false">CONCATENATE("    ",Q58,", ",R58,", ",S58,", ",T58,", ",U58,", /* ASCII ",N58," (",O58,"), character: ",P58," */")</f>
         <v>    0xE0, 0x10, 0x0E, 0x10, 0xE0, /* ASCII 89 (0x59), character: 'Y' */</v>
       </c>
+      <c r="W58" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q58,2))</f>
+        <v>224</v>
+      </c>
+      <c r="X58" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R58,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Y58" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S58,2))</f>
+        <v>14</v>
+      </c>
+      <c r="Z58" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T58,2))</f>
+        <v>16</v>
+      </c>
+      <c r="AA58" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U58,2))</f>
+        <v>224</v>
+      </c>
+      <c r="AB58" s="1" t="n">
+        <f aca="false">IF(W58=0,IF(X58=0,IF(Y58=0,IF(Z58=0,IF(AA58=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC58" s="1" t="n">
+        <f aca="false">IF(AA58=0,IF(Z58=0,IF(Y58=0,IF(X58=0,IF(W58=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD58" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC58*16)+AB58,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0"/>
@@ -3883,6 +5724,38 @@
         <f aca="false">CONCATENATE("    ",Q59,", ",R59,", ",S59,", ",T59,", ",U59,", /* ASCII ",N59," (",O59,"), character: ",P59," */")</f>
         <v>    0x86, 0x8A, 0x92, 0xA2, 0xC2, /* ASCII 90 (0x5A), character: 'Z' */</v>
       </c>
+      <c r="W59" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q59,2))</f>
+        <v>134</v>
+      </c>
+      <c r="X59" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R59,2))</f>
+        <v>138</v>
+      </c>
+      <c r="Y59" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S59,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Z59" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T59,2))</f>
+        <v>162</v>
+      </c>
+      <c r="AA59" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U59,2))</f>
+        <v>194</v>
+      </c>
+      <c r="AB59" s="1" t="n">
+        <f aca="false">IF(W59=0,IF(X59=0,IF(Y59=0,IF(Z59=0,IF(AA59=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC59" s="1" t="n">
+        <f aca="false">IF(AA59=0,IF(Z59=0,IF(Y59=0,IF(X59=0,IF(W59=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD59" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC59*16)+AB59,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0"/>
@@ -3950,6 +5823,38 @@
         <f aca="false">CONCATENATE("    ",Q60,", ",R60,", ",S60,", ",T60,", ",U60,", /* ASCII ",N60," (",O60,"), character: ",P60," */")</f>
         <v>    0x00, 0xFE, 0x82, 0x82, 0x00, /* ASCII 91 (0x5B), character: '[' */</v>
       </c>
+      <c r="W60" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q60,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X60" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R60,2))</f>
+        <v>254</v>
+      </c>
+      <c r="Y60" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S60,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Z60" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T60,2))</f>
+        <v>130</v>
+      </c>
+      <c r="AA60" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U60,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB60" s="1" t="n">
+        <f aca="false">IF(W60=0,IF(X60=0,IF(Y60=0,IF(Z60=0,IF(AA60=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC60" s="1" t="n">
+        <f aca="false">IF(AA60=0,IF(Z60=0,IF(Y60=0,IF(X60=0,IF(W60=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD60" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC60*16)+AB60,2),",")</f>
+        <v>0x41,</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0"/>
@@ -4017,6 +5922,38 @@
         <f aca="false">CONCATENATE("    ",Q61,", ",R61,", ",S61,", ",T61,", ",U61,", /* ASCII ",N61," (",O61,"), character: ",P61," */")</f>
         <v>    0x00, 0xC0, 0x30, 0x0C, 0x03, /* ASCII 92 (0x5C), character: '\' */</v>
       </c>
+      <c r="W61" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q61,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X61" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R61,2))</f>
+        <v>192</v>
+      </c>
+      <c r="Y61" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S61,2))</f>
+        <v>48</v>
+      </c>
+      <c r="Z61" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T61,2))</f>
+        <v>12</v>
+      </c>
+      <c r="AA61" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U61,2))</f>
+        <v>3</v>
+      </c>
+      <c r="AB61" s="1" t="n">
+        <f aca="false">IF(W61=0,IF(X61=0,IF(Y61=0,IF(Z61=0,IF(AA61=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC61" s="1" t="n">
+        <f aca="false">IF(AA61=0,IF(Z61=0,IF(Y61=0,IF(X61=0,IF(W61=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD61" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC61*16)+AB61,2),",")</f>
+        <v>0x51,</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0"/>
@@ -4083,6 +6020,38 @@
       <c r="V62" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q62,", ",R62,", ",S62,", ",T62,", ",U62,", /* ASCII ",N62," (",O62,"), character: ",P62," */")</f>
         <v>    0x00, 0x82, 0x82, 0xFE, 0x00, /* ASCII 93 (0x5D), character: ']' */</v>
+      </c>
+      <c r="W62" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q62,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X62" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R62,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Y62" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S62,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Z62" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T62,2))</f>
+        <v>254</v>
+      </c>
+      <c r="AA62" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U62,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB62" s="1" t="n">
+        <f aca="false">IF(W62=0,IF(X62=0,IF(Y62=0,IF(Z62=0,IF(AA62=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC62" s="1" t="n">
+        <f aca="false">IF(AA62=0,IF(Z62=0,IF(Y62=0,IF(X62=0,IF(W62=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD62" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC62*16)+AB62,2),",")</f>
+        <v>0x41,</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4145,6 +6114,38 @@
       <c r="V63" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q63,", ",R63,", ",S63,", ",T63,", ",U63,", /* ASCII ",N63," (",O63,"), character: ",P63," */")</f>
         <v>    0x10, 0x20, 0x40, 0x20, 0x10, /* ASCII 94 (0x5E), character: '^' */</v>
+      </c>
+      <c r="W63" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q63,2))</f>
+        <v>16</v>
+      </c>
+      <c r="X63" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R63,2))</f>
+        <v>32</v>
+      </c>
+      <c r="Y63" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S63,2))</f>
+        <v>64</v>
+      </c>
+      <c r="Z63" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T63,2))</f>
+        <v>32</v>
+      </c>
+      <c r="AA63" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U63,2))</f>
+        <v>16</v>
+      </c>
+      <c r="AB63" s="1" t="n">
+        <f aca="false">IF(W63=0,IF(X63=0,IF(Y63=0,IF(Z63=0,IF(AA63=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC63" s="1" t="n">
+        <f aca="false">IF(AA63=0,IF(Z63=0,IF(Y63=0,IF(X63=0,IF(W63=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD63" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC63*16)+AB63,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4202,6 +6203,38 @@
         <f aca="false">CONCATENATE("    ",Q64,", ",R64,", ",S64,", ",T64,", ",U64,", /* ASCII ",N64," (",O64,"), character: ",P64," */")</f>
         <v>    0x02, 0x02, 0x02, 0x02, 0x02, /* ASCII 95 (0x5F), character: '_' */</v>
       </c>
+      <c r="W64" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q64,2))</f>
+        <v>2</v>
+      </c>
+      <c r="X64" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R64,2))</f>
+        <v>2</v>
+      </c>
+      <c r="Y64" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S64,2))</f>
+        <v>2</v>
+      </c>
+      <c r="Z64" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T64,2))</f>
+        <v>2</v>
+      </c>
+      <c r="AA64" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U64,2))</f>
+        <v>2</v>
+      </c>
+      <c r="AB64" s="1" t="n">
+        <f aca="false">IF(W64=0,IF(X64=0,IF(Y64=0,IF(Z64=0,IF(AA64=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC64" s="1" t="n">
+        <f aca="false">IF(AA64=0,IF(Z64=0,IF(Y64=0,IF(X64=0,IF(W64=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD64" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC64*16)+AB64,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0"/>
@@ -4258,6 +6291,38 @@
         <f aca="false">CONCATENATE("    ",Q65,", ",R65,", ",S65,", ",T65,", ",U65,", /* ASCII ",N65," (",O65,"), character: ",P65," */")</f>
         <v>    0x00, 0x80, 0x60, 0x00, 0x00, /* ASCII 96 (0x60), character: '`' */</v>
       </c>
+      <c r="W65" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q65,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X65" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R65,2))</f>
+        <v>128</v>
+      </c>
+      <c r="Y65" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S65,2))</f>
+        <v>96</v>
+      </c>
+      <c r="Z65" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T65,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AA65" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U65,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB65" s="1" t="n">
+        <f aca="false">IF(W65=0,IF(X65=0,IF(Y65=0,IF(Z65=0,IF(AA65=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC65" s="1" t="n">
+        <f aca="false">IF(AA65=0,IF(Z65=0,IF(Y65=0,IF(X65=0,IF(W65=0,5,1),2),3),4),5)</f>
+        <v>3</v>
+      </c>
+      <c r="AD65" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC65*16)+AB65,2),",")</f>
+        <v>0x31,</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0"/>
@@ -4325,6 +6390,38 @@
       <c r="V66" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q66,", ",R66,", ",S66,", ",T66,", ",U66,", /* ASCII ",N66," (",O66,"), character: ",P66," */")</f>
         <v>    0x24, 0x4A, 0x4A, 0x3E, 0x00, /* ASCII 97 (0x61), character: 'a' */</v>
+      </c>
+      <c r="W66" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q66,2))</f>
+        <v>36</v>
+      </c>
+      <c r="X66" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R66,2))</f>
+        <v>74</v>
+      </c>
+      <c r="Y66" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S66,2))</f>
+        <v>74</v>
+      </c>
+      <c r="Z66" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T66,2))</f>
+        <v>62</v>
+      </c>
+      <c r="AA66" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U66,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB66" s="1" t="n">
+        <f aca="false">IF(W66=0,IF(X66=0,IF(Y66=0,IF(Z66=0,IF(AA66=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC66" s="1" t="n">
+        <f aca="false">IF(AA66=0,IF(Z66=0,IF(Y66=0,IF(X66=0,IF(W66=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD66" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC66*16)+AB66,2),",")</f>
+        <v>0x40,</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4379,6 +6476,38 @@
         <f aca="false">CONCATENATE("    ",Q67,", ",R67,", ",S67,", ",T67,", ",U67,", /* ASCII ",N67," (",O67,"), character: ",P67," */")</f>
         <v>    0x00, 0xFE, 0x12, 0x12, 0x0C, /* ASCII 98 (0x62), character: 'b' */</v>
       </c>
+      <c r="W67" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q67,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X67" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R67,2))</f>
+        <v>254</v>
+      </c>
+      <c r="Y67" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S67,2))</f>
+        <v>18</v>
+      </c>
+      <c r="Z67" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T67,2))</f>
+        <v>18</v>
+      </c>
+      <c r="AA67" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U67,2))</f>
+        <v>12</v>
+      </c>
+      <c r="AB67" s="1" t="n">
+        <f aca="false">IF(W67=0,IF(X67=0,IF(Y67=0,IF(Z67=0,IF(AA67=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC67" s="1" t="n">
+        <f aca="false">IF(AA67=0,IF(Z67=0,IF(Y67=0,IF(X67=0,IF(W67=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD67" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC67*16)+AB67,2),",")</f>
+        <v>0x51,</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0"/>
@@ -4445,6 +6574,38 @@
       <c r="V68" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q68,", ",R68,", ",S68,", ",T68,", ",U68,", /* ASCII ",N68," (",O68,"), character: ",P68," */")</f>
         <v>    0x0C, 0x12, 0x12, 0x12, 0x00, /* ASCII 99 (0x63), character: 'c' */</v>
+      </c>
+      <c r="W68" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q68,2))</f>
+        <v>12</v>
+      </c>
+      <c r="X68" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R68,2))</f>
+        <v>18</v>
+      </c>
+      <c r="Y68" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S68,2))</f>
+        <v>18</v>
+      </c>
+      <c r="Z68" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T68,2))</f>
+        <v>18</v>
+      </c>
+      <c r="AA68" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U68,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB68" s="1" t="n">
+        <f aca="false">IF(W68=0,IF(X68=0,IF(Y68=0,IF(Z68=0,IF(AA68=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC68" s="1" t="n">
+        <f aca="false">IF(AA68=0,IF(Z68=0,IF(Y68=0,IF(X68=0,IF(W68=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD68" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC68*16)+AB68,2),",")</f>
+        <v>0x40,</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4514,6 +6675,38 @@
         <f aca="false">CONCATENATE("    ",Q69,", ",R69,", ",S69,", ",T69,", ",U69,", /* ASCII ",N69," (",O69,"), character: ",P69," */")</f>
         <v>    0x00, 0x0C, 0x12, 0x12, 0xFE, /* ASCII 100 (0x64), character: 'd' */</v>
       </c>
+      <c r="W69" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q69,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X69" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R69,2))</f>
+        <v>12</v>
+      </c>
+      <c r="Y69" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S69,2))</f>
+        <v>18</v>
+      </c>
+      <c r="Z69" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T69,2))</f>
+        <v>18</v>
+      </c>
+      <c r="AA69" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U69,2))</f>
+        <v>254</v>
+      </c>
+      <c r="AB69" s="1" t="n">
+        <f aca="false">IF(W69=0,IF(X69=0,IF(Y69=0,IF(Z69=0,IF(AA69=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC69" s="1" t="n">
+        <f aca="false">IF(AA69=0,IF(Z69=0,IF(Y69=0,IF(X69=0,IF(W69=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD69" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC69*16)+AB69,2),",")</f>
+        <v>0x51,</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0"/>
@@ -4577,6 +6770,38 @@
         <f aca="false">CONCATENATE("    ",Q70,", ",R70,", ",S70,", ",T70,", ",U70,", /* ASCII ",N70," (",O70,"), character: ",P70," */")</f>
         <v>    0x1C, 0x2A, 0x2A, 0x10, 0x00, /* ASCII 101 (0x65), character: 'e' */</v>
       </c>
+      <c r="W70" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q70,2))</f>
+        <v>28</v>
+      </c>
+      <c r="X70" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R70,2))</f>
+        <v>42</v>
+      </c>
+      <c r="Y70" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S70,2))</f>
+        <v>42</v>
+      </c>
+      <c r="Z70" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T70,2))</f>
+        <v>16</v>
+      </c>
+      <c r="AA70" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U70,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB70" s="1" t="n">
+        <f aca="false">IF(W70=0,IF(X70=0,IF(Y70=0,IF(Z70=0,IF(AA70=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC70" s="1" t="n">
+        <f aca="false">IF(AA70=0,IF(Z70=0,IF(Y70=0,IF(X70=0,IF(W70=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD70" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC70*16)+AB70,2),",")</f>
+        <v>0x40,</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0"/>
@@ -4640,6 +6865,38 @@
         <f aca="false">CONCATENATE("    ",Q71,", ",R71,", ",S71,", ",T71,", ",U71,", /* ASCII ",N71," (",O71,"), character: ",P71," */")</f>
         <v>    0x3E, 0x48, 0x40, 0x20, 0x00, /* ASCII 102 (0x66), character: 'f' */</v>
       </c>
+      <c r="W71" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q71,2))</f>
+        <v>62</v>
+      </c>
+      <c r="X71" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R71,2))</f>
+        <v>72</v>
+      </c>
+      <c r="Y71" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S71,2))</f>
+        <v>64</v>
+      </c>
+      <c r="Z71" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T71,2))</f>
+        <v>32</v>
+      </c>
+      <c r="AA71" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U71,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB71" s="1" t="n">
+        <f aca="false">IF(W71=0,IF(X71=0,IF(Y71=0,IF(Z71=0,IF(AA71=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC71" s="1" t="n">
+        <f aca="false">IF(AA71=0,IF(Z71=0,IF(Y71=0,IF(X71=0,IF(W71=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD71" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC71*16)+AB71,2),",")</f>
+        <v>0x40,</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0"/>
@@ -4701,6 +6958,38 @@
         <f aca="false">CONCATENATE("    ",Q72,", ",R72,", ",S72,", ",T72,", ",U72,", /* ASCII ",N72," (",O72,"), character: ",P72," */")</f>
         <v>    0x12, 0x29, 0x29, 0x3E, 0x00, /* ASCII 103 (0x67), character: 'g' */</v>
       </c>
+      <c r="W72" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q72,2))</f>
+        <v>18</v>
+      </c>
+      <c r="X72" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R72,2))</f>
+        <v>41</v>
+      </c>
+      <c r="Y72" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S72,2))</f>
+        <v>41</v>
+      </c>
+      <c r="Z72" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T72,2))</f>
+        <v>62</v>
+      </c>
+      <c r="AA72" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U72,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB72" s="1" t="n">
+        <f aca="false">IF(W72=0,IF(X72=0,IF(Y72=0,IF(Z72=0,IF(AA72=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC72" s="1" t="n">
+        <f aca="false">IF(AA72=0,IF(Z72=0,IF(Y72=0,IF(X72=0,IF(W72=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD72" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC72*16)+AB72,2),",")</f>
+        <v>0x40,</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0"/>
@@ -4765,6 +7054,38 @@
       <c r="V73" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q73,", ",R73,", ",S73,", ",T73,", ",U73,", /* ASCII ",N73," (",O73,"), character: ",P73," */")</f>
         <v>    0x7E, 0x08, 0x08, 0x06, 0x00, /* ASCII 104 (0x68), character: 'h' */</v>
+      </c>
+      <c r="W73" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q73,2))</f>
+        <v>126</v>
+      </c>
+      <c r="X73" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R73,2))</f>
+        <v>8</v>
+      </c>
+      <c r="Y73" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S73,2))</f>
+        <v>8</v>
+      </c>
+      <c r="Z73" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T73,2))</f>
+        <v>6</v>
+      </c>
+      <c r="AA73" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U73,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB73" s="1" t="n">
+        <f aca="false">IF(W73=0,IF(X73=0,IF(Y73=0,IF(Z73=0,IF(AA73=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC73" s="1" t="n">
+        <f aca="false">IF(AA73=0,IF(Z73=0,IF(Y73=0,IF(X73=0,IF(W73=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD73" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC73*16)+AB73,2),",")</f>
+        <v>0x40,</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4826,6 +7147,38 @@
         <f aca="false">CONCATENATE("    ",Q74,", ",R74,", ",S74,", ",T74,", ",U74,", /* ASCII ",N74," (",O74,"), character: ",P74," */")</f>
         <v>    0x00, 0x12, 0x5E, 0x02, 0x00, /* ASCII 105 (0x69), character: 'i' */</v>
       </c>
+      <c r="W74" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q74,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X74" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R74,2))</f>
+        <v>18</v>
+      </c>
+      <c r="Y74" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S74,2))</f>
+        <v>94</v>
+      </c>
+      <c r="Z74" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T74,2))</f>
+        <v>2</v>
+      </c>
+      <c r="AA74" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U74,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB74" s="1" t="n">
+        <f aca="false">IF(W74=0,IF(X74=0,IF(Y74=0,IF(Z74=0,IF(AA74=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC74" s="1" t="n">
+        <f aca="false">IF(AA74=0,IF(Z74=0,IF(Y74=0,IF(X74=0,IF(W74=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD74" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC74*16)+AB74,2),",")</f>
+        <v>0x41,</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0"/>
@@ -4887,6 +7240,38 @@
       <c r="V75" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q75,", ",R75,", ",S75,", ",T75,", ",U75,", /* ASCII ",N75," (",O75,"), character: ",P75," */")</f>
         <v>    0x00, 0x02, 0x11, 0x5E, 0x10, /* ASCII 106 (0x6A), character: 'j' */</v>
+      </c>
+      <c r="W75" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q75,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X75" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R75,2))</f>
+        <v>2</v>
+      </c>
+      <c r="Y75" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S75,2))</f>
+        <v>17</v>
+      </c>
+      <c r="Z75" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T75,2))</f>
+        <v>94</v>
+      </c>
+      <c r="AA75" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U75,2))</f>
+        <v>16</v>
+      </c>
+      <c r="AB75" s="1" t="n">
+        <f aca="false">IF(W75=0,IF(X75=0,IF(Y75=0,IF(Z75=0,IF(AA75=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC75" s="1" t="n">
+        <f aca="false">IF(AA75=0,IF(Z75=0,IF(Y75=0,IF(X75=0,IF(W75=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD75" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC75*16)+AB75,2),",")</f>
+        <v>0x51,</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4944,6 +7329,38 @@
         <f aca="false">CONCATENATE("    ",Q76,", ",R76,", ",S76,", ",T76,", ",U76,", /* ASCII ",N76," (",O76,"), character: ",P76," */")</f>
         <v>    0x00, 0xFE, 0x08, 0x16, 0x00, /* ASCII 107 (0x6B), character: 'k' */</v>
       </c>
+      <c r="W76" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q76,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X76" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R76,2))</f>
+        <v>254</v>
+      </c>
+      <c r="Y76" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S76,2))</f>
+        <v>8</v>
+      </c>
+      <c r="Z76" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T76,2))</f>
+        <v>22</v>
+      </c>
+      <c r="AA76" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U76,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB76" s="1" t="n">
+        <f aca="false">IF(W76=0,IF(X76=0,IF(Y76=0,IF(Z76=0,IF(AA76=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC76" s="1" t="n">
+        <f aca="false">IF(AA76=0,IF(Z76=0,IF(Y76=0,IF(X76=0,IF(W76=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD76" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC76*16)+AB76,2),",")</f>
+        <v>0x41,</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0"/>
@@ -5011,6 +7428,38 @@
       <c r="V77" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q77,", ",R77,", ",S77,", ",T77,", ",U77,", /* ASCII ",N77," (",O77,"), character: ",P77," */")</f>
         <v>    0x00, 0x42, 0x7E, 0x02, 0x00, /* ASCII 108 (0x6C), character: 'l' */</v>
+      </c>
+      <c r="W77" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q77,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X77" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R77,2))</f>
+        <v>66</v>
+      </c>
+      <c r="Y77" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S77,2))</f>
+        <v>126</v>
+      </c>
+      <c r="Z77" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T77,2))</f>
+        <v>2</v>
+      </c>
+      <c r="AA77" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U77,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB77" s="1" t="n">
+        <f aca="false">IF(W77=0,IF(X77=0,IF(Y77=0,IF(Z77=0,IF(AA77=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC77" s="1" t="n">
+        <f aca="false">IF(AA77=0,IF(Z77=0,IF(Y77=0,IF(X77=0,IF(W77=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD77" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC77*16)+AB77,2),",")</f>
+        <v>0x41,</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5065,6 +7514,38 @@
         <f aca="false">CONCATENATE("    ",Q78,", ",R78,", ",S78,", ",T78,", ",U78,", /* ASCII ",N78," (",O78,"), character: ",P78," */")</f>
         <v>    0x1E, 0x10, 0x0E, 0x10, 0x0E, /* ASCII 109 (0x6D), character: 'm' */</v>
       </c>
+      <c r="W78" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q78,2))</f>
+        <v>30</v>
+      </c>
+      <c r="X78" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R78,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Y78" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S78,2))</f>
+        <v>14</v>
+      </c>
+      <c r="Z78" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T78,2))</f>
+        <v>16</v>
+      </c>
+      <c r="AA78" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U78,2))</f>
+        <v>14</v>
+      </c>
+      <c r="AB78" s="1" t="n">
+        <f aca="false">IF(W78=0,IF(X78=0,IF(Y78=0,IF(Z78=0,IF(AA78=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC78" s="1" t="n">
+        <f aca="false">IF(AA78=0,IF(Z78=0,IF(Y78=0,IF(X78=0,IF(W78=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD78" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC78*16)+AB78,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0"/>
@@ -5132,6 +7613,38 @@
         <f aca="false">CONCATENATE("    ",Q79,", ",R79,", ",S79,", ",T79,", ",U79,", /* ASCII ",N79," (",O79,"), character: ",P79," */")</f>
         <v>    0x1E, 0x10, 0x10, 0x0E, 0x00, /* ASCII 110 (0x6E), character: 'n' */</v>
       </c>
+      <c r="W79" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q79,2))</f>
+        <v>30</v>
+      </c>
+      <c r="X79" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R79,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Y79" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S79,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Z79" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T79,2))</f>
+        <v>14</v>
+      </c>
+      <c r="AA79" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U79,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB79" s="1" t="n">
+        <f aca="false">IF(W79=0,IF(X79=0,IF(Y79=0,IF(Z79=0,IF(AA79=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC79" s="1" t="n">
+        <f aca="false">IF(AA79=0,IF(Z79=0,IF(Y79=0,IF(X79=0,IF(W79=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD79" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC79*16)+AB79,2),",")</f>
+        <v>0x40,</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="n">
@@ -5201,6 +7714,38 @@
       <c r="V80" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q80,", ",R80,", ",S80,", ",T80,", ",U80,", /* ASCII ",N80," (",O80,"), character: ",P80," */")</f>
         <v>    0x0C, 0x12, 0x12, 0x0C, 0x00, /* ASCII 111 (0x6F), character: 'o' */</v>
+      </c>
+      <c r="W80" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q80,2))</f>
+        <v>12</v>
+      </c>
+      <c r="X80" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R80,2))</f>
+        <v>18</v>
+      </c>
+      <c r="Y80" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S80,2))</f>
+        <v>18</v>
+      </c>
+      <c r="Z80" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T80,2))</f>
+        <v>12</v>
+      </c>
+      <c r="AA80" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U80,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB80" s="1" t="n">
+        <f aca="false">IF(W80=0,IF(X80=0,IF(Y80=0,IF(Z80=0,IF(AA80=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC80" s="1" t="n">
+        <f aca="false">IF(AA80=0,IF(Z80=0,IF(Y80=0,IF(X80=0,IF(W80=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD80" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC80*16)+AB80,2),",")</f>
+        <v>0x40,</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5263,6 +7808,38 @@
         <f aca="false">CONCATENATE("    ",Q81,", ",R81,", ",S81,", ",T81,", ",U81,", /* ASCII ",N81," (",O81,"), character: ",P81," */")</f>
         <v>    0x00, 0x3F, 0x24, 0x24, 0x18, /* ASCII 112 (0x70), character: 'p' */</v>
       </c>
+      <c r="W81" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q81,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X81" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R81,2))</f>
+        <v>63</v>
+      </c>
+      <c r="Y81" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S81,2))</f>
+        <v>36</v>
+      </c>
+      <c r="Z81" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T81,2))</f>
+        <v>36</v>
+      </c>
+      <c r="AA81" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U81,2))</f>
+        <v>24</v>
+      </c>
+      <c r="AB81" s="1" t="n">
+        <f aca="false">IF(W81=0,IF(X81=0,IF(Y81=0,IF(Z81=0,IF(AA81=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC81" s="1" t="n">
+        <f aca="false">IF(AA81=0,IF(Z81=0,IF(Y81=0,IF(X81=0,IF(W81=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD81" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC81*16)+AB81,2),",")</f>
+        <v>0x51,</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0"/>
@@ -5323,6 +7900,38 @@
       <c r="V82" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q82,", ",R82,", ",S82,", ",T82,", ",U82,", /* ASCII ",N82," (",O82,"), character: ",P82," */")</f>
         <v>    0x18, 0x24, 0x24, 0x3F, 0x00, /* ASCII 113 (0x71), character: 'q' */</v>
+      </c>
+      <c r="W82" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q82,2))</f>
+        <v>24</v>
+      </c>
+      <c r="X82" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R82,2))</f>
+        <v>36</v>
+      </c>
+      <c r="Y82" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S82,2))</f>
+        <v>36</v>
+      </c>
+      <c r="Z82" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T82,2))</f>
+        <v>63</v>
+      </c>
+      <c r="AA82" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U82,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB82" s="1" t="n">
+        <f aca="false">IF(W82=0,IF(X82=0,IF(Y82=0,IF(Z82=0,IF(AA82=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC82" s="1" t="n">
+        <f aca="false">IF(AA82=0,IF(Z82=0,IF(Y82=0,IF(X82=0,IF(W82=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD82" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC82*16)+AB82,2),",")</f>
+        <v>0x40,</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5383,6 +7992,38 @@
         <f aca="false">CONCATENATE("    ",Q83,", ",R83,", ",S83,", ",T83,", ",U83,", /* ASCII ",N83," (",O83,"), character: ",P83," */")</f>
         <v>    0x1E, 0x08, 0x10, 0x08, 0x00, /* ASCII 114 (0x72), character: 'r' */</v>
       </c>
+      <c r="W83" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q83,2))</f>
+        <v>30</v>
+      </c>
+      <c r="X83" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R83,2))</f>
+        <v>8</v>
+      </c>
+      <c r="Y83" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S83,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Z83" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T83,2))</f>
+        <v>8</v>
+      </c>
+      <c r="AA83" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U83,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB83" s="1" t="n">
+        <f aca="false">IF(W83=0,IF(X83=0,IF(Y83=0,IF(Z83=0,IF(AA83=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC83" s="1" t="n">
+        <f aca="false">IF(AA83=0,IF(Z83=0,IF(Y83=0,IF(X83=0,IF(W83=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD83" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC83*16)+AB83,2),",")</f>
+        <v>0x40,</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0"/>
@@ -5441,6 +8082,38 @@
       <c r="V84" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q84,", ",R84,", ",S84,", ",T84,", ",U84,", /* ASCII ",N84," (",O84,"), character: ",P84," */")</f>
         <v>    0x12, 0x2A, 0x2A, 0x24, 0x00, /* ASCII 115 (0x73), character: 's' */</v>
+      </c>
+      <c r="W84" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q84,2))</f>
+        <v>18</v>
+      </c>
+      <c r="X84" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R84,2))</f>
+        <v>42</v>
+      </c>
+      <c r="Y84" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S84,2))</f>
+        <v>42</v>
+      </c>
+      <c r="Z84" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T84,2))</f>
+        <v>36</v>
+      </c>
+      <c r="AA84" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U84,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB84" s="1" t="n">
+        <f aca="false">IF(W84=0,IF(X84=0,IF(Y84=0,IF(Z84=0,IF(AA84=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC84" s="1" t="n">
+        <f aca="false">IF(AA84=0,IF(Z84=0,IF(Y84=0,IF(X84=0,IF(W84=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD84" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC84*16)+AB84,2),",")</f>
+        <v>0x40,</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5498,6 +8171,38 @@
         <f aca="false">CONCATENATE("    ",Q85,", ",R85,", ",S85,", ",T85,", ",U85,", /* ASCII ",N85," (",O85,"), character: ",P85," */")</f>
         <v>    0x10, 0x3E, 0x11, 0x02, 0x00, /* ASCII 116 (0x74), character: 't' */</v>
       </c>
+      <c r="W85" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q85,2))</f>
+        <v>16</v>
+      </c>
+      <c r="X85" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R85,2))</f>
+        <v>62</v>
+      </c>
+      <c r="Y85" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S85,2))</f>
+        <v>17</v>
+      </c>
+      <c r="Z85" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T85,2))</f>
+        <v>2</v>
+      </c>
+      <c r="AA85" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U85,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB85" s="1" t="n">
+        <f aca="false">IF(W85=0,IF(X85=0,IF(Y85=0,IF(Z85=0,IF(AA85=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC85" s="1" t="n">
+        <f aca="false">IF(AA85=0,IF(Z85=0,IF(Y85=0,IF(X85=0,IF(W85=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD85" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC85*16)+AB85,2),",")</f>
+        <v>0x40,</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0"/>
@@ -5554,6 +8259,38 @@
         <f aca="false">CONCATENATE("    ",Q86,", ",R86,", ",S86,", ",T86,", ",U86,", /* ASCII ",N86," (",O86,"), character: ",P86," */")</f>
         <v>    0x1C, 0x02, 0x02, 0x1C, 0x00, /* ASCII 117 (0x75), character: 'u' */</v>
       </c>
+      <c r="W86" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q86,2))</f>
+        <v>28</v>
+      </c>
+      <c r="X86" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R86,2))</f>
+        <v>2</v>
+      </c>
+      <c r="Y86" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S86,2))</f>
+        <v>2</v>
+      </c>
+      <c r="Z86" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T86,2))</f>
+        <v>28</v>
+      </c>
+      <c r="AA86" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U86,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB86" s="1" t="n">
+        <f aca="false">IF(W86=0,IF(X86=0,IF(Y86=0,IF(Z86=0,IF(AA86=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC86" s="1" t="n">
+        <f aca="false">IF(AA86=0,IF(Z86=0,IF(Y86=0,IF(X86=0,IF(W86=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD86" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC86*16)+AB86,2),",")</f>
+        <v>0x40,</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0"/>
@@ -5610,6 +8347,38 @@
         <f aca="false">CONCATENATE("    ",Q87,", ",R87,", ",S87,", ",T87,", ",U87,", /* ASCII ",N87," (",O87,"), character: ",P87," */")</f>
         <v>    0x18, 0x04, 0x02, 0x04, 0x18, /* ASCII 118 (0x76), character: 'v' */</v>
       </c>
+      <c r="W87" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q87,2))</f>
+        <v>24</v>
+      </c>
+      <c r="X87" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R87,2))</f>
+        <v>4</v>
+      </c>
+      <c r="Y87" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S87,2))</f>
+        <v>2</v>
+      </c>
+      <c r="Z87" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T87,2))</f>
+        <v>4</v>
+      </c>
+      <c r="AA87" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U87,2))</f>
+        <v>24</v>
+      </c>
+      <c r="AB87" s="1" t="n">
+        <f aca="false">IF(W87=0,IF(X87=0,IF(Y87=0,IF(Z87=0,IF(AA87=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC87" s="1" t="n">
+        <f aca="false">IF(AA87=0,IF(Z87=0,IF(Y87=0,IF(X87=0,IF(W87=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD87" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC87*16)+AB87,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0"/>
@@ -5677,6 +8446,38 @@
       <c r="V88" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q88,", ",R88,", ",S88,", ",T88,", ",U88,", /* ASCII ",N88," (",O88,"), character: ",P88," */")</f>
         <v>    0x1C, 0x02, 0x1C, 0x02, 0x1C, /* ASCII 119 (0x77), character: 'w' */</v>
+      </c>
+      <c r="W88" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q88,2))</f>
+        <v>28</v>
+      </c>
+      <c r="X88" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R88,2))</f>
+        <v>2</v>
+      </c>
+      <c r="Y88" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S88,2))</f>
+        <v>28</v>
+      </c>
+      <c r="Z88" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T88,2))</f>
+        <v>2</v>
+      </c>
+      <c r="AA88" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U88,2))</f>
+        <v>28</v>
+      </c>
+      <c r="AB88" s="1" t="n">
+        <f aca="false">IF(W88=0,IF(X88=0,IF(Y88=0,IF(Z88=0,IF(AA88=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC88" s="1" t="n">
+        <f aca="false">IF(AA88=0,IF(Z88=0,IF(Y88=0,IF(X88=0,IF(W88=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD88" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC88*16)+AB88,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5731,6 +8532,38 @@
         <f aca="false">CONCATENATE("    ",Q89,", ",R89,", ",S89,", ",T89,", ",U89,", /* ASCII ",N89," (",O89,"), character: ",P89," */")</f>
         <v>    0x22, 0x14, 0x08, 0x14, 0x22, /* ASCII 120 (0x78), character: 'x' */</v>
       </c>
+      <c r="W89" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q89,2))</f>
+        <v>34</v>
+      </c>
+      <c r="X89" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R89,2))</f>
+        <v>20</v>
+      </c>
+      <c r="Y89" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S89,2))</f>
+        <v>8</v>
+      </c>
+      <c r="Z89" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T89,2))</f>
+        <v>20</v>
+      </c>
+      <c r="AA89" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U89,2))</f>
+        <v>34</v>
+      </c>
+      <c r="AB89" s="1" t="n">
+        <f aca="false">IF(W89=0,IF(X89=0,IF(Y89=0,IF(Z89=0,IF(AA89=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC89" s="1" t="n">
+        <f aca="false">IF(AA89=0,IF(Z89=0,IF(Y89=0,IF(X89=0,IF(W89=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD89" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC89*16)+AB89,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0"/>
@@ -5798,6 +8631,38 @@
         <f aca="false">CONCATENATE("    ",Q90,", ",R90,", ",S90,", ",T90,", ",U90,", /* ASCII ",N90," (",O90,"), character: ",P90," */")</f>
         <v>    0x39, 0x05, 0x05, 0x3E, 0x00, /* ASCII 121 (0x79), character: 'y' */</v>
       </c>
+      <c r="W90" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q90,2))</f>
+        <v>57</v>
+      </c>
+      <c r="X90" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R90,2))</f>
+        <v>5</v>
+      </c>
+      <c r="Y90" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S90,2))</f>
+        <v>5</v>
+      </c>
+      <c r="Z90" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T90,2))</f>
+        <v>62</v>
+      </c>
+      <c r="AA90" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U90,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB90" s="1" t="n">
+        <f aca="false">IF(W90=0,IF(X90=0,IF(Y90=0,IF(Z90=0,IF(AA90=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC90" s="1" t="n">
+        <f aca="false">IF(AA90=0,IF(Z90=0,IF(Y90=0,IF(X90=0,IF(W90=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD90" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC90*16)+AB90,2),",")</f>
+        <v>0x40,</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="n">
@@ -5867,6 +8732,38 @@
       <c r="V91" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q91,", ",R91,", ",S91,", ",T91,", ",U91,", /* ASCII ",N91," (",O91,"), character: ",P91," */")</f>
         <v>    0x00, 0x26, 0x2A, 0x32, 0x00, /* ASCII 122 (0x7A), character: 'z' */</v>
+      </c>
+      <c r="W91" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q91,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X91" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R91,2))</f>
+        <v>38</v>
+      </c>
+      <c r="Y91" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S91,2))</f>
+        <v>42</v>
+      </c>
+      <c r="Z91" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T91,2))</f>
+        <v>50</v>
+      </c>
+      <c r="AA91" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U91,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB91" s="1" t="n">
+        <f aca="false">IF(W91=0,IF(X91=0,IF(Y91=0,IF(Z91=0,IF(AA91=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC91" s="1" t="n">
+        <f aca="false">IF(AA91=0,IF(Z91=0,IF(Y91=0,IF(X91=0,IF(W91=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD91" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC91*16)+AB91,2),",")</f>
+        <v>0x41,</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5929,6 +8826,38 @@
         <f aca="false">CONCATENATE("    ",Q92,", ",R92,", ",S92,", ",T92,", ",U92,", /* ASCII ",N92," (",O92,"), character: ",P92," */")</f>
         <v>    0x00, 0x10, 0x7C, 0x82, 0x00, /* ASCII 123 (0x7B), character: '{' */</v>
       </c>
+      <c r="W92" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q92,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X92" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R92,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Y92" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S92,2))</f>
+        <v>124</v>
+      </c>
+      <c r="Z92" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T92,2))</f>
+        <v>130</v>
+      </c>
+      <c r="AA92" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U92,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB92" s="1" t="n">
+        <f aca="false">IF(W92=0,IF(X92=0,IF(Y92=0,IF(Z92=0,IF(AA92=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC92" s="1" t="n">
+        <f aca="false">IF(AA92=0,IF(Z92=0,IF(Y92=0,IF(X92=0,IF(W92=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD92" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC92*16)+AB92,2),",")</f>
+        <v>0x41,</v>
+      </c>
     </row>
     <row r="93" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0"/>
@@ -5990,6 +8919,38 @@
         <f aca="false">CONCATENATE("    ",Q93,", ",R93,", ",S93,", ",T93,", ",U93,", /* ASCII ",N93," (",O93,"), character: ",P93," */")</f>
         <v>    0x00, 0x00, 0xFF, 0x00, 0x00, /* ASCII 124 (0x7C), character: '|' */</v>
       </c>
+      <c r="W93" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q93,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X93" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R93,2))</f>
+        <v>0</v>
+      </c>
+      <c r="Y93" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S93,2))</f>
+        <v>255</v>
+      </c>
+      <c r="Z93" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T93,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AA93" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U93,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB93" s="1" t="n">
+        <f aca="false">IF(W93=0,IF(X93=0,IF(Y93=0,IF(Z93=0,IF(AA93=0,0,4),3),2),1),0)</f>
+        <v>2</v>
+      </c>
+      <c r="AC93" s="1" t="n">
+        <f aca="false">IF(AA93=0,IF(Z93=0,IF(Y93=0,IF(X93=0,IF(W93=0,5,1),2),3),4),5)</f>
+        <v>3</v>
+      </c>
+      <c r="AD93" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC93*16)+AB93,2),",")</f>
+        <v>0x32,</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0"/>
@@ -6051,6 +9012,38 @@
         <f aca="false">CONCATENATE("    ",Q94,", ",R94,", ",S94,", ",T94,", ",U94,", /* ASCII ",N94," (",O94,"), character: ",P94," */")</f>
         <v>    0x00, 0x82, 0x7C, 0x10, 0x00, /* ASCII 125 (0x7D), character: '}' */</v>
       </c>
+      <c r="W94" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q94,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X94" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R94,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Y94" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S94,2))</f>
+        <v>124</v>
+      </c>
+      <c r="Z94" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T94,2))</f>
+        <v>16</v>
+      </c>
+      <c r="AA94" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U94,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB94" s="1" t="n">
+        <f aca="false">IF(W94=0,IF(X94=0,IF(Y94=0,IF(Z94=0,IF(AA94=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC94" s="1" t="n">
+        <f aca="false">IF(AA94=0,IF(Z94=0,IF(Y94=0,IF(X94=0,IF(W94=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD94" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC94*16)+AB94,2),",")</f>
+        <v>0x41,</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0"/>
@@ -6111,6 +9104,38 @@
       <c r="V95" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q95,", ",R95,", ",S95,", ",T95,", ",U95,", /* ASCII ",N95," (",O95,"), character: ",P95," */")</f>
         <v>    0x10, 0x20, 0x10, 0x08, 0x10, /* ASCII 126 (0x7E), character: '~' */</v>
+      </c>
+      <c r="W95" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q95,2))</f>
+        <v>16</v>
+      </c>
+      <c r="X95" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R95,2))</f>
+        <v>32</v>
+      </c>
+      <c r="Y95" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S95,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Z95" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T95,2))</f>
+        <v>8</v>
+      </c>
+      <c r="AA95" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U95,2))</f>
+        <v>16</v>
+      </c>
+      <c r="AB95" s="1" t="n">
+        <f aca="false">IF(W95=0,IF(X95=0,IF(Y95=0,IF(Z95=0,IF(AA95=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC95" s="1" t="n">
+        <f aca="false">IF(AA95=0,IF(Z95=0,IF(Y95=0,IF(X95=0,IF(W95=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD95" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC95*16)+AB95,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6170,6 +9195,38 @@
         <f aca="false">CONCATENATE("    ",Q96,", ",R96,", ",S96,", ",T96,", ",U96,", /* ASCII ",N96," (",O96,"), character: ",P96," */")</f>
         <v>    0x00, 0xE0, 0xA0, 0xE0, 0x00, /* ASCII 127 (0x7F), character: '' */</v>
       </c>
+      <c r="W96" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q96,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X96" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R96,2))</f>
+        <v>224</v>
+      </c>
+      <c r="Y96" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S96,2))</f>
+        <v>160</v>
+      </c>
+      <c r="Z96" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T96,2))</f>
+        <v>224</v>
+      </c>
+      <c r="AA96" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U96,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB96" s="1" t="n">
+        <f aca="false">IF(W96=0,IF(X96=0,IF(Y96=0,IF(Z96=0,IF(AA96=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC96" s="1" t="n">
+        <f aca="false">IF(AA96=0,IF(Z96=0,IF(Y96=0,IF(X96=0,IF(W96=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD96" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC96*16)+AB96,2),",")</f>
+        <v>0x41,</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0"/>
@@ -6227,6 +9284,38 @@
       <c r="V97" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q97,", ",R97,", ",S97,", ",T97,", ",U97,", /* ASCII ",N97," (",O97,"), character: ",P97," */")</f>
         <v>    0x28, 0x7C, 0xAA, 0x82, 0x44, /* ASCII 128 (0x80), character: '€' */</v>
+      </c>
+      <c r="W97" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q97,2))</f>
+        <v>40</v>
+      </c>
+      <c r="X97" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R97,2))</f>
+        <v>124</v>
+      </c>
+      <c r="Y97" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S97,2))</f>
+        <v>170</v>
+      </c>
+      <c r="Z97" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T97,2))</f>
+        <v>130</v>
+      </c>
+      <c r="AA97" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U97,2))</f>
+        <v>68</v>
+      </c>
+      <c r="AB97" s="1" t="n">
+        <f aca="false">IF(W97=0,IF(X97=0,IF(Y97=0,IF(Z97=0,IF(AA97=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC97" s="1" t="n">
+        <f aca="false">IF(AA97=0,IF(Z97=0,IF(Y97=0,IF(X97=0,IF(W97=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD97" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC97*16)+AB97,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12217,9 +15306,7 @@
         <f aca="false">D$3</f>
         <v>7</v>
       </c>
-      <c r="E355" s="0" t="n">
-        <v>1</v>
-      </c>
+      <c r="E355" s="0"/>
       <c r="F355" s="0" t="n">
         <v>1</v>
       </c>
@@ -12229,12 +15316,10 @@
       <c r="H355" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I355" s="0" t="n">
-        <v>1</v>
-      </c>
+      <c r="I355" s="0"/>
       <c r="J355" s="2" t="str">
         <f aca="false">E363</f>
-        <v>0xFE</v>
+        <v>0x7C</v>
       </c>
       <c r="L355" s="0"/>
       <c r="Q355" s="0"/>
@@ -12340,7 +15425,7 @@
       </c>
       <c r="J359" s="2" t="str">
         <f aca="false">I363</f>
-        <v>0xFA</v>
+        <v>0x7A</v>
       </c>
       <c r="L359" s="0"/>
       <c r="Q359" s="0"/>
@@ -12372,9 +15457,7 @@
         <f aca="false">D$9</f>
         <v>1</v>
       </c>
-      <c r="E361" s="0" t="n">
-        <v>1</v>
-      </c>
+      <c r="E361" s="0"/>
       <c r="F361" s="0" t="n">
         <v>1</v>
       </c>
@@ -12415,7 +15498,7 @@
       <c r="D363" s="0"/>
       <c r="E363" s="2" t="str">
         <f aca="false">CONCATENATE("0x",DEC2HEX(SUM(IF(E362=1,2^$D362,0),IF(E361=1,2^$D361,0),IF(E360=1,2^$D360,0),IF(E359=1,2^$D359,0),IF(E358=1,2^$D358,0),IF(E357=1,2^$D357,0),IF(E356=1,2^$D356,0),IF(E355=1,2^$D355,0)),2))</f>
-        <v>0xFE</v>
+        <v>0x7C</v>
       </c>
       <c r="F363" s="2" t="str">
         <f aca="false">CONCATENATE("0x",DEC2HEX(SUM(IF(F362=1,2^$D362,0),IF(F361=1,2^$D361,0),IF(F360=1,2^$D360,0),IF(F359=1,2^$D359,0),IF(F358=1,2^$D358,0),IF(F357=1,2^$D357,0),IF(F356=1,2^$D356,0),IF(F355=1,2^$D355,0)),2))</f>
@@ -12431,7 +15514,7 @@
       </c>
       <c r="I363" s="2" t="str">
         <f aca="false">CONCATENATE("0x",DEC2HEX(SUM(IF(I362=1,2^$D362,0),IF(I361=1,2^$D361,0),IF(I360=1,2^$D360,0),IF(I359=1,2^$D359,0),IF(I358=1,2^$D358,0),IF(I357=1,2^$D357,0),IF(I356=1,2^$D356,0),IF(I355=1,2^$D355,0)),2))</f>
-        <v>0xFA</v>
+        <v>0x7A</v>
       </c>
       <c r="J363" s="0"/>
       <c r="L363" s="0"/>
@@ -28715,7 +31798,7 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="str">
         <f aca="false">Sheet1!V2</f>
-        <v>    0x00, 0xFB, 0xFB, 0x00, 0x00, /* ASCII 33 (0x21), character: '!' */</v>
+        <v>    0x00, 0x60, 0xFA, 0x60, 0x00, /* ASCII 33 (0x21), character: '!' */</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28901,7 +31984,7 @@
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="str">
         <f aca="false">Sheet1!V33</f>
-        <v>    0xFE, 0x82, 0xBA, 0xAA, 0xFA, /* ASCII 64 (0x40), character: '@' */</v>
+        <v>    0x7C, 0x82, 0xBA, 0xAA, 0x7A, /* ASCII 64 (0x40), character: '@' */</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Revert "commit before I revert"
This reverts commit 419d4417a7e27c2ab40ffa7b2de50b0e5587a0b5.
</commit_message>
<xml_diff>
--- a/CharCreator.xlsx
+++ b/CharCreator.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -93,12 +93,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -110,7 +116,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -134,6 +140,12 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -153,22 +165,19 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Lit" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Lit1" xfId="21" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <font>
-        <sz val="10"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
 </styleSheet>
@@ -179,10 +188,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AD1067"/>
+  <dimension ref="A1:V1067"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A337" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V364" activeCellId="0" sqref="V364"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1028" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L1059" activeCellId="0" sqref="L1059"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -196,10 +205,8 @@
     <col collapsed="false" hidden="false" max="14" min="14" style="1" width="6.57142857142857"/>
     <col collapsed="false" hidden="false" max="16" min="15" style="1" width="9.14285714285714"/>
     <col collapsed="false" hidden="false" max="21" min="17" style="1" width="6.57142857142857"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="21.015306122449"/>
-    <col collapsed="false" hidden="false" max="27" min="23" style="1" width="4.53571428571429"/>
-    <col collapsed="false" hidden="false" max="29" min="28" style="1" width="2.56632653061224"/>
-    <col collapsed="false" hidden="false" max="256" min="30" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="84.280612244898"/>
+    <col collapsed="false" hidden="false" max="256" min="23" style="1" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
@@ -261,38 +268,6 @@
         <f aca="false">CONCATENATE("    ",Q1,", ",R1,", ",S1,", ",T1,", ",U1,", /* ASCII ",N1," (",O1,"), character: ",P1," */")</f>
         <v>    0x00, 0x00, 0x00, 0x00, 0x00, /* ASCII 32 (0x20), character: ' ' */</v>
       </c>
-      <c r="W1" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q1,2))</f>
-        <v>0</v>
-      </c>
-      <c r="X1" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R1,2))</f>
-        <v>0</v>
-      </c>
-      <c r="Y1" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S1,2))</f>
-        <v>0</v>
-      </c>
-      <c r="Z1" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T1,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AA1" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U1,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB1" s="1" t="n">
-        <f aca="false">IF(W1=0,IF(X1=0,IF(Y1=0,IF(Z1=0,IF(AA1=0,1,4),3),2),1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="AC1" s="1" t="n">
-        <f aca="false">IF(AA1=0,IF(Z1=0,IF(Y1=0,IF(X1=0,IF(W1=0,3,1),2),3),4),5)</f>
-        <v>3</v>
-      </c>
-      <c r="AD1" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC1*16)+AB1,2),",")</f>
-        <v>0x31,</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
@@ -347,15 +322,15 @@
       </c>
       <c r="R2" s="2" t="str">
         <f aca="false">INDEX(F:F,$M2+8,1)</f>
-        <v>0x60</v>
+        <v>0xFB</v>
       </c>
       <c r="S2" s="2" t="str">
         <f aca="false">INDEX(G:G,$M2+8,1)</f>
-        <v>0xFA</v>
+        <v>0xFB</v>
       </c>
       <c r="T2" s="2" t="str">
         <f aca="false">INDEX(H:H,$M2+8,1)</f>
-        <v>0x60</v>
+        <v>0x00</v>
       </c>
       <c r="U2" s="2" t="str">
         <f aca="false">INDEX(I:I,$M2+8,1)</f>
@@ -363,39 +338,7 @@
       </c>
       <c r="V2" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q2,", ",R2,", ",S2,", ",T2,", ",U2,", /* ASCII ",N2," (",O2,"), character: ",P2," */")</f>
-        <v>    0x00, 0x60, 0xFA, 0x60, 0x00, /* ASCII 33 (0x21), character: '!' */</v>
-      </c>
-      <c r="W2" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q2,2))</f>
-        <v>0</v>
-      </c>
-      <c r="X2" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R2,2))</f>
-        <v>96</v>
-      </c>
-      <c r="Y2" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S2,2))</f>
-        <v>250</v>
-      </c>
-      <c r="Z2" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T2,2))</f>
-        <v>96</v>
-      </c>
-      <c r="AA2" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U2,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB2" s="1" t="n">
-        <f aca="false">IF(W2=0,IF(X2=0,IF(Y2=0,IF(Z2=0,IF(AA2=0,0,4),3),2),1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="AC2" s="1" t="n">
-        <f aca="false">IF(AA2=0,IF(Z2=0,IF(Y2=0,IF(X2=0,IF(W2=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD2" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC2*16)+AB2,2),",")</f>
-        <v>0x41,</v>
+        <v>    0x00, 0xFB, 0xFB, 0x00, 0x00, /* ASCII 33 (0x21), character: '!' */</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -470,38 +413,6 @@
         <f aca="false">CONCATENATE("    ",Q3,", ",R3,", ",S3,", ",T3,", ",U3,", /* ASCII ",N3," (",O3,"), character: ",P3," */")</f>
         <v>    0x20, 0xC0, 0x00, 0x20, 0xC0, /* ASCII 34 (0x22), character: '"' */</v>
       </c>
-      <c r="W3" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q3,2))</f>
-        <v>32</v>
-      </c>
-      <c r="X3" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R3,2))</f>
-        <v>192</v>
-      </c>
-      <c r="Y3" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S3,2))</f>
-        <v>0</v>
-      </c>
-      <c r="Z3" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T3,2))</f>
-        <v>32</v>
-      </c>
-      <c r="AA3" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U3,2))</f>
-        <v>192</v>
-      </c>
-      <c r="AB3" s="1" t="n">
-        <f aca="false">IF(W3=0,IF(X3=0,IF(Y3=0,IF(Z3=0,IF(AA3=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC3" s="1" t="n">
-        <f aca="false">IF(AA3=0,IF(Z3=0,IF(Y3=0,IF(X3=0,IF(W3=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD3" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC3*16)+AB3,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
@@ -561,38 +472,6 @@
         <f aca="false">CONCATENATE("    ",Q4,", ",R4,", ",S4,", ",T4,", ",U4,", /* ASCII ",N4," (",O4,"), character: ",P4," */")</f>
         <v>    0x28, 0x7C, 0x28, 0x7C, 0x28, /* ASCII 35 (0x23), character: '#' */</v>
       </c>
-      <c r="W4" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q4,2))</f>
-        <v>40</v>
-      </c>
-      <c r="X4" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R4,2))</f>
-        <v>124</v>
-      </c>
-      <c r="Y4" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S4,2))</f>
-        <v>40</v>
-      </c>
-      <c r="Z4" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T4,2))</f>
-        <v>124</v>
-      </c>
-      <c r="AA4" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U4,2))</f>
-        <v>40</v>
-      </c>
-      <c r="AB4" s="1" t="n">
-        <f aca="false">IF(W4=0,IF(X4=0,IF(Y4=0,IF(Z4=0,IF(AA4=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC4" s="1" t="n">
-        <f aca="false">IF(AA4=0,IF(Z4=0,IF(Y4=0,IF(X4=0,IF(W4=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD4" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC4*16)+AB4,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0"/>
@@ -652,38 +531,6 @@
         <f aca="false">CONCATENATE("    ",Q5,", ",R5,", ",S5,", ",T5,", ",U5,", /* ASCII ",N5," (",O5,"), character: ",P5," */")</f>
         <v>    0x24, 0x54, 0xFE, 0x54, 0x48, /* ASCII 36 (0x24), character: '$' */</v>
       </c>
-      <c r="W5" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q5,2))</f>
-        <v>36</v>
-      </c>
-      <c r="X5" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R5,2))</f>
-        <v>84</v>
-      </c>
-      <c r="Y5" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S5,2))</f>
-        <v>254</v>
-      </c>
-      <c r="Z5" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T5,2))</f>
-        <v>84</v>
-      </c>
-      <c r="AA5" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U5,2))</f>
-        <v>72</v>
-      </c>
-      <c r="AB5" s="1" t="n">
-        <f aca="false">IF(W5=0,IF(X5=0,IF(Y5=0,IF(Z5=0,IF(AA5=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC5" s="1" t="n">
-        <f aca="false">IF(AA5=0,IF(Z5=0,IF(Y5=0,IF(X5=0,IF(W5=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD5" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC5*16)+AB5,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0"/>
@@ -743,38 +590,6 @@
         <f aca="false">CONCATENATE("    ",Q6,", ",R6,", ",S6,", ",T6,", ",U6,", /* ASCII ",N6," (",O6,"), character: ",P6," */")</f>
         <v>    0x64, 0x68, 0x10, 0x2C, 0x4C, /* ASCII 37 (0x25), character: '%' */</v>
       </c>
-      <c r="W6" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q6,2))</f>
-        <v>100</v>
-      </c>
-      <c r="X6" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R6,2))</f>
-        <v>104</v>
-      </c>
-      <c r="Y6" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S6,2))</f>
-        <v>16</v>
-      </c>
-      <c r="Z6" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T6,2))</f>
-        <v>44</v>
-      </c>
-      <c r="AA6" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U6,2))</f>
-        <v>76</v>
-      </c>
-      <c r="AB6" s="1" t="n">
-        <f aca="false">IF(W6=0,IF(X6=0,IF(Y6=0,IF(Z6=0,IF(AA6=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC6" s="1" t="n">
-        <f aca="false">IF(AA6=0,IF(Z6=0,IF(Y6=0,IF(X6=0,IF(W6=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD6" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC6*16)+AB6,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0"/>
@@ -833,38 +648,6 @@
       <c r="V7" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q7,", ",R7,", ",S7,", ",T7,", ",U7,", /* ASCII ",N7," (",O7,"), character: ",P7," */")</f>
         <v>    0x34, 0x4A, 0x4A, 0x24, 0x0A, /* ASCII 38 (0x26), character: '&amp;' */</v>
-      </c>
-      <c r="W7" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q7,2))</f>
-        <v>52</v>
-      </c>
-      <c r="X7" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R7,2))</f>
-        <v>74</v>
-      </c>
-      <c r="Y7" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S7,2))</f>
-        <v>74</v>
-      </c>
-      <c r="Z7" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T7,2))</f>
-        <v>36</v>
-      </c>
-      <c r="AA7" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U7,2))</f>
-        <v>10</v>
-      </c>
-      <c r="AB7" s="1" t="n">
-        <f aca="false">IF(W7=0,IF(X7=0,IF(Y7=0,IF(Z7=0,IF(AA7=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC7" s="1" t="n">
-        <f aca="false">IF(AA7=0,IF(Z7=0,IF(Y7=0,IF(X7=0,IF(W7=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD7" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC7*16)+AB7,2),",")</f>
-        <v>0x50,</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -922,38 +705,6 @@
         <f aca="false">CONCATENATE("    ",Q8,", ",R8,", ",S8,", ",T8,", ",U8,", /* ASCII ",N8," (",O8,"), character: ",P8," */")</f>
         <v>    0x20, 0xC0, 0x00, 0x00, 0x00, /* ASCII 39 (0x27), character: ''' */</v>
       </c>
-      <c r="W8" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q8,2))</f>
-        <v>32</v>
-      </c>
-      <c r="X8" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R8,2))</f>
-        <v>192</v>
-      </c>
-      <c r="Y8" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S8,2))</f>
-        <v>0</v>
-      </c>
-      <c r="Z8" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T8,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AA8" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U8,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB8" s="1" t="n">
-        <f aca="false">IF(W8=0,IF(X8=0,IF(Y8=0,IF(Z8=0,IF(AA8=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC8" s="1" t="n">
-        <f aca="false">IF(AA8=0,IF(Z8=0,IF(Y8=0,IF(X8=0,IF(W8=0,5,1),2),3),4),5)</f>
-        <v>2</v>
-      </c>
-      <c r="AD8" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC8*16)+AB8,2),",")</f>
-        <v>0x20,</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0"/>
@@ -1010,38 +761,6 @@
         <f aca="false">CONCATENATE("    ",Q9,", ",R9,", ",S9,", ",T9,", ",U9,", /* ASCII ",N9," (",O9,"), character: ",P9," */")</f>
         <v>    0x00, 0x38, 0x44, 0x82, 0x00, /* ASCII 40 (0x28), character: '(' */</v>
       </c>
-      <c r="W9" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q9,2))</f>
-        <v>0</v>
-      </c>
-      <c r="X9" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R9,2))</f>
-        <v>56</v>
-      </c>
-      <c r="Y9" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S9,2))</f>
-        <v>68</v>
-      </c>
-      <c r="Z9" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T9,2))</f>
-        <v>130</v>
-      </c>
-      <c r="AA9" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U9,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB9" s="1" t="n">
-        <f aca="false">IF(W9=0,IF(X9=0,IF(Y9=0,IF(Z9=0,IF(AA9=0,0,4),3),2),1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="AC9" s="1" t="n">
-        <f aca="false">IF(AA9=0,IF(Z9=0,IF(Y9=0,IF(X9=0,IF(W9=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD9" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC9*16)+AB9,2),",")</f>
-        <v>0x41,</v>
-      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0"/>
@@ -1097,38 +816,6 @@
         <f aca="false">CONCATENATE("    ",Q10,", ",R10,", ",S10,", ",T10,", ",U10,", /* ASCII ",N10," (",O10,"), character: ",P10," */")</f>
         <v>    0x00, 0x82, 0x44, 0x38, 0x00, /* ASCII 41 (0x29), character: ')' */</v>
       </c>
-      <c r="W10" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q10,2))</f>
-        <v>0</v>
-      </c>
-      <c r="X10" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R10,2))</f>
-        <v>130</v>
-      </c>
-      <c r="Y10" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S10,2))</f>
-        <v>68</v>
-      </c>
-      <c r="Z10" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T10,2))</f>
-        <v>56</v>
-      </c>
-      <c r="AA10" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U10,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB10" s="1" t="n">
-        <f aca="false">IF(W10=0,IF(X10=0,IF(Y10=0,IF(Z10=0,IF(AA10=0,0,4),3),2),1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="AC10" s="1" t="n">
-        <f aca="false">IF(AA10=0,IF(Z10=0,IF(Y10=0,IF(X10=0,IF(W10=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD10" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC10*16)+AB10,2),",")</f>
-        <v>0x41,</v>
-      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0"/>
@@ -1196,38 +883,6 @@
       <c r="V11" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q11,", ",R11,", ",S11,", ",T11,", ",U11,", /* ASCII ",N11," (",O11,"), character: ",P11," */")</f>
         <v>    0x28, 0x10, 0x7C, 0x10, 0x28, /* ASCII 42 (0x2A), character: '*' */</v>
-      </c>
-      <c r="W11" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q11,2))</f>
-        <v>40</v>
-      </c>
-      <c r="X11" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R11,2))</f>
-        <v>16</v>
-      </c>
-      <c r="Y11" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S11,2))</f>
-        <v>124</v>
-      </c>
-      <c r="Z11" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T11,2))</f>
-        <v>16</v>
-      </c>
-      <c r="AA11" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U11,2))</f>
-        <v>40</v>
-      </c>
-      <c r="AB11" s="1" t="n">
-        <f aca="false">IF(W11=0,IF(X11=0,IF(Y11=0,IF(Z11=0,IF(AA11=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC11" s="1" t="n">
-        <f aca="false">IF(AA11=0,IF(Z11=0,IF(Y11=0,IF(X11=0,IF(W11=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD11" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC11*16)+AB11,2),",")</f>
-        <v>0x50,</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1282,38 +937,6 @@
         <f aca="false">CONCATENATE("    ",Q12,", ",R12,", ",S12,", ",T12,", ",U12,", /* ASCII ",N12," (",O12,"), character: ",P12," */")</f>
         <v>    0x10, 0x10, 0x7C, 0x10, 0x10, /* ASCII 43 (0x2B), character: '+' */</v>
       </c>
-      <c r="W12" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q12,2))</f>
-        <v>16</v>
-      </c>
-      <c r="X12" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R12,2))</f>
-        <v>16</v>
-      </c>
-      <c r="Y12" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S12,2))</f>
-        <v>124</v>
-      </c>
-      <c r="Z12" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T12,2))</f>
-        <v>16</v>
-      </c>
-      <c r="AA12" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U12,2))</f>
-        <v>16</v>
-      </c>
-      <c r="AB12" s="1" t="n">
-        <f aca="false">IF(W12=0,IF(X12=0,IF(Y12=0,IF(Z12=0,IF(AA12=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC12" s="1" t="n">
-        <f aca="false">IF(AA12=0,IF(Z12=0,IF(Y12=0,IF(X12=0,IF(W12=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD12" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC12*16)+AB12,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0"/>
@@ -1381,38 +1004,6 @@
         <f aca="false">CONCATENATE("    ",Q13,", ",R13,", ",S13,", ",T13,", ",U13,", /* ASCII ",N13," (",O13,"), character: ",P13," */")</f>
         <v>    0x00, 0x0D, 0x0E, 0x00, 0x00, /* ASCII 44 (0x2C), character: ',' */</v>
       </c>
-      <c r="W13" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q13,2))</f>
-        <v>0</v>
-      </c>
-      <c r="X13" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R13,2))</f>
-        <v>13</v>
-      </c>
-      <c r="Y13" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S13,2))</f>
-        <v>14</v>
-      </c>
-      <c r="Z13" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T13,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AA13" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U13,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB13" s="1" t="n">
-        <f aca="false">IF(W13=0,IF(X13=0,IF(Y13=0,IF(Z13=0,IF(AA13=0,0,4),3),2),1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="AC13" s="1" t="n">
-        <f aca="false">IF(AA13=0,IF(Z13=0,IF(Y13=0,IF(X13=0,IF(W13=0,5,1),2),3),4),5)</f>
-        <v>3</v>
-      </c>
-      <c r="AD13" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC13*16)+AB13,2),",")</f>
-        <v>0x31,</v>
-      </c>
     </row>
     <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
@@ -1432,7 +1023,9 @@
         <v>7</v>
       </c>
       <c r="E14" s="0"/>
-      <c r="F14" s="0"/>
+      <c r="F14" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="G14" s="2" t="n">
         <v>1</v>
       </c>
@@ -1482,38 +1075,6 @@
       <c r="V14" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q14,", ",R14,", ",S14,", ",T14,", ",U14,", /* ASCII ",N14," (",O14,"), character: ",P14," */")</f>
         <v>    0x10, 0x10, 0x10, 0x10, 0x00, /* ASCII 45 (0x2D), character: '-' */</v>
-      </c>
-      <c r="W14" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q14,2))</f>
-        <v>16</v>
-      </c>
-      <c r="X14" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R14,2))</f>
-        <v>16</v>
-      </c>
-      <c r="Y14" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S14,2))</f>
-        <v>16</v>
-      </c>
-      <c r="Z14" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T14,2))</f>
-        <v>16</v>
-      </c>
-      <c r="AA14" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U14,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB14" s="1" t="n">
-        <f aca="false">IF(W14=0,IF(X14=0,IF(Y14=0,IF(Z14=0,IF(AA14=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC14" s="1" t="n">
-        <f aca="false">IF(AA14=0,IF(Z14=0,IF(Y14=0,IF(X14=0,IF(W14=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD14" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC14*16)+AB14,2),",")</f>
-        <v>0x40,</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1531,13 +1092,11 @@
       <c r="G15" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H15" s="0" t="n">
-        <v>1</v>
-      </c>
+      <c r="H15" s="0"/>
       <c r="I15" s="0"/>
       <c r="J15" s="2" t="str">
         <f aca="false">F22</f>
-        <v>0x60</v>
+        <v>0xFB</v>
       </c>
       <c r="L15" s="0"/>
       <c r="M15" s="2" t="n">
@@ -1579,38 +1138,6 @@
       <c r="V15" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q15,", ",R15,", ",S15,", ",T15,", ",U15,", /* ASCII ",N15," (",O15,"), character: ",P15," */")</f>
         <v>    0x00, 0x06, 0x06, 0x00, 0x00, /* ASCII 46 (0x2E), character: '.' */</v>
-      </c>
-      <c r="W15" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q15,2))</f>
-        <v>0</v>
-      </c>
-      <c r="X15" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R15,2))</f>
-        <v>6</v>
-      </c>
-      <c r="Y15" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S15,2))</f>
-        <v>6</v>
-      </c>
-      <c r="Z15" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T15,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AA15" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U15,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB15" s="1" t="n">
-        <f aca="false">IF(W15=0,IF(X15=0,IF(Y15=0,IF(Z15=0,IF(AA15=0,0,4),3),2),1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="AC15" s="1" t="n">
-        <f aca="false">IF(AA15=0,IF(Z15=0,IF(Y15=0,IF(X15=0,IF(W15=0,5,1),2),3),4),5)</f>
-        <v>3</v>
-      </c>
-      <c r="AD15" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC15*16)+AB15,2),",")</f>
-        <v>0x31,</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1628,13 +1155,11 @@
       <c r="G16" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H16" s="0" t="n">
-        <v>1</v>
-      </c>
+      <c r="H16" s="0"/>
       <c r="I16" s="0"/>
       <c r="J16" s="2" t="str">
         <f aca="false">G22</f>
-        <v>0xFA</v>
+        <v>0xFB</v>
       </c>
       <c r="L16" s="0"/>
       <c r="M16" s="2" t="n">
@@ -1676,38 +1201,6 @@
       <c r="V16" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q16,", ",R16,", ",S16,", ",T16,", ",U16,", /* ASCII ",N16," (",O16,"), character: ",P16," */")</f>
         <v>    0x03, 0x0C, 0x30, 0xC0, 0x00, /* ASCII 47 (0x2F), character: '/' */</v>
-      </c>
-      <c r="W16" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q16,2))</f>
-        <v>3</v>
-      </c>
-      <c r="X16" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R16,2))</f>
-        <v>12</v>
-      </c>
-      <c r="Y16" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S16,2))</f>
-        <v>48</v>
-      </c>
-      <c r="Z16" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T16,2))</f>
-        <v>192</v>
-      </c>
-      <c r="AA16" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U16,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB16" s="1" t="n">
-        <f aca="false">IF(W16=0,IF(X16=0,IF(Y16=0,IF(Z16=0,IF(AA16=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC16" s="1" t="n">
-        <f aca="false">IF(AA16=0,IF(Z16=0,IF(Y16=0,IF(X16=0,IF(W16=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD16" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC16*16)+AB16,2),",")</f>
-        <v>0x40,</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1719,7 +1212,9 @@
         <v>4</v>
       </c>
       <c r="E17" s="0"/>
-      <c r="F17" s="0"/>
+      <c r="F17" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="G17" s="2" t="n">
         <v>1</v>
       </c>
@@ -1727,7 +1222,7 @@
       <c r="I17" s="0"/>
       <c r="J17" s="2" t="str">
         <f aca="false">H22</f>
-        <v>0x60</v>
+        <v>0x00</v>
       </c>
       <c r="L17" s="0"/>
       <c r="M17" s="2" t="n">
@@ -1769,38 +1264,6 @@
       <c r="V17" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q17,", ",R17,", ",S17,", ",T17,", ",U17,", /* ASCII ",N17," (",O17,"), character: ",P17," */")</f>
         <v>    0x7C, 0x8A, 0x92, 0xA2, 0x7C, /* ASCII 48 (0x30), character: '0' */</v>
-      </c>
-      <c r="W17" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q17,2))</f>
-        <v>124</v>
-      </c>
-      <c r="X17" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R17,2))</f>
-        <v>138</v>
-      </c>
-      <c r="Y17" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S17,2))</f>
-        <v>146</v>
-      </c>
-      <c r="Z17" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T17,2))</f>
-        <v>162</v>
-      </c>
-      <c r="AA17" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U17,2))</f>
-        <v>124</v>
-      </c>
-      <c r="AB17" s="1" t="n">
-        <f aca="false">IF(W17=0,IF(X17=0,IF(Y17=0,IF(Z17=0,IF(AA17=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC17" s="1" t="n">
-        <f aca="false">IF(AA17=0,IF(Z17=0,IF(Y17=0,IF(X17=0,IF(W17=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD17" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC17*16)+AB17,2),",")</f>
-        <v>0x50,</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1812,7 +1275,9 @@
         <v>3</v>
       </c>
       <c r="E18" s="0"/>
-      <c r="F18" s="0"/>
+      <c r="F18" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="G18" s="2" t="n">
         <v>1</v>
       </c>
@@ -1862,38 +1327,6 @@
       <c r="V18" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q18,", ",R18,", ",S18,", ",T18,", ",U18,", /* ASCII ",N18," (",O18,"), character: ",P18," */")</f>
         <v>    0x00, 0x42, 0xFE, 0x02, 0x00, /* ASCII 49 (0x31), character: '1' */</v>
-      </c>
-      <c r="W18" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q18,2))</f>
-        <v>0</v>
-      </c>
-      <c r="X18" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R18,2))</f>
-        <v>66</v>
-      </c>
-      <c r="Y18" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S18,2))</f>
-        <v>254</v>
-      </c>
-      <c r="Z18" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T18,2))</f>
-        <v>2</v>
-      </c>
-      <c r="AA18" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U18,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB18" s="1" t="n">
-        <f aca="false">IF(W18=0,IF(X18=0,IF(Y18=0,IF(Z18=0,IF(AA18=0,0,4),3),2),1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="AC18" s="1" t="n">
-        <f aca="false">IF(AA18=0,IF(Z18=0,IF(Y18=0,IF(X18=0,IF(W18=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD18" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC18*16)+AB18,2),",")</f>
-        <v>0x41,</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1951,38 +1384,6 @@
         <f aca="false">CONCATENATE("    ",Q19,", ",R19,", ",S19,", ",T19,", ",U19,", /* ASCII ",N19," (",O19,"), character: ",P19," */")</f>
         <v>    0x46, 0x8A, 0x92, 0x92, 0x62, /* ASCII 50 (0x32), character: '2' */</v>
       </c>
-      <c r="W19" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q19,2))</f>
-        <v>70</v>
-      </c>
-      <c r="X19" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R19,2))</f>
-        <v>138</v>
-      </c>
-      <c r="Y19" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S19,2))</f>
-        <v>146</v>
-      </c>
-      <c r="Z19" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T19,2))</f>
-        <v>146</v>
-      </c>
-      <c r="AA19" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U19,2))</f>
-        <v>98</v>
-      </c>
-      <c r="AB19" s="1" t="n">
-        <f aca="false">IF(W19=0,IF(X19=0,IF(Y19=0,IF(Z19=0,IF(AA19=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC19" s="1" t="n">
-        <f aca="false">IF(AA19=0,IF(Z19=0,IF(Y19=0,IF(X19=0,IF(W19=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD19" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC19*16)+AB19,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0"/>
@@ -1993,7 +1394,9 @@
         <v>1</v>
       </c>
       <c r="E20" s="0"/>
-      <c r="F20" s="0"/>
+      <c r="F20" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="G20" s="2" t="n">
         <v>1</v>
       </c>
@@ -2041,40 +1444,8 @@
         <f aca="false">CONCATENATE("    ",Q20,", ",R20,", ",S20,", ",T20,", ",U20,", /* ASCII ",N20," (",O20,"), character: ",P20," */")</f>
         <v>    0x44, 0x92, 0x92, 0x92, 0x6C, /* ASCII 51 (0x33), character: '3' */</v>
       </c>
-      <c r="W20" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q20,2))</f>
-        <v>68</v>
-      </c>
-      <c r="X20" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R20,2))</f>
-        <v>146</v>
-      </c>
-      <c r="Y20" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S20,2))</f>
-        <v>146</v>
-      </c>
-      <c r="Z20" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T20,2))</f>
-        <v>146</v>
-      </c>
-      <c r="AA20" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U20,2))</f>
-        <v>108</v>
-      </c>
-      <c r="AB20" s="1" t="n">
-        <f aca="false">IF(W20=0,IF(X20=0,IF(Y20=0,IF(Z20=0,IF(AA20=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC20" s="1" t="n">
-        <f aca="false">IF(AA20=0,IF(Z20=0,IF(Y20=0,IF(X20=0,IF(W20=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD20" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC20*16)+AB20,2),",")</f>
-        <v>0x50,</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="21" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0"/>
       <c r="B21" s="0"/>
       <c r="C21" s="0"/>
@@ -2083,8 +1454,12 @@
         <v>0</v>
       </c>
       <c r="E21" s="0"/>
-      <c r="F21" s="0"/>
-      <c r="G21" s="0"/>
+      <c r="F21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="H21" s="0"/>
       <c r="I21" s="0"/>
       <c r="J21" s="0"/>
@@ -2128,38 +1503,6 @@
       <c r="V21" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q21,", ",R21,", ",S21,", ",T21,", ",U21,", /* ASCII ",N21," (",O21,"), character: ",P21," */")</f>
         <v>    0x38, 0xE8, 0xC8, 0xFE, 0x08, /* ASCII 52 (0x34), character: '4' */</v>
-      </c>
-      <c r="W21" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q21,2))</f>
-        <v>56</v>
-      </c>
-      <c r="X21" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R21,2))</f>
-        <v>232</v>
-      </c>
-      <c r="Y21" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S21,2))</f>
-        <v>200</v>
-      </c>
-      <c r="Z21" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T21,2))</f>
-        <v>254</v>
-      </c>
-      <c r="AA21" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U21,2))</f>
-        <v>8</v>
-      </c>
-      <c r="AB21" s="1" t="n">
-        <f aca="false">IF(W21=0,IF(X21=0,IF(Y21=0,IF(Z21=0,IF(AA21=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC21" s="1" t="n">
-        <f aca="false">IF(AA21=0,IF(Z21=0,IF(Y21=0,IF(X21=0,IF(W21=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD21" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC21*16)+AB21,2),",")</f>
-        <v>0x50,</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2173,15 +1516,15 @@
       </c>
       <c r="F22" s="2" t="str">
         <f aca="false">CONCATENATE("0x",DEC2HEX(SUM(IF(F21=1,2^$D21,0),IF(F20=1,2^$D20,0),IF(F19=1,2^$D19,0),IF(F18=1,2^$D18,0),IF(F17=1,2^$D17,0),IF(F16=1,2^$D16,0),IF(F15=1,2^$D15,0),IF(F14=1,2^$D14,0)),2))</f>
-        <v>0x60</v>
+        <v>0xFB</v>
       </c>
       <c r="G22" s="2" t="str">
         <f aca="false">CONCATENATE("0x",DEC2HEX(SUM(IF(G21=1,2^$D21,0),IF(G20=1,2^$D20,0),IF(G19=1,2^$D19,0),IF(G18=1,2^$D18,0),IF(G17=1,2^$D17,0),IF(G16=1,2^$D16,0),IF(G15=1,2^$D15,0),IF(G14=1,2^$D14,0)),2))</f>
-        <v>0xFA</v>
+        <v>0xFB</v>
       </c>
       <c r="H22" s="2" t="str">
         <f aca="false">CONCATENATE("0x",DEC2HEX(SUM(IF(H21=1,2^$D21,0),IF(H20=1,2^$D20,0),IF(H19=1,2^$D19,0),IF(H18=1,2^$D18,0),IF(H17=1,2^$D17,0),IF(H16=1,2^$D16,0),IF(H15=1,2^$D15,0),IF(H14=1,2^$D14,0)),2))</f>
-        <v>0x60</v>
+        <v>0x00</v>
       </c>
       <c r="I22" s="2" t="str">
         <f aca="false">CONCATENATE("0x",DEC2HEX(SUM(IF(I21=1,2^$D21,0),IF(I20=1,2^$D20,0),IF(I19=1,2^$D19,0),IF(I18=1,2^$D18,0),IF(I17=1,2^$D17,0),IF(I16=1,2^$D16,0),IF(I15=1,2^$D15,0),IF(I14=1,2^$D14,0)),2))</f>
@@ -2228,38 +1571,6 @@
       <c r="V22" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q22,", ",R22,", ",S22,", ",T22,", ",U22,", /* ASCII ",N22," (",O22,"), character: ",P22," */")</f>
         <v>    0xF4, 0x92, 0x92, 0x92, 0x8C, /* ASCII 53 (0x35), character: '5' */</v>
-      </c>
-      <c r="W22" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q22,2))</f>
-        <v>244</v>
-      </c>
-      <c r="X22" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R22,2))</f>
-        <v>146</v>
-      </c>
-      <c r="Y22" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S22,2))</f>
-        <v>146</v>
-      </c>
-      <c r="Z22" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T22,2))</f>
-        <v>146</v>
-      </c>
-      <c r="AA22" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U22,2))</f>
-        <v>140</v>
-      </c>
-      <c r="AB22" s="1" t="n">
-        <f aca="false">IF(W22=0,IF(X22=0,IF(Y22=0,IF(Z22=0,IF(AA22=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC22" s="1" t="n">
-        <f aca="false">IF(AA22=0,IF(Z22=0,IF(Y22=0,IF(X22=0,IF(W22=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD22" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC22*16)+AB22,2),",")</f>
-        <v>0x50,</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2314,38 +1625,6 @@
         <f aca="false">CONCATENATE("    ",Q23,", ",R23,", ",S23,", ",T23,", ",U23,", /* ASCII ",N23," (",O23,"), character: ",P23," */")</f>
         <v>    0x7C, 0x92, 0x92, 0x92, 0x4C, /* ASCII 54 (0x36), character: '6' */</v>
       </c>
-      <c r="W23" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q23,2))</f>
-        <v>124</v>
-      </c>
-      <c r="X23" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R23,2))</f>
-        <v>146</v>
-      </c>
-      <c r="Y23" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S23,2))</f>
-        <v>146</v>
-      </c>
-      <c r="Z23" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T23,2))</f>
-        <v>146</v>
-      </c>
-      <c r="AA23" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U23,2))</f>
-        <v>76</v>
-      </c>
-      <c r="AB23" s="1" t="n">
-        <f aca="false">IF(W23=0,IF(X23=0,IF(Y23=0,IF(Z23=0,IF(AA23=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC23" s="1" t="n">
-        <f aca="false">IF(AA23=0,IF(Z23=0,IF(Y23=0,IF(X23=0,IF(W23=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD23" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC23*16)+AB23,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0"/>
@@ -2413,38 +1692,6 @@
         <f aca="false">CONCATENATE("    ",Q24,", ",R24,", ",S24,", ",T24,", ",U24,", /* ASCII ",N24," (",O24,"), character: ",P24," */")</f>
         <v>    0x80, 0x88, 0x9E, 0xA8, 0xC0, /* ASCII 55 (0x37), character: '7' */</v>
       </c>
-      <c r="W24" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q24,2))</f>
-        <v>128</v>
-      </c>
-      <c r="X24" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R24,2))</f>
-        <v>136</v>
-      </c>
-      <c r="Y24" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S24,2))</f>
-        <v>158</v>
-      </c>
-      <c r="Z24" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T24,2))</f>
-        <v>168</v>
-      </c>
-      <c r="AA24" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U24,2))</f>
-        <v>192</v>
-      </c>
-      <c r="AB24" s="1" t="n">
-        <f aca="false">IF(W24=0,IF(X24=0,IF(Y24=0,IF(Z24=0,IF(AA24=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC24" s="1" t="n">
-        <f aca="false">IF(AA24=0,IF(Z24=0,IF(Y24=0,IF(X24=0,IF(W24=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD24" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC24*16)+AB24,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
@@ -2516,38 +1763,6 @@
       <c r="V25" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q25,", ",R25,", ",S25,", ",T25,", ",U25,", /* ASCII ",N25," (",O25,"), character: ",P25," */")</f>
         <v>    0x6C, 0x92, 0x92, 0x92, 0x6C, /* ASCII 56 (0x38), character: '8' */</v>
-      </c>
-      <c r="W25" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q25,2))</f>
-        <v>108</v>
-      </c>
-      <c r="X25" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R25,2))</f>
-        <v>146</v>
-      </c>
-      <c r="Y25" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S25,2))</f>
-        <v>146</v>
-      </c>
-      <c r="Z25" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T25,2))</f>
-        <v>146</v>
-      </c>
-      <c r="AA25" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U25,2))</f>
-        <v>108</v>
-      </c>
-      <c r="AB25" s="1" t="n">
-        <f aca="false">IF(W25=0,IF(X25=0,IF(Y25=0,IF(Z25=0,IF(AA25=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC25" s="1" t="n">
-        <f aca="false">IF(AA25=0,IF(Z25=0,IF(Y25=0,IF(X25=0,IF(W25=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD25" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC25*16)+AB25,2),",")</f>
-        <v>0x50,</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2612,38 +1827,6 @@
         <f aca="false">CONCATENATE("    ",Q26,", ",R26,", ",S26,", ",T26,", ",U26,", /* ASCII ",N26," (",O26,"), character: ",P26," */")</f>
         <v>    0x64, 0x92, 0x92, 0x92, 0x7C, /* ASCII 57 (0x39), character: '9' */</v>
       </c>
-      <c r="W26" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q26,2))</f>
-        <v>100</v>
-      </c>
-      <c r="X26" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R26,2))</f>
-        <v>146</v>
-      </c>
-      <c r="Y26" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S26,2))</f>
-        <v>146</v>
-      </c>
-      <c r="Z26" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T26,2))</f>
-        <v>146</v>
-      </c>
-      <c r="AA26" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U26,2))</f>
-        <v>124</v>
-      </c>
-      <c r="AB26" s="1" t="n">
-        <f aca="false">IF(W26=0,IF(X26=0,IF(Y26=0,IF(Z26=0,IF(AA26=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC26" s="1" t="n">
-        <f aca="false">IF(AA26=0,IF(Z26=0,IF(Y26=0,IF(X26=0,IF(W26=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD26" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC26*16)+AB26,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0"/>
@@ -2706,38 +1889,6 @@
       <c r="V27" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q27,", ",R27,", ",S27,", ",T27,", ",U27,", /* ASCII ",N27," (",O27,"), character: ",P27," */")</f>
         <v>    0x00, 0x6C, 0x6C, 0x00, 0x00, /* ASCII 58 (0x3A), character: ':' */</v>
-      </c>
-      <c r="W27" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q27,2))</f>
-        <v>0</v>
-      </c>
-      <c r="X27" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R27,2))</f>
-        <v>108</v>
-      </c>
-      <c r="Y27" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S27,2))</f>
-        <v>108</v>
-      </c>
-      <c r="Z27" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T27,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AA27" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U27,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB27" s="1" t="n">
-        <f aca="false">IF(W27=0,IF(X27=0,IF(Y27=0,IF(Z27=0,IF(AA27=0,0,4),3),2),1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="AC27" s="1" t="n">
-        <f aca="false">IF(AA27=0,IF(Z27=0,IF(Y27=0,IF(X27=0,IF(W27=0,5,1),2),3),4),5)</f>
-        <v>3</v>
-      </c>
-      <c r="AD27" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC27*16)+AB27,2),",")</f>
-        <v>0x31,</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2798,38 +1949,6 @@
         <f aca="false">CONCATENATE("    ",Q28,", ",R28,", ",S28,", ",T28,", ",U28,", /* ASCII ",N28," (",O28,"), character: ",P28," */")</f>
         <v>    0x00, 0x6D, 0x6E, 0x00, 0x00, /* ASCII 59 (0x3B), character: ';' */</v>
       </c>
-      <c r="W28" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q28,2))</f>
-        <v>0</v>
-      </c>
-      <c r="X28" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R28,2))</f>
-        <v>109</v>
-      </c>
-      <c r="Y28" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S28,2))</f>
-        <v>110</v>
-      </c>
-      <c r="Z28" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T28,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AA28" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U28,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB28" s="1" t="n">
-        <f aca="false">IF(W28=0,IF(X28=0,IF(Y28=0,IF(Z28=0,IF(AA28=0,0,4),3),2),1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="AC28" s="1" t="n">
-        <f aca="false">IF(AA28=0,IF(Z28=0,IF(Y28=0,IF(X28=0,IF(W28=0,5,1),2),3),4),5)</f>
-        <v>3</v>
-      </c>
-      <c r="AD28" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC28*16)+AB28,2),",")</f>
-        <v>0x31,</v>
-      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0"/>
@@ -2888,38 +2007,6 @@
       <c r="V29" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q29,", ",R29,", ",S29,", ",T29,", ",U29,", /* ASCII ",N29," (",O29,"), character: ",P29," */")</f>
         <v>    0x00, 0x10, 0x28, 0x44, 0x82, /* ASCII 60 (0x3C), character: '&lt;' */</v>
-      </c>
-      <c r="W29" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q29,2))</f>
-        <v>0</v>
-      </c>
-      <c r="X29" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R29,2))</f>
-        <v>16</v>
-      </c>
-      <c r="Y29" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S29,2))</f>
-        <v>40</v>
-      </c>
-      <c r="Z29" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T29,2))</f>
-        <v>68</v>
-      </c>
-      <c r="AA29" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U29,2))</f>
-        <v>130</v>
-      </c>
-      <c r="AB29" s="1" t="n">
-        <f aca="false">IF(W29=0,IF(X29=0,IF(Y29=0,IF(Z29=0,IF(AA29=0,0,4),3),2),1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="AC29" s="1" t="n">
-        <f aca="false">IF(AA29=0,IF(Z29=0,IF(Y29=0,IF(X29=0,IF(W29=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD29" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC29*16)+AB29,2),",")</f>
-        <v>0x51,</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2977,38 +2064,6 @@
         <f aca="false">CONCATENATE("    ",Q30,", ",R30,", ",S30,", ",T30,", ",U30,", /* ASCII ",N30," (",O30,"), character: ",P30," */")</f>
         <v>    0x28, 0x28, 0x28, 0x28, 0x28, /* ASCII 61 (0x3D), character: '=' */</v>
       </c>
-      <c r="W30" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q30,2))</f>
-        <v>40</v>
-      </c>
-      <c r="X30" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R30,2))</f>
-        <v>40</v>
-      </c>
-      <c r="Y30" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S30,2))</f>
-        <v>40</v>
-      </c>
-      <c r="Z30" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T30,2))</f>
-        <v>40</v>
-      </c>
-      <c r="AA30" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U30,2))</f>
-        <v>40</v>
-      </c>
-      <c r="AB30" s="1" t="n">
-        <f aca="false">IF(W30=0,IF(X30=0,IF(Y30=0,IF(Z30=0,IF(AA30=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC30" s="1" t="n">
-        <f aca="false">IF(AA30=0,IF(Z30=0,IF(Y30=0,IF(X30=0,IF(W30=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD30" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC30*16)+AB30,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0"/>
@@ -3065,38 +2120,6 @@
         <f aca="false">CONCATENATE("    ",Q31,", ",R31,", ",S31,", ",T31,", ",U31,", /* ASCII ",N31," (",O31,"), character: ",P31," */")</f>
         <v>    0x82, 0x44, 0x28, 0x10, 0x00, /* ASCII 62 (0x3E), character: '&gt;' */</v>
       </c>
-      <c r="W31" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q31,2))</f>
-        <v>130</v>
-      </c>
-      <c r="X31" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R31,2))</f>
-        <v>68</v>
-      </c>
-      <c r="Y31" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S31,2))</f>
-        <v>40</v>
-      </c>
-      <c r="Z31" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T31,2))</f>
-        <v>16</v>
-      </c>
-      <c r="AA31" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U31,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB31" s="1" t="n">
-        <f aca="false">IF(W31=0,IF(X31=0,IF(Y31=0,IF(Z31=0,IF(AA31=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC31" s="1" t="n">
-        <f aca="false">IF(AA31=0,IF(Z31=0,IF(Y31=0,IF(X31=0,IF(W31=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD31" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC31*16)+AB31,2),",")</f>
-        <v>0x40,</v>
-      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0"/>
@@ -3153,38 +2176,6 @@
         <f aca="false">CONCATENATE("    ",Q32,", ",R32,", ",S32,", ",T32,", ",U32,", /* ASCII ",N32," (",O32,"), character: ",P32," */")</f>
         <v>    0x40, 0x80, 0x9A, 0xA0, 0x40, /* ASCII 63 (0x3F), character: '?' */</v>
       </c>
-      <c r="W32" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q32,2))</f>
-        <v>64</v>
-      </c>
-      <c r="X32" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R32,2))</f>
-        <v>128</v>
-      </c>
-      <c r="Y32" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S32,2))</f>
-        <v>154</v>
-      </c>
-      <c r="Z32" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T32,2))</f>
-        <v>160</v>
-      </c>
-      <c r="AA32" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U32,2))</f>
-        <v>64</v>
-      </c>
-      <c r="AB32" s="1" t="n">
-        <f aca="false">IF(W32=0,IF(X32=0,IF(Y32=0,IF(Z32=0,IF(AA32=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC32" s="1" t="n">
-        <f aca="false">IF(AA32=0,IF(Z32=0,IF(Y32=0,IF(X32=0,IF(W32=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD32" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC32*16)+AB32,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
@@ -3231,7 +2222,7 @@
       </c>
       <c r="Q33" s="2" t="str">
         <f aca="false">INDEX(E:E,$M33+8,1)</f>
-        <v>0x7C</v>
+        <v>0xFE</v>
       </c>
       <c r="R33" s="2" t="str">
         <f aca="false">INDEX(F:F,$M33+8,1)</f>
@@ -3247,43 +2238,11 @@
       </c>
       <c r="U33" s="2" t="str">
         <f aca="false">INDEX(I:I,$M33+8,1)</f>
-        <v>0x7A</v>
+        <v>0xFA</v>
       </c>
       <c r="V33" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q33,", ",R33,", ",S33,", ",T33,", ",U33,", /* ASCII ",N33," (",O33,"), character: ",P33," */")</f>
-        <v>    0x7C, 0x82, 0xBA, 0xAA, 0x7A, /* ASCII 64 (0x40), character: '@' */</v>
-      </c>
-      <c r="W33" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q33,2))</f>
-        <v>124</v>
-      </c>
-      <c r="X33" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R33,2))</f>
-        <v>130</v>
-      </c>
-      <c r="Y33" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S33,2))</f>
-        <v>186</v>
-      </c>
-      <c r="Z33" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T33,2))</f>
-        <v>170</v>
-      </c>
-      <c r="AA33" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U33,2))</f>
-        <v>122</v>
-      </c>
-      <c r="AB33" s="1" t="n">
-        <f aca="false">IF(W33=0,IF(X33=0,IF(Y33=0,IF(Z33=0,IF(AA33=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC33" s="1" t="n">
-        <f aca="false">IF(AA33=0,IF(Z33=0,IF(Y33=0,IF(X33=0,IF(W33=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD33" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC33*16)+AB33,2),",")</f>
-        <v>0x50,</v>
+        <v>    0xFE, 0x82, 0xBA, 0xAA, 0xFA, /* ASCII 64 (0x40), character: '@' */</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3338,38 +2297,6 @@
         <f aca="false">CONCATENATE("    ",Q34,", ",R34,", ",S34,", ",T34,", ",U34,", /* ASCII ",N34," (",O34,"), character: ",P34," */")</f>
         <v>    0x3E, 0x48, 0x88, 0x48, 0x3E, /* ASCII 65 (0x41), character: 'A' */</v>
       </c>
-      <c r="W34" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q34,2))</f>
-        <v>62</v>
-      </c>
-      <c r="X34" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R34,2))</f>
-        <v>72</v>
-      </c>
-      <c r="Y34" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S34,2))</f>
-        <v>136</v>
-      </c>
-      <c r="Z34" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T34,2))</f>
-        <v>72</v>
-      </c>
-      <c r="AA34" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U34,2))</f>
-        <v>62</v>
-      </c>
-      <c r="AB34" s="1" t="n">
-        <f aca="false">IF(W34=0,IF(X34=0,IF(Y34=0,IF(Z34=0,IF(AA34=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC34" s="1" t="n">
-        <f aca="false">IF(AA34=0,IF(Z34=0,IF(Y34=0,IF(X34=0,IF(W34=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD34" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC34*16)+AB34,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0"/>
@@ -3436,38 +2363,6 @@
       <c r="V35" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q35,", ",R35,", ",S35,", ",T35,", ",U35,", /* ASCII ",N35," (",O35,"), character: ",P35," */")</f>
         <v>    0xFE, 0x92, 0x92, 0x92, 0x6C, /* ASCII 66 (0x42), character: 'B' */</v>
-      </c>
-      <c r="W35" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q35,2))</f>
-        <v>254</v>
-      </c>
-      <c r="X35" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R35,2))</f>
-        <v>146</v>
-      </c>
-      <c r="Y35" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S35,2))</f>
-        <v>146</v>
-      </c>
-      <c r="Z35" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T35,2))</f>
-        <v>146</v>
-      </c>
-      <c r="AA35" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U35,2))</f>
-        <v>108</v>
-      </c>
-      <c r="AB35" s="1" t="n">
-        <f aca="false">IF(W35=0,IF(X35=0,IF(Y35=0,IF(Z35=0,IF(AA35=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC35" s="1" t="n">
-        <f aca="false">IF(AA35=0,IF(Z35=0,IF(Y35=0,IF(X35=0,IF(W35=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD35" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC35*16)+AB35,2),",")</f>
-        <v>0x50,</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3537,38 +2432,6 @@
         <f aca="false">CONCATENATE("    ",Q36,", ",R36,", ",S36,", ",T36,", ",U36,", /* ASCII ",N36," (",O36,"), character: ",P36," */")</f>
         <v>    0x7C, 0x82, 0x82, 0x82, 0x44, /* ASCII 67 (0x43), character: 'C' */</v>
       </c>
-      <c r="W36" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q36,2))</f>
-        <v>124</v>
-      </c>
-      <c r="X36" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R36,2))</f>
-        <v>130</v>
-      </c>
-      <c r="Y36" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S36,2))</f>
-        <v>130</v>
-      </c>
-      <c r="Z36" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T36,2))</f>
-        <v>130</v>
-      </c>
-      <c r="AA36" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U36,2))</f>
-        <v>68</v>
-      </c>
-      <c r="AB36" s="1" t="n">
-        <f aca="false">IF(W36=0,IF(X36=0,IF(Y36=0,IF(Z36=0,IF(AA36=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC36" s="1" t="n">
-        <f aca="false">IF(AA36=0,IF(Z36=0,IF(Y36=0,IF(X36=0,IF(W36=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD36" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC36*16)+AB36,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="37" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0"/>
@@ -3632,38 +2495,6 @@
         <f aca="false">CONCATENATE("    ",Q37,", ",R37,", ",S37,", ",T37,", ",U37,", /* ASCII ",N37," (",O37,"), character: ",P37," */")</f>
         <v>    0xFE, 0x82, 0x82, 0x82, 0x7C, /* ASCII 68 (0x44), character: 'D' */</v>
       </c>
-      <c r="W37" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q37,2))</f>
-        <v>254</v>
-      </c>
-      <c r="X37" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R37,2))</f>
-        <v>130</v>
-      </c>
-      <c r="Y37" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S37,2))</f>
-        <v>130</v>
-      </c>
-      <c r="Z37" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T37,2))</f>
-        <v>130</v>
-      </c>
-      <c r="AA37" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U37,2))</f>
-        <v>124</v>
-      </c>
-      <c r="AB37" s="1" t="n">
-        <f aca="false">IF(W37=0,IF(X37=0,IF(Y37=0,IF(Z37=0,IF(AA37=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC37" s="1" t="n">
-        <f aca="false">IF(AA37=0,IF(Z37=0,IF(Y37=0,IF(X37=0,IF(W37=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD37" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC37*16)+AB37,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="38" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0"/>
@@ -3733,38 +2564,6 @@
         <f aca="false">CONCATENATE("    ",Q38,", ",R38,", ",S38,", ",T38,", ",U38,", /* ASCII ",N38," (",O38,"), character: ",P38," */")</f>
         <v>    0xFE, 0x92, 0x92, 0x92, 0x82, /* ASCII 69 (0x45), character: 'E' */</v>
       </c>
-      <c r="W38" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q38,2))</f>
-        <v>254</v>
-      </c>
-      <c r="X38" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R38,2))</f>
-        <v>146</v>
-      </c>
-      <c r="Y38" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S38,2))</f>
-        <v>146</v>
-      </c>
-      <c r="Z38" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T38,2))</f>
-        <v>146</v>
-      </c>
-      <c r="AA38" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U38,2))</f>
-        <v>130</v>
-      </c>
-      <c r="AB38" s="1" t="n">
-        <f aca="false">IF(W38=0,IF(X38=0,IF(Y38=0,IF(Z38=0,IF(AA38=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC38" s="1" t="n">
-        <f aca="false">IF(AA38=0,IF(Z38=0,IF(Y38=0,IF(X38=0,IF(W38=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD38" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC38*16)+AB38,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="39" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0"/>
@@ -3828,38 +2627,6 @@
         <f aca="false">CONCATENATE("    ",Q39,", ",R39,", ",S39,", ",T39,", ",U39,", /* ASCII ",N39," (",O39,"), character: ",P39," */")</f>
         <v>    0xFE, 0x90, 0x90, 0x90, 0x80, /* ASCII 70 (0x46), character: 'F' */</v>
       </c>
-      <c r="W39" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q39,2))</f>
-        <v>254</v>
-      </c>
-      <c r="X39" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R39,2))</f>
-        <v>144</v>
-      </c>
-      <c r="Y39" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S39,2))</f>
-        <v>144</v>
-      </c>
-      <c r="Z39" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T39,2))</f>
-        <v>144</v>
-      </c>
-      <c r="AA39" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U39,2))</f>
-        <v>128</v>
-      </c>
-      <c r="AB39" s="1" t="n">
-        <f aca="false">IF(W39=0,IF(X39=0,IF(Y39=0,IF(Z39=0,IF(AA39=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC39" s="1" t="n">
-        <f aca="false">IF(AA39=0,IF(Z39=0,IF(Y39=0,IF(X39=0,IF(W39=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD39" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC39*16)+AB39,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="40" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0"/>
@@ -3928,38 +2695,6 @@
       <c r="V40" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q40,", ",R40,", ",S40,", ",T40,", ",U40,", /* ASCII ",N40," (",O40,"), character: ",P40," */")</f>
         <v>    0x7C, 0x82, 0x8A, 0x8A, 0x4C, /* ASCII 71 (0x47), character: 'G' */</v>
-      </c>
-      <c r="W40" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q40,2))</f>
-        <v>124</v>
-      </c>
-      <c r="X40" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R40,2))</f>
-        <v>130</v>
-      </c>
-      <c r="Y40" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S40,2))</f>
-        <v>138</v>
-      </c>
-      <c r="Z40" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T40,2))</f>
-        <v>138</v>
-      </c>
-      <c r="AA40" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U40,2))</f>
-        <v>76</v>
-      </c>
-      <c r="AB40" s="1" t="n">
-        <f aca="false">IF(W40=0,IF(X40=0,IF(Y40=0,IF(Z40=0,IF(AA40=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC40" s="1" t="n">
-        <f aca="false">IF(AA40=0,IF(Z40=0,IF(Y40=0,IF(X40=0,IF(W40=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD40" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC40*16)+AB40,2),",")</f>
-        <v>0x50,</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4020,38 +2755,6 @@
       <c r="V41" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q41,", ",R41,", ",S41,", ",T41,", ",U41,", /* ASCII ",N41," (",O41,"), character: ",P41," */")</f>
         <v>    0xFE, 0x10, 0x10, 0x10, 0xFE, /* ASCII 72 (0x48), character: 'H' */</v>
-      </c>
-      <c r="W41" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q41,2))</f>
-        <v>254</v>
-      </c>
-      <c r="X41" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R41,2))</f>
-        <v>16</v>
-      </c>
-      <c r="Y41" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S41,2))</f>
-        <v>16</v>
-      </c>
-      <c r="Z41" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T41,2))</f>
-        <v>16</v>
-      </c>
-      <c r="AA41" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U41,2))</f>
-        <v>254</v>
-      </c>
-      <c r="AB41" s="1" t="n">
-        <f aca="false">IF(W41=0,IF(X41=0,IF(Y41=0,IF(Z41=0,IF(AA41=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC41" s="1" t="n">
-        <f aca="false">IF(AA41=0,IF(Z41=0,IF(Y41=0,IF(X41=0,IF(W41=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD41" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC41*16)+AB41,2),",")</f>
-        <v>0x50,</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4109,38 +2812,6 @@
         <f aca="false">CONCATENATE("    ",Q42,", ",R42,", ",S42,", ",T42,", ",U42,", /* ASCII ",N42," (",O42,"), character: ",P42," */")</f>
         <v>    0x00, 0x82, 0xFE, 0x82, 0x00, /* ASCII 73 (0x49), character: 'I' */</v>
       </c>
-      <c r="W42" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q42,2))</f>
-        <v>0</v>
-      </c>
-      <c r="X42" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R42,2))</f>
-        <v>130</v>
-      </c>
-      <c r="Y42" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S42,2))</f>
-        <v>254</v>
-      </c>
-      <c r="Z42" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T42,2))</f>
-        <v>130</v>
-      </c>
-      <c r="AA42" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U42,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB42" s="1" t="n">
-        <f aca="false">IF(W42=0,IF(X42=0,IF(Y42=0,IF(Z42=0,IF(AA42=0,0,4),3),2),1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="AC42" s="1" t="n">
-        <f aca="false">IF(AA42=0,IF(Z42=0,IF(Y42=0,IF(X42=0,IF(W42=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD42" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC42*16)+AB42,2),",")</f>
-        <v>0x41,</v>
-      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0"/>
@@ -4197,38 +2868,6 @@
         <f aca="false">CONCATENATE("    ",Q43,", ",R43,", ",S43,", ",T43,", ",U43,", /* ASCII ",N43," (",O43,"), character: ",P43," */")</f>
         <v>    0x0C, 0x02, 0x82, 0xFC, 0x80, /* ASCII 74 (0x4A), character: 'J' */</v>
       </c>
-      <c r="W43" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q43,2))</f>
-        <v>12</v>
-      </c>
-      <c r="X43" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R43,2))</f>
-        <v>2</v>
-      </c>
-      <c r="Y43" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S43,2))</f>
-        <v>130</v>
-      </c>
-      <c r="Z43" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T43,2))</f>
-        <v>252</v>
-      </c>
-      <c r="AA43" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U43,2))</f>
-        <v>128</v>
-      </c>
-      <c r="AB43" s="1" t="n">
-        <f aca="false">IF(W43=0,IF(X43=0,IF(Y43=0,IF(Z43=0,IF(AA43=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC43" s="1" t="n">
-        <f aca="false">IF(AA43=0,IF(Z43=0,IF(Y43=0,IF(X43=0,IF(W43=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD43" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC43*16)+AB43,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0"/>
@@ -4296,38 +2935,6 @@
       <c r="V44" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q44,", ",R44,", ",S44,", ",T44,", ",U44,", /* ASCII ",N44," (",O44,"), character: ",P44," */")</f>
         <v>    0xFE, 0x10, 0x28, 0x44, 0x82, /* ASCII 75 (0x4B), character: 'K' */</v>
-      </c>
-      <c r="W44" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q44,2))</f>
-        <v>254</v>
-      </c>
-      <c r="X44" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R44,2))</f>
-        <v>16</v>
-      </c>
-      <c r="Y44" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S44,2))</f>
-        <v>40</v>
-      </c>
-      <c r="Z44" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T44,2))</f>
-        <v>68</v>
-      </c>
-      <c r="AA44" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U44,2))</f>
-        <v>130</v>
-      </c>
-      <c r="AB44" s="1" t="n">
-        <f aca="false">IF(W44=0,IF(X44=0,IF(Y44=0,IF(Z44=0,IF(AA44=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC44" s="1" t="n">
-        <f aca="false">IF(AA44=0,IF(Z44=0,IF(Y44=0,IF(X44=0,IF(W44=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD44" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC44*16)+AB44,2),",")</f>
-        <v>0x50,</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4382,38 +2989,6 @@
         <f aca="false">CONCATENATE("    ",Q45,", ",R45,", ",S45,", ",T45,", ",U45,", /* ASCII ",N45," (",O45,"), character: ",P45," */")</f>
         <v>    0xFE, 0x02, 0x02, 0x02, 0x02, /* ASCII 76 (0x4C), character: 'L' */</v>
       </c>
-      <c r="W45" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q45,2))</f>
-        <v>254</v>
-      </c>
-      <c r="X45" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R45,2))</f>
-        <v>2</v>
-      </c>
-      <c r="Y45" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S45,2))</f>
-        <v>2</v>
-      </c>
-      <c r="Z45" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T45,2))</f>
-        <v>2</v>
-      </c>
-      <c r="AA45" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U45,2))</f>
-        <v>2</v>
-      </c>
-      <c r="AB45" s="1" t="n">
-        <f aca="false">IF(W45=0,IF(X45=0,IF(Y45=0,IF(Z45=0,IF(AA45=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC45" s="1" t="n">
-        <f aca="false">IF(AA45=0,IF(Z45=0,IF(Y45=0,IF(X45=0,IF(W45=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD45" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC45*16)+AB45,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0"/>
@@ -4481,38 +3056,6 @@
         <f aca="false">CONCATENATE("    ",Q46,", ",R46,", ",S46,", ",T46,", ",U46,", /* ASCII ",N46," (",O46,"), character: ",P46," */")</f>
         <v>    0xFE, 0x40, 0x20, 0x40, 0xFE, /* ASCII 77 (0x4D), character: 'M' */</v>
       </c>
-      <c r="W46" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q46,2))</f>
-        <v>254</v>
-      </c>
-      <c r="X46" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R46,2))</f>
-        <v>64</v>
-      </c>
-      <c r="Y46" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S46,2))</f>
-        <v>32</v>
-      </c>
-      <c r="Z46" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T46,2))</f>
-        <v>64</v>
-      </c>
-      <c r="AA46" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U46,2))</f>
-        <v>254</v>
-      </c>
-      <c r="AB46" s="1" t="n">
-        <f aca="false">IF(W46=0,IF(X46=0,IF(Y46=0,IF(Z46=0,IF(AA46=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC46" s="1" t="n">
-        <f aca="false">IF(AA46=0,IF(Z46=0,IF(Y46=0,IF(X46=0,IF(W46=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD46" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC46*16)+AB46,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="47" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="n">
@@ -4582,38 +3125,6 @@
       <c r="V47" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q47,", ",R47,", ",S47,", ",T47,", ",U47,", /* ASCII ",N47," (",O47,"), character: ",P47," */")</f>
         <v>    0xFE, 0x20, 0x10, 0x08, 0xFE, /* ASCII 78 (0x4E), character: 'N' */</v>
-      </c>
-      <c r="W47" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q47,2))</f>
-        <v>254</v>
-      </c>
-      <c r="X47" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R47,2))</f>
-        <v>32</v>
-      </c>
-      <c r="Y47" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S47,2))</f>
-        <v>16</v>
-      </c>
-      <c r="Z47" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T47,2))</f>
-        <v>8</v>
-      </c>
-      <c r="AA47" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U47,2))</f>
-        <v>254</v>
-      </c>
-      <c r="AB47" s="1" t="n">
-        <f aca="false">IF(W47=0,IF(X47=0,IF(Y47=0,IF(Z47=0,IF(AA47=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC47" s="1" t="n">
-        <f aca="false">IF(AA47=0,IF(Z47=0,IF(Y47=0,IF(X47=0,IF(W47=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD47" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC47*16)+AB47,2),",")</f>
-        <v>0x50,</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4682,38 +3193,6 @@
         <f aca="false">CONCATENATE("    ",Q48,", ",R48,", ",S48,", ",T48,", ",U48,", /* ASCII ",N48," (",O48,"), character: ",P48," */")</f>
         <v>    0x7C, 0x82, 0x82, 0x82, 0x7C, /* ASCII 79 (0x4F), character: 'O' */</v>
       </c>
-      <c r="W48" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q48,2))</f>
-        <v>124</v>
-      </c>
-      <c r="X48" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R48,2))</f>
-        <v>130</v>
-      </c>
-      <c r="Y48" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S48,2))</f>
-        <v>130</v>
-      </c>
-      <c r="Z48" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T48,2))</f>
-        <v>130</v>
-      </c>
-      <c r="AA48" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U48,2))</f>
-        <v>124</v>
-      </c>
-      <c r="AB48" s="1" t="n">
-        <f aca="false">IF(W48=0,IF(X48=0,IF(Y48=0,IF(Z48=0,IF(AA48=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC48" s="1" t="n">
-        <f aca="false">IF(AA48=0,IF(Z48=0,IF(Y48=0,IF(X48=0,IF(W48=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD48" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC48*16)+AB48,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="49" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0"/>
@@ -4777,38 +3256,6 @@
         <f aca="false">CONCATENATE("    ",Q49,", ",R49,", ",S49,", ",T49,", ",U49,", /* ASCII ",N49," (",O49,"), character: ",P49," */")</f>
         <v>    0xFE, 0x90, 0x90, 0x90, 0x60, /* ASCII 80 (0x50), character: 'P' */</v>
       </c>
-      <c r="W49" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q49,2))</f>
-        <v>254</v>
-      </c>
-      <c r="X49" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R49,2))</f>
-        <v>144</v>
-      </c>
-      <c r="Y49" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S49,2))</f>
-        <v>144</v>
-      </c>
-      <c r="Z49" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T49,2))</f>
-        <v>144</v>
-      </c>
-      <c r="AA49" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U49,2))</f>
-        <v>96</v>
-      </c>
-      <c r="AB49" s="1" t="n">
-        <f aca="false">IF(W49=0,IF(X49=0,IF(Y49=0,IF(Z49=0,IF(AA49=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC49" s="1" t="n">
-        <f aca="false">IF(AA49=0,IF(Z49=0,IF(Y49=0,IF(X49=0,IF(W49=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD49" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC49*16)+AB49,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="50" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0"/>
@@ -4874,38 +3321,6 @@
         <f aca="false">CONCATENATE("    ",Q50,", ",R50,", ",S50,", ",T50,", ",U50,", /* ASCII ",N50," (",O50,"), character: ",P50," */")</f>
         <v>    0x7C, 0x82, 0x86, 0x82, 0x7D, /* ASCII 81 (0x51), character: 'Q' */</v>
       </c>
-      <c r="W50" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q50,2))</f>
-        <v>124</v>
-      </c>
-      <c r="X50" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R50,2))</f>
-        <v>130</v>
-      </c>
-      <c r="Y50" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S50,2))</f>
-        <v>134</v>
-      </c>
-      <c r="Z50" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T50,2))</f>
-        <v>130</v>
-      </c>
-      <c r="AA50" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U50,2))</f>
-        <v>125</v>
-      </c>
-      <c r="AB50" s="1" t="n">
-        <f aca="false">IF(W50=0,IF(X50=0,IF(Y50=0,IF(Z50=0,IF(AA50=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC50" s="1" t="n">
-        <f aca="false">IF(AA50=0,IF(Z50=0,IF(Y50=0,IF(X50=0,IF(W50=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD50" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC50*16)+AB50,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="51" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0"/>
@@ -4968,38 +3383,6 @@
       <c r="V51" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q51,", ",R51,", ",S51,", ",T51,", ",U51,", /* ASCII ",N51," (",O51,"), character: ",P51," */")</f>
         <v>    0xFE, 0x90, 0x90, 0x90, 0x6E, /* ASCII 82 (0x52), character: 'R' */</v>
-      </c>
-      <c r="W51" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q51,2))</f>
-        <v>254</v>
-      </c>
-      <c r="X51" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R51,2))</f>
-        <v>144</v>
-      </c>
-      <c r="Y51" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S51,2))</f>
-        <v>144</v>
-      </c>
-      <c r="Z51" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T51,2))</f>
-        <v>144</v>
-      </c>
-      <c r="AA51" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U51,2))</f>
-        <v>110</v>
-      </c>
-      <c r="AB51" s="1" t="n">
-        <f aca="false">IF(W51=0,IF(X51=0,IF(Y51=0,IF(Z51=0,IF(AA51=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC51" s="1" t="n">
-        <f aca="false">IF(AA51=0,IF(Z51=0,IF(Y51=0,IF(X51=0,IF(W51=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD51" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC51*16)+AB51,2),",")</f>
-        <v>0x50,</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5065,38 +3448,6 @@
         <f aca="false">CONCATENATE("    ",Q52,", ",R52,", ",S52,", ",T52,", ",U52,", /* ASCII ",N52," (",O52,"), character: ",P52," */")</f>
         <v>    0x62, 0x92, 0x92, 0x92, 0x8C, /* ASCII 83 (0x53), character: 'S' */</v>
       </c>
-      <c r="W52" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q52,2))</f>
-        <v>98</v>
-      </c>
-      <c r="X52" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R52,2))</f>
-        <v>146</v>
-      </c>
-      <c r="Y52" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S52,2))</f>
-        <v>146</v>
-      </c>
-      <c r="Z52" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T52,2))</f>
-        <v>146</v>
-      </c>
-      <c r="AA52" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U52,2))</f>
-        <v>140</v>
-      </c>
-      <c r="AB52" s="1" t="n">
-        <f aca="false">IF(W52=0,IF(X52=0,IF(Y52=0,IF(Z52=0,IF(AA52=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC52" s="1" t="n">
-        <f aca="false">IF(AA52=0,IF(Z52=0,IF(Y52=0,IF(X52=0,IF(W52=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD52" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC52*16)+AB52,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="53" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0"/>
@@ -5154,38 +3505,6 @@
       <c r="V53" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q53,", ",R53,", ",S53,", ",T53,", ",U53,", /* ASCII ",N53," (",O53,"), character: ",P53," */")</f>
         <v>    0x80, 0x80, 0xFE, 0x80, 0x80, /* ASCII 84 (0x54), character: 'T' */</v>
-      </c>
-      <c r="W53" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q53,2))</f>
-        <v>128</v>
-      </c>
-      <c r="X53" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R53,2))</f>
-        <v>128</v>
-      </c>
-      <c r="Y53" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S53,2))</f>
-        <v>254</v>
-      </c>
-      <c r="Z53" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T53,2))</f>
-        <v>128</v>
-      </c>
-      <c r="AA53" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U53,2))</f>
-        <v>128</v>
-      </c>
-      <c r="AB53" s="1" t="n">
-        <f aca="false">IF(W53=0,IF(X53=0,IF(Y53=0,IF(Z53=0,IF(AA53=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC53" s="1" t="n">
-        <f aca="false">IF(AA53=0,IF(Z53=0,IF(Y53=0,IF(X53=0,IF(W53=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD53" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC53*16)+AB53,2),",")</f>
-        <v>0x50,</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5243,38 +3562,6 @@
         <f aca="false">CONCATENATE("    ",Q54,", ",R54,", ",S54,", ",T54,", ",U54,", /* ASCII ",N54," (",O54,"), character: ",P54," */")</f>
         <v>    0xFC, 0x02, 0x02, 0x02, 0xFC, /* ASCII 85 (0x55), character: 'U' */</v>
       </c>
-      <c r="W54" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q54,2))</f>
-        <v>252</v>
-      </c>
-      <c r="X54" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R54,2))</f>
-        <v>2</v>
-      </c>
-      <c r="Y54" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S54,2))</f>
-        <v>2</v>
-      </c>
-      <c r="Z54" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T54,2))</f>
-        <v>2</v>
-      </c>
-      <c r="AA54" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U54,2))</f>
-        <v>252</v>
-      </c>
-      <c r="AB54" s="1" t="n">
-        <f aca="false">IF(W54=0,IF(X54=0,IF(Y54=0,IF(Z54=0,IF(AA54=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC54" s="1" t="n">
-        <f aca="false">IF(AA54=0,IF(Z54=0,IF(Y54=0,IF(X54=0,IF(W54=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD54" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC54*16)+AB54,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0"/>
@@ -5342,38 +3629,6 @@
       <c r="V55" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q55,", ",R55,", ",S55,", ",T55,", ",U55,", /* ASCII ",N55," (",O55,"), character: ",P55," */")</f>
         <v>    0xE0, 0x38, 0x0E, 0x38, 0xE0, /* ASCII 86 (0x56), character: 'V' */</v>
-      </c>
-      <c r="W55" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q55,2))</f>
-        <v>224</v>
-      </c>
-      <c r="X55" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R55,2))</f>
-        <v>56</v>
-      </c>
-      <c r="Y55" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S55,2))</f>
-        <v>14</v>
-      </c>
-      <c r="Z55" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T55,2))</f>
-        <v>56</v>
-      </c>
-      <c r="AA55" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U55,2))</f>
-        <v>224</v>
-      </c>
-      <c r="AB55" s="1" t="n">
-        <f aca="false">IF(W55=0,IF(X55=0,IF(Y55=0,IF(Z55=0,IF(AA55=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC55" s="1" t="n">
-        <f aca="false">IF(AA55=0,IF(Z55=0,IF(Y55=0,IF(X55=0,IF(W55=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD55" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC55*16)+AB55,2),",")</f>
-        <v>0x50,</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5428,38 +3683,6 @@
         <f aca="false">CONCATENATE("    ",Q56,", ",R56,", ",S56,", ",T56,", ",U56,", /* ASCII ",N56," (",O56,"), character: ",P56," */")</f>
         <v>    0xFC, 0x02, 0x0C, 0x02, 0xFC, /* ASCII 87 (0x57), character: 'W' */</v>
       </c>
-      <c r="W56" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q56,2))</f>
-        <v>252</v>
-      </c>
-      <c r="X56" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R56,2))</f>
-        <v>2</v>
-      </c>
-      <c r="Y56" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S56,2))</f>
-        <v>12</v>
-      </c>
-      <c r="Z56" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T56,2))</f>
-        <v>2</v>
-      </c>
-      <c r="AA56" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U56,2))</f>
-        <v>252</v>
-      </c>
-      <c r="AB56" s="1" t="n">
-        <f aca="false">IF(W56=0,IF(X56=0,IF(Y56=0,IF(Z56=0,IF(AA56=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC56" s="1" t="n">
-        <f aca="false">IF(AA56=0,IF(Z56=0,IF(Y56=0,IF(X56=0,IF(W56=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD56" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC56*16)+AB56,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0"/>
@@ -5526,38 +3749,6 @@
       <c r="V57" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q57,", ",R57,", ",S57,", ",T57,", ",U57,", /* ASCII ",N57," (",O57,"), character: ",P57," */")</f>
         <v>    0xC6, 0x28, 0x10, 0x28, 0xC6, /* ASCII 88 (0x58), character: 'X' */</v>
-      </c>
-      <c r="W57" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q57,2))</f>
-        <v>198</v>
-      </c>
-      <c r="X57" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R57,2))</f>
-        <v>40</v>
-      </c>
-      <c r="Y57" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S57,2))</f>
-        <v>16</v>
-      </c>
-      <c r="Z57" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T57,2))</f>
-        <v>40</v>
-      </c>
-      <c r="AA57" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U57,2))</f>
-        <v>198</v>
-      </c>
-      <c r="AB57" s="1" t="n">
-        <f aca="false">IF(W57=0,IF(X57=0,IF(Y57=0,IF(Z57=0,IF(AA57=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC57" s="1" t="n">
-        <f aca="false">IF(AA57=0,IF(Z57=0,IF(Y57=0,IF(X57=0,IF(W57=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD57" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC57*16)+AB57,2),",")</f>
-        <v>0x50,</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5627,38 +3818,6 @@
         <f aca="false">CONCATENATE("    ",Q58,", ",R58,", ",S58,", ",T58,", ",U58,", /* ASCII ",N58," (",O58,"), character: ",P58," */")</f>
         <v>    0xE0, 0x10, 0x0E, 0x10, 0xE0, /* ASCII 89 (0x59), character: 'Y' */</v>
       </c>
-      <c r="W58" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q58,2))</f>
-        <v>224</v>
-      </c>
-      <c r="X58" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R58,2))</f>
-        <v>16</v>
-      </c>
-      <c r="Y58" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S58,2))</f>
-        <v>14</v>
-      </c>
-      <c r="Z58" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T58,2))</f>
-        <v>16</v>
-      </c>
-      <c r="AA58" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U58,2))</f>
-        <v>224</v>
-      </c>
-      <c r="AB58" s="1" t="n">
-        <f aca="false">IF(W58=0,IF(X58=0,IF(Y58=0,IF(Z58=0,IF(AA58=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC58" s="1" t="n">
-        <f aca="false">IF(AA58=0,IF(Z58=0,IF(Y58=0,IF(X58=0,IF(W58=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD58" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC58*16)+AB58,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="59" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0"/>
@@ -5724,38 +3883,6 @@
         <f aca="false">CONCATENATE("    ",Q59,", ",R59,", ",S59,", ",T59,", ",U59,", /* ASCII ",N59," (",O59,"), character: ",P59," */")</f>
         <v>    0x86, 0x8A, 0x92, 0xA2, 0xC2, /* ASCII 90 (0x5A), character: 'Z' */</v>
       </c>
-      <c r="W59" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q59,2))</f>
-        <v>134</v>
-      </c>
-      <c r="X59" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R59,2))</f>
-        <v>138</v>
-      </c>
-      <c r="Y59" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S59,2))</f>
-        <v>146</v>
-      </c>
-      <c r="Z59" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T59,2))</f>
-        <v>162</v>
-      </c>
-      <c r="AA59" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U59,2))</f>
-        <v>194</v>
-      </c>
-      <c r="AB59" s="1" t="n">
-        <f aca="false">IF(W59=0,IF(X59=0,IF(Y59=0,IF(Z59=0,IF(AA59=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC59" s="1" t="n">
-        <f aca="false">IF(AA59=0,IF(Z59=0,IF(Y59=0,IF(X59=0,IF(W59=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD59" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC59*16)+AB59,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="60" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0"/>
@@ -5823,38 +3950,6 @@
         <f aca="false">CONCATENATE("    ",Q60,", ",R60,", ",S60,", ",T60,", ",U60,", /* ASCII ",N60," (",O60,"), character: ",P60," */")</f>
         <v>    0x00, 0xFE, 0x82, 0x82, 0x00, /* ASCII 91 (0x5B), character: '[' */</v>
       </c>
-      <c r="W60" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q60,2))</f>
-        <v>0</v>
-      </c>
-      <c r="X60" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R60,2))</f>
-        <v>254</v>
-      </c>
-      <c r="Y60" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S60,2))</f>
-        <v>130</v>
-      </c>
-      <c r="Z60" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T60,2))</f>
-        <v>130</v>
-      </c>
-      <c r="AA60" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U60,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB60" s="1" t="n">
-        <f aca="false">IF(W60=0,IF(X60=0,IF(Y60=0,IF(Z60=0,IF(AA60=0,0,4),3),2),1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="AC60" s="1" t="n">
-        <f aca="false">IF(AA60=0,IF(Z60=0,IF(Y60=0,IF(X60=0,IF(W60=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD60" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC60*16)+AB60,2),",")</f>
-        <v>0x41,</v>
-      </c>
     </row>
     <row r="61" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0"/>
@@ -5922,38 +4017,6 @@
         <f aca="false">CONCATENATE("    ",Q61,", ",R61,", ",S61,", ",T61,", ",U61,", /* ASCII ",N61," (",O61,"), character: ",P61," */")</f>
         <v>    0x00, 0xC0, 0x30, 0x0C, 0x03, /* ASCII 92 (0x5C), character: '\' */</v>
       </c>
-      <c r="W61" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q61,2))</f>
-        <v>0</v>
-      </c>
-      <c r="X61" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R61,2))</f>
-        <v>192</v>
-      </c>
-      <c r="Y61" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S61,2))</f>
-        <v>48</v>
-      </c>
-      <c r="Z61" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T61,2))</f>
-        <v>12</v>
-      </c>
-      <c r="AA61" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U61,2))</f>
-        <v>3</v>
-      </c>
-      <c r="AB61" s="1" t="n">
-        <f aca="false">IF(W61=0,IF(X61=0,IF(Y61=0,IF(Z61=0,IF(AA61=0,0,4),3),2),1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="AC61" s="1" t="n">
-        <f aca="false">IF(AA61=0,IF(Z61=0,IF(Y61=0,IF(X61=0,IF(W61=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD61" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC61*16)+AB61,2),",")</f>
-        <v>0x51,</v>
-      </c>
     </row>
     <row r="62" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0"/>
@@ -6020,38 +4083,6 @@
       <c r="V62" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q62,", ",R62,", ",S62,", ",T62,", ",U62,", /* ASCII ",N62," (",O62,"), character: ",P62," */")</f>
         <v>    0x00, 0x82, 0x82, 0xFE, 0x00, /* ASCII 93 (0x5D), character: ']' */</v>
-      </c>
-      <c r="W62" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q62,2))</f>
-        <v>0</v>
-      </c>
-      <c r="X62" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R62,2))</f>
-        <v>130</v>
-      </c>
-      <c r="Y62" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S62,2))</f>
-        <v>130</v>
-      </c>
-      <c r="Z62" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T62,2))</f>
-        <v>254</v>
-      </c>
-      <c r="AA62" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U62,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB62" s="1" t="n">
-        <f aca="false">IF(W62=0,IF(X62=0,IF(Y62=0,IF(Z62=0,IF(AA62=0,0,4),3),2),1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="AC62" s="1" t="n">
-        <f aca="false">IF(AA62=0,IF(Z62=0,IF(Y62=0,IF(X62=0,IF(W62=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD62" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC62*16)+AB62,2),",")</f>
-        <v>0x41,</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6114,38 +4145,6 @@
       <c r="V63" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q63,", ",R63,", ",S63,", ",T63,", ",U63,", /* ASCII ",N63," (",O63,"), character: ",P63," */")</f>
         <v>    0x10, 0x20, 0x40, 0x20, 0x10, /* ASCII 94 (0x5E), character: '^' */</v>
-      </c>
-      <c r="W63" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q63,2))</f>
-        <v>16</v>
-      </c>
-      <c r="X63" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R63,2))</f>
-        <v>32</v>
-      </c>
-      <c r="Y63" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S63,2))</f>
-        <v>64</v>
-      </c>
-      <c r="Z63" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T63,2))</f>
-        <v>32</v>
-      </c>
-      <c r="AA63" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U63,2))</f>
-        <v>16</v>
-      </c>
-      <c r="AB63" s="1" t="n">
-        <f aca="false">IF(W63=0,IF(X63=0,IF(Y63=0,IF(Z63=0,IF(AA63=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC63" s="1" t="n">
-        <f aca="false">IF(AA63=0,IF(Z63=0,IF(Y63=0,IF(X63=0,IF(W63=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD63" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC63*16)+AB63,2),",")</f>
-        <v>0x50,</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6203,38 +4202,6 @@
         <f aca="false">CONCATENATE("    ",Q64,", ",R64,", ",S64,", ",T64,", ",U64,", /* ASCII ",N64," (",O64,"), character: ",P64," */")</f>
         <v>    0x02, 0x02, 0x02, 0x02, 0x02, /* ASCII 95 (0x5F), character: '_' */</v>
       </c>
-      <c r="W64" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q64,2))</f>
-        <v>2</v>
-      </c>
-      <c r="X64" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R64,2))</f>
-        <v>2</v>
-      </c>
-      <c r="Y64" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S64,2))</f>
-        <v>2</v>
-      </c>
-      <c r="Z64" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T64,2))</f>
-        <v>2</v>
-      </c>
-      <c r="AA64" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U64,2))</f>
-        <v>2</v>
-      </c>
-      <c r="AB64" s="1" t="n">
-        <f aca="false">IF(W64=0,IF(X64=0,IF(Y64=0,IF(Z64=0,IF(AA64=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC64" s="1" t="n">
-        <f aca="false">IF(AA64=0,IF(Z64=0,IF(Y64=0,IF(X64=0,IF(W64=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD64" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC64*16)+AB64,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0"/>
@@ -6291,38 +4258,6 @@
         <f aca="false">CONCATENATE("    ",Q65,", ",R65,", ",S65,", ",T65,", ",U65,", /* ASCII ",N65," (",O65,"), character: ",P65," */")</f>
         <v>    0x00, 0x80, 0x60, 0x00, 0x00, /* ASCII 96 (0x60), character: '`' */</v>
       </c>
-      <c r="W65" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q65,2))</f>
-        <v>0</v>
-      </c>
-      <c r="X65" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R65,2))</f>
-        <v>128</v>
-      </c>
-      <c r="Y65" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S65,2))</f>
-        <v>96</v>
-      </c>
-      <c r="Z65" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T65,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AA65" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U65,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB65" s="1" t="n">
-        <f aca="false">IF(W65=0,IF(X65=0,IF(Y65=0,IF(Z65=0,IF(AA65=0,0,4),3),2),1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="AC65" s="1" t="n">
-        <f aca="false">IF(AA65=0,IF(Z65=0,IF(Y65=0,IF(X65=0,IF(W65=0,5,1),2),3),4),5)</f>
-        <v>3</v>
-      </c>
-      <c r="AD65" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC65*16)+AB65,2),",")</f>
-        <v>0x31,</v>
-      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0"/>
@@ -6390,38 +4325,6 @@
       <c r="V66" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q66,", ",R66,", ",S66,", ",T66,", ",U66,", /* ASCII ",N66," (",O66,"), character: ",P66," */")</f>
         <v>    0x24, 0x4A, 0x4A, 0x3E, 0x00, /* ASCII 97 (0x61), character: 'a' */</v>
-      </c>
-      <c r="W66" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q66,2))</f>
-        <v>36</v>
-      </c>
-      <c r="X66" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R66,2))</f>
-        <v>74</v>
-      </c>
-      <c r="Y66" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S66,2))</f>
-        <v>74</v>
-      </c>
-      <c r="Z66" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T66,2))</f>
-        <v>62</v>
-      </c>
-      <c r="AA66" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U66,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB66" s="1" t="n">
-        <f aca="false">IF(W66=0,IF(X66=0,IF(Y66=0,IF(Z66=0,IF(AA66=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC66" s="1" t="n">
-        <f aca="false">IF(AA66=0,IF(Z66=0,IF(Y66=0,IF(X66=0,IF(W66=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD66" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC66*16)+AB66,2),",")</f>
-        <v>0x40,</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6476,38 +4379,6 @@
         <f aca="false">CONCATENATE("    ",Q67,", ",R67,", ",S67,", ",T67,", ",U67,", /* ASCII ",N67," (",O67,"), character: ",P67," */")</f>
         <v>    0x00, 0xFE, 0x12, 0x12, 0x0C, /* ASCII 98 (0x62), character: 'b' */</v>
       </c>
-      <c r="W67" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q67,2))</f>
-        <v>0</v>
-      </c>
-      <c r="X67" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R67,2))</f>
-        <v>254</v>
-      </c>
-      <c r="Y67" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S67,2))</f>
-        <v>18</v>
-      </c>
-      <c r="Z67" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T67,2))</f>
-        <v>18</v>
-      </c>
-      <c r="AA67" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U67,2))</f>
-        <v>12</v>
-      </c>
-      <c r="AB67" s="1" t="n">
-        <f aca="false">IF(W67=0,IF(X67=0,IF(Y67=0,IF(Z67=0,IF(AA67=0,0,4),3),2),1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="AC67" s="1" t="n">
-        <f aca="false">IF(AA67=0,IF(Z67=0,IF(Y67=0,IF(X67=0,IF(W67=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD67" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC67*16)+AB67,2),",")</f>
-        <v>0x51,</v>
-      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0"/>
@@ -6574,38 +4445,6 @@
       <c r="V68" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q68,", ",R68,", ",S68,", ",T68,", ",U68,", /* ASCII ",N68," (",O68,"), character: ",P68," */")</f>
         <v>    0x0C, 0x12, 0x12, 0x12, 0x00, /* ASCII 99 (0x63), character: 'c' */</v>
-      </c>
-      <c r="W68" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q68,2))</f>
-        <v>12</v>
-      </c>
-      <c r="X68" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R68,2))</f>
-        <v>18</v>
-      </c>
-      <c r="Y68" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S68,2))</f>
-        <v>18</v>
-      </c>
-      <c r="Z68" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T68,2))</f>
-        <v>18</v>
-      </c>
-      <c r="AA68" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U68,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB68" s="1" t="n">
-        <f aca="false">IF(W68=0,IF(X68=0,IF(Y68=0,IF(Z68=0,IF(AA68=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC68" s="1" t="n">
-        <f aca="false">IF(AA68=0,IF(Z68=0,IF(Y68=0,IF(X68=0,IF(W68=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD68" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC68*16)+AB68,2),",")</f>
-        <v>0x40,</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6675,38 +4514,6 @@
         <f aca="false">CONCATENATE("    ",Q69,", ",R69,", ",S69,", ",T69,", ",U69,", /* ASCII ",N69," (",O69,"), character: ",P69," */")</f>
         <v>    0x00, 0x0C, 0x12, 0x12, 0xFE, /* ASCII 100 (0x64), character: 'd' */</v>
       </c>
-      <c r="W69" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q69,2))</f>
-        <v>0</v>
-      </c>
-      <c r="X69" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R69,2))</f>
-        <v>12</v>
-      </c>
-      <c r="Y69" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S69,2))</f>
-        <v>18</v>
-      </c>
-      <c r="Z69" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T69,2))</f>
-        <v>18</v>
-      </c>
-      <c r="AA69" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U69,2))</f>
-        <v>254</v>
-      </c>
-      <c r="AB69" s="1" t="n">
-        <f aca="false">IF(W69=0,IF(X69=0,IF(Y69=0,IF(Z69=0,IF(AA69=0,0,4),3),2),1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="AC69" s="1" t="n">
-        <f aca="false">IF(AA69=0,IF(Z69=0,IF(Y69=0,IF(X69=0,IF(W69=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD69" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC69*16)+AB69,2),",")</f>
-        <v>0x51,</v>
-      </c>
     </row>
     <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0"/>
@@ -6770,38 +4577,6 @@
         <f aca="false">CONCATENATE("    ",Q70,", ",R70,", ",S70,", ",T70,", ",U70,", /* ASCII ",N70," (",O70,"), character: ",P70," */")</f>
         <v>    0x1C, 0x2A, 0x2A, 0x10, 0x00, /* ASCII 101 (0x65), character: 'e' */</v>
       </c>
-      <c r="W70" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q70,2))</f>
-        <v>28</v>
-      </c>
-      <c r="X70" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R70,2))</f>
-        <v>42</v>
-      </c>
-      <c r="Y70" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S70,2))</f>
-        <v>42</v>
-      </c>
-      <c r="Z70" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T70,2))</f>
-        <v>16</v>
-      </c>
-      <c r="AA70" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U70,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB70" s="1" t="n">
-        <f aca="false">IF(W70=0,IF(X70=0,IF(Y70=0,IF(Z70=0,IF(AA70=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC70" s="1" t="n">
-        <f aca="false">IF(AA70=0,IF(Z70=0,IF(Y70=0,IF(X70=0,IF(W70=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD70" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC70*16)+AB70,2),",")</f>
-        <v>0x40,</v>
-      </c>
     </row>
     <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0"/>
@@ -6865,38 +4640,6 @@
         <f aca="false">CONCATENATE("    ",Q71,", ",R71,", ",S71,", ",T71,", ",U71,", /* ASCII ",N71," (",O71,"), character: ",P71," */")</f>
         <v>    0x3E, 0x48, 0x40, 0x20, 0x00, /* ASCII 102 (0x66), character: 'f' */</v>
       </c>
-      <c r="W71" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q71,2))</f>
-        <v>62</v>
-      </c>
-      <c r="X71" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R71,2))</f>
-        <v>72</v>
-      </c>
-      <c r="Y71" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S71,2))</f>
-        <v>64</v>
-      </c>
-      <c r="Z71" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T71,2))</f>
-        <v>32</v>
-      </c>
-      <c r="AA71" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U71,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB71" s="1" t="n">
-        <f aca="false">IF(W71=0,IF(X71=0,IF(Y71=0,IF(Z71=0,IF(AA71=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC71" s="1" t="n">
-        <f aca="false">IF(AA71=0,IF(Z71=0,IF(Y71=0,IF(X71=0,IF(W71=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD71" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC71*16)+AB71,2),",")</f>
-        <v>0x40,</v>
-      </c>
     </row>
     <row r="72" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0"/>
@@ -6958,38 +4701,6 @@
         <f aca="false">CONCATENATE("    ",Q72,", ",R72,", ",S72,", ",T72,", ",U72,", /* ASCII ",N72," (",O72,"), character: ",P72," */")</f>
         <v>    0x12, 0x29, 0x29, 0x3E, 0x00, /* ASCII 103 (0x67), character: 'g' */</v>
       </c>
-      <c r="W72" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q72,2))</f>
-        <v>18</v>
-      </c>
-      <c r="X72" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R72,2))</f>
-        <v>41</v>
-      </c>
-      <c r="Y72" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S72,2))</f>
-        <v>41</v>
-      </c>
-      <c r="Z72" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T72,2))</f>
-        <v>62</v>
-      </c>
-      <c r="AA72" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U72,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB72" s="1" t="n">
-        <f aca="false">IF(W72=0,IF(X72=0,IF(Y72=0,IF(Z72=0,IF(AA72=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC72" s="1" t="n">
-        <f aca="false">IF(AA72=0,IF(Z72=0,IF(Y72=0,IF(X72=0,IF(W72=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD72" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC72*16)+AB72,2),",")</f>
-        <v>0x40,</v>
-      </c>
     </row>
     <row r="73" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0"/>
@@ -7054,38 +4765,6 @@
       <c r="V73" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q73,", ",R73,", ",S73,", ",T73,", ",U73,", /* ASCII ",N73," (",O73,"), character: ",P73," */")</f>
         <v>    0x7E, 0x08, 0x08, 0x06, 0x00, /* ASCII 104 (0x68), character: 'h' */</v>
-      </c>
-      <c r="W73" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q73,2))</f>
-        <v>126</v>
-      </c>
-      <c r="X73" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R73,2))</f>
-        <v>8</v>
-      </c>
-      <c r="Y73" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S73,2))</f>
-        <v>8</v>
-      </c>
-      <c r="Z73" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T73,2))</f>
-        <v>6</v>
-      </c>
-      <c r="AA73" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U73,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB73" s="1" t="n">
-        <f aca="false">IF(W73=0,IF(X73=0,IF(Y73=0,IF(Z73=0,IF(AA73=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC73" s="1" t="n">
-        <f aca="false">IF(AA73=0,IF(Z73=0,IF(Y73=0,IF(X73=0,IF(W73=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD73" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC73*16)+AB73,2),",")</f>
-        <v>0x40,</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7147,38 +4826,6 @@
         <f aca="false">CONCATENATE("    ",Q74,", ",R74,", ",S74,", ",T74,", ",U74,", /* ASCII ",N74," (",O74,"), character: ",P74," */")</f>
         <v>    0x00, 0x12, 0x5E, 0x02, 0x00, /* ASCII 105 (0x69), character: 'i' */</v>
       </c>
-      <c r="W74" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q74,2))</f>
-        <v>0</v>
-      </c>
-      <c r="X74" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R74,2))</f>
-        <v>18</v>
-      </c>
-      <c r="Y74" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S74,2))</f>
-        <v>94</v>
-      </c>
-      <c r="Z74" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T74,2))</f>
-        <v>2</v>
-      </c>
-      <c r="AA74" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U74,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB74" s="1" t="n">
-        <f aca="false">IF(W74=0,IF(X74=0,IF(Y74=0,IF(Z74=0,IF(AA74=0,0,4),3),2),1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="AC74" s="1" t="n">
-        <f aca="false">IF(AA74=0,IF(Z74=0,IF(Y74=0,IF(X74=0,IF(W74=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD74" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC74*16)+AB74,2),",")</f>
-        <v>0x41,</v>
-      </c>
     </row>
     <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0"/>
@@ -7240,38 +4887,6 @@
       <c r="V75" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q75,", ",R75,", ",S75,", ",T75,", ",U75,", /* ASCII ",N75," (",O75,"), character: ",P75," */")</f>
         <v>    0x00, 0x02, 0x11, 0x5E, 0x10, /* ASCII 106 (0x6A), character: 'j' */</v>
-      </c>
-      <c r="W75" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q75,2))</f>
-        <v>0</v>
-      </c>
-      <c r="X75" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R75,2))</f>
-        <v>2</v>
-      </c>
-      <c r="Y75" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S75,2))</f>
-        <v>17</v>
-      </c>
-      <c r="Z75" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T75,2))</f>
-        <v>94</v>
-      </c>
-      <c r="AA75" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U75,2))</f>
-        <v>16</v>
-      </c>
-      <c r="AB75" s="1" t="n">
-        <f aca="false">IF(W75=0,IF(X75=0,IF(Y75=0,IF(Z75=0,IF(AA75=0,0,4),3),2),1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="AC75" s="1" t="n">
-        <f aca="false">IF(AA75=0,IF(Z75=0,IF(Y75=0,IF(X75=0,IF(W75=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD75" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC75*16)+AB75,2),",")</f>
-        <v>0x51,</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7329,38 +4944,6 @@
         <f aca="false">CONCATENATE("    ",Q76,", ",R76,", ",S76,", ",T76,", ",U76,", /* ASCII ",N76," (",O76,"), character: ",P76," */")</f>
         <v>    0x00, 0xFE, 0x08, 0x16, 0x00, /* ASCII 107 (0x6B), character: 'k' */</v>
       </c>
-      <c r="W76" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q76,2))</f>
-        <v>0</v>
-      </c>
-      <c r="X76" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R76,2))</f>
-        <v>254</v>
-      </c>
-      <c r="Y76" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S76,2))</f>
-        <v>8</v>
-      </c>
-      <c r="Z76" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T76,2))</f>
-        <v>22</v>
-      </c>
-      <c r="AA76" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U76,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB76" s="1" t="n">
-        <f aca="false">IF(W76=0,IF(X76=0,IF(Y76=0,IF(Z76=0,IF(AA76=0,0,4),3),2),1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="AC76" s="1" t="n">
-        <f aca="false">IF(AA76=0,IF(Z76=0,IF(Y76=0,IF(X76=0,IF(W76=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD76" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC76*16)+AB76,2),",")</f>
-        <v>0x41,</v>
-      </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0"/>
@@ -7428,38 +5011,6 @@
       <c r="V77" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q77,", ",R77,", ",S77,", ",T77,", ",U77,", /* ASCII ",N77," (",O77,"), character: ",P77," */")</f>
         <v>    0x00, 0x42, 0x7E, 0x02, 0x00, /* ASCII 108 (0x6C), character: 'l' */</v>
-      </c>
-      <c r="W77" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q77,2))</f>
-        <v>0</v>
-      </c>
-      <c r="X77" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R77,2))</f>
-        <v>66</v>
-      </c>
-      <c r="Y77" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S77,2))</f>
-        <v>126</v>
-      </c>
-      <c r="Z77" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T77,2))</f>
-        <v>2</v>
-      </c>
-      <c r="AA77" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U77,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB77" s="1" t="n">
-        <f aca="false">IF(W77=0,IF(X77=0,IF(Y77=0,IF(Z77=0,IF(AA77=0,0,4),3),2),1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="AC77" s="1" t="n">
-        <f aca="false">IF(AA77=0,IF(Z77=0,IF(Y77=0,IF(X77=0,IF(W77=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD77" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC77*16)+AB77,2),",")</f>
-        <v>0x41,</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7514,38 +5065,6 @@
         <f aca="false">CONCATENATE("    ",Q78,", ",R78,", ",S78,", ",T78,", ",U78,", /* ASCII ",N78," (",O78,"), character: ",P78," */")</f>
         <v>    0x1E, 0x10, 0x0E, 0x10, 0x0E, /* ASCII 109 (0x6D), character: 'm' */</v>
       </c>
-      <c r="W78" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q78,2))</f>
-        <v>30</v>
-      </c>
-      <c r="X78" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R78,2))</f>
-        <v>16</v>
-      </c>
-      <c r="Y78" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S78,2))</f>
-        <v>14</v>
-      </c>
-      <c r="Z78" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T78,2))</f>
-        <v>16</v>
-      </c>
-      <c r="AA78" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U78,2))</f>
-        <v>14</v>
-      </c>
-      <c r="AB78" s="1" t="n">
-        <f aca="false">IF(W78=0,IF(X78=0,IF(Y78=0,IF(Z78=0,IF(AA78=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC78" s="1" t="n">
-        <f aca="false">IF(AA78=0,IF(Z78=0,IF(Y78=0,IF(X78=0,IF(W78=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD78" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC78*16)+AB78,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0"/>
@@ -7613,38 +5132,6 @@
         <f aca="false">CONCATENATE("    ",Q79,", ",R79,", ",S79,", ",T79,", ",U79,", /* ASCII ",N79," (",O79,"), character: ",P79," */")</f>
         <v>    0x1E, 0x10, 0x10, 0x0E, 0x00, /* ASCII 110 (0x6E), character: 'n' */</v>
       </c>
-      <c r="W79" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q79,2))</f>
-        <v>30</v>
-      </c>
-      <c r="X79" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R79,2))</f>
-        <v>16</v>
-      </c>
-      <c r="Y79" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S79,2))</f>
-        <v>16</v>
-      </c>
-      <c r="Z79" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T79,2))</f>
-        <v>14</v>
-      </c>
-      <c r="AA79" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U79,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB79" s="1" t="n">
-        <f aca="false">IF(W79=0,IF(X79=0,IF(Y79=0,IF(Z79=0,IF(AA79=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC79" s="1" t="n">
-        <f aca="false">IF(AA79=0,IF(Z79=0,IF(Y79=0,IF(X79=0,IF(W79=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD79" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC79*16)+AB79,2),",")</f>
-        <v>0x40,</v>
-      </c>
     </row>
     <row r="80" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="n">
@@ -7714,38 +5201,6 @@
       <c r="V80" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q80,", ",R80,", ",S80,", ",T80,", ",U80,", /* ASCII ",N80," (",O80,"), character: ",P80," */")</f>
         <v>    0x0C, 0x12, 0x12, 0x0C, 0x00, /* ASCII 111 (0x6F), character: 'o' */</v>
-      </c>
-      <c r="W80" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q80,2))</f>
-        <v>12</v>
-      </c>
-      <c r="X80" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R80,2))</f>
-        <v>18</v>
-      </c>
-      <c r="Y80" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S80,2))</f>
-        <v>18</v>
-      </c>
-      <c r="Z80" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T80,2))</f>
-        <v>12</v>
-      </c>
-      <c r="AA80" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U80,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB80" s="1" t="n">
-        <f aca="false">IF(W80=0,IF(X80=0,IF(Y80=0,IF(Z80=0,IF(AA80=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC80" s="1" t="n">
-        <f aca="false">IF(AA80=0,IF(Z80=0,IF(Y80=0,IF(X80=0,IF(W80=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD80" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC80*16)+AB80,2),",")</f>
-        <v>0x40,</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7808,38 +5263,6 @@
         <f aca="false">CONCATENATE("    ",Q81,", ",R81,", ",S81,", ",T81,", ",U81,", /* ASCII ",N81," (",O81,"), character: ",P81," */")</f>
         <v>    0x00, 0x3F, 0x24, 0x24, 0x18, /* ASCII 112 (0x70), character: 'p' */</v>
       </c>
-      <c r="W81" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q81,2))</f>
-        <v>0</v>
-      </c>
-      <c r="X81" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R81,2))</f>
-        <v>63</v>
-      </c>
-      <c r="Y81" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S81,2))</f>
-        <v>36</v>
-      </c>
-      <c r="Z81" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T81,2))</f>
-        <v>36</v>
-      </c>
-      <c r="AA81" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U81,2))</f>
-        <v>24</v>
-      </c>
-      <c r="AB81" s="1" t="n">
-        <f aca="false">IF(W81=0,IF(X81=0,IF(Y81=0,IF(Z81=0,IF(AA81=0,0,4),3),2),1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="AC81" s="1" t="n">
-        <f aca="false">IF(AA81=0,IF(Z81=0,IF(Y81=0,IF(X81=0,IF(W81=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD81" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC81*16)+AB81,2),",")</f>
-        <v>0x51,</v>
-      </c>
     </row>
     <row r="82" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0"/>
@@ -7900,38 +5323,6 @@
       <c r="V82" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q82,", ",R82,", ",S82,", ",T82,", ",U82,", /* ASCII ",N82," (",O82,"), character: ",P82," */")</f>
         <v>    0x18, 0x24, 0x24, 0x3F, 0x00, /* ASCII 113 (0x71), character: 'q' */</v>
-      </c>
-      <c r="W82" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q82,2))</f>
-        <v>24</v>
-      </c>
-      <c r="X82" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R82,2))</f>
-        <v>36</v>
-      </c>
-      <c r="Y82" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S82,2))</f>
-        <v>36</v>
-      </c>
-      <c r="Z82" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T82,2))</f>
-        <v>63</v>
-      </c>
-      <c r="AA82" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U82,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB82" s="1" t="n">
-        <f aca="false">IF(W82=0,IF(X82=0,IF(Y82=0,IF(Z82=0,IF(AA82=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC82" s="1" t="n">
-        <f aca="false">IF(AA82=0,IF(Z82=0,IF(Y82=0,IF(X82=0,IF(W82=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD82" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC82*16)+AB82,2),",")</f>
-        <v>0x40,</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7992,38 +5383,6 @@
         <f aca="false">CONCATENATE("    ",Q83,", ",R83,", ",S83,", ",T83,", ",U83,", /* ASCII ",N83," (",O83,"), character: ",P83," */")</f>
         <v>    0x1E, 0x08, 0x10, 0x08, 0x00, /* ASCII 114 (0x72), character: 'r' */</v>
       </c>
-      <c r="W83" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q83,2))</f>
-        <v>30</v>
-      </c>
-      <c r="X83" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R83,2))</f>
-        <v>8</v>
-      </c>
-      <c r="Y83" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S83,2))</f>
-        <v>16</v>
-      </c>
-      <c r="Z83" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T83,2))</f>
-        <v>8</v>
-      </c>
-      <c r="AA83" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U83,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB83" s="1" t="n">
-        <f aca="false">IF(W83=0,IF(X83=0,IF(Y83=0,IF(Z83=0,IF(AA83=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC83" s="1" t="n">
-        <f aca="false">IF(AA83=0,IF(Z83=0,IF(Y83=0,IF(X83=0,IF(W83=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD83" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC83*16)+AB83,2),",")</f>
-        <v>0x40,</v>
-      </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0"/>
@@ -8082,38 +5441,6 @@
       <c r="V84" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q84,", ",R84,", ",S84,", ",T84,", ",U84,", /* ASCII ",N84," (",O84,"), character: ",P84," */")</f>
         <v>    0x12, 0x2A, 0x2A, 0x24, 0x00, /* ASCII 115 (0x73), character: 's' */</v>
-      </c>
-      <c r="W84" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q84,2))</f>
-        <v>18</v>
-      </c>
-      <c r="X84" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R84,2))</f>
-        <v>42</v>
-      </c>
-      <c r="Y84" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S84,2))</f>
-        <v>42</v>
-      </c>
-      <c r="Z84" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T84,2))</f>
-        <v>36</v>
-      </c>
-      <c r="AA84" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U84,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB84" s="1" t="n">
-        <f aca="false">IF(W84=0,IF(X84=0,IF(Y84=0,IF(Z84=0,IF(AA84=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC84" s="1" t="n">
-        <f aca="false">IF(AA84=0,IF(Z84=0,IF(Y84=0,IF(X84=0,IF(W84=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD84" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC84*16)+AB84,2),",")</f>
-        <v>0x40,</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8171,38 +5498,6 @@
         <f aca="false">CONCATENATE("    ",Q85,", ",R85,", ",S85,", ",T85,", ",U85,", /* ASCII ",N85," (",O85,"), character: ",P85," */")</f>
         <v>    0x10, 0x3E, 0x11, 0x02, 0x00, /* ASCII 116 (0x74), character: 't' */</v>
       </c>
-      <c r="W85" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q85,2))</f>
-        <v>16</v>
-      </c>
-      <c r="X85" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R85,2))</f>
-        <v>62</v>
-      </c>
-      <c r="Y85" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S85,2))</f>
-        <v>17</v>
-      </c>
-      <c r="Z85" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T85,2))</f>
-        <v>2</v>
-      </c>
-      <c r="AA85" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U85,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB85" s="1" t="n">
-        <f aca="false">IF(W85=0,IF(X85=0,IF(Y85=0,IF(Z85=0,IF(AA85=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC85" s="1" t="n">
-        <f aca="false">IF(AA85=0,IF(Z85=0,IF(Y85=0,IF(X85=0,IF(W85=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD85" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC85*16)+AB85,2),",")</f>
-        <v>0x40,</v>
-      </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0"/>
@@ -8259,38 +5554,6 @@
         <f aca="false">CONCATENATE("    ",Q86,", ",R86,", ",S86,", ",T86,", ",U86,", /* ASCII ",N86," (",O86,"), character: ",P86," */")</f>
         <v>    0x1C, 0x02, 0x02, 0x1C, 0x00, /* ASCII 117 (0x75), character: 'u' */</v>
       </c>
-      <c r="W86" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q86,2))</f>
-        <v>28</v>
-      </c>
-      <c r="X86" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R86,2))</f>
-        <v>2</v>
-      </c>
-      <c r="Y86" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S86,2))</f>
-        <v>2</v>
-      </c>
-      <c r="Z86" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T86,2))</f>
-        <v>28</v>
-      </c>
-      <c r="AA86" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U86,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB86" s="1" t="n">
-        <f aca="false">IF(W86=0,IF(X86=0,IF(Y86=0,IF(Z86=0,IF(AA86=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC86" s="1" t="n">
-        <f aca="false">IF(AA86=0,IF(Z86=0,IF(Y86=0,IF(X86=0,IF(W86=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD86" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC86*16)+AB86,2),",")</f>
-        <v>0x40,</v>
-      </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0"/>
@@ -8347,38 +5610,6 @@
         <f aca="false">CONCATENATE("    ",Q87,", ",R87,", ",S87,", ",T87,", ",U87,", /* ASCII ",N87," (",O87,"), character: ",P87," */")</f>
         <v>    0x18, 0x04, 0x02, 0x04, 0x18, /* ASCII 118 (0x76), character: 'v' */</v>
       </c>
-      <c r="W87" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q87,2))</f>
-        <v>24</v>
-      </c>
-      <c r="X87" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R87,2))</f>
-        <v>4</v>
-      </c>
-      <c r="Y87" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S87,2))</f>
-        <v>2</v>
-      </c>
-      <c r="Z87" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T87,2))</f>
-        <v>4</v>
-      </c>
-      <c r="AA87" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U87,2))</f>
-        <v>24</v>
-      </c>
-      <c r="AB87" s="1" t="n">
-        <f aca="false">IF(W87=0,IF(X87=0,IF(Y87=0,IF(Z87=0,IF(AA87=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC87" s="1" t="n">
-        <f aca="false">IF(AA87=0,IF(Z87=0,IF(Y87=0,IF(X87=0,IF(W87=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD87" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC87*16)+AB87,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0"/>
@@ -8446,38 +5677,6 @@
       <c r="V88" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q88,", ",R88,", ",S88,", ",T88,", ",U88,", /* ASCII ",N88," (",O88,"), character: ",P88," */")</f>
         <v>    0x1C, 0x02, 0x1C, 0x02, 0x1C, /* ASCII 119 (0x77), character: 'w' */</v>
-      </c>
-      <c r="W88" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q88,2))</f>
-        <v>28</v>
-      </c>
-      <c r="X88" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R88,2))</f>
-        <v>2</v>
-      </c>
-      <c r="Y88" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S88,2))</f>
-        <v>28</v>
-      </c>
-      <c r="Z88" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T88,2))</f>
-        <v>2</v>
-      </c>
-      <c r="AA88" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U88,2))</f>
-        <v>28</v>
-      </c>
-      <c r="AB88" s="1" t="n">
-        <f aca="false">IF(W88=0,IF(X88=0,IF(Y88=0,IF(Z88=0,IF(AA88=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC88" s="1" t="n">
-        <f aca="false">IF(AA88=0,IF(Z88=0,IF(Y88=0,IF(X88=0,IF(W88=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD88" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC88*16)+AB88,2),",")</f>
-        <v>0x50,</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8532,38 +5731,6 @@
         <f aca="false">CONCATENATE("    ",Q89,", ",R89,", ",S89,", ",T89,", ",U89,", /* ASCII ",N89," (",O89,"), character: ",P89," */")</f>
         <v>    0x22, 0x14, 0x08, 0x14, 0x22, /* ASCII 120 (0x78), character: 'x' */</v>
       </c>
-      <c r="W89" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q89,2))</f>
-        <v>34</v>
-      </c>
-      <c r="X89" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R89,2))</f>
-        <v>20</v>
-      </c>
-      <c r="Y89" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S89,2))</f>
-        <v>8</v>
-      </c>
-      <c r="Z89" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T89,2))</f>
-        <v>20</v>
-      </c>
-      <c r="AA89" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U89,2))</f>
-        <v>34</v>
-      </c>
-      <c r="AB89" s="1" t="n">
-        <f aca="false">IF(W89=0,IF(X89=0,IF(Y89=0,IF(Z89=0,IF(AA89=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC89" s="1" t="n">
-        <f aca="false">IF(AA89=0,IF(Z89=0,IF(Y89=0,IF(X89=0,IF(W89=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD89" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC89*16)+AB89,2),",")</f>
-        <v>0x50,</v>
-      </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0"/>
@@ -8631,38 +5798,6 @@
         <f aca="false">CONCATENATE("    ",Q90,", ",R90,", ",S90,", ",T90,", ",U90,", /* ASCII ",N90," (",O90,"), character: ",P90," */")</f>
         <v>    0x39, 0x05, 0x05, 0x3E, 0x00, /* ASCII 121 (0x79), character: 'y' */</v>
       </c>
-      <c r="W90" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q90,2))</f>
-        <v>57</v>
-      </c>
-      <c r="X90" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R90,2))</f>
-        <v>5</v>
-      </c>
-      <c r="Y90" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S90,2))</f>
-        <v>5</v>
-      </c>
-      <c r="Z90" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T90,2))</f>
-        <v>62</v>
-      </c>
-      <c r="AA90" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U90,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB90" s="1" t="n">
-        <f aca="false">IF(W90=0,IF(X90=0,IF(Y90=0,IF(Z90=0,IF(AA90=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC90" s="1" t="n">
-        <f aca="false">IF(AA90=0,IF(Z90=0,IF(Y90=0,IF(X90=0,IF(W90=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD90" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC90*16)+AB90,2),",")</f>
-        <v>0x40,</v>
-      </c>
     </row>
     <row r="91" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="n">
@@ -8732,38 +5867,6 @@
       <c r="V91" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q91,", ",R91,", ",S91,", ",T91,", ",U91,", /* ASCII ",N91," (",O91,"), character: ",P91," */")</f>
         <v>    0x00, 0x26, 0x2A, 0x32, 0x00, /* ASCII 122 (0x7A), character: 'z' */</v>
-      </c>
-      <c r="W91" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q91,2))</f>
-        <v>0</v>
-      </c>
-      <c r="X91" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R91,2))</f>
-        <v>38</v>
-      </c>
-      <c r="Y91" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S91,2))</f>
-        <v>42</v>
-      </c>
-      <c r="Z91" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T91,2))</f>
-        <v>50</v>
-      </c>
-      <c r="AA91" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U91,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB91" s="1" t="n">
-        <f aca="false">IF(W91=0,IF(X91=0,IF(Y91=0,IF(Z91=0,IF(AA91=0,0,4),3),2),1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="AC91" s="1" t="n">
-        <f aca="false">IF(AA91=0,IF(Z91=0,IF(Y91=0,IF(X91=0,IF(W91=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD91" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC91*16)+AB91,2),",")</f>
-        <v>0x41,</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8826,38 +5929,6 @@
         <f aca="false">CONCATENATE("    ",Q92,", ",R92,", ",S92,", ",T92,", ",U92,", /* ASCII ",N92," (",O92,"), character: ",P92," */")</f>
         <v>    0x00, 0x10, 0x7C, 0x82, 0x00, /* ASCII 123 (0x7B), character: '{' */</v>
       </c>
-      <c r="W92" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q92,2))</f>
-        <v>0</v>
-      </c>
-      <c r="X92" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R92,2))</f>
-        <v>16</v>
-      </c>
-      <c r="Y92" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S92,2))</f>
-        <v>124</v>
-      </c>
-      <c r="Z92" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T92,2))</f>
-        <v>130</v>
-      </c>
-      <c r="AA92" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U92,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB92" s="1" t="n">
-        <f aca="false">IF(W92=0,IF(X92=0,IF(Y92=0,IF(Z92=0,IF(AA92=0,0,4),3),2),1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="AC92" s="1" t="n">
-        <f aca="false">IF(AA92=0,IF(Z92=0,IF(Y92=0,IF(X92=0,IF(W92=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD92" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC92*16)+AB92,2),",")</f>
-        <v>0x41,</v>
-      </c>
     </row>
     <row r="93" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0"/>
@@ -8919,38 +5990,6 @@
         <f aca="false">CONCATENATE("    ",Q93,", ",R93,", ",S93,", ",T93,", ",U93,", /* ASCII ",N93," (",O93,"), character: ",P93," */")</f>
         <v>    0x00, 0x00, 0xFF, 0x00, 0x00, /* ASCII 124 (0x7C), character: '|' */</v>
       </c>
-      <c r="W93" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q93,2))</f>
-        <v>0</v>
-      </c>
-      <c r="X93" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R93,2))</f>
-        <v>0</v>
-      </c>
-      <c r="Y93" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S93,2))</f>
-        <v>255</v>
-      </c>
-      <c r="Z93" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T93,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AA93" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U93,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB93" s="1" t="n">
-        <f aca="false">IF(W93=0,IF(X93=0,IF(Y93=0,IF(Z93=0,IF(AA93=0,0,4),3),2),1),0)</f>
-        <v>2</v>
-      </c>
-      <c r="AC93" s="1" t="n">
-        <f aca="false">IF(AA93=0,IF(Z93=0,IF(Y93=0,IF(X93=0,IF(W93=0,5,1),2),3),4),5)</f>
-        <v>3</v>
-      </c>
-      <c r="AD93" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC93*16)+AB93,2),",")</f>
-        <v>0x32,</v>
-      </c>
     </row>
     <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0"/>
@@ -9012,38 +6051,6 @@
         <f aca="false">CONCATENATE("    ",Q94,", ",R94,", ",S94,", ",T94,", ",U94,", /* ASCII ",N94," (",O94,"), character: ",P94," */")</f>
         <v>    0x00, 0x82, 0x7C, 0x10, 0x00, /* ASCII 125 (0x7D), character: '}' */</v>
       </c>
-      <c r="W94" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q94,2))</f>
-        <v>0</v>
-      </c>
-      <c r="X94" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R94,2))</f>
-        <v>130</v>
-      </c>
-      <c r="Y94" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S94,2))</f>
-        <v>124</v>
-      </c>
-      <c r="Z94" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T94,2))</f>
-        <v>16</v>
-      </c>
-      <c r="AA94" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U94,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB94" s="1" t="n">
-        <f aca="false">IF(W94=0,IF(X94=0,IF(Y94=0,IF(Z94=0,IF(AA94=0,0,4),3),2),1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="AC94" s="1" t="n">
-        <f aca="false">IF(AA94=0,IF(Z94=0,IF(Y94=0,IF(X94=0,IF(W94=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD94" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC94*16)+AB94,2),",")</f>
-        <v>0x41,</v>
-      </c>
     </row>
     <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0"/>
@@ -9104,38 +6111,6 @@
       <c r="V95" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q95,", ",R95,", ",S95,", ",T95,", ",U95,", /* ASCII ",N95," (",O95,"), character: ",P95," */")</f>
         <v>    0x10, 0x20, 0x10, 0x08, 0x10, /* ASCII 126 (0x7E), character: '~' */</v>
-      </c>
-      <c r="W95" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q95,2))</f>
-        <v>16</v>
-      </c>
-      <c r="X95" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R95,2))</f>
-        <v>32</v>
-      </c>
-      <c r="Y95" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S95,2))</f>
-        <v>16</v>
-      </c>
-      <c r="Z95" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T95,2))</f>
-        <v>8</v>
-      </c>
-      <c r="AA95" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U95,2))</f>
-        <v>16</v>
-      </c>
-      <c r="AB95" s="1" t="n">
-        <f aca="false">IF(W95=0,IF(X95=0,IF(Y95=0,IF(Z95=0,IF(AA95=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC95" s="1" t="n">
-        <f aca="false">IF(AA95=0,IF(Z95=0,IF(Y95=0,IF(X95=0,IF(W95=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD95" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC95*16)+AB95,2),",")</f>
-        <v>0x50,</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9195,38 +6170,6 @@
         <f aca="false">CONCATENATE("    ",Q96,", ",R96,", ",S96,", ",T96,", ",U96,", /* ASCII ",N96," (",O96,"), character: ",P96," */")</f>
         <v>    0x00, 0xE0, 0xA0, 0xE0, 0x00, /* ASCII 127 (0x7F), character: '' */</v>
       </c>
-      <c r="W96" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q96,2))</f>
-        <v>0</v>
-      </c>
-      <c r="X96" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R96,2))</f>
-        <v>224</v>
-      </c>
-      <c r="Y96" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S96,2))</f>
-        <v>160</v>
-      </c>
-      <c r="Z96" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T96,2))</f>
-        <v>224</v>
-      </c>
-      <c r="AA96" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U96,2))</f>
-        <v>0</v>
-      </c>
-      <c r="AB96" s="1" t="n">
-        <f aca="false">IF(W96=0,IF(X96=0,IF(Y96=0,IF(Z96=0,IF(AA96=0,0,4),3),2),1),0)</f>
-        <v>1</v>
-      </c>
-      <c r="AC96" s="1" t="n">
-        <f aca="false">IF(AA96=0,IF(Z96=0,IF(Y96=0,IF(X96=0,IF(W96=0,5,1),2),3),4),5)</f>
-        <v>4</v>
-      </c>
-      <c r="AD96" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC96*16)+AB96,2),",")</f>
-        <v>0x41,</v>
-      </c>
     </row>
     <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0"/>
@@ -9284,38 +6227,6 @@
       <c r="V97" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q97,", ",R97,", ",S97,", ",T97,", ",U97,", /* ASCII ",N97," (",O97,"), character: ",P97," */")</f>
         <v>    0x28, 0x7C, 0xAA, 0x82, 0x44, /* ASCII 128 (0x80), character: '€' */</v>
-      </c>
-      <c r="W97" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(Q97,2))</f>
-        <v>40</v>
-      </c>
-      <c r="X97" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(R97,2))</f>
-        <v>124</v>
-      </c>
-      <c r="Y97" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(S97,2))</f>
-        <v>170</v>
-      </c>
-      <c r="Z97" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(T97,2))</f>
-        <v>130</v>
-      </c>
-      <c r="AA97" s="1" t="n">
-        <f aca="false">HEX2DEC(RIGHT(U97,2))</f>
-        <v>68</v>
-      </c>
-      <c r="AB97" s="1" t="n">
-        <f aca="false">IF(W97=0,IF(X97=0,IF(Y97=0,IF(Z97=0,IF(AA97=0,0,4),3),2),1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC97" s="1" t="n">
-        <f aca="false">IF(AA97=0,IF(Z97=0,IF(Y97=0,IF(X97=0,IF(W97=0,5,1),2),3),4),5)</f>
-        <v>5</v>
-      </c>
-      <c r="AD97" s="1" t="str">
-        <f aca="false">CONCATENATE("0x",DEC2HEX((AC97*16)+AB97,2),",")</f>
-        <v>0x50,</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15306,7 +12217,9 @@
         <f aca="false">D$3</f>
         <v>7</v>
       </c>
-      <c r="E355" s="0"/>
+      <c r="E355" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="F355" s="0" t="n">
         <v>1</v>
       </c>
@@ -15316,10 +12229,12 @@
       <c r="H355" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I355" s="0"/>
+      <c r="I355" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="J355" s="2" t="str">
         <f aca="false">E363</f>
-        <v>0x7C</v>
+        <v>0xFE</v>
       </c>
       <c r="L355" s="0"/>
       <c r="Q355" s="0"/>
@@ -15425,7 +12340,7 @@
       </c>
       <c r="J359" s="2" t="str">
         <f aca="false">I363</f>
-        <v>0x7A</v>
+        <v>0xFA</v>
       </c>
       <c r="L359" s="0"/>
       <c r="Q359" s="0"/>
@@ -15457,7 +12372,9 @@
         <f aca="false">D$9</f>
         <v>1</v>
       </c>
-      <c r="E361" s="0"/>
+      <c r="E361" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="F361" s="0" t="n">
         <v>1</v>
       </c>
@@ -15498,7 +12415,7 @@
       <c r="D363" s="0"/>
       <c r="E363" s="2" t="str">
         <f aca="false">CONCATENATE("0x",DEC2HEX(SUM(IF(E362=1,2^$D362,0),IF(E361=1,2^$D361,0),IF(E360=1,2^$D360,0),IF(E359=1,2^$D359,0),IF(E358=1,2^$D358,0),IF(E357=1,2^$D357,0),IF(E356=1,2^$D356,0),IF(E355=1,2^$D355,0)),2))</f>
-        <v>0x7C</v>
+        <v>0xFE</v>
       </c>
       <c r="F363" s="2" t="str">
         <f aca="false">CONCATENATE("0x",DEC2HEX(SUM(IF(F362=1,2^$D362,0),IF(F361=1,2^$D361,0),IF(F360=1,2^$D360,0),IF(F359=1,2^$D359,0),IF(F358=1,2^$D358,0),IF(F357=1,2^$D357,0),IF(F356=1,2^$D356,0),IF(F355=1,2^$D355,0)),2))</f>
@@ -15514,7 +12431,7 @@
       </c>
       <c r="I363" s="2" t="str">
         <f aca="false">CONCATENATE("0x",DEC2HEX(SUM(IF(I362=1,2^$D362,0),IF(I361=1,2^$D361,0),IF(I360=1,2^$D360,0),IF(I359=1,2^$D359,0),IF(I358=1,2^$D358,0),IF(I357=1,2^$D357,0),IF(I356=1,2^$D356,0),IF(I355=1,2^$D355,0)),2))</f>
-        <v>0x7A</v>
+        <v>0xFA</v>
       </c>
       <c r="J363" s="0"/>
       <c r="L363" s="0"/>
@@ -31798,7 +28715,7 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="str">
         <f aca="false">Sheet1!V2</f>
-        <v>    0x00, 0x60, 0xFA, 0x60, 0x00, /* ASCII 33 (0x21), character: '!' */</v>
+        <v>    0x00, 0xFB, 0xFB, 0x00, 0x00, /* ASCII 33 (0x21), character: '!' */</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31984,7 +28901,7 @@
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="str">
         <f aca="false">Sheet1!V33</f>
-        <v>    0x7C, 0x82, 0xBA, 0xAA, 0x7A, /* ASCII 64 (0x40), character: '@' */</v>
+        <v>    0xFE, 0x82, 0xBA, 0xAA, 0xFA, /* ASCII 64 (0x40), character: '@' */</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Revert "Revert "commit before I revert""
This reverts commit 2d45093b48a51f5e68c998fda31418e8e672edf3.
</commit_message>
<xml_diff>
--- a/CharCreator.xlsx
+++ b/CharCreator.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -93,18 +93,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -116,7 +110,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -140,12 +134,6 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -165,19 +153,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Lit" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Lit1" xfId="21" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <font>
+        <sz val="10"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
     </dxf>
   </dxfs>
 </styleSheet>
@@ -188,10 +179,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V1067"/>
+  <dimension ref="A1:AD1067"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1028" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1059" activeCellId="0" sqref="L1059"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A337" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V364" activeCellId="0" sqref="V364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -205,8 +196,10 @@
     <col collapsed="false" hidden="false" max="14" min="14" style="1" width="6.57142857142857"/>
     <col collapsed="false" hidden="false" max="16" min="15" style="1" width="9.14285714285714"/>
     <col collapsed="false" hidden="false" max="21" min="17" style="1" width="6.57142857142857"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="84.280612244898"/>
-    <col collapsed="false" hidden="false" max="256" min="23" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="21.015306122449"/>
+    <col collapsed="false" hidden="false" max="27" min="23" style="1" width="4.53571428571429"/>
+    <col collapsed="false" hidden="false" max="29" min="28" style="1" width="2.56632653061224"/>
+    <col collapsed="false" hidden="false" max="256" min="30" style="1" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
@@ -268,6 +261,38 @@
         <f aca="false">CONCATENATE("    ",Q1,", ",R1,", ",S1,", ",T1,", ",U1,", /* ASCII ",N1," (",O1,"), character: ",P1," */")</f>
         <v>    0x00, 0x00, 0x00, 0x00, 0x00, /* ASCII 32 (0x20), character: ' ' */</v>
       </c>
+      <c r="W1" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q1,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X1" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R1,2))</f>
+        <v>0</v>
+      </c>
+      <c r="Y1" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S1,2))</f>
+        <v>0</v>
+      </c>
+      <c r="Z1" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T1,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AA1" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U1,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB1" s="1" t="n">
+        <f aca="false">IF(W1=0,IF(X1=0,IF(Y1=0,IF(Z1=0,IF(AA1=0,1,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC1" s="1" t="n">
+        <f aca="false">IF(AA1=0,IF(Z1=0,IF(Y1=0,IF(X1=0,IF(W1=0,3,1),2),3),4),5)</f>
+        <v>3</v>
+      </c>
+      <c r="AD1" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC1*16)+AB1,2),",")</f>
+        <v>0x31,</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
@@ -322,15 +347,15 @@
       </c>
       <c r="R2" s="2" t="str">
         <f aca="false">INDEX(F:F,$M2+8,1)</f>
-        <v>0xFB</v>
+        <v>0x60</v>
       </c>
       <c r="S2" s="2" t="str">
         <f aca="false">INDEX(G:G,$M2+8,1)</f>
-        <v>0xFB</v>
+        <v>0xFA</v>
       </c>
       <c r="T2" s="2" t="str">
         <f aca="false">INDEX(H:H,$M2+8,1)</f>
-        <v>0x00</v>
+        <v>0x60</v>
       </c>
       <c r="U2" s="2" t="str">
         <f aca="false">INDEX(I:I,$M2+8,1)</f>
@@ -338,7 +363,39 @@
       </c>
       <c r="V2" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q2,", ",R2,", ",S2,", ",T2,", ",U2,", /* ASCII ",N2," (",O2,"), character: ",P2," */")</f>
-        <v>    0x00, 0xFB, 0xFB, 0x00, 0x00, /* ASCII 33 (0x21), character: '!' */</v>
+        <v>    0x00, 0x60, 0xFA, 0x60, 0x00, /* ASCII 33 (0x21), character: '!' */</v>
+      </c>
+      <c r="W2" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q2,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X2" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R2,2))</f>
+        <v>96</v>
+      </c>
+      <c r="Y2" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S2,2))</f>
+        <v>250</v>
+      </c>
+      <c r="Z2" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T2,2))</f>
+        <v>96</v>
+      </c>
+      <c r="AA2" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U2,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB2" s="1" t="n">
+        <f aca="false">IF(W2=0,IF(X2=0,IF(Y2=0,IF(Z2=0,IF(AA2=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC2" s="1" t="n">
+        <f aca="false">IF(AA2=0,IF(Z2=0,IF(Y2=0,IF(X2=0,IF(W2=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD2" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC2*16)+AB2,2),",")</f>
+        <v>0x41,</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -413,6 +470,38 @@
         <f aca="false">CONCATENATE("    ",Q3,", ",R3,", ",S3,", ",T3,", ",U3,", /* ASCII ",N3," (",O3,"), character: ",P3," */")</f>
         <v>    0x20, 0xC0, 0x00, 0x20, 0xC0, /* ASCII 34 (0x22), character: '"' */</v>
       </c>
+      <c r="W3" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q3,2))</f>
+        <v>32</v>
+      </c>
+      <c r="X3" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R3,2))</f>
+        <v>192</v>
+      </c>
+      <c r="Y3" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S3,2))</f>
+        <v>0</v>
+      </c>
+      <c r="Z3" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T3,2))</f>
+        <v>32</v>
+      </c>
+      <c r="AA3" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U3,2))</f>
+        <v>192</v>
+      </c>
+      <c r="AB3" s="1" t="n">
+        <f aca="false">IF(W3=0,IF(X3=0,IF(Y3=0,IF(Z3=0,IF(AA3=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC3" s="1" t="n">
+        <f aca="false">IF(AA3=0,IF(Z3=0,IF(Y3=0,IF(X3=0,IF(W3=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD3" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC3*16)+AB3,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
@@ -472,6 +561,38 @@
         <f aca="false">CONCATENATE("    ",Q4,", ",R4,", ",S4,", ",T4,", ",U4,", /* ASCII ",N4," (",O4,"), character: ",P4," */")</f>
         <v>    0x28, 0x7C, 0x28, 0x7C, 0x28, /* ASCII 35 (0x23), character: '#' */</v>
       </c>
+      <c r="W4" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q4,2))</f>
+        <v>40</v>
+      </c>
+      <c r="X4" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R4,2))</f>
+        <v>124</v>
+      </c>
+      <c r="Y4" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S4,2))</f>
+        <v>40</v>
+      </c>
+      <c r="Z4" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T4,2))</f>
+        <v>124</v>
+      </c>
+      <c r="AA4" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U4,2))</f>
+        <v>40</v>
+      </c>
+      <c r="AB4" s="1" t="n">
+        <f aca="false">IF(W4=0,IF(X4=0,IF(Y4=0,IF(Z4=0,IF(AA4=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC4" s="1" t="n">
+        <f aca="false">IF(AA4=0,IF(Z4=0,IF(Y4=0,IF(X4=0,IF(W4=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD4" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC4*16)+AB4,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0"/>
@@ -531,6 +652,38 @@
         <f aca="false">CONCATENATE("    ",Q5,", ",R5,", ",S5,", ",T5,", ",U5,", /* ASCII ",N5," (",O5,"), character: ",P5," */")</f>
         <v>    0x24, 0x54, 0xFE, 0x54, 0x48, /* ASCII 36 (0x24), character: '$' */</v>
       </c>
+      <c r="W5" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q5,2))</f>
+        <v>36</v>
+      </c>
+      <c r="X5" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R5,2))</f>
+        <v>84</v>
+      </c>
+      <c r="Y5" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S5,2))</f>
+        <v>254</v>
+      </c>
+      <c r="Z5" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T5,2))</f>
+        <v>84</v>
+      </c>
+      <c r="AA5" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U5,2))</f>
+        <v>72</v>
+      </c>
+      <c r="AB5" s="1" t="n">
+        <f aca="false">IF(W5=0,IF(X5=0,IF(Y5=0,IF(Z5=0,IF(AA5=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC5" s="1" t="n">
+        <f aca="false">IF(AA5=0,IF(Z5=0,IF(Y5=0,IF(X5=0,IF(W5=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD5" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC5*16)+AB5,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0"/>
@@ -590,6 +743,38 @@
         <f aca="false">CONCATENATE("    ",Q6,", ",R6,", ",S6,", ",T6,", ",U6,", /* ASCII ",N6," (",O6,"), character: ",P6," */")</f>
         <v>    0x64, 0x68, 0x10, 0x2C, 0x4C, /* ASCII 37 (0x25), character: '%' */</v>
       </c>
+      <c r="W6" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q6,2))</f>
+        <v>100</v>
+      </c>
+      <c r="X6" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R6,2))</f>
+        <v>104</v>
+      </c>
+      <c r="Y6" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S6,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Z6" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T6,2))</f>
+        <v>44</v>
+      </c>
+      <c r="AA6" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U6,2))</f>
+        <v>76</v>
+      </c>
+      <c r="AB6" s="1" t="n">
+        <f aca="false">IF(W6=0,IF(X6=0,IF(Y6=0,IF(Z6=0,IF(AA6=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC6" s="1" t="n">
+        <f aca="false">IF(AA6=0,IF(Z6=0,IF(Y6=0,IF(X6=0,IF(W6=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD6" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC6*16)+AB6,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0"/>
@@ -648,6 +833,38 @@
       <c r="V7" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q7,", ",R7,", ",S7,", ",T7,", ",U7,", /* ASCII ",N7," (",O7,"), character: ",P7," */")</f>
         <v>    0x34, 0x4A, 0x4A, 0x24, 0x0A, /* ASCII 38 (0x26), character: '&amp;' */</v>
+      </c>
+      <c r="W7" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q7,2))</f>
+        <v>52</v>
+      </c>
+      <c r="X7" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R7,2))</f>
+        <v>74</v>
+      </c>
+      <c r="Y7" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S7,2))</f>
+        <v>74</v>
+      </c>
+      <c r="Z7" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T7,2))</f>
+        <v>36</v>
+      </c>
+      <c r="AA7" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U7,2))</f>
+        <v>10</v>
+      </c>
+      <c r="AB7" s="1" t="n">
+        <f aca="false">IF(W7=0,IF(X7=0,IF(Y7=0,IF(Z7=0,IF(AA7=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC7" s="1" t="n">
+        <f aca="false">IF(AA7=0,IF(Z7=0,IF(Y7=0,IF(X7=0,IF(W7=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD7" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC7*16)+AB7,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -705,6 +922,38 @@
         <f aca="false">CONCATENATE("    ",Q8,", ",R8,", ",S8,", ",T8,", ",U8,", /* ASCII ",N8," (",O8,"), character: ",P8," */")</f>
         <v>    0x20, 0xC0, 0x00, 0x00, 0x00, /* ASCII 39 (0x27), character: ''' */</v>
       </c>
+      <c r="W8" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q8,2))</f>
+        <v>32</v>
+      </c>
+      <c r="X8" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R8,2))</f>
+        <v>192</v>
+      </c>
+      <c r="Y8" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S8,2))</f>
+        <v>0</v>
+      </c>
+      <c r="Z8" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T8,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AA8" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U8,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB8" s="1" t="n">
+        <f aca="false">IF(W8=0,IF(X8=0,IF(Y8=0,IF(Z8=0,IF(AA8=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC8" s="1" t="n">
+        <f aca="false">IF(AA8=0,IF(Z8=0,IF(Y8=0,IF(X8=0,IF(W8=0,5,1),2),3),4),5)</f>
+        <v>2</v>
+      </c>
+      <c r="AD8" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC8*16)+AB8,2),",")</f>
+        <v>0x20,</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0"/>
@@ -761,6 +1010,38 @@
         <f aca="false">CONCATENATE("    ",Q9,", ",R9,", ",S9,", ",T9,", ",U9,", /* ASCII ",N9," (",O9,"), character: ",P9," */")</f>
         <v>    0x00, 0x38, 0x44, 0x82, 0x00, /* ASCII 40 (0x28), character: '(' */</v>
       </c>
+      <c r="W9" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q9,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X9" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R9,2))</f>
+        <v>56</v>
+      </c>
+      <c r="Y9" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S9,2))</f>
+        <v>68</v>
+      </c>
+      <c r="Z9" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T9,2))</f>
+        <v>130</v>
+      </c>
+      <c r="AA9" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U9,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB9" s="1" t="n">
+        <f aca="false">IF(W9=0,IF(X9=0,IF(Y9=0,IF(Z9=0,IF(AA9=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC9" s="1" t="n">
+        <f aca="false">IF(AA9=0,IF(Z9=0,IF(Y9=0,IF(X9=0,IF(W9=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD9" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC9*16)+AB9,2),",")</f>
+        <v>0x41,</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0"/>
@@ -816,6 +1097,38 @@
         <f aca="false">CONCATENATE("    ",Q10,", ",R10,", ",S10,", ",T10,", ",U10,", /* ASCII ",N10," (",O10,"), character: ",P10," */")</f>
         <v>    0x00, 0x82, 0x44, 0x38, 0x00, /* ASCII 41 (0x29), character: ')' */</v>
       </c>
+      <c r="W10" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q10,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X10" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R10,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Y10" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S10,2))</f>
+        <v>68</v>
+      </c>
+      <c r="Z10" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T10,2))</f>
+        <v>56</v>
+      </c>
+      <c r="AA10" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U10,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB10" s="1" t="n">
+        <f aca="false">IF(W10=0,IF(X10=0,IF(Y10=0,IF(Z10=0,IF(AA10=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC10" s="1" t="n">
+        <f aca="false">IF(AA10=0,IF(Z10=0,IF(Y10=0,IF(X10=0,IF(W10=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD10" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC10*16)+AB10,2),",")</f>
+        <v>0x41,</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0"/>
@@ -883,6 +1196,38 @@
       <c r="V11" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q11,", ",R11,", ",S11,", ",T11,", ",U11,", /* ASCII ",N11," (",O11,"), character: ",P11," */")</f>
         <v>    0x28, 0x10, 0x7C, 0x10, 0x28, /* ASCII 42 (0x2A), character: '*' */</v>
+      </c>
+      <c r="W11" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q11,2))</f>
+        <v>40</v>
+      </c>
+      <c r="X11" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R11,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Y11" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S11,2))</f>
+        <v>124</v>
+      </c>
+      <c r="Z11" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T11,2))</f>
+        <v>16</v>
+      </c>
+      <c r="AA11" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U11,2))</f>
+        <v>40</v>
+      </c>
+      <c r="AB11" s="1" t="n">
+        <f aca="false">IF(W11=0,IF(X11=0,IF(Y11=0,IF(Z11=0,IF(AA11=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC11" s="1" t="n">
+        <f aca="false">IF(AA11=0,IF(Z11=0,IF(Y11=0,IF(X11=0,IF(W11=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD11" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC11*16)+AB11,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -937,6 +1282,38 @@
         <f aca="false">CONCATENATE("    ",Q12,", ",R12,", ",S12,", ",T12,", ",U12,", /* ASCII ",N12," (",O12,"), character: ",P12," */")</f>
         <v>    0x10, 0x10, 0x7C, 0x10, 0x10, /* ASCII 43 (0x2B), character: '+' */</v>
       </c>
+      <c r="W12" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q12,2))</f>
+        <v>16</v>
+      </c>
+      <c r="X12" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R12,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Y12" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S12,2))</f>
+        <v>124</v>
+      </c>
+      <c r="Z12" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T12,2))</f>
+        <v>16</v>
+      </c>
+      <c r="AA12" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U12,2))</f>
+        <v>16</v>
+      </c>
+      <c r="AB12" s="1" t="n">
+        <f aca="false">IF(W12=0,IF(X12=0,IF(Y12=0,IF(Z12=0,IF(AA12=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC12" s="1" t="n">
+        <f aca="false">IF(AA12=0,IF(Z12=0,IF(Y12=0,IF(X12=0,IF(W12=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD12" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC12*16)+AB12,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0"/>
@@ -1004,6 +1381,38 @@
         <f aca="false">CONCATENATE("    ",Q13,", ",R13,", ",S13,", ",T13,", ",U13,", /* ASCII ",N13," (",O13,"), character: ",P13," */")</f>
         <v>    0x00, 0x0D, 0x0E, 0x00, 0x00, /* ASCII 44 (0x2C), character: ',' */</v>
       </c>
+      <c r="W13" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q13,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X13" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R13,2))</f>
+        <v>13</v>
+      </c>
+      <c r="Y13" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S13,2))</f>
+        <v>14</v>
+      </c>
+      <c r="Z13" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T13,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AA13" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U13,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB13" s="1" t="n">
+        <f aca="false">IF(W13=0,IF(X13=0,IF(Y13=0,IF(Z13=0,IF(AA13=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC13" s="1" t="n">
+        <f aca="false">IF(AA13=0,IF(Z13=0,IF(Y13=0,IF(X13=0,IF(W13=0,5,1),2),3),4),5)</f>
+        <v>3</v>
+      </c>
+      <c r="AD13" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC13*16)+AB13,2),",")</f>
+        <v>0x31,</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
@@ -1023,9 +1432,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="0"/>
-      <c r="F14" s="0" t="n">
-        <v>1</v>
-      </c>
+      <c r="F14" s="0"/>
       <c r="G14" s="2" t="n">
         <v>1</v>
       </c>
@@ -1075,6 +1482,38 @@
       <c r="V14" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q14,", ",R14,", ",S14,", ",T14,", ",U14,", /* ASCII ",N14," (",O14,"), character: ",P14," */")</f>
         <v>    0x10, 0x10, 0x10, 0x10, 0x00, /* ASCII 45 (0x2D), character: '-' */</v>
+      </c>
+      <c r="W14" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q14,2))</f>
+        <v>16</v>
+      </c>
+      <c r="X14" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R14,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Y14" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S14,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Z14" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T14,2))</f>
+        <v>16</v>
+      </c>
+      <c r="AA14" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U14,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB14" s="1" t="n">
+        <f aca="false">IF(W14=0,IF(X14=0,IF(Y14=0,IF(Z14=0,IF(AA14=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC14" s="1" t="n">
+        <f aca="false">IF(AA14=0,IF(Z14=0,IF(Y14=0,IF(X14=0,IF(W14=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD14" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC14*16)+AB14,2),",")</f>
+        <v>0x40,</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1092,11 +1531,13 @@
       <c r="G15" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H15" s="0"/>
+      <c r="H15" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="I15" s="0"/>
       <c r="J15" s="2" t="str">
         <f aca="false">F22</f>
-        <v>0xFB</v>
+        <v>0x60</v>
       </c>
       <c r="L15" s="0"/>
       <c r="M15" s="2" t="n">
@@ -1138,6 +1579,38 @@
       <c r="V15" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q15,", ",R15,", ",S15,", ",T15,", ",U15,", /* ASCII ",N15," (",O15,"), character: ",P15," */")</f>
         <v>    0x00, 0x06, 0x06, 0x00, 0x00, /* ASCII 46 (0x2E), character: '.' */</v>
+      </c>
+      <c r="W15" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q15,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X15" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R15,2))</f>
+        <v>6</v>
+      </c>
+      <c r="Y15" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S15,2))</f>
+        <v>6</v>
+      </c>
+      <c r="Z15" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T15,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AA15" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U15,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB15" s="1" t="n">
+        <f aca="false">IF(W15=0,IF(X15=0,IF(Y15=0,IF(Z15=0,IF(AA15=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC15" s="1" t="n">
+        <f aca="false">IF(AA15=0,IF(Z15=0,IF(Y15=0,IF(X15=0,IF(W15=0,5,1),2),3),4),5)</f>
+        <v>3</v>
+      </c>
+      <c r="AD15" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC15*16)+AB15,2),",")</f>
+        <v>0x31,</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1155,11 +1628,13 @@
       <c r="G16" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H16" s="0"/>
+      <c r="H16" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="I16" s="0"/>
       <c r="J16" s="2" t="str">
         <f aca="false">G22</f>
-        <v>0xFB</v>
+        <v>0xFA</v>
       </c>
       <c r="L16" s="0"/>
       <c r="M16" s="2" t="n">
@@ -1201,6 +1676,38 @@
       <c r="V16" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q16,", ",R16,", ",S16,", ",T16,", ",U16,", /* ASCII ",N16," (",O16,"), character: ",P16," */")</f>
         <v>    0x03, 0x0C, 0x30, 0xC0, 0x00, /* ASCII 47 (0x2F), character: '/' */</v>
+      </c>
+      <c r="W16" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q16,2))</f>
+        <v>3</v>
+      </c>
+      <c r="X16" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R16,2))</f>
+        <v>12</v>
+      </c>
+      <c r="Y16" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S16,2))</f>
+        <v>48</v>
+      </c>
+      <c r="Z16" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T16,2))</f>
+        <v>192</v>
+      </c>
+      <c r="AA16" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U16,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB16" s="1" t="n">
+        <f aca="false">IF(W16=0,IF(X16=0,IF(Y16=0,IF(Z16=0,IF(AA16=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC16" s="1" t="n">
+        <f aca="false">IF(AA16=0,IF(Z16=0,IF(Y16=0,IF(X16=0,IF(W16=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD16" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC16*16)+AB16,2),",")</f>
+        <v>0x40,</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1212,9 +1719,7 @@
         <v>4</v>
       </c>
       <c r="E17" s="0"/>
-      <c r="F17" s="0" t="n">
-        <v>1</v>
-      </c>
+      <c r="F17" s="0"/>
       <c r="G17" s="2" t="n">
         <v>1</v>
       </c>
@@ -1222,7 +1727,7 @@
       <c r="I17" s="0"/>
       <c r="J17" s="2" t="str">
         <f aca="false">H22</f>
-        <v>0x00</v>
+        <v>0x60</v>
       </c>
       <c r="L17" s="0"/>
       <c r="M17" s="2" t="n">
@@ -1264,6 +1769,38 @@
       <c r="V17" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q17,", ",R17,", ",S17,", ",T17,", ",U17,", /* ASCII ",N17," (",O17,"), character: ",P17," */")</f>
         <v>    0x7C, 0x8A, 0x92, 0xA2, 0x7C, /* ASCII 48 (0x30), character: '0' */</v>
+      </c>
+      <c r="W17" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q17,2))</f>
+        <v>124</v>
+      </c>
+      <c r="X17" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R17,2))</f>
+        <v>138</v>
+      </c>
+      <c r="Y17" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S17,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Z17" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T17,2))</f>
+        <v>162</v>
+      </c>
+      <c r="AA17" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U17,2))</f>
+        <v>124</v>
+      </c>
+      <c r="AB17" s="1" t="n">
+        <f aca="false">IF(W17=0,IF(X17=0,IF(Y17=0,IF(Z17=0,IF(AA17=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC17" s="1" t="n">
+        <f aca="false">IF(AA17=0,IF(Z17=0,IF(Y17=0,IF(X17=0,IF(W17=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD17" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC17*16)+AB17,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1275,9 +1812,7 @@
         <v>3</v>
       </c>
       <c r="E18" s="0"/>
-      <c r="F18" s="0" t="n">
-        <v>1</v>
-      </c>
+      <c r="F18" s="0"/>
       <c r="G18" s="2" t="n">
         <v>1</v>
       </c>
@@ -1327,6 +1862,38 @@
       <c r="V18" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q18,", ",R18,", ",S18,", ",T18,", ",U18,", /* ASCII ",N18," (",O18,"), character: ",P18," */")</f>
         <v>    0x00, 0x42, 0xFE, 0x02, 0x00, /* ASCII 49 (0x31), character: '1' */</v>
+      </c>
+      <c r="W18" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q18,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X18" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R18,2))</f>
+        <v>66</v>
+      </c>
+      <c r="Y18" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S18,2))</f>
+        <v>254</v>
+      </c>
+      <c r="Z18" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T18,2))</f>
+        <v>2</v>
+      </c>
+      <c r="AA18" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U18,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB18" s="1" t="n">
+        <f aca="false">IF(W18=0,IF(X18=0,IF(Y18=0,IF(Z18=0,IF(AA18=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC18" s="1" t="n">
+        <f aca="false">IF(AA18=0,IF(Z18=0,IF(Y18=0,IF(X18=0,IF(W18=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD18" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC18*16)+AB18,2),",")</f>
+        <v>0x41,</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1384,6 +1951,38 @@
         <f aca="false">CONCATENATE("    ",Q19,", ",R19,", ",S19,", ",T19,", ",U19,", /* ASCII ",N19," (",O19,"), character: ",P19," */")</f>
         <v>    0x46, 0x8A, 0x92, 0x92, 0x62, /* ASCII 50 (0x32), character: '2' */</v>
       </c>
+      <c r="W19" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q19,2))</f>
+        <v>70</v>
+      </c>
+      <c r="X19" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R19,2))</f>
+        <v>138</v>
+      </c>
+      <c r="Y19" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S19,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Z19" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T19,2))</f>
+        <v>146</v>
+      </c>
+      <c r="AA19" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U19,2))</f>
+        <v>98</v>
+      </c>
+      <c r="AB19" s="1" t="n">
+        <f aca="false">IF(W19=0,IF(X19=0,IF(Y19=0,IF(Z19=0,IF(AA19=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC19" s="1" t="n">
+        <f aca="false">IF(AA19=0,IF(Z19=0,IF(Y19=0,IF(X19=0,IF(W19=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD19" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC19*16)+AB19,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0"/>
@@ -1394,9 +1993,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="0"/>
-      <c r="F20" s="0" t="n">
-        <v>1</v>
-      </c>
+      <c r="F20" s="0"/>
       <c r="G20" s="2" t="n">
         <v>1</v>
       </c>
@@ -1444,8 +2041,40 @@
         <f aca="false">CONCATENATE("    ",Q20,", ",R20,", ",S20,", ",T20,", ",U20,", /* ASCII ",N20," (",O20,"), character: ",P20," */")</f>
         <v>    0x44, 0x92, 0x92, 0x92, 0x6C, /* ASCII 51 (0x33), character: '3' */</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="W20" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q20,2))</f>
+        <v>68</v>
+      </c>
+      <c r="X20" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R20,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Y20" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S20,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Z20" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T20,2))</f>
+        <v>146</v>
+      </c>
+      <c r="AA20" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U20,2))</f>
+        <v>108</v>
+      </c>
+      <c r="AB20" s="1" t="n">
+        <f aca="false">IF(W20=0,IF(X20=0,IF(Y20=0,IF(Z20=0,IF(AA20=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC20" s="1" t="n">
+        <f aca="false">IF(AA20=0,IF(Z20=0,IF(Y20=0,IF(X20=0,IF(W20=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD20" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC20*16)+AB20,2),",")</f>
+        <v>0x50,</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0"/>
       <c r="B21" s="0"/>
       <c r="C21" s="0"/>
@@ -1454,12 +2083,8 @@
         <v>0</v>
       </c>
       <c r="E21" s="0"/>
-      <c r="F21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G21" s="0" t="n">
-        <v>1</v>
-      </c>
+      <c r="F21" s="0"/>
+      <c r="G21" s="0"/>
       <c r="H21" s="0"/>
       <c r="I21" s="0"/>
       <c r="J21" s="0"/>
@@ -1503,6 +2128,38 @@
       <c r="V21" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q21,", ",R21,", ",S21,", ",T21,", ",U21,", /* ASCII ",N21," (",O21,"), character: ",P21," */")</f>
         <v>    0x38, 0xE8, 0xC8, 0xFE, 0x08, /* ASCII 52 (0x34), character: '4' */</v>
+      </c>
+      <c r="W21" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q21,2))</f>
+        <v>56</v>
+      </c>
+      <c r="X21" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R21,2))</f>
+        <v>232</v>
+      </c>
+      <c r="Y21" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S21,2))</f>
+        <v>200</v>
+      </c>
+      <c r="Z21" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T21,2))</f>
+        <v>254</v>
+      </c>
+      <c r="AA21" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U21,2))</f>
+        <v>8</v>
+      </c>
+      <c r="AB21" s="1" t="n">
+        <f aca="false">IF(W21=0,IF(X21=0,IF(Y21=0,IF(Z21=0,IF(AA21=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC21" s="1" t="n">
+        <f aca="false">IF(AA21=0,IF(Z21=0,IF(Y21=0,IF(X21=0,IF(W21=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD21" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC21*16)+AB21,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1516,15 +2173,15 @@
       </c>
       <c r="F22" s="2" t="str">
         <f aca="false">CONCATENATE("0x",DEC2HEX(SUM(IF(F21=1,2^$D21,0),IF(F20=1,2^$D20,0),IF(F19=1,2^$D19,0),IF(F18=1,2^$D18,0),IF(F17=1,2^$D17,0),IF(F16=1,2^$D16,0),IF(F15=1,2^$D15,0),IF(F14=1,2^$D14,0)),2))</f>
-        <v>0xFB</v>
+        <v>0x60</v>
       </c>
       <c r="G22" s="2" t="str">
         <f aca="false">CONCATENATE("0x",DEC2HEX(SUM(IF(G21=1,2^$D21,0),IF(G20=1,2^$D20,0),IF(G19=1,2^$D19,0),IF(G18=1,2^$D18,0),IF(G17=1,2^$D17,0),IF(G16=1,2^$D16,0),IF(G15=1,2^$D15,0),IF(G14=1,2^$D14,0)),2))</f>
-        <v>0xFB</v>
+        <v>0xFA</v>
       </c>
       <c r="H22" s="2" t="str">
         <f aca="false">CONCATENATE("0x",DEC2HEX(SUM(IF(H21=1,2^$D21,0),IF(H20=1,2^$D20,0),IF(H19=1,2^$D19,0),IF(H18=1,2^$D18,0),IF(H17=1,2^$D17,0),IF(H16=1,2^$D16,0),IF(H15=1,2^$D15,0),IF(H14=1,2^$D14,0)),2))</f>
-        <v>0x00</v>
+        <v>0x60</v>
       </c>
       <c r="I22" s="2" t="str">
         <f aca="false">CONCATENATE("0x",DEC2HEX(SUM(IF(I21=1,2^$D21,0),IF(I20=1,2^$D20,0),IF(I19=1,2^$D19,0),IF(I18=1,2^$D18,0),IF(I17=1,2^$D17,0),IF(I16=1,2^$D16,0),IF(I15=1,2^$D15,0),IF(I14=1,2^$D14,0)),2))</f>
@@ -1571,6 +2228,38 @@
       <c r="V22" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q22,", ",R22,", ",S22,", ",T22,", ",U22,", /* ASCII ",N22," (",O22,"), character: ",P22," */")</f>
         <v>    0xF4, 0x92, 0x92, 0x92, 0x8C, /* ASCII 53 (0x35), character: '5' */</v>
+      </c>
+      <c r="W22" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q22,2))</f>
+        <v>244</v>
+      </c>
+      <c r="X22" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R22,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Y22" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S22,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Z22" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T22,2))</f>
+        <v>146</v>
+      </c>
+      <c r="AA22" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U22,2))</f>
+        <v>140</v>
+      </c>
+      <c r="AB22" s="1" t="n">
+        <f aca="false">IF(W22=0,IF(X22=0,IF(Y22=0,IF(Z22=0,IF(AA22=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC22" s="1" t="n">
+        <f aca="false">IF(AA22=0,IF(Z22=0,IF(Y22=0,IF(X22=0,IF(W22=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD22" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC22*16)+AB22,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1625,6 +2314,38 @@
         <f aca="false">CONCATENATE("    ",Q23,", ",R23,", ",S23,", ",T23,", ",U23,", /* ASCII ",N23," (",O23,"), character: ",P23," */")</f>
         <v>    0x7C, 0x92, 0x92, 0x92, 0x4C, /* ASCII 54 (0x36), character: '6' */</v>
       </c>
+      <c r="W23" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q23,2))</f>
+        <v>124</v>
+      </c>
+      <c r="X23" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R23,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Y23" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S23,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Z23" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T23,2))</f>
+        <v>146</v>
+      </c>
+      <c r="AA23" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U23,2))</f>
+        <v>76</v>
+      </c>
+      <c r="AB23" s="1" t="n">
+        <f aca="false">IF(W23=0,IF(X23=0,IF(Y23=0,IF(Z23=0,IF(AA23=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC23" s="1" t="n">
+        <f aca="false">IF(AA23=0,IF(Z23=0,IF(Y23=0,IF(X23=0,IF(W23=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD23" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC23*16)+AB23,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0"/>
@@ -1692,6 +2413,38 @@
         <f aca="false">CONCATENATE("    ",Q24,", ",R24,", ",S24,", ",T24,", ",U24,", /* ASCII ",N24," (",O24,"), character: ",P24," */")</f>
         <v>    0x80, 0x88, 0x9E, 0xA8, 0xC0, /* ASCII 55 (0x37), character: '7' */</v>
       </c>
+      <c r="W24" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q24,2))</f>
+        <v>128</v>
+      </c>
+      <c r="X24" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R24,2))</f>
+        <v>136</v>
+      </c>
+      <c r="Y24" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S24,2))</f>
+        <v>158</v>
+      </c>
+      <c r="Z24" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T24,2))</f>
+        <v>168</v>
+      </c>
+      <c r="AA24" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U24,2))</f>
+        <v>192</v>
+      </c>
+      <c r="AB24" s="1" t="n">
+        <f aca="false">IF(W24=0,IF(X24=0,IF(Y24=0,IF(Z24=0,IF(AA24=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC24" s="1" t="n">
+        <f aca="false">IF(AA24=0,IF(Z24=0,IF(Y24=0,IF(X24=0,IF(W24=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD24" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC24*16)+AB24,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
@@ -1763,6 +2516,38 @@
       <c r="V25" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q25,", ",R25,", ",S25,", ",T25,", ",U25,", /* ASCII ",N25," (",O25,"), character: ",P25," */")</f>
         <v>    0x6C, 0x92, 0x92, 0x92, 0x6C, /* ASCII 56 (0x38), character: '8' */</v>
+      </c>
+      <c r="W25" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q25,2))</f>
+        <v>108</v>
+      </c>
+      <c r="X25" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R25,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Y25" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S25,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Z25" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T25,2))</f>
+        <v>146</v>
+      </c>
+      <c r="AA25" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U25,2))</f>
+        <v>108</v>
+      </c>
+      <c r="AB25" s="1" t="n">
+        <f aca="false">IF(W25=0,IF(X25=0,IF(Y25=0,IF(Z25=0,IF(AA25=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC25" s="1" t="n">
+        <f aca="false">IF(AA25=0,IF(Z25=0,IF(Y25=0,IF(X25=0,IF(W25=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD25" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC25*16)+AB25,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1827,6 +2612,38 @@
         <f aca="false">CONCATENATE("    ",Q26,", ",R26,", ",S26,", ",T26,", ",U26,", /* ASCII ",N26," (",O26,"), character: ",P26," */")</f>
         <v>    0x64, 0x92, 0x92, 0x92, 0x7C, /* ASCII 57 (0x39), character: '9' */</v>
       </c>
+      <c r="W26" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q26,2))</f>
+        <v>100</v>
+      </c>
+      <c r="X26" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R26,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Y26" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S26,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Z26" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T26,2))</f>
+        <v>146</v>
+      </c>
+      <c r="AA26" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U26,2))</f>
+        <v>124</v>
+      </c>
+      <c r="AB26" s="1" t="n">
+        <f aca="false">IF(W26=0,IF(X26=0,IF(Y26=0,IF(Z26=0,IF(AA26=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC26" s="1" t="n">
+        <f aca="false">IF(AA26=0,IF(Z26=0,IF(Y26=0,IF(X26=0,IF(W26=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD26" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC26*16)+AB26,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0"/>
@@ -1889,6 +2706,38 @@
       <c r="V27" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q27,", ",R27,", ",S27,", ",T27,", ",U27,", /* ASCII ",N27," (",O27,"), character: ",P27," */")</f>
         <v>    0x00, 0x6C, 0x6C, 0x00, 0x00, /* ASCII 58 (0x3A), character: ':' */</v>
+      </c>
+      <c r="W27" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q27,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X27" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R27,2))</f>
+        <v>108</v>
+      </c>
+      <c r="Y27" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S27,2))</f>
+        <v>108</v>
+      </c>
+      <c r="Z27" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T27,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AA27" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U27,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB27" s="1" t="n">
+        <f aca="false">IF(W27=0,IF(X27=0,IF(Y27=0,IF(Z27=0,IF(AA27=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC27" s="1" t="n">
+        <f aca="false">IF(AA27=0,IF(Z27=0,IF(Y27=0,IF(X27=0,IF(W27=0,5,1),2),3),4),5)</f>
+        <v>3</v>
+      </c>
+      <c r="AD27" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC27*16)+AB27,2),",")</f>
+        <v>0x31,</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1949,6 +2798,38 @@
         <f aca="false">CONCATENATE("    ",Q28,", ",R28,", ",S28,", ",T28,", ",U28,", /* ASCII ",N28," (",O28,"), character: ",P28," */")</f>
         <v>    0x00, 0x6D, 0x6E, 0x00, 0x00, /* ASCII 59 (0x3B), character: ';' */</v>
       </c>
+      <c r="W28" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q28,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X28" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R28,2))</f>
+        <v>109</v>
+      </c>
+      <c r="Y28" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S28,2))</f>
+        <v>110</v>
+      </c>
+      <c r="Z28" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T28,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AA28" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U28,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB28" s="1" t="n">
+        <f aca="false">IF(W28=0,IF(X28=0,IF(Y28=0,IF(Z28=0,IF(AA28=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC28" s="1" t="n">
+        <f aca="false">IF(AA28=0,IF(Z28=0,IF(Y28=0,IF(X28=0,IF(W28=0,5,1),2),3),4),5)</f>
+        <v>3</v>
+      </c>
+      <c r="AD28" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC28*16)+AB28,2),",")</f>
+        <v>0x31,</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0"/>
@@ -2007,6 +2888,38 @@
       <c r="V29" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q29,", ",R29,", ",S29,", ",T29,", ",U29,", /* ASCII ",N29," (",O29,"), character: ",P29," */")</f>
         <v>    0x00, 0x10, 0x28, 0x44, 0x82, /* ASCII 60 (0x3C), character: '&lt;' */</v>
+      </c>
+      <c r="W29" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q29,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X29" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R29,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Y29" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S29,2))</f>
+        <v>40</v>
+      </c>
+      <c r="Z29" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T29,2))</f>
+        <v>68</v>
+      </c>
+      <c r="AA29" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U29,2))</f>
+        <v>130</v>
+      </c>
+      <c r="AB29" s="1" t="n">
+        <f aca="false">IF(W29=0,IF(X29=0,IF(Y29=0,IF(Z29=0,IF(AA29=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC29" s="1" t="n">
+        <f aca="false">IF(AA29=0,IF(Z29=0,IF(Y29=0,IF(X29=0,IF(W29=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD29" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC29*16)+AB29,2),",")</f>
+        <v>0x51,</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2064,6 +2977,38 @@
         <f aca="false">CONCATENATE("    ",Q30,", ",R30,", ",S30,", ",T30,", ",U30,", /* ASCII ",N30," (",O30,"), character: ",P30," */")</f>
         <v>    0x28, 0x28, 0x28, 0x28, 0x28, /* ASCII 61 (0x3D), character: '=' */</v>
       </c>
+      <c r="W30" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q30,2))</f>
+        <v>40</v>
+      </c>
+      <c r="X30" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R30,2))</f>
+        <v>40</v>
+      </c>
+      <c r="Y30" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S30,2))</f>
+        <v>40</v>
+      </c>
+      <c r="Z30" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T30,2))</f>
+        <v>40</v>
+      </c>
+      <c r="AA30" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U30,2))</f>
+        <v>40</v>
+      </c>
+      <c r="AB30" s="1" t="n">
+        <f aca="false">IF(W30=0,IF(X30=0,IF(Y30=0,IF(Z30=0,IF(AA30=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC30" s="1" t="n">
+        <f aca="false">IF(AA30=0,IF(Z30=0,IF(Y30=0,IF(X30=0,IF(W30=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD30" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC30*16)+AB30,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0"/>
@@ -2120,6 +3065,38 @@
         <f aca="false">CONCATENATE("    ",Q31,", ",R31,", ",S31,", ",T31,", ",U31,", /* ASCII ",N31," (",O31,"), character: ",P31," */")</f>
         <v>    0x82, 0x44, 0x28, 0x10, 0x00, /* ASCII 62 (0x3E), character: '&gt;' */</v>
       </c>
+      <c r="W31" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q31,2))</f>
+        <v>130</v>
+      </c>
+      <c r="X31" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R31,2))</f>
+        <v>68</v>
+      </c>
+      <c r="Y31" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S31,2))</f>
+        <v>40</v>
+      </c>
+      <c r="Z31" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T31,2))</f>
+        <v>16</v>
+      </c>
+      <c r="AA31" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U31,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB31" s="1" t="n">
+        <f aca="false">IF(W31=0,IF(X31=0,IF(Y31=0,IF(Z31=0,IF(AA31=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC31" s="1" t="n">
+        <f aca="false">IF(AA31=0,IF(Z31=0,IF(Y31=0,IF(X31=0,IF(W31=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD31" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC31*16)+AB31,2),",")</f>
+        <v>0x40,</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0"/>
@@ -2176,6 +3153,38 @@
         <f aca="false">CONCATENATE("    ",Q32,", ",R32,", ",S32,", ",T32,", ",U32,", /* ASCII ",N32," (",O32,"), character: ",P32," */")</f>
         <v>    0x40, 0x80, 0x9A, 0xA0, 0x40, /* ASCII 63 (0x3F), character: '?' */</v>
       </c>
+      <c r="W32" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q32,2))</f>
+        <v>64</v>
+      </c>
+      <c r="X32" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R32,2))</f>
+        <v>128</v>
+      </c>
+      <c r="Y32" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S32,2))</f>
+        <v>154</v>
+      </c>
+      <c r="Z32" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T32,2))</f>
+        <v>160</v>
+      </c>
+      <c r="AA32" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U32,2))</f>
+        <v>64</v>
+      </c>
+      <c r="AB32" s="1" t="n">
+        <f aca="false">IF(W32=0,IF(X32=0,IF(Y32=0,IF(Z32=0,IF(AA32=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC32" s="1" t="n">
+        <f aca="false">IF(AA32=0,IF(Z32=0,IF(Y32=0,IF(X32=0,IF(W32=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD32" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC32*16)+AB32,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
@@ -2222,7 +3231,7 @@
       </c>
       <c r="Q33" s="2" t="str">
         <f aca="false">INDEX(E:E,$M33+8,1)</f>
-        <v>0xFE</v>
+        <v>0x7C</v>
       </c>
       <c r="R33" s="2" t="str">
         <f aca="false">INDEX(F:F,$M33+8,1)</f>
@@ -2238,11 +3247,43 @@
       </c>
       <c r="U33" s="2" t="str">
         <f aca="false">INDEX(I:I,$M33+8,1)</f>
-        <v>0xFA</v>
+        <v>0x7A</v>
       </c>
       <c r="V33" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q33,", ",R33,", ",S33,", ",T33,", ",U33,", /* ASCII ",N33," (",O33,"), character: ",P33," */")</f>
-        <v>    0xFE, 0x82, 0xBA, 0xAA, 0xFA, /* ASCII 64 (0x40), character: '@' */</v>
+        <v>    0x7C, 0x82, 0xBA, 0xAA, 0x7A, /* ASCII 64 (0x40), character: '@' */</v>
+      </c>
+      <c r="W33" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q33,2))</f>
+        <v>124</v>
+      </c>
+      <c r="X33" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R33,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Y33" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S33,2))</f>
+        <v>186</v>
+      </c>
+      <c r="Z33" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T33,2))</f>
+        <v>170</v>
+      </c>
+      <c r="AA33" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U33,2))</f>
+        <v>122</v>
+      </c>
+      <c r="AB33" s="1" t="n">
+        <f aca="false">IF(W33=0,IF(X33=0,IF(Y33=0,IF(Z33=0,IF(AA33=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC33" s="1" t="n">
+        <f aca="false">IF(AA33=0,IF(Z33=0,IF(Y33=0,IF(X33=0,IF(W33=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD33" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC33*16)+AB33,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2297,6 +3338,38 @@
         <f aca="false">CONCATENATE("    ",Q34,", ",R34,", ",S34,", ",T34,", ",U34,", /* ASCII ",N34," (",O34,"), character: ",P34," */")</f>
         <v>    0x3E, 0x48, 0x88, 0x48, 0x3E, /* ASCII 65 (0x41), character: 'A' */</v>
       </c>
+      <c r="W34" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q34,2))</f>
+        <v>62</v>
+      </c>
+      <c r="X34" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R34,2))</f>
+        <v>72</v>
+      </c>
+      <c r="Y34" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S34,2))</f>
+        <v>136</v>
+      </c>
+      <c r="Z34" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T34,2))</f>
+        <v>72</v>
+      </c>
+      <c r="AA34" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U34,2))</f>
+        <v>62</v>
+      </c>
+      <c r="AB34" s="1" t="n">
+        <f aca="false">IF(W34=0,IF(X34=0,IF(Y34=0,IF(Z34=0,IF(AA34=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC34" s="1" t="n">
+        <f aca="false">IF(AA34=0,IF(Z34=0,IF(Y34=0,IF(X34=0,IF(W34=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD34" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC34*16)+AB34,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0"/>
@@ -2363,6 +3436,38 @@
       <c r="V35" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q35,", ",R35,", ",S35,", ",T35,", ",U35,", /* ASCII ",N35," (",O35,"), character: ",P35," */")</f>
         <v>    0xFE, 0x92, 0x92, 0x92, 0x6C, /* ASCII 66 (0x42), character: 'B' */</v>
+      </c>
+      <c r="W35" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q35,2))</f>
+        <v>254</v>
+      </c>
+      <c r="X35" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R35,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Y35" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S35,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Z35" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T35,2))</f>
+        <v>146</v>
+      </c>
+      <c r="AA35" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U35,2))</f>
+        <v>108</v>
+      </c>
+      <c r="AB35" s="1" t="n">
+        <f aca="false">IF(W35=0,IF(X35=0,IF(Y35=0,IF(Z35=0,IF(AA35=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC35" s="1" t="n">
+        <f aca="false">IF(AA35=0,IF(Z35=0,IF(Y35=0,IF(X35=0,IF(W35=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD35" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC35*16)+AB35,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2432,6 +3537,38 @@
         <f aca="false">CONCATENATE("    ",Q36,", ",R36,", ",S36,", ",T36,", ",U36,", /* ASCII ",N36," (",O36,"), character: ",P36," */")</f>
         <v>    0x7C, 0x82, 0x82, 0x82, 0x44, /* ASCII 67 (0x43), character: 'C' */</v>
       </c>
+      <c r="W36" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q36,2))</f>
+        <v>124</v>
+      </c>
+      <c r="X36" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R36,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Y36" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S36,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Z36" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T36,2))</f>
+        <v>130</v>
+      </c>
+      <c r="AA36" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U36,2))</f>
+        <v>68</v>
+      </c>
+      <c r="AB36" s="1" t="n">
+        <f aca="false">IF(W36=0,IF(X36=0,IF(Y36=0,IF(Z36=0,IF(AA36=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC36" s="1" t="n">
+        <f aca="false">IF(AA36=0,IF(Z36=0,IF(Y36=0,IF(X36=0,IF(W36=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD36" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC36*16)+AB36,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0"/>
@@ -2495,6 +3632,38 @@
         <f aca="false">CONCATENATE("    ",Q37,", ",R37,", ",S37,", ",T37,", ",U37,", /* ASCII ",N37," (",O37,"), character: ",P37," */")</f>
         <v>    0xFE, 0x82, 0x82, 0x82, 0x7C, /* ASCII 68 (0x44), character: 'D' */</v>
       </c>
+      <c r="W37" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q37,2))</f>
+        <v>254</v>
+      </c>
+      <c r="X37" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R37,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Y37" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S37,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Z37" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T37,2))</f>
+        <v>130</v>
+      </c>
+      <c r="AA37" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U37,2))</f>
+        <v>124</v>
+      </c>
+      <c r="AB37" s="1" t="n">
+        <f aca="false">IF(W37=0,IF(X37=0,IF(Y37=0,IF(Z37=0,IF(AA37=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC37" s="1" t="n">
+        <f aca="false">IF(AA37=0,IF(Z37=0,IF(Y37=0,IF(X37=0,IF(W37=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD37" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC37*16)+AB37,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0"/>
@@ -2564,6 +3733,38 @@
         <f aca="false">CONCATENATE("    ",Q38,", ",R38,", ",S38,", ",T38,", ",U38,", /* ASCII ",N38," (",O38,"), character: ",P38," */")</f>
         <v>    0xFE, 0x92, 0x92, 0x92, 0x82, /* ASCII 69 (0x45), character: 'E' */</v>
       </c>
+      <c r="W38" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q38,2))</f>
+        <v>254</v>
+      </c>
+      <c r="X38" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R38,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Y38" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S38,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Z38" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T38,2))</f>
+        <v>146</v>
+      </c>
+      <c r="AA38" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U38,2))</f>
+        <v>130</v>
+      </c>
+      <c r="AB38" s="1" t="n">
+        <f aca="false">IF(W38=0,IF(X38=0,IF(Y38=0,IF(Z38=0,IF(AA38=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC38" s="1" t="n">
+        <f aca="false">IF(AA38=0,IF(Z38=0,IF(Y38=0,IF(X38=0,IF(W38=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD38" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC38*16)+AB38,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0"/>
@@ -2627,6 +3828,38 @@
         <f aca="false">CONCATENATE("    ",Q39,", ",R39,", ",S39,", ",T39,", ",U39,", /* ASCII ",N39," (",O39,"), character: ",P39," */")</f>
         <v>    0xFE, 0x90, 0x90, 0x90, 0x80, /* ASCII 70 (0x46), character: 'F' */</v>
       </c>
+      <c r="W39" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q39,2))</f>
+        <v>254</v>
+      </c>
+      <c r="X39" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R39,2))</f>
+        <v>144</v>
+      </c>
+      <c r="Y39" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S39,2))</f>
+        <v>144</v>
+      </c>
+      <c r="Z39" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T39,2))</f>
+        <v>144</v>
+      </c>
+      <c r="AA39" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U39,2))</f>
+        <v>128</v>
+      </c>
+      <c r="AB39" s="1" t="n">
+        <f aca="false">IF(W39=0,IF(X39=0,IF(Y39=0,IF(Z39=0,IF(AA39=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC39" s="1" t="n">
+        <f aca="false">IF(AA39=0,IF(Z39=0,IF(Y39=0,IF(X39=0,IF(W39=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD39" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC39*16)+AB39,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0"/>
@@ -2695,6 +3928,38 @@
       <c r="V40" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q40,", ",R40,", ",S40,", ",T40,", ",U40,", /* ASCII ",N40," (",O40,"), character: ",P40," */")</f>
         <v>    0x7C, 0x82, 0x8A, 0x8A, 0x4C, /* ASCII 71 (0x47), character: 'G' */</v>
+      </c>
+      <c r="W40" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q40,2))</f>
+        <v>124</v>
+      </c>
+      <c r="X40" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R40,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Y40" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S40,2))</f>
+        <v>138</v>
+      </c>
+      <c r="Z40" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T40,2))</f>
+        <v>138</v>
+      </c>
+      <c r="AA40" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U40,2))</f>
+        <v>76</v>
+      </c>
+      <c r="AB40" s="1" t="n">
+        <f aca="false">IF(W40=0,IF(X40=0,IF(Y40=0,IF(Z40=0,IF(AA40=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC40" s="1" t="n">
+        <f aca="false">IF(AA40=0,IF(Z40=0,IF(Y40=0,IF(X40=0,IF(W40=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD40" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC40*16)+AB40,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2755,6 +4020,38 @@
       <c r="V41" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q41,", ",R41,", ",S41,", ",T41,", ",U41,", /* ASCII ",N41," (",O41,"), character: ",P41," */")</f>
         <v>    0xFE, 0x10, 0x10, 0x10, 0xFE, /* ASCII 72 (0x48), character: 'H' */</v>
+      </c>
+      <c r="W41" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q41,2))</f>
+        <v>254</v>
+      </c>
+      <c r="X41" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R41,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Y41" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S41,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Z41" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T41,2))</f>
+        <v>16</v>
+      </c>
+      <c r="AA41" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U41,2))</f>
+        <v>254</v>
+      </c>
+      <c r="AB41" s="1" t="n">
+        <f aca="false">IF(W41=0,IF(X41=0,IF(Y41=0,IF(Z41=0,IF(AA41=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC41" s="1" t="n">
+        <f aca="false">IF(AA41=0,IF(Z41=0,IF(Y41=0,IF(X41=0,IF(W41=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD41" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC41*16)+AB41,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2812,6 +4109,38 @@
         <f aca="false">CONCATENATE("    ",Q42,", ",R42,", ",S42,", ",T42,", ",U42,", /* ASCII ",N42," (",O42,"), character: ",P42," */")</f>
         <v>    0x00, 0x82, 0xFE, 0x82, 0x00, /* ASCII 73 (0x49), character: 'I' */</v>
       </c>
+      <c r="W42" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q42,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X42" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R42,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Y42" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S42,2))</f>
+        <v>254</v>
+      </c>
+      <c r="Z42" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T42,2))</f>
+        <v>130</v>
+      </c>
+      <c r="AA42" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U42,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB42" s="1" t="n">
+        <f aca="false">IF(W42=0,IF(X42=0,IF(Y42=0,IF(Z42=0,IF(AA42=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC42" s="1" t="n">
+        <f aca="false">IF(AA42=0,IF(Z42=0,IF(Y42=0,IF(X42=0,IF(W42=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD42" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC42*16)+AB42,2),",")</f>
+        <v>0x41,</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0"/>
@@ -2868,6 +4197,38 @@
         <f aca="false">CONCATENATE("    ",Q43,", ",R43,", ",S43,", ",T43,", ",U43,", /* ASCII ",N43," (",O43,"), character: ",P43," */")</f>
         <v>    0x0C, 0x02, 0x82, 0xFC, 0x80, /* ASCII 74 (0x4A), character: 'J' */</v>
       </c>
+      <c r="W43" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q43,2))</f>
+        <v>12</v>
+      </c>
+      <c r="X43" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R43,2))</f>
+        <v>2</v>
+      </c>
+      <c r="Y43" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S43,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Z43" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T43,2))</f>
+        <v>252</v>
+      </c>
+      <c r="AA43" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U43,2))</f>
+        <v>128</v>
+      </c>
+      <c r="AB43" s="1" t="n">
+        <f aca="false">IF(W43=0,IF(X43=0,IF(Y43=0,IF(Z43=0,IF(AA43=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC43" s="1" t="n">
+        <f aca="false">IF(AA43=0,IF(Z43=0,IF(Y43=0,IF(X43=0,IF(W43=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD43" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC43*16)+AB43,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0"/>
@@ -2935,6 +4296,38 @@
       <c r="V44" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q44,", ",R44,", ",S44,", ",T44,", ",U44,", /* ASCII ",N44," (",O44,"), character: ",P44," */")</f>
         <v>    0xFE, 0x10, 0x28, 0x44, 0x82, /* ASCII 75 (0x4B), character: 'K' */</v>
+      </c>
+      <c r="W44" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q44,2))</f>
+        <v>254</v>
+      </c>
+      <c r="X44" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R44,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Y44" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S44,2))</f>
+        <v>40</v>
+      </c>
+      <c r="Z44" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T44,2))</f>
+        <v>68</v>
+      </c>
+      <c r="AA44" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U44,2))</f>
+        <v>130</v>
+      </c>
+      <c r="AB44" s="1" t="n">
+        <f aca="false">IF(W44=0,IF(X44=0,IF(Y44=0,IF(Z44=0,IF(AA44=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC44" s="1" t="n">
+        <f aca="false">IF(AA44=0,IF(Z44=0,IF(Y44=0,IF(X44=0,IF(W44=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD44" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC44*16)+AB44,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2989,6 +4382,38 @@
         <f aca="false">CONCATENATE("    ",Q45,", ",R45,", ",S45,", ",T45,", ",U45,", /* ASCII ",N45," (",O45,"), character: ",P45," */")</f>
         <v>    0xFE, 0x02, 0x02, 0x02, 0x02, /* ASCII 76 (0x4C), character: 'L' */</v>
       </c>
+      <c r="W45" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q45,2))</f>
+        <v>254</v>
+      </c>
+      <c r="X45" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R45,2))</f>
+        <v>2</v>
+      </c>
+      <c r="Y45" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S45,2))</f>
+        <v>2</v>
+      </c>
+      <c r="Z45" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T45,2))</f>
+        <v>2</v>
+      </c>
+      <c r="AA45" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U45,2))</f>
+        <v>2</v>
+      </c>
+      <c r="AB45" s="1" t="n">
+        <f aca="false">IF(W45=0,IF(X45=0,IF(Y45=0,IF(Z45=0,IF(AA45=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC45" s="1" t="n">
+        <f aca="false">IF(AA45=0,IF(Z45=0,IF(Y45=0,IF(X45=0,IF(W45=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD45" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC45*16)+AB45,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0"/>
@@ -3056,6 +4481,38 @@
         <f aca="false">CONCATENATE("    ",Q46,", ",R46,", ",S46,", ",T46,", ",U46,", /* ASCII ",N46," (",O46,"), character: ",P46," */")</f>
         <v>    0xFE, 0x40, 0x20, 0x40, 0xFE, /* ASCII 77 (0x4D), character: 'M' */</v>
       </c>
+      <c r="W46" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q46,2))</f>
+        <v>254</v>
+      </c>
+      <c r="X46" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R46,2))</f>
+        <v>64</v>
+      </c>
+      <c r="Y46" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S46,2))</f>
+        <v>32</v>
+      </c>
+      <c r="Z46" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T46,2))</f>
+        <v>64</v>
+      </c>
+      <c r="AA46" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U46,2))</f>
+        <v>254</v>
+      </c>
+      <c r="AB46" s="1" t="n">
+        <f aca="false">IF(W46=0,IF(X46=0,IF(Y46=0,IF(Z46=0,IF(AA46=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC46" s="1" t="n">
+        <f aca="false">IF(AA46=0,IF(Z46=0,IF(Y46=0,IF(X46=0,IF(W46=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD46" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC46*16)+AB46,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="n">
@@ -3125,6 +4582,38 @@
       <c r="V47" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q47,", ",R47,", ",S47,", ",T47,", ",U47,", /* ASCII ",N47," (",O47,"), character: ",P47," */")</f>
         <v>    0xFE, 0x20, 0x10, 0x08, 0xFE, /* ASCII 78 (0x4E), character: 'N' */</v>
+      </c>
+      <c r="W47" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q47,2))</f>
+        <v>254</v>
+      </c>
+      <c r="X47" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R47,2))</f>
+        <v>32</v>
+      </c>
+      <c r="Y47" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S47,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Z47" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T47,2))</f>
+        <v>8</v>
+      </c>
+      <c r="AA47" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U47,2))</f>
+        <v>254</v>
+      </c>
+      <c r="AB47" s="1" t="n">
+        <f aca="false">IF(W47=0,IF(X47=0,IF(Y47=0,IF(Z47=0,IF(AA47=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC47" s="1" t="n">
+        <f aca="false">IF(AA47=0,IF(Z47=0,IF(Y47=0,IF(X47=0,IF(W47=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD47" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC47*16)+AB47,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3193,6 +4682,38 @@
         <f aca="false">CONCATENATE("    ",Q48,", ",R48,", ",S48,", ",T48,", ",U48,", /* ASCII ",N48," (",O48,"), character: ",P48," */")</f>
         <v>    0x7C, 0x82, 0x82, 0x82, 0x7C, /* ASCII 79 (0x4F), character: 'O' */</v>
       </c>
+      <c r="W48" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q48,2))</f>
+        <v>124</v>
+      </c>
+      <c r="X48" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R48,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Y48" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S48,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Z48" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T48,2))</f>
+        <v>130</v>
+      </c>
+      <c r="AA48" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U48,2))</f>
+        <v>124</v>
+      </c>
+      <c r="AB48" s="1" t="n">
+        <f aca="false">IF(W48=0,IF(X48=0,IF(Y48=0,IF(Z48=0,IF(AA48=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC48" s="1" t="n">
+        <f aca="false">IF(AA48=0,IF(Z48=0,IF(Y48=0,IF(X48=0,IF(W48=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD48" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC48*16)+AB48,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0"/>
@@ -3256,6 +4777,38 @@
         <f aca="false">CONCATENATE("    ",Q49,", ",R49,", ",S49,", ",T49,", ",U49,", /* ASCII ",N49," (",O49,"), character: ",P49," */")</f>
         <v>    0xFE, 0x90, 0x90, 0x90, 0x60, /* ASCII 80 (0x50), character: 'P' */</v>
       </c>
+      <c r="W49" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q49,2))</f>
+        <v>254</v>
+      </c>
+      <c r="X49" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R49,2))</f>
+        <v>144</v>
+      </c>
+      <c r="Y49" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S49,2))</f>
+        <v>144</v>
+      </c>
+      <c r="Z49" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T49,2))</f>
+        <v>144</v>
+      </c>
+      <c r="AA49" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U49,2))</f>
+        <v>96</v>
+      </c>
+      <c r="AB49" s="1" t="n">
+        <f aca="false">IF(W49=0,IF(X49=0,IF(Y49=0,IF(Z49=0,IF(AA49=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC49" s="1" t="n">
+        <f aca="false">IF(AA49=0,IF(Z49=0,IF(Y49=0,IF(X49=0,IF(W49=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD49" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC49*16)+AB49,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0"/>
@@ -3321,6 +4874,38 @@
         <f aca="false">CONCATENATE("    ",Q50,", ",R50,", ",S50,", ",T50,", ",U50,", /* ASCII ",N50," (",O50,"), character: ",P50," */")</f>
         <v>    0x7C, 0x82, 0x86, 0x82, 0x7D, /* ASCII 81 (0x51), character: 'Q' */</v>
       </c>
+      <c r="W50" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q50,2))</f>
+        <v>124</v>
+      </c>
+      <c r="X50" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R50,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Y50" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S50,2))</f>
+        <v>134</v>
+      </c>
+      <c r="Z50" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T50,2))</f>
+        <v>130</v>
+      </c>
+      <c r="AA50" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U50,2))</f>
+        <v>125</v>
+      </c>
+      <c r="AB50" s="1" t="n">
+        <f aca="false">IF(W50=0,IF(X50=0,IF(Y50=0,IF(Z50=0,IF(AA50=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC50" s="1" t="n">
+        <f aca="false">IF(AA50=0,IF(Z50=0,IF(Y50=0,IF(X50=0,IF(W50=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD50" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC50*16)+AB50,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0"/>
@@ -3383,6 +4968,38 @@
       <c r="V51" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q51,", ",R51,", ",S51,", ",T51,", ",U51,", /* ASCII ",N51," (",O51,"), character: ",P51," */")</f>
         <v>    0xFE, 0x90, 0x90, 0x90, 0x6E, /* ASCII 82 (0x52), character: 'R' */</v>
+      </c>
+      <c r="W51" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q51,2))</f>
+        <v>254</v>
+      </c>
+      <c r="X51" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R51,2))</f>
+        <v>144</v>
+      </c>
+      <c r="Y51" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S51,2))</f>
+        <v>144</v>
+      </c>
+      <c r="Z51" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T51,2))</f>
+        <v>144</v>
+      </c>
+      <c r="AA51" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U51,2))</f>
+        <v>110</v>
+      </c>
+      <c r="AB51" s="1" t="n">
+        <f aca="false">IF(W51=0,IF(X51=0,IF(Y51=0,IF(Z51=0,IF(AA51=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC51" s="1" t="n">
+        <f aca="false">IF(AA51=0,IF(Z51=0,IF(Y51=0,IF(X51=0,IF(W51=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD51" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC51*16)+AB51,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3448,6 +5065,38 @@
         <f aca="false">CONCATENATE("    ",Q52,", ",R52,", ",S52,", ",T52,", ",U52,", /* ASCII ",N52," (",O52,"), character: ",P52," */")</f>
         <v>    0x62, 0x92, 0x92, 0x92, 0x8C, /* ASCII 83 (0x53), character: 'S' */</v>
       </c>
+      <c r="W52" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q52,2))</f>
+        <v>98</v>
+      </c>
+      <c r="X52" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R52,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Y52" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S52,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Z52" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T52,2))</f>
+        <v>146</v>
+      </c>
+      <c r="AA52" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U52,2))</f>
+        <v>140</v>
+      </c>
+      <c r="AB52" s="1" t="n">
+        <f aca="false">IF(W52=0,IF(X52=0,IF(Y52=0,IF(Z52=0,IF(AA52=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC52" s="1" t="n">
+        <f aca="false">IF(AA52=0,IF(Z52=0,IF(Y52=0,IF(X52=0,IF(W52=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD52" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC52*16)+AB52,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0"/>
@@ -3505,6 +5154,38 @@
       <c r="V53" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q53,", ",R53,", ",S53,", ",T53,", ",U53,", /* ASCII ",N53," (",O53,"), character: ",P53," */")</f>
         <v>    0x80, 0x80, 0xFE, 0x80, 0x80, /* ASCII 84 (0x54), character: 'T' */</v>
+      </c>
+      <c r="W53" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q53,2))</f>
+        <v>128</v>
+      </c>
+      <c r="X53" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R53,2))</f>
+        <v>128</v>
+      </c>
+      <c r="Y53" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S53,2))</f>
+        <v>254</v>
+      </c>
+      <c r="Z53" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T53,2))</f>
+        <v>128</v>
+      </c>
+      <c r="AA53" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U53,2))</f>
+        <v>128</v>
+      </c>
+      <c r="AB53" s="1" t="n">
+        <f aca="false">IF(W53=0,IF(X53=0,IF(Y53=0,IF(Z53=0,IF(AA53=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC53" s="1" t="n">
+        <f aca="false">IF(AA53=0,IF(Z53=0,IF(Y53=0,IF(X53=0,IF(W53=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD53" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC53*16)+AB53,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3562,6 +5243,38 @@
         <f aca="false">CONCATENATE("    ",Q54,", ",R54,", ",S54,", ",T54,", ",U54,", /* ASCII ",N54," (",O54,"), character: ",P54," */")</f>
         <v>    0xFC, 0x02, 0x02, 0x02, 0xFC, /* ASCII 85 (0x55), character: 'U' */</v>
       </c>
+      <c r="W54" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q54,2))</f>
+        <v>252</v>
+      </c>
+      <c r="X54" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R54,2))</f>
+        <v>2</v>
+      </c>
+      <c r="Y54" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S54,2))</f>
+        <v>2</v>
+      </c>
+      <c r="Z54" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T54,2))</f>
+        <v>2</v>
+      </c>
+      <c r="AA54" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U54,2))</f>
+        <v>252</v>
+      </c>
+      <c r="AB54" s="1" t="n">
+        <f aca="false">IF(W54=0,IF(X54=0,IF(Y54=0,IF(Z54=0,IF(AA54=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC54" s="1" t="n">
+        <f aca="false">IF(AA54=0,IF(Z54=0,IF(Y54=0,IF(X54=0,IF(W54=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD54" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC54*16)+AB54,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0"/>
@@ -3629,6 +5342,38 @@
       <c r="V55" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q55,", ",R55,", ",S55,", ",T55,", ",U55,", /* ASCII ",N55," (",O55,"), character: ",P55," */")</f>
         <v>    0xE0, 0x38, 0x0E, 0x38, 0xE0, /* ASCII 86 (0x56), character: 'V' */</v>
+      </c>
+      <c r="W55" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q55,2))</f>
+        <v>224</v>
+      </c>
+      <c r="X55" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R55,2))</f>
+        <v>56</v>
+      </c>
+      <c r="Y55" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S55,2))</f>
+        <v>14</v>
+      </c>
+      <c r="Z55" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T55,2))</f>
+        <v>56</v>
+      </c>
+      <c r="AA55" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U55,2))</f>
+        <v>224</v>
+      </c>
+      <c r="AB55" s="1" t="n">
+        <f aca="false">IF(W55=0,IF(X55=0,IF(Y55=0,IF(Z55=0,IF(AA55=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC55" s="1" t="n">
+        <f aca="false">IF(AA55=0,IF(Z55=0,IF(Y55=0,IF(X55=0,IF(W55=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD55" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC55*16)+AB55,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3683,6 +5428,38 @@
         <f aca="false">CONCATENATE("    ",Q56,", ",R56,", ",S56,", ",T56,", ",U56,", /* ASCII ",N56," (",O56,"), character: ",P56," */")</f>
         <v>    0xFC, 0x02, 0x0C, 0x02, 0xFC, /* ASCII 87 (0x57), character: 'W' */</v>
       </c>
+      <c r="W56" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q56,2))</f>
+        <v>252</v>
+      </c>
+      <c r="X56" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R56,2))</f>
+        <v>2</v>
+      </c>
+      <c r="Y56" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S56,2))</f>
+        <v>12</v>
+      </c>
+      <c r="Z56" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T56,2))</f>
+        <v>2</v>
+      </c>
+      <c r="AA56" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U56,2))</f>
+        <v>252</v>
+      </c>
+      <c r="AB56" s="1" t="n">
+        <f aca="false">IF(W56=0,IF(X56=0,IF(Y56=0,IF(Z56=0,IF(AA56=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC56" s="1" t="n">
+        <f aca="false">IF(AA56=0,IF(Z56=0,IF(Y56=0,IF(X56=0,IF(W56=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD56" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC56*16)+AB56,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0"/>
@@ -3749,6 +5526,38 @@
       <c r="V57" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q57,", ",R57,", ",S57,", ",T57,", ",U57,", /* ASCII ",N57," (",O57,"), character: ",P57," */")</f>
         <v>    0xC6, 0x28, 0x10, 0x28, 0xC6, /* ASCII 88 (0x58), character: 'X' */</v>
+      </c>
+      <c r="W57" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q57,2))</f>
+        <v>198</v>
+      </c>
+      <c r="X57" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R57,2))</f>
+        <v>40</v>
+      </c>
+      <c r="Y57" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S57,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Z57" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T57,2))</f>
+        <v>40</v>
+      </c>
+      <c r="AA57" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U57,2))</f>
+        <v>198</v>
+      </c>
+      <c r="AB57" s="1" t="n">
+        <f aca="false">IF(W57=0,IF(X57=0,IF(Y57=0,IF(Z57=0,IF(AA57=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC57" s="1" t="n">
+        <f aca="false">IF(AA57=0,IF(Z57=0,IF(Y57=0,IF(X57=0,IF(W57=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD57" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC57*16)+AB57,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3818,6 +5627,38 @@
         <f aca="false">CONCATENATE("    ",Q58,", ",R58,", ",S58,", ",T58,", ",U58,", /* ASCII ",N58," (",O58,"), character: ",P58," */")</f>
         <v>    0xE0, 0x10, 0x0E, 0x10, 0xE0, /* ASCII 89 (0x59), character: 'Y' */</v>
       </c>
+      <c r="W58" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q58,2))</f>
+        <v>224</v>
+      </c>
+      <c r="X58" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R58,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Y58" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S58,2))</f>
+        <v>14</v>
+      </c>
+      <c r="Z58" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T58,2))</f>
+        <v>16</v>
+      </c>
+      <c r="AA58" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U58,2))</f>
+        <v>224</v>
+      </c>
+      <c r="AB58" s="1" t="n">
+        <f aca="false">IF(W58=0,IF(X58=0,IF(Y58=0,IF(Z58=0,IF(AA58=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC58" s="1" t="n">
+        <f aca="false">IF(AA58=0,IF(Z58=0,IF(Y58=0,IF(X58=0,IF(W58=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD58" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC58*16)+AB58,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0"/>
@@ -3883,6 +5724,38 @@
         <f aca="false">CONCATENATE("    ",Q59,", ",R59,", ",S59,", ",T59,", ",U59,", /* ASCII ",N59," (",O59,"), character: ",P59," */")</f>
         <v>    0x86, 0x8A, 0x92, 0xA2, 0xC2, /* ASCII 90 (0x5A), character: 'Z' */</v>
       </c>
+      <c r="W59" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q59,2))</f>
+        <v>134</v>
+      </c>
+      <c r="X59" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R59,2))</f>
+        <v>138</v>
+      </c>
+      <c r="Y59" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S59,2))</f>
+        <v>146</v>
+      </c>
+      <c r="Z59" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T59,2))</f>
+        <v>162</v>
+      </c>
+      <c r="AA59" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U59,2))</f>
+        <v>194</v>
+      </c>
+      <c r="AB59" s="1" t="n">
+        <f aca="false">IF(W59=0,IF(X59=0,IF(Y59=0,IF(Z59=0,IF(AA59=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC59" s="1" t="n">
+        <f aca="false">IF(AA59=0,IF(Z59=0,IF(Y59=0,IF(X59=0,IF(W59=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD59" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC59*16)+AB59,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0"/>
@@ -3950,6 +5823,38 @@
         <f aca="false">CONCATENATE("    ",Q60,", ",R60,", ",S60,", ",T60,", ",U60,", /* ASCII ",N60," (",O60,"), character: ",P60," */")</f>
         <v>    0x00, 0xFE, 0x82, 0x82, 0x00, /* ASCII 91 (0x5B), character: '[' */</v>
       </c>
+      <c r="W60" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q60,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X60" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R60,2))</f>
+        <v>254</v>
+      </c>
+      <c r="Y60" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S60,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Z60" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T60,2))</f>
+        <v>130</v>
+      </c>
+      <c r="AA60" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U60,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB60" s="1" t="n">
+        <f aca="false">IF(W60=0,IF(X60=0,IF(Y60=0,IF(Z60=0,IF(AA60=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC60" s="1" t="n">
+        <f aca="false">IF(AA60=0,IF(Z60=0,IF(Y60=0,IF(X60=0,IF(W60=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD60" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC60*16)+AB60,2),",")</f>
+        <v>0x41,</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0"/>
@@ -4017,6 +5922,38 @@
         <f aca="false">CONCATENATE("    ",Q61,", ",R61,", ",S61,", ",T61,", ",U61,", /* ASCII ",N61," (",O61,"), character: ",P61," */")</f>
         <v>    0x00, 0xC0, 0x30, 0x0C, 0x03, /* ASCII 92 (0x5C), character: '\' */</v>
       </c>
+      <c r="W61" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q61,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X61" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R61,2))</f>
+        <v>192</v>
+      </c>
+      <c r="Y61" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S61,2))</f>
+        <v>48</v>
+      </c>
+      <c r="Z61" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T61,2))</f>
+        <v>12</v>
+      </c>
+      <c r="AA61" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U61,2))</f>
+        <v>3</v>
+      </c>
+      <c r="AB61" s="1" t="n">
+        <f aca="false">IF(W61=0,IF(X61=0,IF(Y61=0,IF(Z61=0,IF(AA61=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC61" s="1" t="n">
+        <f aca="false">IF(AA61=0,IF(Z61=0,IF(Y61=0,IF(X61=0,IF(W61=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD61" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC61*16)+AB61,2),",")</f>
+        <v>0x51,</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0"/>
@@ -4083,6 +6020,38 @@
       <c r="V62" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q62,", ",R62,", ",S62,", ",T62,", ",U62,", /* ASCII ",N62," (",O62,"), character: ",P62," */")</f>
         <v>    0x00, 0x82, 0x82, 0xFE, 0x00, /* ASCII 93 (0x5D), character: ']' */</v>
+      </c>
+      <c r="W62" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q62,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X62" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R62,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Y62" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S62,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Z62" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T62,2))</f>
+        <v>254</v>
+      </c>
+      <c r="AA62" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U62,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB62" s="1" t="n">
+        <f aca="false">IF(W62=0,IF(X62=0,IF(Y62=0,IF(Z62=0,IF(AA62=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC62" s="1" t="n">
+        <f aca="false">IF(AA62=0,IF(Z62=0,IF(Y62=0,IF(X62=0,IF(W62=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD62" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC62*16)+AB62,2),",")</f>
+        <v>0x41,</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4145,6 +6114,38 @@
       <c r="V63" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q63,", ",R63,", ",S63,", ",T63,", ",U63,", /* ASCII ",N63," (",O63,"), character: ",P63," */")</f>
         <v>    0x10, 0x20, 0x40, 0x20, 0x10, /* ASCII 94 (0x5E), character: '^' */</v>
+      </c>
+      <c r="W63" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q63,2))</f>
+        <v>16</v>
+      </c>
+      <c r="X63" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R63,2))</f>
+        <v>32</v>
+      </c>
+      <c r="Y63" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S63,2))</f>
+        <v>64</v>
+      </c>
+      <c r="Z63" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T63,2))</f>
+        <v>32</v>
+      </c>
+      <c r="AA63" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U63,2))</f>
+        <v>16</v>
+      </c>
+      <c r="AB63" s="1" t="n">
+        <f aca="false">IF(W63=0,IF(X63=0,IF(Y63=0,IF(Z63=0,IF(AA63=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC63" s="1" t="n">
+        <f aca="false">IF(AA63=0,IF(Z63=0,IF(Y63=0,IF(X63=0,IF(W63=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD63" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC63*16)+AB63,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4202,6 +6203,38 @@
         <f aca="false">CONCATENATE("    ",Q64,", ",R64,", ",S64,", ",T64,", ",U64,", /* ASCII ",N64," (",O64,"), character: ",P64," */")</f>
         <v>    0x02, 0x02, 0x02, 0x02, 0x02, /* ASCII 95 (0x5F), character: '_' */</v>
       </c>
+      <c r="W64" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q64,2))</f>
+        <v>2</v>
+      </c>
+      <c r="X64" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R64,2))</f>
+        <v>2</v>
+      </c>
+      <c r="Y64" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S64,2))</f>
+        <v>2</v>
+      </c>
+      <c r="Z64" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T64,2))</f>
+        <v>2</v>
+      </c>
+      <c r="AA64" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U64,2))</f>
+        <v>2</v>
+      </c>
+      <c r="AB64" s="1" t="n">
+        <f aca="false">IF(W64=0,IF(X64=0,IF(Y64=0,IF(Z64=0,IF(AA64=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC64" s="1" t="n">
+        <f aca="false">IF(AA64=0,IF(Z64=0,IF(Y64=0,IF(X64=0,IF(W64=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD64" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC64*16)+AB64,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0"/>
@@ -4258,6 +6291,38 @@
         <f aca="false">CONCATENATE("    ",Q65,", ",R65,", ",S65,", ",T65,", ",U65,", /* ASCII ",N65," (",O65,"), character: ",P65," */")</f>
         <v>    0x00, 0x80, 0x60, 0x00, 0x00, /* ASCII 96 (0x60), character: '`' */</v>
       </c>
+      <c r="W65" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q65,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X65" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R65,2))</f>
+        <v>128</v>
+      </c>
+      <c r="Y65" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S65,2))</f>
+        <v>96</v>
+      </c>
+      <c r="Z65" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T65,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AA65" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U65,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB65" s="1" t="n">
+        <f aca="false">IF(W65=0,IF(X65=0,IF(Y65=0,IF(Z65=0,IF(AA65=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC65" s="1" t="n">
+        <f aca="false">IF(AA65=0,IF(Z65=0,IF(Y65=0,IF(X65=0,IF(W65=0,5,1),2),3),4),5)</f>
+        <v>3</v>
+      </c>
+      <c r="AD65" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC65*16)+AB65,2),",")</f>
+        <v>0x31,</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0"/>
@@ -4325,6 +6390,38 @@
       <c r="V66" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q66,", ",R66,", ",S66,", ",T66,", ",U66,", /* ASCII ",N66," (",O66,"), character: ",P66," */")</f>
         <v>    0x24, 0x4A, 0x4A, 0x3E, 0x00, /* ASCII 97 (0x61), character: 'a' */</v>
+      </c>
+      <c r="W66" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q66,2))</f>
+        <v>36</v>
+      </c>
+      <c r="X66" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R66,2))</f>
+        <v>74</v>
+      </c>
+      <c r="Y66" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S66,2))</f>
+        <v>74</v>
+      </c>
+      <c r="Z66" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T66,2))</f>
+        <v>62</v>
+      </c>
+      <c r="AA66" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U66,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB66" s="1" t="n">
+        <f aca="false">IF(W66=0,IF(X66=0,IF(Y66=0,IF(Z66=0,IF(AA66=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC66" s="1" t="n">
+        <f aca="false">IF(AA66=0,IF(Z66=0,IF(Y66=0,IF(X66=0,IF(W66=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD66" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC66*16)+AB66,2),",")</f>
+        <v>0x40,</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4379,6 +6476,38 @@
         <f aca="false">CONCATENATE("    ",Q67,", ",R67,", ",S67,", ",T67,", ",U67,", /* ASCII ",N67," (",O67,"), character: ",P67," */")</f>
         <v>    0x00, 0xFE, 0x12, 0x12, 0x0C, /* ASCII 98 (0x62), character: 'b' */</v>
       </c>
+      <c r="W67" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q67,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X67" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R67,2))</f>
+        <v>254</v>
+      </c>
+      <c r="Y67" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S67,2))</f>
+        <v>18</v>
+      </c>
+      <c r="Z67" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T67,2))</f>
+        <v>18</v>
+      </c>
+      <c r="AA67" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U67,2))</f>
+        <v>12</v>
+      </c>
+      <c r="AB67" s="1" t="n">
+        <f aca="false">IF(W67=0,IF(X67=0,IF(Y67=0,IF(Z67=0,IF(AA67=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC67" s="1" t="n">
+        <f aca="false">IF(AA67=0,IF(Z67=0,IF(Y67=0,IF(X67=0,IF(W67=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD67" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC67*16)+AB67,2),",")</f>
+        <v>0x51,</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0"/>
@@ -4445,6 +6574,38 @@
       <c r="V68" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q68,", ",R68,", ",S68,", ",T68,", ",U68,", /* ASCII ",N68," (",O68,"), character: ",P68," */")</f>
         <v>    0x0C, 0x12, 0x12, 0x12, 0x00, /* ASCII 99 (0x63), character: 'c' */</v>
+      </c>
+      <c r="W68" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q68,2))</f>
+        <v>12</v>
+      </c>
+      <c r="X68" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R68,2))</f>
+        <v>18</v>
+      </c>
+      <c r="Y68" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S68,2))</f>
+        <v>18</v>
+      </c>
+      <c r="Z68" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T68,2))</f>
+        <v>18</v>
+      </c>
+      <c r="AA68" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U68,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB68" s="1" t="n">
+        <f aca="false">IF(W68=0,IF(X68=0,IF(Y68=0,IF(Z68=0,IF(AA68=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC68" s="1" t="n">
+        <f aca="false">IF(AA68=0,IF(Z68=0,IF(Y68=0,IF(X68=0,IF(W68=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD68" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC68*16)+AB68,2),",")</f>
+        <v>0x40,</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4514,6 +6675,38 @@
         <f aca="false">CONCATENATE("    ",Q69,", ",R69,", ",S69,", ",T69,", ",U69,", /* ASCII ",N69," (",O69,"), character: ",P69," */")</f>
         <v>    0x00, 0x0C, 0x12, 0x12, 0xFE, /* ASCII 100 (0x64), character: 'd' */</v>
       </c>
+      <c r="W69" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q69,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X69" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R69,2))</f>
+        <v>12</v>
+      </c>
+      <c r="Y69" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S69,2))</f>
+        <v>18</v>
+      </c>
+      <c r="Z69" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T69,2))</f>
+        <v>18</v>
+      </c>
+      <c r="AA69" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U69,2))</f>
+        <v>254</v>
+      </c>
+      <c r="AB69" s="1" t="n">
+        <f aca="false">IF(W69=0,IF(X69=0,IF(Y69=0,IF(Z69=0,IF(AA69=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC69" s="1" t="n">
+        <f aca="false">IF(AA69=0,IF(Z69=0,IF(Y69=0,IF(X69=0,IF(W69=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD69" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC69*16)+AB69,2),",")</f>
+        <v>0x51,</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0"/>
@@ -4577,6 +6770,38 @@
         <f aca="false">CONCATENATE("    ",Q70,", ",R70,", ",S70,", ",T70,", ",U70,", /* ASCII ",N70," (",O70,"), character: ",P70," */")</f>
         <v>    0x1C, 0x2A, 0x2A, 0x10, 0x00, /* ASCII 101 (0x65), character: 'e' */</v>
       </c>
+      <c r="W70" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q70,2))</f>
+        <v>28</v>
+      </c>
+      <c r="X70" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R70,2))</f>
+        <v>42</v>
+      </c>
+      <c r="Y70" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S70,2))</f>
+        <v>42</v>
+      </c>
+      <c r="Z70" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T70,2))</f>
+        <v>16</v>
+      </c>
+      <c r="AA70" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U70,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB70" s="1" t="n">
+        <f aca="false">IF(W70=0,IF(X70=0,IF(Y70=0,IF(Z70=0,IF(AA70=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC70" s="1" t="n">
+        <f aca="false">IF(AA70=0,IF(Z70=0,IF(Y70=0,IF(X70=0,IF(W70=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD70" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC70*16)+AB70,2),",")</f>
+        <v>0x40,</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0"/>
@@ -4640,6 +6865,38 @@
         <f aca="false">CONCATENATE("    ",Q71,", ",R71,", ",S71,", ",T71,", ",U71,", /* ASCII ",N71," (",O71,"), character: ",P71," */")</f>
         <v>    0x3E, 0x48, 0x40, 0x20, 0x00, /* ASCII 102 (0x66), character: 'f' */</v>
       </c>
+      <c r="W71" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q71,2))</f>
+        <v>62</v>
+      </c>
+      <c r="X71" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R71,2))</f>
+        <v>72</v>
+      </c>
+      <c r="Y71" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S71,2))</f>
+        <v>64</v>
+      </c>
+      <c r="Z71" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T71,2))</f>
+        <v>32</v>
+      </c>
+      <c r="AA71" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U71,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB71" s="1" t="n">
+        <f aca="false">IF(W71=0,IF(X71=0,IF(Y71=0,IF(Z71=0,IF(AA71=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC71" s="1" t="n">
+        <f aca="false">IF(AA71=0,IF(Z71=0,IF(Y71=0,IF(X71=0,IF(W71=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD71" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC71*16)+AB71,2),",")</f>
+        <v>0x40,</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0"/>
@@ -4701,6 +6958,38 @@
         <f aca="false">CONCATENATE("    ",Q72,", ",R72,", ",S72,", ",T72,", ",U72,", /* ASCII ",N72," (",O72,"), character: ",P72," */")</f>
         <v>    0x12, 0x29, 0x29, 0x3E, 0x00, /* ASCII 103 (0x67), character: 'g' */</v>
       </c>
+      <c r="W72" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q72,2))</f>
+        <v>18</v>
+      </c>
+      <c r="X72" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R72,2))</f>
+        <v>41</v>
+      </c>
+      <c r="Y72" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S72,2))</f>
+        <v>41</v>
+      </c>
+      <c r="Z72" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T72,2))</f>
+        <v>62</v>
+      </c>
+      <c r="AA72" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U72,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB72" s="1" t="n">
+        <f aca="false">IF(W72=0,IF(X72=0,IF(Y72=0,IF(Z72=0,IF(AA72=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC72" s="1" t="n">
+        <f aca="false">IF(AA72=0,IF(Z72=0,IF(Y72=0,IF(X72=0,IF(W72=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD72" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC72*16)+AB72,2),",")</f>
+        <v>0x40,</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0"/>
@@ -4765,6 +7054,38 @@
       <c r="V73" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q73,", ",R73,", ",S73,", ",T73,", ",U73,", /* ASCII ",N73," (",O73,"), character: ",P73," */")</f>
         <v>    0x7E, 0x08, 0x08, 0x06, 0x00, /* ASCII 104 (0x68), character: 'h' */</v>
+      </c>
+      <c r="W73" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q73,2))</f>
+        <v>126</v>
+      </c>
+      <c r="X73" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R73,2))</f>
+        <v>8</v>
+      </c>
+      <c r="Y73" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S73,2))</f>
+        <v>8</v>
+      </c>
+      <c r="Z73" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T73,2))</f>
+        <v>6</v>
+      </c>
+      <c r="AA73" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U73,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB73" s="1" t="n">
+        <f aca="false">IF(W73=0,IF(X73=0,IF(Y73=0,IF(Z73=0,IF(AA73=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC73" s="1" t="n">
+        <f aca="false">IF(AA73=0,IF(Z73=0,IF(Y73=0,IF(X73=0,IF(W73=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD73" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC73*16)+AB73,2),",")</f>
+        <v>0x40,</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4826,6 +7147,38 @@
         <f aca="false">CONCATENATE("    ",Q74,", ",R74,", ",S74,", ",T74,", ",U74,", /* ASCII ",N74," (",O74,"), character: ",P74," */")</f>
         <v>    0x00, 0x12, 0x5E, 0x02, 0x00, /* ASCII 105 (0x69), character: 'i' */</v>
       </c>
+      <c r="W74" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q74,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X74" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R74,2))</f>
+        <v>18</v>
+      </c>
+      <c r="Y74" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S74,2))</f>
+        <v>94</v>
+      </c>
+      <c r="Z74" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T74,2))</f>
+        <v>2</v>
+      </c>
+      <c r="AA74" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U74,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB74" s="1" t="n">
+        <f aca="false">IF(W74=0,IF(X74=0,IF(Y74=0,IF(Z74=0,IF(AA74=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC74" s="1" t="n">
+        <f aca="false">IF(AA74=0,IF(Z74=0,IF(Y74=0,IF(X74=0,IF(W74=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD74" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC74*16)+AB74,2),",")</f>
+        <v>0x41,</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0"/>
@@ -4887,6 +7240,38 @@
       <c r="V75" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q75,", ",R75,", ",S75,", ",T75,", ",U75,", /* ASCII ",N75," (",O75,"), character: ",P75," */")</f>
         <v>    0x00, 0x02, 0x11, 0x5E, 0x10, /* ASCII 106 (0x6A), character: 'j' */</v>
+      </c>
+      <c r="W75" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q75,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X75" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R75,2))</f>
+        <v>2</v>
+      </c>
+      <c r="Y75" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S75,2))</f>
+        <v>17</v>
+      </c>
+      <c r="Z75" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T75,2))</f>
+        <v>94</v>
+      </c>
+      <c r="AA75" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U75,2))</f>
+        <v>16</v>
+      </c>
+      <c r="AB75" s="1" t="n">
+        <f aca="false">IF(W75=0,IF(X75=0,IF(Y75=0,IF(Z75=0,IF(AA75=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC75" s="1" t="n">
+        <f aca="false">IF(AA75=0,IF(Z75=0,IF(Y75=0,IF(X75=0,IF(W75=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD75" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC75*16)+AB75,2),",")</f>
+        <v>0x51,</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4944,6 +7329,38 @@
         <f aca="false">CONCATENATE("    ",Q76,", ",R76,", ",S76,", ",T76,", ",U76,", /* ASCII ",N76," (",O76,"), character: ",P76," */")</f>
         <v>    0x00, 0xFE, 0x08, 0x16, 0x00, /* ASCII 107 (0x6B), character: 'k' */</v>
       </c>
+      <c r="W76" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q76,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X76" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R76,2))</f>
+        <v>254</v>
+      </c>
+      <c r="Y76" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S76,2))</f>
+        <v>8</v>
+      </c>
+      <c r="Z76" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T76,2))</f>
+        <v>22</v>
+      </c>
+      <c r="AA76" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U76,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB76" s="1" t="n">
+        <f aca="false">IF(W76=0,IF(X76=0,IF(Y76=0,IF(Z76=0,IF(AA76=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC76" s="1" t="n">
+        <f aca="false">IF(AA76=0,IF(Z76=0,IF(Y76=0,IF(X76=0,IF(W76=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD76" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC76*16)+AB76,2),",")</f>
+        <v>0x41,</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0"/>
@@ -5011,6 +7428,38 @@
       <c r="V77" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q77,", ",R77,", ",S77,", ",T77,", ",U77,", /* ASCII ",N77," (",O77,"), character: ",P77," */")</f>
         <v>    0x00, 0x42, 0x7E, 0x02, 0x00, /* ASCII 108 (0x6C), character: 'l' */</v>
+      </c>
+      <c r="W77" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q77,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X77" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R77,2))</f>
+        <v>66</v>
+      </c>
+      <c r="Y77" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S77,2))</f>
+        <v>126</v>
+      </c>
+      <c r="Z77" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T77,2))</f>
+        <v>2</v>
+      </c>
+      <c r="AA77" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U77,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB77" s="1" t="n">
+        <f aca="false">IF(W77=0,IF(X77=0,IF(Y77=0,IF(Z77=0,IF(AA77=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC77" s="1" t="n">
+        <f aca="false">IF(AA77=0,IF(Z77=0,IF(Y77=0,IF(X77=0,IF(W77=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD77" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC77*16)+AB77,2),",")</f>
+        <v>0x41,</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5065,6 +7514,38 @@
         <f aca="false">CONCATENATE("    ",Q78,", ",R78,", ",S78,", ",T78,", ",U78,", /* ASCII ",N78," (",O78,"), character: ",P78," */")</f>
         <v>    0x1E, 0x10, 0x0E, 0x10, 0x0E, /* ASCII 109 (0x6D), character: 'm' */</v>
       </c>
+      <c r="W78" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q78,2))</f>
+        <v>30</v>
+      </c>
+      <c r="X78" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R78,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Y78" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S78,2))</f>
+        <v>14</v>
+      </c>
+      <c r="Z78" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T78,2))</f>
+        <v>16</v>
+      </c>
+      <c r="AA78" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U78,2))</f>
+        <v>14</v>
+      </c>
+      <c r="AB78" s="1" t="n">
+        <f aca="false">IF(W78=0,IF(X78=0,IF(Y78=0,IF(Z78=0,IF(AA78=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC78" s="1" t="n">
+        <f aca="false">IF(AA78=0,IF(Z78=0,IF(Y78=0,IF(X78=0,IF(W78=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD78" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC78*16)+AB78,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0"/>
@@ -5132,6 +7613,38 @@
         <f aca="false">CONCATENATE("    ",Q79,", ",R79,", ",S79,", ",T79,", ",U79,", /* ASCII ",N79," (",O79,"), character: ",P79," */")</f>
         <v>    0x1E, 0x10, 0x10, 0x0E, 0x00, /* ASCII 110 (0x6E), character: 'n' */</v>
       </c>
+      <c r="W79" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q79,2))</f>
+        <v>30</v>
+      </c>
+      <c r="X79" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R79,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Y79" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S79,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Z79" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T79,2))</f>
+        <v>14</v>
+      </c>
+      <c r="AA79" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U79,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB79" s="1" t="n">
+        <f aca="false">IF(W79=0,IF(X79=0,IF(Y79=0,IF(Z79=0,IF(AA79=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC79" s="1" t="n">
+        <f aca="false">IF(AA79=0,IF(Z79=0,IF(Y79=0,IF(X79=0,IF(W79=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD79" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC79*16)+AB79,2),",")</f>
+        <v>0x40,</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="n">
@@ -5201,6 +7714,38 @@
       <c r="V80" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q80,", ",R80,", ",S80,", ",T80,", ",U80,", /* ASCII ",N80," (",O80,"), character: ",P80," */")</f>
         <v>    0x0C, 0x12, 0x12, 0x0C, 0x00, /* ASCII 111 (0x6F), character: 'o' */</v>
+      </c>
+      <c r="W80" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q80,2))</f>
+        <v>12</v>
+      </c>
+      <c r="X80" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R80,2))</f>
+        <v>18</v>
+      </c>
+      <c r="Y80" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S80,2))</f>
+        <v>18</v>
+      </c>
+      <c r="Z80" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T80,2))</f>
+        <v>12</v>
+      </c>
+      <c r="AA80" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U80,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB80" s="1" t="n">
+        <f aca="false">IF(W80=0,IF(X80=0,IF(Y80=0,IF(Z80=0,IF(AA80=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC80" s="1" t="n">
+        <f aca="false">IF(AA80=0,IF(Z80=0,IF(Y80=0,IF(X80=0,IF(W80=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD80" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC80*16)+AB80,2),",")</f>
+        <v>0x40,</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5263,6 +7808,38 @@
         <f aca="false">CONCATENATE("    ",Q81,", ",R81,", ",S81,", ",T81,", ",U81,", /* ASCII ",N81," (",O81,"), character: ",P81," */")</f>
         <v>    0x00, 0x3F, 0x24, 0x24, 0x18, /* ASCII 112 (0x70), character: 'p' */</v>
       </c>
+      <c r="W81" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q81,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X81" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R81,2))</f>
+        <v>63</v>
+      </c>
+      <c r="Y81" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S81,2))</f>
+        <v>36</v>
+      </c>
+      <c r="Z81" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T81,2))</f>
+        <v>36</v>
+      </c>
+      <c r="AA81" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U81,2))</f>
+        <v>24</v>
+      </c>
+      <c r="AB81" s="1" t="n">
+        <f aca="false">IF(W81=0,IF(X81=0,IF(Y81=0,IF(Z81=0,IF(AA81=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC81" s="1" t="n">
+        <f aca="false">IF(AA81=0,IF(Z81=0,IF(Y81=0,IF(X81=0,IF(W81=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD81" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC81*16)+AB81,2),",")</f>
+        <v>0x51,</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0"/>
@@ -5323,6 +7900,38 @@
       <c r="V82" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q82,", ",R82,", ",S82,", ",T82,", ",U82,", /* ASCII ",N82," (",O82,"), character: ",P82," */")</f>
         <v>    0x18, 0x24, 0x24, 0x3F, 0x00, /* ASCII 113 (0x71), character: 'q' */</v>
+      </c>
+      <c r="W82" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q82,2))</f>
+        <v>24</v>
+      </c>
+      <c r="X82" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R82,2))</f>
+        <v>36</v>
+      </c>
+      <c r="Y82" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S82,2))</f>
+        <v>36</v>
+      </c>
+      <c r="Z82" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T82,2))</f>
+        <v>63</v>
+      </c>
+      <c r="AA82" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U82,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB82" s="1" t="n">
+        <f aca="false">IF(W82=0,IF(X82=0,IF(Y82=0,IF(Z82=0,IF(AA82=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC82" s="1" t="n">
+        <f aca="false">IF(AA82=0,IF(Z82=0,IF(Y82=0,IF(X82=0,IF(W82=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD82" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC82*16)+AB82,2),",")</f>
+        <v>0x40,</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5383,6 +7992,38 @@
         <f aca="false">CONCATENATE("    ",Q83,", ",R83,", ",S83,", ",T83,", ",U83,", /* ASCII ",N83," (",O83,"), character: ",P83," */")</f>
         <v>    0x1E, 0x08, 0x10, 0x08, 0x00, /* ASCII 114 (0x72), character: 'r' */</v>
       </c>
+      <c r="W83" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q83,2))</f>
+        <v>30</v>
+      </c>
+      <c r="X83" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R83,2))</f>
+        <v>8</v>
+      </c>
+      <c r="Y83" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S83,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Z83" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T83,2))</f>
+        <v>8</v>
+      </c>
+      <c r="AA83" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U83,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB83" s="1" t="n">
+        <f aca="false">IF(W83=0,IF(X83=0,IF(Y83=0,IF(Z83=0,IF(AA83=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC83" s="1" t="n">
+        <f aca="false">IF(AA83=0,IF(Z83=0,IF(Y83=0,IF(X83=0,IF(W83=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD83" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC83*16)+AB83,2),",")</f>
+        <v>0x40,</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0"/>
@@ -5441,6 +8082,38 @@
       <c r="V84" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q84,", ",R84,", ",S84,", ",T84,", ",U84,", /* ASCII ",N84," (",O84,"), character: ",P84," */")</f>
         <v>    0x12, 0x2A, 0x2A, 0x24, 0x00, /* ASCII 115 (0x73), character: 's' */</v>
+      </c>
+      <c r="W84" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q84,2))</f>
+        <v>18</v>
+      </c>
+      <c r="X84" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R84,2))</f>
+        <v>42</v>
+      </c>
+      <c r="Y84" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S84,2))</f>
+        <v>42</v>
+      </c>
+      <c r="Z84" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T84,2))</f>
+        <v>36</v>
+      </c>
+      <c r="AA84" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U84,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB84" s="1" t="n">
+        <f aca="false">IF(W84=0,IF(X84=0,IF(Y84=0,IF(Z84=0,IF(AA84=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC84" s="1" t="n">
+        <f aca="false">IF(AA84=0,IF(Z84=0,IF(Y84=0,IF(X84=0,IF(W84=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD84" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC84*16)+AB84,2),",")</f>
+        <v>0x40,</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5498,6 +8171,38 @@
         <f aca="false">CONCATENATE("    ",Q85,", ",R85,", ",S85,", ",T85,", ",U85,", /* ASCII ",N85," (",O85,"), character: ",P85," */")</f>
         <v>    0x10, 0x3E, 0x11, 0x02, 0x00, /* ASCII 116 (0x74), character: 't' */</v>
       </c>
+      <c r="W85" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q85,2))</f>
+        <v>16</v>
+      </c>
+      <c r="X85" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R85,2))</f>
+        <v>62</v>
+      </c>
+      <c r="Y85" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S85,2))</f>
+        <v>17</v>
+      </c>
+      <c r="Z85" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T85,2))</f>
+        <v>2</v>
+      </c>
+      <c r="AA85" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U85,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB85" s="1" t="n">
+        <f aca="false">IF(W85=0,IF(X85=0,IF(Y85=0,IF(Z85=0,IF(AA85=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC85" s="1" t="n">
+        <f aca="false">IF(AA85=0,IF(Z85=0,IF(Y85=0,IF(X85=0,IF(W85=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD85" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC85*16)+AB85,2),",")</f>
+        <v>0x40,</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0"/>
@@ -5554,6 +8259,38 @@
         <f aca="false">CONCATENATE("    ",Q86,", ",R86,", ",S86,", ",T86,", ",U86,", /* ASCII ",N86," (",O86,"), character: ",P86," */")</f>
         <v>    0x1C, 0x02, 0x02, 0x1C, 0x00, /* ASCII 117 (0x75), character: 'u' */</v>
       </c>
+      <c r="W86" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q86,2))</f>
+        <v>28</v>
+      </c>
+      <c r="X86" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R86,2))</f>
+        <v>2</v>
+      </c>
+      <c r="Y86" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S86,2))</f>
+        <v>2</v>
+      </c>
+      <c r="Z86" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T86,2))</f>
+        <v>28</v>
+      </c>
+      <c r="AA86" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U86,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB86" s="1" t="n">
+        <f aca="false">IF(W86=0,IF(X86=0,IF(Y86=0,IF(Z86=0,IF(AA86=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC86" s="1" t="n">
+        <f aca="false">IF(AA86=0,IF(Z86=0,IF(Y86=0,IF(X86=0,IF(W86=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD86" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC86*16)+AB86,2),",")</f>
+        <v>0x40,</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0"/>
@@ -5610,6 +8347,38 @@
         <f aca="false">CONCATENATE("    ",Q87,", ",R87,", ",S87,", ",T87,", ",U87,", /* ASCII ",N87," (",O87,"), character: ",P87," */")</f>
         <v>    0x18, 0x04, 0x02, 0x04, 0x18, /* ASCII 118 (0x76), character: 'v' */</v>
       </c>
+      <c r="W87" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q87,2))</f>
+        <v>24</v>
+      </c>
+      <c r="X87" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R87,2))</f>
+        <v>4</v>
+      </c>
+      <c r="Y87" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S87,2))</f>
+        <v>2</v>
+      </c>
+      <c r="Z87" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T87,2))</f>
+        <v>4</v>
+      </c>
+      <c r="AA87" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U87,2))</f>
+        <v>24</v>
+      </c>
+      <c r="AB87" s="1" t="n">
+        <f aca="false">IF(W87=0,IF(X87=0,IF(Y87=0,IF(Z87=0,IF(AA87=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC87" s="1" t="n">
+        <f aca="false">IF(AA87=0,IF(Z87=0,IF(Y87=0,IF(X87=0,IF(W87=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD87" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC87*16)+AB87,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0"/>
@@ -5677,6 +8446,38 @@
       <c r="V88" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q88,", ",R88,", ",S88,", ",T88,", ",U88,", /* ASCII ",N88," (",O88,"), character: ",P88," */")</f>
         <v>    0x1C, 0x02, 0x1C, 0x02, 0x1C, /* ASCII 119 (0x77), character: 'w' */</v>
+      </c>
+      <c r="W88" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q88,2))</f>
+        <v>28</v>
+      </c>
+      <c r="X88" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R88,2))</f>
+        <v>2</v>
+      </c>
+      <c r="Y88" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S88,2))</f>
+        <v>28</v>
+      </c>
+      <c r="Z88" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T88,2))</f>
+        <v>2</v>
+      </c>
+      <c r="AA88" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U88,2))</f>
+        <v>28</v>
+      </c>
+      <c r="AB88" s="1" t="n">
+        <f aca="false">IF(W88=0,IF(X88=0,IF(Y88=0,IF(Z88=0,IF(AA88=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC88" s="1" t="n">
+        <f aca="false">IF(AA88=0,IF(Z88=0,IF(Y88=0,IF(X88=0,IF(W88=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD88" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC88*16)+AB88,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5731,6 +8532,38 @@
         <f aca="false">CONCATENATE("    ",Q89,", ",R89,", ",S89,", ",T89,", ",U89,", /* ASCII ",N89," (",O89,"), character: ",P89," */")</f>
         <v>    0x22, 0x14, 0x08, 0x14, 0x22, /* ASCII 120 (0x78), character: 'x' */</v>
       </c>
+      <c r="W89" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q89,2))</f>
+        <v>34</v>
+      </c>
+      <c r="X89" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R89,2))</f>
+        <v>20</v>
+      </c>
+      <c r="Y89" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S89,2))</f>
+        <v>8</v>
+      </c>
+      <c r="Z89" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T89,2))</f>
+        <v>20</v>
+      </c>
+      <c r="AA89" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U89,2))</f>
+        <v>34</v>
+      </c>
+      <c r="AB89" s="1" t="n">
+        <f aca="false">IF(W89=0,IF(X89=0,IF(Y89=0,IF(Z89=0,IF(AA89=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC89" s="1" t="n">
+        <f aca="false">IF(AA89=0,IF(Z89=0,IF(Y89=0,IF(X89=0,IF(W89=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD89" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC89*16)+AB89,2),",")</f>
+        <v>0x50,</v>
+      </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0"/>
@@ -5798,6 +8631,38 @@
         <f aca="false">CONCATENATE("    ",Q90,", ",R90,", ",S90,", ",T90,", ",U90,", /* ASCII ",N90," (",O90,"), character: ",P90," */")</f>
         <v>    0x39, 0x05, 0x05, 0x3E, 0x00, /* ASCII 121 (0x79), character: 'y' */</v>
       </c>
+      <c r="W90" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q90,2))</f>
+        <v>57</v>
+      </c>
+      <c r="X90" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R90,2))</f>
+        <v>5</v>
+      </c>
+      <c r="Y90" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S90,2))</f>
+        <v>5</v>
+      </c>
+      <c r="Z90" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T90,2))</f>
+        <v>62</v>
+      </c>
+      <c r="AA90" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U90,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB90" s="1" t="n">
+        <f aca="false">IF(W90=0,IF(X90=0,IF(Y90=0,IF(Z90=0,IF(AA90=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC90" s="1" t="n">
+        <f aca="false">IF(AA90=0,IF(Z90=0,IF(Y90=0,IF(X90=0,IF(W90=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD90" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC90*16)+AB90,2),",")</f>
+        <v>0x40,</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="n">
@@ -5867,6 +8732,38 @@
       <c r="V91" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q91,", ",R91,", ",S91,", ",T91,", ",U91,", /* ASCII ",N91," (",O91,"), character: ",P91," */")</f>
         <v>    0x00, 0x26, 0x2A, 0x32, 0x00, /* ASCII 122 (0x7A), character: 'z' */</v>
+      </c>
+      <c r="W91" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q91,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X91" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R91,2))</f>
+        <v>38</v>
+      </c>
+      <c r="Y91" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S91,2))</f>
+        <v>42</v>
+      </c>
+      <c r="Z91" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T91,2))</f>
+        <v>50</v>
+      </c>
+      <c r="AA91" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U91,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB91" s="1" t="n">
+        <f aca="false">IF(W91=0,IF(X91=0,IF(Y91=0,IF(Z91=0,IF(AA91=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC91" s="1" t="n">
+        <f aca="false">IF(AA91=0,IF(Z91=0,IF(Y91=0,IF(X91=0,IF(W91=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD91" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC91*16)+AB91,2),",")</f>
+        <v>0x41,</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5929,6 +8826,38 @@
         <f aca="false">CONCATENATE("    ",Q92,", ",R92,", ",S92,", ",T92,", ",U92,", /* ASCII ",N92," (",O92,"), character: ",P92," */")</f>
         <v>    0x00, 0x10, 0x7C, 0x82, 0x00, /* ASCII 123 (0x7B), character: '{' */</v>
       </c>
+      <c r="W92" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q92,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X92" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R92,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Y92" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S92,2))</f>
+        <v>124</v>
+      </c>
+      <c r="Z92" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T92,2))</f>
+        <v>130</v>
+      </c>
+      <c r="AA92" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U92,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB92" s="1" t="n">
+        <f aca="false">IF(W92=0,IF(X92=0,IF(Y92=0,IF(Z92=0,IF(AA92=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC92" s="1" t="n">
+        <f aca="false">IF(AA92=0,IF(Z92=0,IF(Y92=0,IF(X92=0,IF(W92=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD92" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC92*16)+AB92,2),",")</f>
+        <v>0x41,</v>
+      </c>
     </row>
     <row r="93" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0"/>
@@ -5990,6 +8919,38 @@
         <f aca="false">CONCATENATE("    ",Q93,", ",R93,", ",S93,", ",T93,", ",U93,", /* ASCII ",N93," (",O93,"), character: ",P93," */")</f>
         <v>    0x00, 0x00, 0xFF, 0x00, 0x00, /* ASCII 124 (0x7C), character: '|' */</v>
       </c>
+      <c r="W93" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q93,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X93" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R93,2))</f>
+        <v>0</v>
+      </c>
+      <c r="Y93" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S93,2))</f>
+        <v>255</v>
+      </c>
+      <c r="Z93" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T93,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AA93" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U93,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB93" s="1" t="n">
+        <f aca="false">IF(W93=0,IF(X93=0,IF(Y93=0,IF(Z93=0,IF(AA93=0,0,4),3),2),1),0)</f>
+        <v>2</v>
+      </c>
+      <c r="AC93" s="1" t="n">
+        <f aca="false">IF(AA93=0,IF(Z93=0,IF(Y93=0,IF(X93=0,IF(W93=0,5,1),2),3),4),5)</f>
+        <v>3</v>
+      </c>
+      <c r="AD93" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC93*16)+AB93,2),",")</f>
+        <v>0x32,</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0"/>
@@ -6051,6 +9012,38 @@
         <f aca="false">CONCATENATE("    ",Q94,", ",R94,", ",S94,", ",T94,", ",U94,", /* ASCII ",N94," (",O94,"), character: ",P94," */")</f>
         <v>    0x00, 0x82, 0x7C, 0x10, 0x00, /* ASCII 125 (0x7D), character: '}' */</v>
       </c>
+      <c r="W94" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q94,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X94" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R94,2))</f>
+        <v>130</v>
+      </c>
+      <c r="Y94" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S94,2))</f>
+        <v>124</v>
+      </c>
+      <c r="Z94" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T94,2))</f>
+        <v>16</v>
+      </c>
+      <c r="AA94" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U94,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB94" s="1" t="n">
+        <f aca="false">IF(W94=0,IF(X94=0,IF(Y94=0,IF(Z94=0,IF(AA94=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC94" s="1" t="n">
+        <f aca="false">IF(AA94=0,IF(Z94=0,IF(Y94=0,IF(X94=0,IF(W94=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD94" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC94*16)+AB94,2),",")</f>
+        <v>0x41,</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0"/>
@@ -6111,6 +9104,38 @@
       <c r="V95" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q95,", ",R95,", ",S95,", ",T95,", ",U95,", /* ASCII ",N95," (",O95,"), character: ",P95," */")</f>
         <v>    0x10, 0x20, 0x10, 0x08, 0x10, /* ASCII 126 (0x7E), character: '~' */</v>
+      </c>
+      <c r="W95" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q95,2))</f>
+        <v>16</v>
+      </c>
+      <c r="X95" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R95,2))</f>
+        <v>32</v>
+      </c>
+      <c r="Y95" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S95,2))</f>
+        <v>16</v>
+      </c>
+      <c r="Z95" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T95,2))</f>
+        <v>8</v>
+      </c>
+      <c r="AA95" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U95,2))</f>
+        <v>16</v>
+      </c>
+      <c r="AB95" s="1" t="n">
+        <f aca="false">IF(W95=0,IF(X95=0,IF(Y95=0,IF(Z95=0,IF(AA95=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC95" s="1" t="n">
+        <f aca="false">IF(AA95=0,IF(Z95=0,IF(Y95=0,IF(X95=0,IF(W95=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD95" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC95*16)+AB95,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6170,6 +9195,38 @@
         <f aca="false">CONCATENATE("    ",Q96,", ",R96,", ",S96,", ",T96,", ",U96,", /* ASCII ",N96," (",O96,"), character: ",P96," */")</f>
         <v>    0x00, 0xE0, 0xA0, 0xE0, 0x00, /* ASCII 127 (0x7F), character: '' */</v>
       </c>
+      <c r="W96" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q96,2))</f>
+        <v>0</v>
+      </c>
+      <c r="X96" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R96,2))</f>
+        <v>224</v>
+      </c>
+      <c r="Y96" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S96,2))</f>
+        <v>160</v>
+      </c>
+      <c r="Z96" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T96,2))</f>
+        <v>224</v>
+      </c>
+      <c r="AA96" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U96,2))</f>
+        <v>0</v>
+      </c>
+      <c r="AB96" s="1" t="n">
+        <f aca="false">IF(W96=0,IF(X96=0,IF(Y96=0,IF(Z96=0,IF(AA96=0,0,4),3),2),1),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC96" s="1" t="n">
+        <f aca="false">IF(AA96=0,IF(Z96=0,IF(Y96=0,IF(X96=0,IF(W96=0,5,1),2),3),4),5)</f>
+        <v>4</v>
+      </c>
+      <c r="AD96" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC96*16)+AB96,2),",")</f>
+        <v>0x41,</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0"/>
@@ -6227,6 +9284,38 @@
       <c r="V97" s="3" t="str">
         <f aca="false">CONCATENATE("    ",Q97,", ",R97,", ",S97,", ",T97,", ",U97,", /* ASCII ",N97," (",O97,"), character: ",P97," */")</f>
         <v>    0x28, 0x7C, 0xAA, 0x82, 0x44, /* ASCII 128 (0x80), character: '€' */</v>
+      </c>
+      <c r="W97" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(Q97,2))</f>
+        <v>40</v>
+      </c>
+      <c r="X97" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(R97,2))</f>
+        <v>124</v>
+      </c>
+      <c r="Y97" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(S97,2))</f>
+        <v>170</v>
+      </c>
+      <c r="Z97" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(T97,2))</f>
+        <v>130</v>
+      </c>
+      <c r="AA97" s="1" t="n">
+        <f aca="false">HEX2DEC(RIGHT(U97,2))</f>
+        <v>68</v>
+      </c>
+      <c r="AB97" s="1" t="n">
+        <f aca="false">IF(W97=0,IF(X97=0,IF(Y97=0,IF(Z97=0,IF(AA97=0,0,4),3),2),1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC97" s="1" t="n">
+        <f aca="false">IF(AA97=0,IF(Z97=0,IF(Y97=0,IF(X97=0,IF(W97=0,5,1),2),3),4),5)</f>
+        <v>5</v>
+      </c>
+      <c r="AD97" s="1" t="str">
+        <f aca="false">CONCATENATE("0x",DEC2HEX((AC97*16)+AB97,2),",")</f>
+        <v>0x50,</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12217,9 +15306,7 @@
         <f aca="false">D$3</f>
         <v>7</v>
       </c>
-      <c r="E355" s="0" t="n">
-        <v>1</v>
-      </c>
+      <c r="E355" s="0"/>
       <c r="F355" s="0" t="n">
         <v>1</v>
       </c>
@@ -12229,12 +15316,10 @@
       <c r="H355" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I355" s="0" t="n">
-        <v>1</v>
-      </c>
+      <c r="I355" s="0"/>
       <c r="J355" s="2" t="str">
         <f aca="false">E363</f>
-        <v>0xFE</v>
+        <v>0x7C</v>
       </c>
       <c r="L355" s="0"/>
       <c r="Q355" s="0"/>
@@ -12340,7 +15425,7 @@
       </c>
       <c r="J359" s="2" t="str">
         <f aca="false">I363</f>
-        <v>0xFA</v>
+        <v>0x7A</v>
       </c>
       <c r="L359" s="0"/>
       <c r="Q359" s="0"/>
@@ -12372,9 +15457,7 @@
         <f aca="false">D$9</f>
         <v>1</v>
       </c>
-      <c r="E361" s="0" t="n">
-        <v>1</v>
-      </c>
+      <c r="E361" s="0"/>
       <c r="F361" s="0" t="n">
         <v>1</v>
       </c>
@@ -12415,7 +15498,7 @@
       <c r="D363" s="0"/>
       <c r="E363" s="2" t="str">
         <f aca="false">CONCATENATE("0x",DEC2HEX(SUM(IF(E362=1,2^$D362,0),IF(E361=1,2^$D361,0),IF(E360=1,2^$D360,0),IF(E359=1,2^$D359,0),IF(E358=1,2^$D358,0),IF(E357=1,2^$D357,0),IF(E356=1,2^$D356,0),IF(E355=1,2^$D355,0)),2))</f>
-        <v>0xFE</v>
+        <v>0x7C</v>
       </c>
       <c r="F363" s="2" t="str">
         <f aca="false">CONCATENATE("0x",DEC2HEX(SUM(IF(F362=1,2^$D362,0),IF(F361=1,2^$D361,0),IF(F360=1,2^$D360,0),IF(F359=1,2^$D359,0),IF(F358=1,2^$D358,0),IF(F357=1,2^$D357,0),IF(F356=1,2^$D356,0),IF(F355=1,2^$D355,0)),2))</f>
@@ -12431,7 +15514,7 @@
       </c>
       <c r="I363" s="2" t="str">
         <f aca="false">CONCATENATE("0x",DEC2HEX(SUM(IF(I362=1,2^$D362,0),IF(I361=1,2^$D361,0),IF(I360=1,2^$D360,0),IF(I359=1,2^$D359,0),IF(I358=1,2^$D358,0),IF(I357=1,2^$D357,0),IF(I356=1,2^$D356,0),IF(I355=1,2^$D355,0)),2))</f>
-        <v>0xFA</v>
+        <v>0x7A</v>
       </c>
       <c r="J363" s="0"/>
       <c r="L363" s="0"/>
@@ -28715,7 +31798,7 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="str">
         <f aca="false">Sheet1!V2</f>
-        <v>    0x00, 0xFB, 0xFB, 0x00, 0x00, /* ASCII 33 (0x21), character: '!' */</v>
+        <v>    0x00, 0x60, 0xFA, 0x60, 0x00, /* ASCII 33 (0x21), character: '!' */</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28901,7 +31984,7 @@
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="str">
         <f aca="false">Sheet1!V33</f>
-        <v>    0xFE, 0x82, 0xBA, 0xAA, 0xFA, /* ASCII 64 (0x40), character: '@' */</v>
+        <v>    0x7C, 0x82, 0xBA, 0xAA, 0x7A, /* ASCII 64 (0x40), character: '@' */</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Slight change to character creator
Changing to add brackets around the lines of character creator as it is
a multidimensional array, and doing the initializer as a single
dimension array causes some warnings.
</commit_message>
<xml_diff>
--- a/CharCreator.xlsx
+++ b/CharCreator.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -49,7 +49,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -90,6 +90,13 @@
       <color rgb="FF000000"/>
       <name val="Monospace"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -135,7 +142,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -152,6 +159,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -163,12 +174,7 @@
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <font>
-        <sz val="10"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
 </styleSheet>
@@ -181,8 +187,8 @@
   </sheetPr>
   <dimension ref="A1:AD1067"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A337" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V364" activeCellId="0" sqref="V364"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A59" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AH103" activeCellId="0" sqref="AH103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -258,8 +264,8 @@
         <v>0x00</v>
       </c>
       <c r="V1" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q1,", ",R1,", ",S1,", ",T1,", ",U1,", /* ASCII ",N1," (",O1,"), character: ",P1," */")</f>
-        <v>    0x00, 0x00, 0x00, 0x00, 0x00, /* ASCII 32 (0x20), character: ' ' */</v>
+        <f aca="false">CONCATENATE("    { ",Q1,", ",R1,", ",S1,", ",T1,", ",U1," }, /* ASCII ",N1," (",O1,"), character: ",P1," */")</f>
+        <v>    { 0x00, 0x00, 0x00, 0x00, 0x00 }, /* ASCII 32 (0x20), character: ' ' */</v>
       </c>
       <c r="W1" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q1,2))</f>
@@ -362,8 +368,8 @@
         <v>0x00</v>
       </c>
       <c r="V2" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q2,", ",R2,", ",S2,", ",T2,", ",U2,", /* ASCII ",N2," (",O2,"), character: ",P2," */")</f>
-        <v>    0x00, 0x60, 0xFA, 0x60, 0x00, /* ASCII 33 (0x21), character: '!' */</v>
+        <f aca="false">CONCATENATE("    { ",Q2,", ",R2,", ",S2,", ",T2,", ",U2," }, /* ASCII ",N2," (",O2,"), character: ",P2," */")</f>
+        <v>    { 0x00, 0x60, 0xFA, 0x60, 0x00 }, /* ASCII 33 (0x21), character: '!' */</v>
       </c>
       <c r="W2" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q2,2))</f>
@@ -467,8 +473,8 @@
         <v>0xC0</v>
       </c>
       <c r="V3" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q3,", ",R3,", ",S3,", ",T3,", ",U3,", /* ASCII ",N3," (",O3,"), character: ",P3," */")</f>
-        <v>    0x20, 0xC0, 0x00, 0x20, 0xC0, /* ASCII 34 (0x22), character: '"' */</v>
+        <f aca="false">CONCATENATE("    { ",Q3,", ",R3,", ",S3,", ",T3,", ",U3," }, /* ASCII ",N3," (",O3,"), character: ",P3," */")</f>
+        <v>    { 0x20, 0xC0, 0x00, 0x20, 0xC0 }, /* ASCII 34 (0x22), character: '"' */</v>
       </c>
       <c r="W3" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q3,2))</f>
@@ -558,8 +564,8 @@
         <v>0x28</v>
       </c>
       <c r="V4" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q4,", ",R4,", ",S4,", ",T4,", ",U4,", /* ASCII ",N4," (",O4,"), character: ",P4," */")</f>
-        <v>    0x28, 0x7C, 0x28, 0x7C, 0x28, /* ASCII 35 (0x23), character: '#' */</v>
+        <f aca="false">CONCATENATE("    { ",Q4,", ",R4,", ",S4,", ",T4,", ",U4," }, /* ASCII ",N4," (",O4,"), character: ",P4," */")</f>
+        <v>    { 0x28, 0x7C, 0x28, 0x7C, 0x28 }, /* ASCII 35 (0x23), character: '#' */</v>
       </c>
       <c r="W4" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q4,2))</f>
@@ -649,8 +655,8 @@
         <v>0x48</v>
       </c>
       <c r="V5" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q5,", ",R5,", ",S5,", ",T5,", ",U5,", /* ASCII ",N5," (",O5,"), character: ",P5," */")</f>
-        <v>    0x24, 0x54, 0xFE, 0x54, 0x48, /* ASCII 36 (0x24), character: '$' */</v>
+        <f aca="false">CONCATENATE("    { ",Q5,", ",R5,", ",S5,", ",T5,", ",U5," }, /* ASCII ",N5," (",O5,"), character: ",P5," */")</f>
+        <v>    { 0x24, 0x54, 0xFE, 0x54, 0x48 }, /* ASCII 36 (0x24), character: '$' */</v>
       </c>
       <c r="W5" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q5,2))</f>
@@ -740,8 +746,8 @@
         <v>0x4C</v>
       </c>
       <c r="V6" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q6,", ",R6,", ",S6,", ",T6,", ",U6,", /* ASCII ",N6," (",O6,"), character: ",P6," */")</f>
-        <v>    0x64, 0x68, 0x10, 0x2C, 0x4C, /* ASCII 37 (0x25), character: '%' */</v>
+        <f aca="false">CONCATENATE("    { ",Q6,", ",R6,", ",S6,", ",T6,", ",U6," }, /* ASCII ",N6," (",O6,"), character: ",P6," */")</f>
+        <v>    { 0x64, 0x68, 0x10, 0x2C, 0x4C }, /* ASCII 37 (0x25), character: '%' */</v>
       </c>
       <c r="W6" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q6,2))</f>
@@ -831,8 +837,8 @@
         <v>0x0A</v>
       </c>
       <c r="V7" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q7,", ",R7,", ",S7,", ",T7,", ",U7,", /* ASCII ",N7," (",O7,"), character: ",P7," */")</f>
-        <v>    0x34, 0x4A, 0x4A, 0x24, 0x0A, /* ASCII 38 (0x26), character: '&amp;' */</v>
+        <f aca="false">CONCATENATE("    { ",Q7,", ",R7,", ",S7,", ",T7,", ",U7," }, /* ASCII ",N7," (",O7,"), character: ",P7," */")</f>
+        <v>    { 0x34, 0x4A, 0x4A, 0x24, 0x0A }, /* ASCII 38 (0x26), character: '&amp;' */</v>
       </c>
       <c r="W7" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q7,2))</f>
@@ -919,8 +925,8 @@
         <v>0x00</v>
       </c>
       <c r="V8" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q8,", ",R8,", ",S8,", ",T8,", ",U8,", /* ASCII ",N8," (",O8,"), character: ",P8," */")</f>
-        <v>    0x20, 0xC0, 0x00, 0x00, 0x00, /* ASCII 39 (0x27), character: ''' */</v>
+        <f aca="false">CONCATENATE("    { ",Q8,", ",R8,", ",S8,", ",T8,", ",U8," }, /* ASCII ",N8," (",O8,"), character: ",P8," */")</f>
+        <v>    { 0x20, 0xC0, 0x00, 0x00, 0x00 }, /* ASCII 39 (0x27), character: ''' */</v>
       </c>
       <c r="W8" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q8,2))</f>
@@ -1007,8 +1013,8 @@
         <v>0x00</v>
       </c>
       <c r="V9" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q9,", ",R9,", ",S9,", ",T9,", ",U9,", /* ASCII ",N9," (",O9,"), character: ",P9," */")</f>
-        <v>    0x00, 0x38, 0x44, 0x82, 0x00, /* ASCII 40 (0x28), character: '(' */</v>
+        <f aca="false">CONCATENATE("    { ",Q9,", ",R9,", ",S9,", ",T9,", ",U9," }, /* ASCII ",N9," (",O9,"), character: ",P9," */")</f>
+        <v>    { 0x00, 0x38, 0x44, 0x82, 0x00 }, /* ASCII 40 (0x28), character: '(' */</v>
       </c>
       <c r="W9" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q9,2))</f>
@@ -1094,8 +1100,8 @@
         <v>0x00</v>
       </c>
       <c r="V10" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q10,", ",R10,", ",S10,", ",T10,", ",U10,", /* ASCII ",N10," (",O10,"), character: ",P10," */")</f>
-        <v>    0x00, 0x82, 0x44, 0x38, 0x00, /* ASCII 41 (0x29), character: ')' */</v>
+        <f aca="false">CONCATENATE("    { ",Q10,", ",R10,", ",S10,", ",T10,", ",U10," }, /* ASCII ",N10," (",O10,"), character: ",P10," */")</f>
+        <v>    { 0x00, 0x82, 0x44, 0x38, 0x00 }, /* ASCII 41 (0x29), character: ')' */</v>
       </c>
       <c r="W10" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q10,2))</f>
@@ -1194,8 +1200,8 @@
         <v>0x28</v>
       </c>
       <c r="V11" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q11,", ",R11,", ",S11,", ",T11,", ",U11,", /* ASCII ",N11," (",O11,"), character: ",P11," */")</f>
-        <v>    0x28, 0x10, 0x7C, 0x10, 0x28, /* ASCII 42 (0x2A), character: '*' */</v>
+        <f aca="false">CONCATENATE("    { ",Q11,", ",R11,", ",S11,", ",T11,", ",U11," }, /* ASCII ",N11," (",O11,"), character: ",P11," */")</f>
+        <v>    { 0x28, 0x10, 0x7C, 0x10, 0x28 }, /* ASCII 42 (0x2A), character: '*' */</v>
       </c>
       <c r="W11" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q11,2))</f>
@@ -1279,8 +1285,8 @@
         <v>0x10</v>
       </c>
       <c r="V12" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q12,", ",R12,", ",S12,", ",T12,", ",U12,", /* ASCII ",N12," (",O12,"), character: ",P12," */")</f>
-        <v>    0x10, 0x10, 0x7C, 0x10, 0x10, /* ASCII 43 (0x2B), character: '+' */</v>
+        <f aca="false">CONCATENATE("    { ",Q12,", ",R12,", ",S12,", ",T12,", ",U12," }, /* ASCII ",N12," (",O12,"), character: ",P12," */")</f>
+        <v>    { 0x10, 0x10, 0x7C, 0x10, 0x10 }, /* ASCII 43 (0x2B), character: '+' */</v>
       </c>
       <c r="W12" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q12,2))</f>
@@ -1378,8 +1384,8 @@
         <v>0x00</v>
       </c>
       <c r="V13" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q13,", ",R13,", ",S13,", ",T13,", ",U13,", /* ASCII ",N13," (",O13,"), character: ",P13," */")</f>
-        <v>    0x00, 0x0D, 0x0E, 0x00, 0x00, /* ASCII 44 (0x2C), character: ',' */</v>
+        <f aca="false">CONCATENATE("    { ",Q13,", ",R13,", ",S13,", ",T13,", ",U13," }, /* ASCII ",N13," (",O13,"), character: ",P13," */")</f>
+        <v>    { 0x00, 0x0D, 0x0E, 0x00, 0x00 }, /* ASCII 44 (0x2C), character: ',' */</v>
       </c>
       <c r="W13" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q13,2))</f>
@@ -1480,8 +1486,8 @@
         <v>0x00</v>
       </c>
       <c r="V14" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q14,", ",R14,", ",S14,", ",T14,", ",U14,", /* ASCII ",N14," (",O14,"), character: ",P14," */")</f>
-        <v>    0x10, 0x10, 0x10, 0x10, 0x00, /* ASCII 45 (0x2D), character: '-' */</v>
+        <f aca="false">CONCATENATE("    { ",Q14,", ",R14,", ",S14,", ",T14,", ",U14," }, /* ASCII ",N14," (",O14,"), character: ",P14," */")</f>
+        <v>    { 0x10, 0x10, 0x10, 0x10, 0x00 }, /* ASCII 45 (0x2D), character: '-' */</v>
       </c>
       <c r="W14" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q14,2))</f>
@@ -1577,8 +1583,8 @@
         <v>0x00</v>
       </c>
       <c r="V15" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q15,", ",R15,", ",S15,", ",T15,", ",U15,", /* ASCII ",N15," (",O15,"), character: ",P15," */")</f>
-        <v>    0x00, 0x06, 0x06, 0x00, 0x00, /* ASCII 46 (0x2E), character: '.' */</v>
+        <f aca="false">CONCATENATE("    { ",Q15,", ",R15,", ",S15,", ",T15,", ",U15," }, /* ASCII ",N15," (",O15,"), character: ",P15," */")</f>
+        <v>    { 0x00, 0x06, 0x06, 0x00, 0x00 }, /* ASCII 46 (0x2E), character: '.' */</v>
       </c>
       <c r="W15" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q15,2))</f>
@@ -1674,8 +1680,8 @@
         <v>0x00</v>
       </c>
       <c r="V16" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q16,", ",R16,", ",S16,", ",T16,", ",U16,", /* ASCII ",N16," (",O16,"), character: ",P16," */")</f>
-        <v>    0x03, 0x0C, 0x30, 0xC0, 0x00, /* ASCII 47 (0x2F), character: '/' */</v>
+        <f aca="false">CONCATENATE("    { ",Q16,", ",R16,", ",S16,", ",T16,", ",U16," }, /* ASCII ",N16," (",O16,"), character: ",P16," */")</f>
+        <v>    { 0x03, 0x0C, 0x30, 0xC0, 0x00 }, /* ASCII 47 (0x2F), character: '/' */</v>
       </c>
       <c r="W16" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q16,2))</f>
@@ -1767,8 +1773,8 @@
         <v>0x7C</v>
       </c>
       <c r="V17" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q17,", ",R17,", ",S17,", ",T17,", ",U17,", /* ASCII ",N17," (",O17,"), character: ",P17," */")</f>
-        <v>    0x7C, 0x8A, 0x92, 0xA2, 0x7C, /* ASCII 48 (0x30), character: '0' */</v>
+        <f aca="false">CONCATENATE("    { ",Q17,", ",R17,", ",S17,", ",T17,", ",U17," }, /* ASCII ",N17," (",O17,"), character: ",P17," */")</f>
+        <v>    { 0x7C, 0x8A, 0x92, 0xA2, 0x7C }, /* ASCII 48 (0x30), character: '0' */</v>
       </c>
       <c r="W17" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q17,2))</f>
@@ -1860,8 +1866,8 @@
         <v>0x00</v>
       </c>
       <c r="V18" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q18,", ",R18,", ",S18,", ",T18,", ",U18,", /* ASCII ",N18," (",O18,"), character: ",P18," */")</f>
-        <v>    0x00, 0x42, 0xFE, 0x02, 0x00, /* ASCII 49 (0x31), character: '1' */</v>
+        <f aca="false">CONCATENATE("    { ",Q18,", ",R18,", ",S18,", ",T18,", ",U18," }, /* ASCII ",N18," (",O18,"), character: ",P18," */")</f>
+        <v>    { 0x00, 0x42, 0xFE, 0x02, 0x00 }, /* ASCII 49 (0x31), character: '1' */</v>
       </c>
       <c r="W18" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q18,2))</f>
@@ -1948,8 +1954,8 @@
         <v>0x62</v>
       </c>
       <c r="V19" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q19,", ",R19,", ",S19,", ",T19,", ",U19,", /* ASCII ",N19," (",O19,"), character: ",P19," */")</f>
-        <v>    0x46, 0x8A, 0x92, 0x92, 0x62, /* ASCII 50 (0x32), character: '2' */</v>
+        <f aca="false">CONCATENATE("    { ",Q19,", ",R19,", ",S19,", ",T19,", ",U19," }, /* ASCII ",N19," (",O19,"), character: ",P19," */")</f>
+        <v>    { 0x46, 0x8A, 0x92, 0x92, 0x62 }, /* ASCII 50 (0x32), character: '2' */</v>
       </c>
       <c r="W19" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q19,2))</f>
@@ -2038,8 +2044,8 @@
         <v>0x6C</v>
       </c>
       <c r="V20" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q20,", ",R20,", ",S20,", ",T20,", ",U20,", /* ASCII ",N20," (",O20,"), character: ",P20," */")</f>
-        <v>    0x44, 0x92, 0x92, 0x92, 0x6C, /* ASCII 51 (0x33), character: '3' */</v>
+        <f aca="false">CONCATENATE("    { ",Q20,", ",R20,", ",S20,", ",T20,", ",U20," }, /* ASCII ",N20," (",O20,"), character: ",P20," */")</f>
+        <v>    { 0x44, 0x92, 0x92, 0x92, 0x6C }, /* ASCII 51 (0x33), character: '3' */</v>
       </c>
       <c r="W20" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q20,2))</f>
@@ -2126,8 +2132,8 @@
         <v>0x08</v>
       </c>
       <c r="V21" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q21,", ",R21,", ",S21,", ",T21,", ",U21,", /* ASCII ",N21," (",O21,"), character: ",P21," */")</f>
-        <v>    0x38, 0xE8, 0xC8, 0xFE, 0x08, /* ASCII 52 (0x34), character: '4' */</v>
+        <f aca="false">CONCATENATE("    { ",Q21,", ",R21,", ",S21,", ",T21,", ",U21," }, /* ASCII ",N21," (",O21,"), character: ",P21," */")</f>
+        <v>    { 0x38, 0xE8, 0xC8, 0xFE, 0x08 }, /* ASCII 52 (0x34), character: '4' */</v>
       </c>
       <c r="W21" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q21,2))</f>
@@ -2226,8 +2232,8 @@
         <v>0x8C</v>
       </c>
       <c r="V22" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q22,", ",R22,", ",S22,", ",T22,", ",U22,", /* ASCII ",N22," (",O22,"), character: ",P22," */")</f>
-        <v>    0xF4, 0x92, 0x92, 0x92, 0x8C, /* ASCII 53 (0x35), character: '5' */</v>
+        <f aca="false">CONCATENATE("    { ",Q22,", ",R22,", ",S22,", ",T22,", ",U22," }, /* ASCII ",N22," (",O22,"), character: ",P22," */")</f>
+        <v>    { 0xF4, 0x92, 0x92, 0x92, 0x8C }, /* ASCII 53 (0x35), character: '5' */</v>
       </c>
       <c r="W22" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q22,2))</f>
@@ -2311,8 +2317,8 @@
         <v>0x4C</v>
       </c>
       <c r="V23" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q23,", ",R23,", ",S23,", ",T23,", ",U23,", /* ASCII ",N23," (",O23,"), character: ",P23," */")</f>
-        <v>    0x7C, 0x92, 0x92, 0x92, 0x4C, /* ASCII 54 (0x36), character: '6' */</v>
+        <f aca="false">CONCATENATE("    { ",Q23,", ",R23,", ",S23,", ",T23,", ",U23," }, /* ASCII ",N23," (",O23,"), character: ",P23," */")</f>
+        <v>    { 0x7C, 0x92, 0x92, 0x92, 0x4C }, /* ASCII 54 (0x36), character: '6' */</v>
       </c>
       <c r="W23" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q23,2))</f>
@@ -2410,8 +2416,8 @@
         <v>0xC0</v>
       </c>
       <c r="V24" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q24,", ",R24,", ",S24,", ",T24,", ",U24,", /* ASCII ",N24," (",O24,"), character: ",P24," */")</f>
-        <v>    0x80, 0x88, 0x9E, 0xA8, 0xC0, /* ASCII 55 (0x37), character: '7' */</v>
+        <f aca="false">CONCATENATE("    { ",Q24,", ",R24,", ",S24,", ",T24,", ",U24," }, /* ASCII ",N24," (",O24,"), character: ",P24," */")</f>
+        <v>    { 0x80, 0x88, 0x9E, 0xA8, 0xC0 }, /* ASCII 55 (0x37), character: '7' */</v>
       </c>
       <c r="W24" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q24,2))</f>
@@ -2514,8 +2520,8 @@
         <v>0x6C</v>
       </c>
       <c r="V25" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q25,", ",R25,", ",S25,", ",T25,", ",U25,", /* ASCII ",N25," (",O25,"), character: ",P25," */")</f>
-        <v>    0x6C, 0x92, 0x92, 0x92, 0x6C, /* ASCII 56 (0x38), character: '8' */</v>
+        <f aca="false">CONCATENATE("    { ",Q25,", ",R25,", ",S25,", ",T25,", ",U25," }, /* ASCII ",N25," (",O25,"), character: ",P25," */")</f>
+        <v>    { 0x6C, 0x92, 0x92, 0x92, 0x6C }, /* ASCII 56 (0x38), character: '8' */</v>
       </c>
       <c r="W25" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q25,2))</f>
@@ -2609,8 +2615,8 @@
         <v>0x7C</v>
       </c>
       <c r="V26" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q26,", ",R26,", ",S26,", ",T26,", ",U26,", /* ASCII ",N26," (",O26,"), character: ",P26," */")</f>
-        <v>    0x64, 0x92, 0x92, 0x92, 0x7C, /* ASCII 57 (0x39), character: '9' */</v>
+        <f aca="false">CONCATENATE("    { ",Q26,", ",R26,", ",S26,", ",T26,", ",U26," }, /* ASCII ",N26," (",O26,"), character: ",P26," */")</f>
+        <v>    { 0x64, 0x92, 0x92, 0x92, 0x7C }, /* ASCII 57 (0x39), character: '9' */</v>
       </c>
       <c r="W26" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q26,2))</f>
@@ -2704,8 +2710,8 @@
         <v>0x00</v>
       </c>
       <c r="V27" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q27,", ",R27,", ",S27,", ",T27,", ",U27,", /* ASCII ",N27," (",O27,"), character: ",P27," */")</f>
-        <v>    0x00, 0x6C, 0x6C, 0x00, 0x00, /* ASCII 58 (0x3A), character: ':' */</v>
+        <f aca="false">CONCATENATE("    { ",Q27,", ",R27,", ",S27,", ",T27,", ",U27," }, /* ASCII ",N27," (",O27,"), character: ",P27," */")</f>
+        <v>    { 0x00, 0x6C, 0x6C, 0x00, 0x00 }, /* ASCII 58 (0x3A), character: ':' */</v>
       </c>
       <c r="W27" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q27,2))</f>
@@ -2795,8 +2801,8 @@
         <v>0x00</v>
       </c>
       <c r="V28" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q28,", ",R28,", ",S28,", ",T28,", ",U28,", /* ASCII ",N28," (",O28,"), character: ",P28," */")</f>
-        <v>    0x00, 0x6D, 0x6E, 0x00, 0x00, /* ASCII 59 (0x3B), character: ';' */</v>
+        <f aca="false">CONCATENATE("    { ",Q28,", ",R28,", ",S28,", ",T28,", ",U28," }, /* ASCII ",N28," (",O28,"), character: ",P28," */")</f>
+        <v>    { 0x00, 0x6D, 0x6E, 0x00, 0x00 }, /* ASCII 59 (0x3B), character: ';' */</v>
       </c>
       <c r="W28" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q28,2))</f>
@@ -2886,8 +2892,8 @@
         <v>0x82</v>
       </c>
       <c r="V29" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q29,", ",R29,", ",S29,", ",T29,", ",U29,", /* ASCII ",N29," (",O29,"), character: ",P29," */")</f>
-        <v>    0x00, 0x10, 0x28, 0x44, 0x82, /* ASCII 60 (0x3C), character: '&lt;' */</v>
+        <f aca="false">CONCATENATE("    { ",Q29,", ",R29,", ",S29,", ",T29,", ",U29," }, /* ASCII ",N29," (",O29,"), character: ",P29," */")</f>
+        <v>    { 0x00, 0x10, 0x28, 0x44, 0x82 }, /* ASCII 60 (0x3C), character: '&lt;' */</v>
       </c>
       <c r="W29" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q29,2))</f>
@@ -2974,8 +2980,8 @@
         <v>0x28</v>
       </c>
       <c r="V30" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q30,", ",R30,", ",S30,", ",T30,", ",U30,", /* ASCII ",N30," (",O30,"), character: ",P30," */")</f>
-        <v>    0x28, 0x28, 0x28, 0x28, 0x28, /* ASCII 61 (0x3D), character: '=' */</v>
+        <f aca="false">CONCATENATE("    { ",Q30,", ",R30,", ",S30,", ",T30,", ",U30," }, /* ASCII ",N30," (",O30,"), character: ",P30," */")</f>
+        <v>    { 0x28, 0x28, 0x28, 0x28, 0x28 }, /* ASCII 61 (0x3D), character: '=' */</v>
       </c>
       <c r="W30" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q30,2))</f>
@@ -3062,8 +3068,8 @@
         <v>0x00</v>
       </c>
       <c r="V31" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q31,", ",R31,", ",S31,", ",T31,", ",U31,", /* ASCII ",N31," (",O31,"), character: ",P31," */")</f>
-        <v>    0x82, 0x44, 0x28, 0x10, 0x00, /* ASCII 62 (0x3E), character: '&gt;' */</v>
+        <f aca="false">CONCATENATE("    { ",Q31,", ",R31,", ",S31,", ",T31,", ",U31," }, /* ASCII ",N31," (",O31,"), character: ",P31," */")</f>
+        <v>    { 0x82, 0x44, 0x28, 0x10, 0x00 }, /* ASCII 62 (0x3E), character: '&gt;' */</v>
       </c>
       <c r="W31" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q31,2))</f>
@@ -3150,8 +3156,8 @@
         <v>0x40</v>
       </c>
       <c r="V32" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q32,", ",R32,", ",S32,", ",T32,", ",U32,", /* ASCII ",N32," (",O32,"), character: ",P32," */")</f>
-        <v>    0x40, 0x80, 0x9A, 0xA0, 0x40, /* ASCII 63 (0x3F), character: '?' */</v>
+        <f aca="false">CONCATENATE("    { ",Q32,", ",R32,", ",S32,", ",T32,", ",U32," }, /* ASCII ",N32," (",O32,"), character: ",P32," */")</f>
+        <v>    { 0x40, 0x80, 0x9A, 0xA0, 0x40 }, /* ASCII 63 (0x3F), character: '?' */</v>
       </c>
       <c r="W32" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q32,2))</f>
@@ -3250,8 +3256,8 @@
         <v>0x7A</v>
       </c>
       <c r="V33" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q33,", ",R33,", ",S33,", ",T33,", ",U33,", /* ASCII ",N33," (",O33,"), character: ",P33," */")</f>
-        <v>    0x7C, 0x82, 0xBA, 0xAA, 0x7A, /* ASCII 64 (0x40), character: '@' */</v>
+        <f aca="false">CONCATENATE("    { ",Q33,", ",R33,", ",S33,", ",T33,", ",U33," }, /* ASCII ",N33," (",O33,"), character: ",P33," */")</f>
+        <v>    { 0x7C, 0x82, 0xBA, 0xAA, 0x7A }, /* ASCII 64 (0x40), character: '@' */</v>
       </c>
       <c r="W33" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q33,2))</f>
@@ -3335,8 +3341,8 @@
         <v>0x3E</v>
       </c>
       <c r="V34" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q34,", ",R34,", ",S34,", ",T34,", ",U34,", /* ASCII ",N34," (",O34,"), character: ",P34," */")</f>
-        <v>    0x3E, 0x48, 0x88, 0x48, 0x3E, /* ASCII 65 (0x41), character: 'A' */</v>
+        <f aca="false">CONCATENATE("    { ",Q34,", ",R34,", ",S34,", ",T34,", ",U34," }, /* ASCII ",N34," (",O34,"), character: ",P34," */")</f>
+        <v>    { 0x3E, 0x48, 0x88, 0x48, 0x3E }, /* ASCII 65 (0x41), character: 'A' */</v>
       </c>
       <c r="W34" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q34,2))</f>
@@ -3434,8 +3440,8 @@
         <v>0x6C</v>
       </c>
       <c r="V35" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q35,", ",R35,", ",S35,", ",T35,", ",U35,", /* ASCII ",N35," (",O35,"), character: ",P35," */")</f>
-        <v>    0xFE, 0x92, 0x92, 0x92, 0x6C, /* ASCII 66 (0x42), character: 'B' */</v>
+        <f aca="false">CONCATENATE("    { ",Q35,", ",R35,", ",S35,", ",T35,", ",U35," }, /* ASCII ",N35," (",O35,"), character: ",P35," */")</f>
+        <v>    { 0xFE, 0x92, 0x92, 0x92, 0x6C }, /* ASCII 66 (0x42), character: 'B' */</v>
       </c>
       <c r="W35" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q35,2))</f>
@@ -3534,8 +3540,8 @@
         <v>0x44</v>
       </c>
       <c r="V36" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q36,", ",R36,", ",S36,", ",T36,", ",U36,", /* ASCII ",N36," (",O36,"), character: ",P36," */")</f>
-        <v>    0x7C, 0x82, 0x82, 0x82, 0x44, /* ASCII 67 (0x43), character: 'C' */</v>
+        <f aca="false">CONCATENATE("    { ",Q36,", ",R36,", ",S36,", ",T36,", ",U36," }, /* ASCII ",N36," (",O36,"), character: ",P36," */")</f>
+        <v>    { 0x7C, 0x82, 0x82, 0x82, 0x44 }, /* ASCII 67 (0x43), character: 'C' */</v>
       </c>
       <c r="W36" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q36,2))</f>
@@ -3629,8 +3635,8 @@
         <v>0x7C</v>
       </c>
       <c r="V37" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q37,", ",R37,", ",S37,", ",T37,", ",U37,", /* ASCII ",N37," (",O37,"), character: ",P37," */")</f>
-        <v>    0xFE, 0x82, 0x82, 0x82, 0x7C, /* ASCII 68 (0x44), character: 'D' */</v>
+        <f aca="false">CONCATENATE("    { ",Q37,", ",R37,", ",S37,", ",T37,", ",U37," }, /* ASCII ",N37," (",O37,"), character: ",P37," */")</f>
+        <v>    { 0xFE, 0x82, 0x82, 0x82, 0x7C }, /* ASCII 68 (0x44), character: 'D' */</v>
       </c>
       <c r="W37" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q37,2))</f>
@@ -3730,8 +3736,8 @@
         <v>0x82</v>
       </c>
       <c r="V38" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q38,", ",R38,", ",S38,", ",T38,", ",U38,", /* ASCII ",N38," (",O38,"), character: ",P38," */")</f>
-        <v>    0xFE, 0x92, 0x92, 0x92, 0x82, /* ASCII 69 (0x45), character: 'E' */</v>
+        <f aca="false">CONCATENATE("    { ",Q38,", ",R38,", ",S38,", ",T38,", ",U38," }, /* ASCII ",N38," (",O38,"), character: ",P38," */")</f>
+        <v>    { 0xFE, 0x92, 0x92, 0x92, 0x82 }, /* ASCII 69 (0x45), character: 'E' */</v>
       </c>
       <c r="W38" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q38,2))</f>
@@ -3825,8 +3831,8 @@
         <v>0x80</v>
       </c>
       <c r="V39" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q39,", ",R39,", ",S39,", ",T39,", ",U39,", /* ASCII ",N39," (",O39,"), character: ",P39," */")</f>
-        <v>    0xFE, 0x90, 0x90, 0x90, 0x80, /* ASCII 70 (0x46), character: 'F' */</v>
+        <f aca="false">CONCATENATE("    { ",Q39,", ",R39,", ",S39,", ",T39,", ",U39," }, /* ASCII ",N39," (",O39,"), character: ",P39," */")</f>
+        <v>    { 0xFE, 0x90, 0x90, 0x90, 0x80 }, /* ASCII 70 (0x46), character: 'F' */</v>
       </c>
       <c r="W39" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q39,2))</f>
@@ -3926,8 +3932,8 @@
         <v>0x4C</v>
       </c>
       <c r="V40" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q40,", ",R40,", ",S40,", ",T40,", ",U40,", /* ASCII ",N40," (",O40,"), character: ",P40," */")</f>
-        <v>    0x7C, 0x82, 0x8A, 0x8A, 0x4C, /* ASCII 71 (0x47), character: 'G' */</v>
+        <f aca="false">CONCATENATE("    { ",Q40,", ",R40,", ",S40,", ",T40,", ",U40," }, /* ASCII ",N40," (",O40,"), character: ",P40," */")</f>
+        <v>    { 0x7C, 0x82, 0x8A, 0x8A, 0x4C }, /* ASCII 71 (0x47), character: 'G' */</v>
       </c>
       <c r="W40" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q40,2))</f>
@@ -4018,8 +4024,8 @@
         <v>0xFE</v>
       </c>
       <c r="V41" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q41,", ",R41,", ",S41,", ",T41,", ",U41,", /* ASCII ",N41," (",O41,"), character: ",P41," */")</f>
-        <v>    0xFE, 0x10, 0x10, 0x10, 0xFE, /* ASCII 72 (0x48), character: 'H' */</v>
+        <f aca="false">CONCATENATE("    { ",Q41,", ",R41,", ",S41,", ",T41,", ",U41," }, /* ASCII ",N41," (",O41,"), character: ",P41," */")</f>
+        <v>    { 0xFE, 0x10, 0x10, 0x10, 0xFE }, /* ASCII 72 (0x48), character: 'H' */</v>
       </c>
       <c r="W41" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q41,2))</f>
@@ -4106,8 +4112,8 @@
         <v>0x00</v>
       </c>
       <c r="V42" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q42,", ",R42,", ",S42,", ",T42,", ",U42,", /* ASCII ",N42," (",O42,"), character: ",P42," */")</f>
-        <v>    0x00, 0x82, 0xFE, 0x82, 0x00, /* ASCII 73 (0x49), character: 'I' */</v>
+        <f aca="false">CONCATENATE("    { ",Q42,", ",R42,", ",S42,", ",T42,", ",U42," }, /* ASCII ",N42," (",O42,"), character: ",P42," */")</f>
+        <v>    { 0x00, 0x82, 0xFE, 0x82, 0x00 }, /* ASCII 73 (0x49), character: 'I' */</v>
       </c>
       <c r="W42" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q42,2))</f>
@@ -4194,8 +4200,8 @@
         <v>0x80</v>
       </c>
       <c r="V43" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q43,", ",R43,", ",S43,", ",T43,", ",U43,", /* ASCII ",N43," (",O43,"), character: ",P43," */")</f>
-        <v>    0x0C, 0x02, 0x82, 0xFC, 0x80, /* ASCII 74 (0x4A), character: 'J' */</v>
+        <f aca="false">CONCATENATE("    { ",Q43,", ",R43,", ",S43,", ",T43,", ",U43," }, /* ASCII ",N43," (",O43,"), character: ",P43," */")</f>
+        <v>    { 0x0C, 0x02, 0x82, 0xFC, 0x80 }, /* ASCII 74 (0x4A), character: 'J' */</v>
       </c>
       <c r="W43" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q43,2))</f>
@@ -4294,8 +4300,8 @@
         <v>0x82</v>
       </c>
       <c r="V44" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q44,", ",R44,", ",S44,", ",T44,", ",U44,", /* ASCII ",N44," (",O44,"), character: ",P44," */")</f>
-        <v>    0xFE, 0x10, 0x28, 0x44, 0x82, /* ASCII 75 (0x4B), character: 'K' */</v>
+        <f aca="false">CONCATENATE("    { ",Q44,", ",R44,", ",S44,", ",T44,", ",U44," }, /* ASCII ",N44," (",O44,"), character: ",P44," */")</f>
+        <v>    { 0xFE, 0x10, 0x28, 0x44, 0x82 }, /* ASCII 75 (0x4B), character: 'K' */</v>
       </c>
       <c r="W44" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q44,2))</f>
@@ -4379,8 +4385,8 @@
         <v>0x02</v>
       </c>
       <c r="V45" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q45,", ",R45,", ",S45,", ",T45,", ",U45,", /* ASCII ",N45," (",O45,"), character: ",P45," */")</f>
-        <v>    0xFE, 0x02, 0x02, 0x02, 0x02, /* ASCII 76 (0x4C), character: 'L' */</v>
+        <f aca="false">CONCATENATE("    { ",Q45,", ",R45,", ",S45,", ",T45,", ",U45," }, /* ASCII ",N45," (",O45,"), character: ",P45," */")</f>
+        <v>    { 0xFE, 0x02, 0x02, 0x02, 0x02 }, /* ASCII 76 (0x4C), character: 'L' */</v>
       </c>
       <c r="W45" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q45,2))</f>
@@ -4478,8 +4484,8 @@
         <v>0xFE</v>
       </c>
       <c r="V46" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q46,", ",R46,", ",S46,", ",T46,", ",U46,", /* ASCII ",N46," (",O46,"), character: ",P46," */")</f>
-        <v>    0xFE, 0x40, 0x20, 0x40, 0xFE, /* ASCII 77 (0x4D), character: 'M' */</v>
+        <f aca="false">CONCATENATE("    { ",Q46,", ",R46,", ",S46,", ",T46,", ",U46," }, /* ASCII ",N46," (",O46,"), character: ",P46," */")</f>
+        <v>    { 0xFE, 0x40, 0x20, 0x40, 0xFE }, /* ASCII 77 (0x4D), character: 'M' */</v>
       </c>
       <c r="W46" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q46,2))</f>
@@ -4580,8 +4586,8 @@
         <v>0xFE</v>
       </c>
       <c r="V47" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q47,", ",R47,", ",S47,", ",T47,", ",U47,", /* ASCII ",N47," (",O47,"), character: ",P47," */")</f>
-        <v>    0xFE, 0x20, 0x10, 0x08, 0xFE, /* ASCII 78 (0x4E), character: 'N' */</v>
+        <f aca="false">CONCATENATE("    { ",Q47,", ",R47,", ",S47,", ",T47,", ",U47," }, /* ASCII ",N47," (",O47,"), character: ",P47," */")</f>
+        <v>    { 0xFE, 0x20, 0x10, 0x08, 0xFE }, /* ASCII 78 (0x4E), character: 'N' */</v>
       </c>
       <c r="W47" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q47,2))</f>
@@ -4679,8 +4685,8 @@
         <v>0x7C</v>
       </c>
       <c r="V48" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q48,", ",R48,", ",S48,", ",T48,", ",U48,", /* ASCII ",N48," (",O48,"), character: ",P48," */")</f>
-        <v>    0x7C, 0x82, 0x82, 0x82, 0x7C, /* ASCII 79 (0x4F), character: 'O' */</v>
+        <f aca="false">CONCATENATE("    { ",Q48,", ",R48,", ",S48,", ",T48,", ",U48," }, /* ASCII ",N48," (",O48,"), character: ",P48," */")</f>
+        <v>    { 0x7C, 0x82, 0x82, 0x82, 0x7C }, /* ASCII 79 (0x4F), character: 'O' */</v>
       </c>
       <c r="W48" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q48,2))</f>
@@ -4774,8 +4780,8 @@
         <v>0x60</v>
       </c>
       <c r="V49" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q49,", ",R49,", ",S49,", ",T49,", ",U49,", /* ASCII ",N49," (",O49,"), character: ",P49," */")</f>
-        <v>    0xFE, 0x90, 0x90, 0x90, 0x60, /* ASCII 80 (0x50), character: 'P' */</v>
+        <f aca="false">CONCATENATE("    { ",Q49,", ",R49,", ",S49,", ",T49,", ",U49," }, /* ASCII ",N49," (",O49,"), character: ",P49," */")</f>
+        <v>    { 0xFE, 0x90, 0x90, 0x90, 0x60 }, /* ASCII 80 (0x50), character: 'P' */</v>
       </c>
       <c r="W49" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q49,2))</f>
@@ -4871,8 +4877,8 @@
         <v>0x7D</v>
       </c>
       <c r="V50" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q50,", ",R50,", ",S50,", ",T50,", ",U50,", /* ASCII ",N50," (",O50,"), character: ",P50," */")</f>
-        <v>    0x7C, 0x82, 0x86, 0x82, 0x7D, /* ASCII 81 (0x51), character: 'Q' */</v>
+        <f aca="false">CONCATENATE("    { ",Q50,", ",R50,", ",S50,", ",T50,", ",U50," }, /* ASCII ",N50," (",O50,"), character: ",P50," */")</f>
+        <v>    { 0x7C, 0x82, 0x86, 0x82, 0x7D }, /* ASCII 81 (0x51), character: 'Q' */</v>
       </c>
       <c r="W50" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q50,2))</f>
@@ -4966,8 +4972,8 @@
         <v>0x6E</v>
       </c>
       <c r="V51" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q51,", ",R51,", ",S51,", ",T51,", ",U51,", /* ASCII ",N51," (",O51,"), character: ",P51," */")</f>
-        <v>    0xFE, 0x90, 0x90, 0x90, 0x6E, /* ASCII 82 (0x52), character: 'R' */</v>
+        <f aca="false">CONCATENATE("    { ",Q51,", ",R51,", ",S51,", ",T51,", ",U51," }, /* ASCII ",N51," (",O51,"), character: ",P51," */")</f>
+        <v>    { 0xFE, 0x90, 0x90, 0x90, 0x6E }, /* ASCII 82 (0x52), character: 'R' */</v>
       </c>
       <c r="W51" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q51,2))</f>
@@ -5062,8 +5068,8 @@
         <v>0x8C</v>
       </c>
       <c r="V52" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q52,", ",R52,", ",S52,", ",T52,", ",U52,", /* ASCII ",N52," (",O52,"), character: ",P52," */")</f>
-        <v>    0x62, 0x92, 0x92, 0x92, 0x8C, /* ASCII 83 (0x53), character: 'S' */</v>
+        <f aca="false">CONCATENATE("    { ",Q52,", ",R52,", ",S52,", ",T52,", ",U52," }, /* ASCII ",N52," (",O52,"), character: ",P52," */")</f>
+        <v>    { 0x62, 0x92, 0x92, 0x92, 0x8C }, /* ASCII 83 (0x53), character: 'S' */</v>
       </c>
       <c r="W52" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q52,2))</f>
@@ -5152,8 +5158,8 @@
         <v>0x80</v>
       </c>
       <c r="V53" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q53,", ",R53,", ",S53,", ",T53,", ",U53,", /* ASCII ",N53," (",O53,"), character: ",P53," */")</f>
-        <v>    0x80, 0x80, 0xFE, 0x80, 0x80, /* ASCII 84 (0x54), character: 'T' */</v>
+        <f aca="false">CONCATENATE("    { ",Q53,", ",R53,", ",S53,", ",T53,", ",U53," }, /* ASCII ",N53," (",O53,"), character: ",P53," */")</f>
+        <v>    { 0x80, 0x80, 0xFE, 0x80, 0x80 }, /* ASCII 84 (0x54), character: 'T' */</v>
       </c>
       <c r="W53" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q53,2))</f>
@@ -5240,8 +5246,8 @@
         <v>0xFC</v>
       </c>
       <c r="V54" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q54,", ",R54,", ",S54,", ",T54,", ",U54,", /* ASCII ",N54," (",O54,"), character: ",P54," */")</f>
-        <v>    0xFC, 0x02, 0x02, 0x02, 0xFC, /* ASCII 85 (0x55), character: 'U' */</v>
+        <f aca="false">CONCATENATE("    { ",Q54,", ",R54,", ",S54,", ",T54,", ",U54," }, /* ASCII ",N54," (",O54,"), character: ",P54," */")</f>
+        <v>    { 0xFC, 0x02, 0x02, 0x02, 0xFC }, /* ASCII 85 (0x55), character: 'U' */</v>
       </c>
       <c r="W54" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q54,2))</f>
@@ -5340,8 +5346,8 @@
         <v>0xE0</v>
       </c>
       <c r="V55" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q55,", ",R55,", ",S55,", ",T55,", ",U55,", /* ASCII ",N55," (",O55,"), character: ",P55," */")</f>
-        <v>    0xE0, 0x38, 0x0E, 0x38, 0xE0, /* ASCII 86 (0x56), character: 'V' */</v>
+        <f aca="false">CONCATENATE("    { ",Q55,", ",R55,", ",S55,", ",T55,", ",U55," }, /* ASCII ",N55," (",O55,"), character: ",P55," */")</f>
+        <v>    { 0xE0, 0x38, 0x0E, 0x38, 0xE0 }, /* ASCII 86 (0x56), character: 'V' */</v>
       </c>
       <c r="W55" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q55,2))</f>
@@ -5425,8 +5431,8 @@
         <v>0xFC</v>
       </c>
       <c r="V56" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q56,", ",R56,", ",S56,", ",T56,", ",U56,", /* ASCII ",N56," (",O56,"), character: ",P56," */")</f>
-        <v>    0xFC, 0x02, 0x0C, 0x02, 0xFC, /* ASCII 87 (0x57), character: 'W' */</v>
+        <f aca="false">CONCATENATE("    { ",Q56,", ",R56,", ",S56,", ",T56,", ",U56," }, /* ASCII ",N56," (",O56,"), character: ",P56," */")</f>
+        <v>    { 0xFC, 0x02, 0x0C, 0x02, 0xFC }, /* ASCII 87 (0x57), character: 'W' */</v>
       </c>
       <c r="W56" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q56,2))</f>
@@ -5524,8 +5530,8 @@
         <v>0xC6</v>
       </c>
       <c r="V57" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q57,", ",R57,", ",S57,", ",T57,", ",U57,", /* ASCII ",N57," (",O57,"), character: ",P57," */")</f>
-        <v>    0xC6, 0x28, 0x10, 0x28, 0xC6, /* ASCII 88 (0x58), character: 'X' */</v>
+        <f aca="false">CONCATENATE("    { ",Q57,", ",R57,", ",S57,", ",T57,", ",U57," }, /* ASCII ",N57," (",O57,"), character: ",P57," */")</f>
+        <v>    { 0xC6, 0x28, 0x10, 0x28, 0xC6 }, /* ASCII 88 (0x58), character: 'X' */</v>
       </c>
       <c r="W57" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q57,2))</f>
@@ -5624,8 +5630,8 @@
         <v>0xE0</v>
       </c>
       <c r="V58" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q58,", ",R58,", ",S58,", ",T58,", ",U58,", /* ASCII ",N58," (",O58,"), character: ",P58," */")</f>
-        <v>    0xE0, 0x10, 0x0E, 0x10, 0xE0, /* ASCII 89 (0x59), character: 'Y' */</v>
+        <f aca="false">CONCATENATE("    { ",Q58,", ",R58,", ",S58,", ",T58,", ",U58," }, /* ASCII ",N58," (",O58,"), character: ",P58," */")</f>
+        <v>    { 0xE0, 0x10, 0x0E, 0x10, 0xE0 }, /* ASCII 89 (0x59), character: 'Y' */</v>
       </c>
       <c r="W58" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q58,2))</f>
@@ -5721,8 +5727,8 @@
         <v>0xC2</v>
       </c>
       <c r="V59" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q59,", ",R59,", ",S59,", ",T59,", ",U59,", /* ASCII ",N59," (",O59,"), character: ",P59," */")</f>
-        <v>    0x86, 0x8A, 0x92, 0xA2, 0xC2, /* ASCII 90 (0x5A), character: 'Z' */</v>
+        <f aca="false">CONCATENATE("    { ",Q59,", ",R59,", ",S59,", ",T59,", ",U59," }, /* ASCII ",N59," (",O59,"), character: ",P59," */")</f>
+        <v>    { 0x86, 0x8A, 0x92, 0xA2, 0xC2 }, /* ASCII 90 (0x5A), character: 'Z' */</v>
       </c>
       <c r="W59" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q59,2))</f>
@@ -5820,8 +5826,8 @@
         <v>0x00</v>
       </c>
       <c r="V60" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q60,", ",R60,", ",S60,", ",T60,", ",U60,", /* ASCII ",N60," (",O60,"), character: ",P60," */")</f>
-        <v>    0x00, 0xFE, 0x82, 0x82, 0x00, /* ASCII 91 (0x5B), character: '[' */</v>
+        <f aca="false">CONCATENATE("    { ",Q60,", ",R60,", ",S60,", ",T60,", ",U60," }, /* ASCII ",N60," (",O60,"), character: ",P60," */")</f>
+        <v>    { 0x00, 0xFE, 0x82, 0x82, 0x00 }, /* ASCII 91 (0x5B), character: '[' */</v>
       </c>
       <c r="W60" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q60,2))</f>
@@ -5919,8 +5925,8 @@
         <v>0x03</v>
       </c>
       <c r="V61" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q61,", ",R61,", ",S61,", ",T61,", ",U61,", /* ASCII ",N61," (",O61,"), character: ",P61," */")</f>
-        <v>    0x00, 0xC0, 0x30, 0x0C, 0x03, /* ASCII 92 (0x5C), character: '\' */</v>
+        <f aca="false">CONCATENATE("    { ",Q61,", ",R61,", ",S61,", ",T61,", ",U61," }, /* ASCII ",N61," (",O61,"), character: ",P61," */")</f>
+        <v>    { 0x00, 0xC0, 0x30, 0x0C, 0x03 }, /* ASCII 92 (0x5C), character: '\' */</v>
       </c>
       <c r="W61" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q61,2))</f>
@@ -6018,8 +6024,8 @@
         <v>0x00</v>
       </c>
       <c r="V62" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q62,", ",R62,", ",S62,", ",T62,", ",U62,", /* ASCII ",N62," (",O62,"), character: ",P62," */")</f>
-        <v>    0x00, 0x82, 0x82, 0xFE, 0x00, /* ASCII 93 (0x5D), character: ']' */</v>
+        <f aca="false">CONCATENATE("    { ",Q62,", ",R62,", ",S62,", ",T62,", ",U62," }, /* ASCII ",N62," (",O62,"), character: ",P62," */")</f>
+        <v>    { 0x00, 0x82, 0x82, 0xFE, 0x00 }, /* ASCII 93 (0x5D), character: ']' */</v>
       </c>
       <c r="W62" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q62,2))</f>
@@ -6112,8 +6118,8 @@
         <v>0x10</v>
       </c>
       <c r="V63" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q63,", ",R63,", ",S63,", ",T63,", ",U63,", /* ASCII ",N63," (",O63,"), character: ",P63," */")</f>
-        <v>    0x10, 0x20, 0x40, 0x20, 0x10, /* ASCII 94 (0x5E), character: '^' */</v>
+        <f aca="false">CONCATENATE("    { ",Q63,", ",R63,", ",S63,", ",T63,", ",U63," }, /* ASCII ",N63," (",O63,"), character: ",P63," */")</f>
+        <v>    { 0x10, 0x20, 0x40, 0x20, 0x10 }, /* ASCII 94 (0x5E), character: '^' */</v>
       </c>
       <c r="W63" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q63,2))</f>
@@ -6200,8 +6206,8 @@
         <v>0x02</v>
       </c>
       <c r="V64" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q64,", ",R64,", ",S64,", ",T64,", ",U64,", /* ASCII ",N64," (",O64,"), character: ",P64," */")</f>
-        <v>    0x02, 0x02, 0x02, 0x02, 0x02, /* ASCII 95 (0x5F), character: '_' */</v>
+        <f aca="false">CONCATENATE("    { ",Q64,", ",R64,", ",S64,", ",T64,", ",U64," }, /* ASCII ",N64," (",O64,"), character: ",P64," */")</f>
+        <v>    { 0x02, 0x02, 0x02, 0x02, 0x02 }, /* ASCII 95 (0x5F), character: '_' */</v>
       </c>
       <c r="W64" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q64,2))</f>
@@ -6288,8 +6294,8 @@
         <v>0x00</v>
       </c>
       <c r="V65" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q65,", ",R65,", ",S65,", ",T65,", ",U65,", /* ASCII ",N65," (",O65,"), character: ",P65," */")</f>
-        <v>    0x00, 0x80, 0x60, 0x00, 0x00, /* ASCII 96 (0x60), character: '`' */</v>
+        <f aca="false">CONCATENATE("    { ",Q65,", ",R65,", ",S65,", ",T65,", ",U65," }, /* ASCII ",N65," (",O65,"), character: ",P65," */")</f>
+        <v>    { 0x00, 0x80, 0x60, 0x00, 0x00 }, /* ASCII 96 (0x60), character: '`' */</v>
       </c>
       <c r="W65" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q65,2))</f>
@@ -6388,8 +6394,8 @@
         <v>0x00</v>
       </c>
       <c r="V66" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q66,", ",R66,", ",S66,", ",T66,", ",U66,", /* ASCII ",N66," (",O66,"), character: ",P66," */")</f>
-        <v>    0x24, 0x4A, 0x4A, 0x3E, 0x00, /* ASCII 97 (0x61), character: 'a' */</v>
+        <f aca="false">CONCATENATE("    { ",Q66,", ",R66,", ",S66,", ",T66,", ",U66," }, /* ASCII ",N66," (",O66,"), character: ",P66," */")</f>
+        <v>    { 0x24, 0x4A, 0x4A, 0x3E, 0x00 }, /* ASCII 97 (0x61), character: 'a' */</v>
       </c>
       <c r="W66" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q66,2))</f>
@@ -6473,8 +6479,8 @@
         <v>0x0C</v>
       </c>
       <c r="V67" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q67,", ",R67,", ",S67,", ",T67,", ",U67,", /* ASCII ",N67," (",O67,"), character: ",P67," */")</f>
-        <v>    0x00, 0xFE, 0x12, 0x12, 0x0C, /* ASCII 98 (0x62), character: 'b' */</v>
+        <f aca="false">CONCATENATE("    { ",Q67,", ",R67,", ",S67,", ",T67,", ",U67," }, /* ASCII ",N67," (",O67,"), character: ",P67," */")</f>
+        <v>    { 0x00, 0xFE, 0x12, 0x12, 0x0C }, /* ASCII 98 (0x62), character: 'b' */</v>
       </c>
       <c r="W67" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q67,2))</f>
@@ -6572,8 +6578,8 @@
         <v>0x00</v>
       </c>
       <c r="V68" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q68,", ",R68,", ",S68,", ",T68,", ",U68,", /* ASCII ",N68," (",O68,"), character: ",P68," */")</f>
-        <v>    0x0C, 0x12, 0x12, 0x12, 0x00, /* ASCII 99 (0x63), character: 'c' */</v>
+        <f aca="false">CONCATENATE("    { ",Q68,", ",R68,", ",S68,", ",T68,", ",U68," }, /* ASCII ",N68," (",O68,"), character: ",P68," */")</f>
+        <v>    { 0x0C, 0x12, 0x12, 0x12, 0x00 }, /* ASCII 99 (0x63), character: 'c' */</v>
       </c>
       <c r="W68" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q68,2))</f>
@@ -6672,8 +6678,8 @@
         <v>0xFE</v>
       </c>
       <c r="V69" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q69,", ",R69,", ",S69,", ",T69,", ",U69,", /* ASCII ",N69," (",O69,"), character: ",P69," */")</f>
-        <v>    0x00, 0x0C, 0x12, 0x12, 0xFE, /* ASCII 100 (0x64), character: 'd' */</v>
+        <f aca="false">CONCATENATE("    { ",Q69,", ",R69,", ",S69,", ",T69,", ",U69," }, /* ASCII ",N69," (",O69,"), character: ",P69," */")</f>
+        <v>    { 0x00, 0x0C, 0x12, 0x12, 0xFE }, /* ASCII 100 (0x64), character: 'd' */</v>
       </c>
       <c r="W69" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q69,2))</f>
@@ -6767,8 +6773,8 @@
         <v>0x00</v>
       </c>
       <c r="V70" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q70,", ",R70,", ",S70,", ",T70,", ",U70,", /* ASCII ",N70," (",O70,"), character: ",P70," */")</f>
-        <v>    0x1C, 0x2A, 0x2A, 0x10, 0x00, /* ASCII 101 (0x65), character: 'e' */</v>
+        <f aca="false">CONCATENATE("    { ",Q70,", ",R70,", ",S70,", ",T70,", ",U70," }, /* ASCII ",N70," (",O70,"), character: ",P70," */")</f>
+        <v>    { 0x1C, 0x2A, 0x2A, 0x10, 0x00 }, /* ASCII 101 (0x65), character: 'e' */</v>
       </c>
       <c r="W70" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q70,2))</f>
@@ -6862,8 +6868,8 @@
         <v>0x00</v>
       </c>
       <c r="V71" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q71,", ",R71,", ",S71,", ",T71,", ",U71,", /* ASCII ",N71," (",O71,"), character: ",P71," */")</f>
-        <v>    0x3E, 0x48, 0x40, 0x20, 0x00, /* ASCII 102 (0x66), character: 'f' */</v>
+        <f aca="false">CONCATENATE("    { ",Q71,", ",R71,", ",S71,", ",T71,", ",U71," }, /* ASCII ",N71," (",O71,"), character: ",P71," */")</f>
+        <v>    { 0x3E, 0x48, 0x40, 0x20, 0x00 }, /* ASCII 102 (0x66), character: 'f' */</v>
       </c>
       <c r="W71" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q71,2))</f>
@@ -6955,8 +6961,8 @@
         <v>0x00</v>
       </c>
       <c r="V72" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q72,", ",R72,", ",S72,", ",T72,", ",U72,", /* ASCII ",N72," (",O72,"), character: ",P72," */")</f>
-        <v>    0x12, 0x29, 0x29, 0x3E, 0x00, /* ASCII 103 (0x67), character: 'g' */</v>
+        <f aca="false">CONCATENATE("    { ",Q72,", ",R72,", ",S72,", ",T72,", ",U72," }, /* ASCII ",N72," (",O72,"), character: ",P72," */")</f>
+        <v>    { 0x12, 0x29, 0x29, 0x3E, 0x00 }, /* ASCII 103 (0x67), character: 'g' */</v>
       </c>
       <c r="W72" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q72,2))</f>
@@ -7052,8 +7058,8 @@
         <v>0x00</v>
       </c>
       <c r="V73" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q73,", ",R73,", ",S73,", ",T73,", ",U73,", /* ASCII ",N73," (",O73,"), character: ",P73," */")</f>
-        <v>    0x7E, 0x08, 0x08, 0x06, 0x00, /* ASCII 104 (0x68), character: 'h' */</v>
+        <f aca="false">CONCATENATE("    { ",Q73,", ",R73,", ",S73,", ",T73,", ",U73," }, /* ASCII ",N73," (",O73,"), character: ",P73," */")</f>
+        <v>    { 0x7E, 0x08, 0x08, 0x06, 0x00 }, /* ASCII 104 (0x68), character: 'h' */</v>
       </c>
       <c r="W73" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q73,2))</f>
@@ -7144,8 +7150,8 @@
         <v>0x00</v>
       </c>
       <c r="V74" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q74,", ",R74,", ",S74,", ",T74,", ",U74,", /* ASCII ",N74," (",O74,"), character: ",P74," */")</f>
-        <v>    0x00, 0x12, 0x5E, 0x02, 0x00, /* ASCII 105 (0x69), character: 'i' */</v>
+        <f aca="false">CONCATENATE("    { ",Q74,", ",R74,", ",S74,", ",T74,", ",U74," }, /* ASCII ",N74," (",O74,"), character: ",P74," */")</f>
+        <v>    { 0x00, 0x12, 0x5E, 0x02, 0x00 }, /* ASCII 105 (0x69), character: 'i' */</v>
       </c>
       <c r="W74" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q74,2))</f>
@@ -7238,8 +7244,8 @@
         <v>0x10</v>
       </c>
       <c r="V75" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q75,", ",R75,", ",S75,", ",T75,", ",U75,", /* ASCII ",N75," (",O75,"), character: ",P75," */")</f>
-        <v>    0x00, 0x02, 0x11, 0x5E, 0x10, /* ASCII 106 (0x6A), character: 'j' */</v>
+        <f aca="false">CONCATENATE("    { ",Q75,", ",R75,", ",S75,", ",T75,", ",U75," }, /* ASCII ",N75," (",O75,"), character: ",P75," */")</f>
+        <v>    { 0x00, 0x02, 0x11, 0x5E, 0x10 }, /* ASCII 106 (0x6A), character: 'j' */</v>
       </c>
       <c r="W75" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q75,2))</f>
@@ -7326,8 +7332,8 @@
         <v>0x00</v>
       </c>
       <c r="V76" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q76,", ",R76,", ",S76,", ",T76,", ",U76,", /* ASCII ",N76," (",O76,"), character: ",P76," */")</f>
-        <v>    0x00, 0xFE, 0x08, 0x16, 0x00, /* ASCII 107 (0x6B), character: 'k' */</v>
+        <f aca="false">CONCATENATE("    { ",Q76,", ",R76,", ",S76,", ",T76,", ",U76," }, /* ASCII ",N76," (",O76,"), character: ",P76," */")</f>
+        <v>    { 0x00, 0xFE, 0x08, 0x16, 0x00 }, /* ASCII 107 (0x6B), character: 'k' */</v>
       </c>
       <c r="W76" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q76,2))</f>
@@ -7426,8 +7432,8 @@
         <v>0x00</v>
       </c>
       <c r="V77" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q77,", ",R77,", ",S77,", ",T77,", ",U77,", /* ASCII ",N77," (",O77,"), character: ",P77," */")</f>
-        <v>    0x00, 0x42, 0x7E, 0x02, 0x00, /* ASCII 108 (0x6C), character: 'l' */</v>
+        <f aca="false">CONCATENATE("    { ",Q77,", ",R77,", ",S77,", ",T77,", ",U77," }, /* ASCII ",N77," (",O77,"), character: ",P77," */")</f>
+        <v>    { 0x00, 0x42, 0x7E, 0x02, 0x00 }, /* ASCII 108 (0x6C), character: 'l' */</v>
       </c>
       <c r="W77" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q77,2))</f>
@@ -7511,8 +7517,8 @@
         <v>0x0E</v>
       </c>
       <c r="V78" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q78,", ",R78,", ",S78,", ",T78,", ",U78,", /* ASCII ",N78," (",O78,"), character: ",P78," */")</f>
-        <v>    0x1E, 0x10, 0x0E, 0x10, 0x0E, /* ASCII 109 (0x6D), character: 'm' */</v>
+        <f aca="false">CONCATENATE("    { ",Q78,", ",R78,", ",S78,", ",T78,", ",U78," }, /* ASCII ",N78," (",O78,"), character: ",P78," */")</f>
+        <v>    { 0x1E, 0x10, 0x0E, 0x10, 0x0E }, /* ASCII 109 (0x6D), character: 'm' */</v>
       </c>
       <c r="W78" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q78,2))</f>
@@ -7610,8 +7616,8 @@
         <v>0x00</v>
       </c>
       <c r="V79" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q79,", ",R79,", ",S79,", ",T79,", ",U79,", /* ASCII ",N79," (",O79,"), character: ",P79," */")</f>
-        <v>    0x1E, 0x10, 0x10, 0x0E, 0x00, /* ASCII 110 (0x6E), character: 'n' */</v>
+        <f aca="false">CONCATENATE("    { ",Q79,", ",R79,", ",S79,", ",T79,", ",U79," }, /* ASCII ",N79," (",O79,"), character: ",P79," */")</f>
+        <v>    { 0x1E, 0x10, 0x10, 0x0E, 0x00 }, /* ASCII 110 (0x6E), character: 'n' */</v>
       </c>
       <c r="W79" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q79,2))</f>
@@ -7712,8 +7718,8 @@
         <v>0x00</v>
       </c>
       <c r="V80" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q80,", ",R80,", ",S80,", ",T80,", ",U80,", /* ASCII ",N80," (",O80,"), character: ",P80," */")</f>
-        <v>    0x0C, 0x12, 0x12, 0x0C, 0x00, /* ASCII 111 (0x6F), character: 'o' */</v>
+        <f aca="false">CONCATENATE("    { ",Q80,", ",R80,", ",S80,", ",T80,", ",U80," }, /* ASCII ",N80," (",O80,"), character: ",P80," */")</f>
+        <v>    { 0x0C, 0x12, 0x12, 0x0C, 0x00 }, /* ASCII 111 (0x6F), character: 'o' */</v>
       </c>
       <c r="W80" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q80,2))</f>
@@ -7805,8 +7811,8 @@
         <v>0x18</v>
       </c>
       <c r="V81" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q81,", ",R81,", ",S81,", ",T81,", ",U81,", /* ASCII ",N81," (",O81,"), character: ",P81," */")</f>
-        <v>    0x00, 0x3F, 0x24, 0x24, 0x18, /* ASCII 112 (0x70), character: 'p' */</v>
+        <f aca="false">CONCATENATE("    { ",Q81,", ",R81,", ",S81,", ",T81,", ",U81," }, /* ASCII ",N81," (",O81,"), character: ",P81," */")</f>
+        <v>    { 0x00, 0x3F, 0x24, 0x24, 0x18 }, /* ASCII 112 (0x70), character: 'p' */</v>
       </c>
       <c r="W81" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q81,2))</f>
@@ -7898,8 +7904,8 @@
         <v>0x00</v>
       </c>
       <c r="V82" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q82,", ",R82,", ",S82,", ",T82,", ",U82,", /* ASCII ",N82," (",O82,"), character: ",P82," */")</f>
-        <v>    0x18, 0x24, 0x24, 0x3F, 0x00, /* ASCII 113 (0x71), character: 'q' */</v>
+        <f aca="false">CONCATENATE("    { ",Q82,", ",R82,", ",S82,", ",T82,", ",U82," }, /* ASCII ",N82," (",O82,"), character: ",P82," */")</f>
+        <v>    { 0x18, 0x24, 0x24, 0x3F, 0x00 }, /* ASCII 113 (0x71), character: 'q' */</v>
       </c>
       <c r="W82" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q82,2))</f>
@@ -7989,8 +7995,8 @@
         <v>0x00</v>
       </c>
       <c r="V83" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q83,", ",R83,", ",S83,", ",T83,", ",U83,", /* ASCII ",N83," (",O83,"), character: ",P83," */")</f>
-        <v>    0x1E, 0x08, 0x10, 0x08, 0x00, /* ASCII 114 (0x72), character: 'r' */</v>
+        <f aca="false">CONCATENATE("    { ",Q83,", ",R83,", ",S83,", ",T83,", ",U83," }, /* ASCII ",N83," (",O83,"), character: ",P83," */")</f>
+        <v>    { 0x1E, 0x08, 0x10, 0x08, 0x00 }, /* ASCII 114 (0x72), character: 'r' */</v>
       </c>
       <c r="W83" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q83,2))</f>
@@ -8080,8 +8086,8 @@
         <v>0x00</v>
       </c>
       <c r="V84" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q84,", ",R84,", ",S84,", ",T84,", ",U84,", /* ASCII ",N84," (",O84,"), character: ",P84," */")</f>
-        <v>    0x12, 0x2A, 0x2A, 0x24, 0x00, /* ASCII 115 (0x73), character: 's' */</v>
+        <f aca="false">CONCATENATE("    { ",Q84,", ",R84,", ",S84,", ",T84,", ",U84," }, /* ASCII ",N84," (",O84,"), character: ",P84," */")</f>
+        <v>    { 0x12, 0x2A, 0x2A, 0x24, 0x00 }, /* ASCII 115 (0x73), character: 's' */</v>
       </c>
       <c r="W84" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q84,2))</f>
@@ -8168,8 +8174,8 @@
         <v>0x00</v>
       </c>
       <c r="V85" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q85,", ",R85,", ",S85,", ",T85,", ",U85,", /* ASCII ",N85," (",O85,"), character: ",P85," */")</f>
-        <v>    0x10, 0x3E, 0x11, 0x02, 0x00, /* ASCII 116 (0x74), character: 't' */</v>
+        <f aca="false">CONCATENATE("    { ",Q85,", ",R85,", ",S85,", ",T85,", ",U85," }, /* ASCII ",N85," (",O85,"), character: ",P85," */")</f>
+        <v>    { 0x10, 0x3E, 0x11, 0x02, 0x00 }, /* ASCII 116 (0x74), character: 't' */</v>
       </c>
       <c r="W85" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q85,2))</f>
@@ -8256,8 +8262,8 @@
         <v>0x00</v>
       </c>
       <c r="V86" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q86,", ",R86,", ",S86,", ",T86,", ",U86,", /* ASCII ",N86," (",O86,"), character: ",P86," */")</f>
-        <v>    0x1C, 0x02, 0x02, 0x1C, 0x00, /* ASCII 117 (0x75), character: 'u' */</v>
+        <f aca="false">CONCATENATE("    { ",Q86,", ",R86,", ",S86,", ",T86,", ",U86," }, /* ASCII ",N86," (",O86,"), character: ",P86," */")</f>
+        <v>    { 0x1C, 0x02, 0x02, 0x1C, 0x00 }, /* ASCII 117 (0x75), character: 'u' */</v>
       </c>
       <c r="W86" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q86,2))</f>
@@ -8344,8 +8350,8 @@
         <v>0x18</v>
       </c>
       <c r="V87" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q87,", ",R87,", ",S87,", ",T87,", ",U87,", /* ASCII ",N87," (",O87,"), character: ",P87," */")</f>
-        <v>    0x18, 0x04, 0x02, 0x04, 0x18, /* ASCII 118 (0x76), character: 'v' */</v>
+        <f aca="false">CONCATENATE("    { ",Q87,", ",R87,", ",S87,", ",T87,", ",U87," }, /* ASCII ",N87," (",O87,"), character: ",P87," */")</f>
+        <v>    { 0x18, 0x04, 0x02, 0x04, 0x18 }, /* ASCII 118 (0x76), character: 'v' */</v>
       </c>
       <c r="W87" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q87,2))</f>
@@ -8444,8 +8450,8 @@
         <v>0x1C</v>
       </c>
       <c r="V88" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q88,", ",R88,", ",S88,", ",T88,", ",U88,", /* ASCII ",N88," (",O88,"), character: ",P88," */")</f>
-        <v>    0x1C, 0x02, 0x1C, 0x02, 0x1C, /* ASCII 119 (0x77), character: 'w' */</v>
+        <f aca="false">CONCATENATE("    { ",Q88,", ",R88,", ",S88,", ",T88,", ",U88," }, /* ASCII ",N88," (",O88,"), character: ",P88," */")</f>
+        <v>    { 0x1C, 0x02, 0x1C, 0x02, 0x1C }, /* ASCII 119 (0x77), character: 'w' */</v>
       </c>
       <c r="W88" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q88,2))</f>
@@ -8529,8 +8535,8 @@
         <v>0x22</v>
       </c>
       <c r="V89" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q89,", ",R89,", ",S89,", ",T89,", ",U89,", /* ASCII ",N89," (",O89,"), character: ",P89," */")</f>
-        <v>    0x22, 0x14, 0x08, 0x14, 0x22, /* ASCII 120 (0x78), character: 'x' */</v>
+        <f aca="false">CONCATENATE("    { ",Q89,", ",R89,", ",S89,", ",T89,", ",U89," }, /* ASCII ",N89," (",O89,"), character: ",P89," */")</f>
+        <v>    { 0x22, 0x14, 0x08, 0x14, 0x22 }, /* ASCII 120 (0x78), character: 'x' */</v>
       </c>
       <c r="W89" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q89,2))</f>
@@ -8628,8 +8634,8 @@
         <v>0x00</v>
       </c>
       <c r="V90" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q90,", ",R90,", ",S90,", ",T90,", ",U90,", /* ASCII ",N90," (",O90,"), character: ",P90," */")</f>
-        <v>    0x39, 0x05, 0x05, 0x3E, 0x00, /* ASCII 121 (0x79), character: 'y' */</v>
+        <f aca="false">CONCATENATE("    { ",Q90,", ",R90,", ",S90,", ",T90,", ",U90," }, /* ASCII ",N90," (",O90,"), character: ",P90," */")</f>
+        <v>    { 0x39, 0x05, 0x05, 0x3E, 0x00 }, /* ASCII 121 (0x79), character: 'y' */</v>
       </c>
       <c r="W90" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q90,2))</f>
@@ -8730,8 +8736,8 @@
         <v>0x00</v>
       </c>
       <c r="V91" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q91,", ",R91,", ",S91,", ",T91,", ",U91,", /* ASCII ",N91," (",O91,"), character: ",P91," */")</f>
-        <v>    0x00, 0x26, 0x2A, 0x32, 0x00, /* ASCII 122 (0x7A), character: 'z' */</v>
+        <f aca="false">CONCATENATE("    { ",Q91,", ",R91,", ",S91,", ",T91,", ",U91," }, /* ASCII ",N91," (",O91,"), character: ",P91," */")</f>
+        <v>    { 0x00, 0x26, 0x2A, 0x32, 0x00 }, /* ASCII 122 (0x7A), character: 'z' */</v>
       </c>
       <c r="W91" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q91,2))</f>
@@ -8823,8 +8829,8 @@
         <v>0x00</v>
       </c>
       <c r="V92" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q92,", ",R92,", ",S92,", ",T92,", ",U92,", /* ASCII ",N92," (",O92,"), character: ",P92," */")</f>
-        <v>    0x00, 0x10, 0x7C, 0x82, 0x00, /* ASCII 123 (0x7B), character: '{' */</v>
+        <f aca="false">CONCATENATE("    { ",Q92,", ",R92,", ",S92,", ",T92,", ",U92," }, /* ASCII ",N92," (",O92,"), character: ",P92," */")</f>
+        <v>    { 0x00, 0x10, 0x7C, 0x82, 0x00 }, /* ASCII 123 (0x7B), character: '{' */</v>
       </c>
       <c r="W92" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q92,2))</f>
@@ -8916,8 +8922,8 @@
         <v>0x00</v>
       </c>
       <c r="V93" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q93,", ",R93,", ",S93,", ",T93,", ",U93,", /* ASCII ",N93," (",O93,"), character: ",P93," */")</f>
-        <v>    0x00, 0x00, 0xFF, 0x00, 0x00, /* ASCII 124 (0x7C), character: '|' */</v>
+        <f aca="false">CONCATENATE("    { ",Q93,", ",R93,", ",S93,", ",T93,", ",U93," }, /* ASCII ",N93," (",O93,"), character: ",P93," */")</f>
+        <v>    { 0x00, 0x00, 0xFF, 0x00, 0x00 }, /* ASCII 124 (0x7C), character: '|' */</v>
       </c>
       <c r="W93" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q93,2))</f>
@@ -9009,8 +9015,8 @@
         <v>0x00</v>
       </c>
       <c r="V94" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q94,", ",R94,", ",S94,", ",T94,", ",U94,", /* ASCII ",N94," (",O94,"), character: ",P94," */")</f>
-        <v>    0x00, 0x82, 0x7C, 0x10, 0x00, /* ASCII 125 (0x7D), character: '}' */</v>
+        <f aca="false">CONCATENATE("    { ",Q94,", ",R94,", ",S94,", ",T94,", ",U94," }, /* ASCII ",N94," (",O94,"), character: ",P94," */")</f>
+        <v>    { 0x00, 0x82, 0x7C, 0x10, 0x00 }, /* ASCII 125 (0x7D), character: '}' */</v>
       </c>
       <c r="W94" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q94,2))</f>
@@ -9102,8 +9108,8 @@
         <v>0x10</v>
       </c>
       <c r="V95" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q95,", ",R95,", ",S95,", ",T95,", ",U95,", /* ASCII ",N95," (",O95,"), character: ",P95," */")</f>
-        <v>    0x10, 0x20, 0x10, 0x08, 0x10, /* ASCII 126 (0x7E), character: '~' */</v>
+        <f aca="false">CONCATENATE("    { ",Q95,", ",R95,", ",S95,", ",T95,", ",U95," }, /* ASCII ",N95," (",O95,"), character: ",P95," */")</f>
+        <v>    { 0x10, 0x20, 0x10, 0x08, 0x10 }, /* ASCII 126 (0x7E), character: '~' */</v>
       </c>
       <c r="W95" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q95,2))</f>
@@ -9192,8 +9198,8 @@
         <v>0x00</v>
       </c>
       <c r="V96" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q96,", ",R96,", ",S96,", ",T96,", ",U96,", /* ASCII ",N96," (",O96,"), character: ",P96," */")</f>
-        <v>    0x00, 0xE0, 0xA0, 0xE0, 0x00, /* ASCII 127 (0x7F), character: '' */</v>
+        <f aca="false">CONCATENATE("    { ",Q96,", ",R96,", ",S96,", ",T96,", ",U96," }, /* ASCII ",N96," (",O96,"), character: ",P96," */")</f>
+        <v>    { 0x00, 0xE0, 0xA0, 0xE0, 0x00 }, /* ASCII 127 (0x7F), character: '' */</v>
       </c>
       <c r="W96" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q96,2))</f>
@@ -9282,8 +9288,8 @@
         <v>0x44</v>
       </c>
       <c r="V97" s="3" t="str">
-        <f aca="false">CONCATENATE("    ",Q97,", ",R97,", ",S97,", ",T97,", ",U97,", /* ASCII ",N97," (",O97,"), character: ",P97," */")</f>
-        <v>    0x28, 0x7C, 0xAA, 0x82, 0x44, /* ASCII 128 (0x80), character: '€' */</v>
+        <f aca="false">CONCATENATE("    { ",Q97,", ",R97,", ",S97,", ",T97,", ",U97," }, /* ASCII ",N97," (",O97,"), character: ",P97," */")</f>
+        <v>    { 0x28, 0x7C, 0xAA, 0x82, 0x44 }, /* ASCII 128 (0x80), character: '€' */</v>
       </c>
       <c r="W97" s="1" t="n">
         <f aca="false">HEX2DEC(RIGHT(Q97,2))</f>
@@ -31760,619 +31766,619 @@
   </sheetPr>
   <dimension ref="A1:A101"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A101" activeCellId="0" sqref="A101"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A79" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D92" activeCellId="0" sqref="D92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="84.280612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="84.280612244898"/>
     <col collapsed="false" hidden="false" max="256" min="2" style="1" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="str">
+      <c r="A1" s="4" t="str">
         <f aca="false">CONCATENATE("#define ASCII_OFFSET     (",Offset,")")</f>
         <v>#define ASCII_OFFSET     (32)</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="str">
+      <c r="A2" s="4" t="str">
         <f aca="false">CONCATENATE("#define CHARACTER_WIDTH    (",Columns,")")</f>
         <v>#define CHARACTER_WIDTH    (5)</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="str">
+      <c r="A3" s="4" t="str">
         <f aca="false">CONCATENATE("uint8_t asciiBitmap[",Rows,"][",Columns,"] = {")</f>
         <v>uint8_t asciiBitmap[97][5] = {</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="str">
+      <c r="A4" s="4" t="str">
         <f aca="false">Sheet1!V1</f>
-        <v>    0x00, 0x00, 0x00, 0x00, 0x00, /* ASCII 32 (0x20), character: ' ' */</v>
+        <v>    { 0x00, 0x00, 0x00, 0x00, 0x00 }, /* ASCII 32 (0x20), character: ' ' */</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="str">
+      <c r="A5" s="4" t="str">
         <f aca="false">Sheet1!V2</f>
-        <v>    0x00, 0x60, 0xFA, 0x60, 0x00, /* ASCII 33 (0x21), character: '!' */</v>
+        <v>    { 0x00, 0x60, 0xFA, 0x60, 0x00 }, /* ASCII 33 (0x21), character: '!' */</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="str">
+      <c r="A6" s="4" t="str">
         <f aca="false">Sheet1!V3</f>
-        <v>    0x20, 0xC0, 0x00, 0x20, 0xC0, /* ASCII 34 (0x22), character: '"' */</v>
+        <v>    { 0x20, 0xC0, 0x00, 0x20, 0xC0 }, /* ASCII 34 (0x22), character: '"' */</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="str">
+      <c r="A7" s="4" t="str">
         <f aca="false">Sheet1!V4</f>
-        <v>    0x28, 0x7C, 0x28, 0x7C, 0x28, /* ASCII 35 (0x23), character: '#' */</v>
+        <v>    { 0x28, 0x7C, 0x28, 0x7C, 0x28 }, /* ASCII 35 (0x23), character: '#' */</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="str">
+      <c r="A8" s="4" t="str">
         <f aca="false">Sheet1!V5</f>
-        <v>    0x24, 0x54, 0xFE, 0x54, 0x48, /* ASCII 36 (0x24), character: '$' */</v>
+        <v>    { 0x24, 0x54, 0xFE, 0x54, 0x48 }, /* ASCII 36 (0x24), character: '$' */</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="str">
+      <c r="A9" s="4" t="str">
         <f aca="false">Sheet1!V6</f>
-        <v>    0x64, 0x68, 0x10, 0x2C, 0x4C, /* ASCII 37 (0x25), character: '%' */</v>
+        <v>    { 0x64, 0x68, 0x10, 0x2C, 0x4C }, /* ASCII 37 (0x25), character: '%' */</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="str">
+      <c r="A10" s="4" t="str">
         <f aca="false">Sheet1!V7</f>
-        <v>    0x34, 0x4A, 0x4A, 0x24, 0x0A, /* ASCII 38 (0x26), character: '&amp;' */</v>
+        <v>    { 0x34, 0x4A, 0x4A, 0x24, 0x0A }, /* ASCII 38 (0x26), character: '&amp;' */</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="str">
+      <c r="A11" s="4" t="str">
         <f aca="false">Sheet1!V8</f>
-        <v>    0x20, 0xC0, 0x00, 0x00, 0x00, /* ASCII 39 (0x27), character: ''' */</v>
+        <v>    { 0x20, 0xC0, 0x00, 0x00, 0x00 }, /* ASCII 39 (0x27), character: ''' */</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="str">
+      <c r="A12" s="4" t="str">
         <f aca="false">Sheet1!V9</f>
-        <v>    0x00, 0x38, 0x44, 0x82, 0x00, /* ASCII 40 (0x28), character: '(' */</v>
+        <v>    { 0x00, 0x38, 0x44, 0x82, 0x00 }, /* ASCII 40 (0x28), character: '(' */</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="str">
+      <c r="A13" s="4" t="str">
         <f aca="false">Sheet1!V10</f>
-        <v>    0x00, 0x82, 0x44, 0x38, 0x00, /* ASCII 41 (0x29), character: ')' */</v>
+        <v>    { 0x00, 0x82, 0x44, 0x38, 0x00 }, /* ASCII 41 (0x29), character: ')' */</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="str">
+      <c r="A14" s="4" t="str">
         <f aca="false">Sheet1!V11</f>
-        <v>    0x28, 0x10, 0x7C, 0x10, 0x28, /* ASCII 42 (0x2A), character: '*' */</v>
+        <v>    { 0x28, 0x10, 0x7C, 0x10, 0x28 }, /* ASCII 42 (0x2A), character: '*' */</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="str">
+      <c r="A15" s="4" t="str">
         <f aca="false">Sheet1!V12</f>
-        <v>    0x10, 0x10, 0x7C, 0x10, 0x10, /* ASCII 43 (0x2B), character: '+' */</v>
+        <v>    { 0x10, 0x10, 0x7C, 0x10, 0x10 }, /* ASCII 43 (0x2B), character: '+' */</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="str">
+      <c r="A16" s="4" t="str">
         <f aca="false">Sheet1!V13</f>
-        <v>    0x00, 0x0D, 0x0E, 0x00, 0x00, /* ASCII 44 (0x2C), character: ',' */</v>
+        <v>    { 0x00, 0x0D, 0x0E, 0x00, 0x00 }, /* ASCII 44 (0x2C), character: ',' */</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="str">
+      <c r="A17" s="4" t="str">
         <f aca="false">Sheet1!V14</f>
-        <v>    0x10, 0x10, 0x10, 0x10, 0x00, /* ASCII 45 (0x2D), character: '-' */</v>
+        <v>    { 0x10, 0x10, 0x10, 0x10, 0x00 }, /* ASCII 45 (0x2D), character: '-' */</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="str">
+      <c r="A18" s="4" t="str">
         <f aca="false">Sheet1!V15</f>
-        <v>    0x00, 0x06, 0x06, 0x00, 0x00, /* ASCII 46 (0x2E), character: '.' */</v>
+        <v>    { 0x00, 0x06, 0x06, 0x00, 0x00 }, /* ASCII 46 (0x2E), character: '.' */</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="str">
+      <c r="A19" s="4" t="str">
         <f aca="false">Sheet1!V16</f>
-        <v>    0x03, 0x0C, 0x30, 0xC0, 0x00, /* ASCII 47 (0x2F), character: '/' */</v>
+        <v>    { 0x03, 0x0C, 0x30, 0xC0, 0x00 }, /* ASCII 47 (0x2F), character: '/' */</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="str">
+      <c r="A20" s="4" t="str">
         <f aca="false">Sheet1!V17</f>
-        <v>    0x7C, 0x8A, 0x92, 0xA2, 0x7C, /* ASCII 48 (0x30), character: '0' */</v>
+        <v>    { 0x7C, 0x8A, 0x92, 0xA2, 0x7C }, /* ASCII 48 (0x30), character: '0' */</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="str">
+      <c r="A21" s="4" t="str">
         <f aca="false">Sheet1!V18</f>
-        <v>    0x00, 0x42, 0xFE, 0x02, 0x00, /* ASCII 49 (0x31), character: '1' */</v>
+        <v>    { 0x00, 0x42, 0xFE, 0x02, 0x00 }, /* ASCII 49 (0x31), character: '1' */</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="str">
+      <c r="A22" s="4" t="str">
         <f aca="false">Sheet1!V19</f>
-        <v>    0x46, 0x8A, 0x92, 0x92, 0x62, /* ASCII 50 (0x32), character: '2' */</v>
+        <v>    { 0x46, 0x8A, 0x92, 0x92, 0x62 }, /* ASCII 50 (0x32), character: '2' */</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="str">
+      <c r="A23" s="4" t="str">
         <f aca="false">Sheet1!V20</f>
-        <v>    0x44, 0x92, 0x92, 0x92, 0x6C, /* ASCII 51 (0x33), character: '3' */</v>
+        <v>    { 0x44, 0x92, 0x92, 0x92, 0x6C }, /* ASCII 51 (0x33), character: '3' */</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="str">
+      <c r="A24" s="4" t="str">
         <f aca="false">Sheet1!V21</f>
-        <v>    0x38, 0xE8, 0xC8, 0xFE, 0x08, /* ASCII 52 (0x34), character: '4' */</v>
+        <v>    { 0x38, 0xE8, 0xC8, 0xFE, 0x08 }, /* ASCII 52 (0x34), character: '4' */</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="str">
+      <c r="A25" s="4" t="str">
         <f aca="false">Sheet1!V22</f>
-        <v>    0xF4, 0x92, 0x92, 0x92, 0x8C, /* ASCII 53 (0x35), character: '5' */</v>
+        <v>    { 0xF4, 0x92, 0x92, 0x92, 0x8C }, /* ASCII 53 (0x35), character: '5' */</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="str">
+      <c r="A26" s="4" t="str">
         <f aca="false">Sheet1!V23</f>
-        <v>    0x7C, 0x92, 0x92, 0x92, 0x4C, /* ASCII 54 (0x36), character: '6' */</v>
+        <v>    { 0x7C, 0x92, 0x92, 0x92, 0x4C }, /* ASCII 54 (0x36), character: '6' */</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="str">
+      <c r="A27" s="4" t="str">
         <f aca="false">Sheet1!V24</f>
-        <v>    0x80, 0x88, 0x9E, 0xA8, 0xC0, /* ASCII 55 (0x37), character: '7' */</v>
+        <v>    { 0x80, 0x88, 0x9E, 0xA8, 0xC0 }, /* ASCII 55 (0x37), character: '7' */</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="str">
+      <c r="A28" s="4" t="str">
         <f aca="false">Sheet1!V25</f>
-        <v>    0x6C, 0x92, 0x92, 0x92, 0x6C, /* ASCII 56 (0x38), character: '8' */</v>
+        <v>    { 0x6C, 0x92, 0x92, 0x92, 0x6C }, /* ASCII 56 (0x38), character: '8' */</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="str">
+      <c r="A29" s="4" t="str">
         <f aca="false">Sheet1!V26</f>
-        <v>    0x64, 0x92, 0x92, 0x92, 0x7C, /* ASCII 57 (0x39), character: '9' */</v>
+        <v>    { 0x64, 0x92, 0x92, 0x92, 0x7C }, /* ASCII 57 (0x39), character: '9' */</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="str">
+      <c r="A30" s="4" t="str">
         <f aca="false">Sheet1!V27</f>
-        <v>    0x00, 0x6C, 0x6C, 0x00, 0x00, /* ASCII 58 (0x3A), character: ':' */</v>
+        <v>    { 0x00, 0x6C, 0x6C, 0x00, 0x00 }, /* ASCII 58 (0x3A), character: ':' */</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="str">
+      <c r="A31" s="4" t="str">
         <f aca="false">Sheet1!V28</f>
-        <v>    0x00, 0x6D, 0x6E, 0x00, 0x00, /* ASCII 59 (0x3B), character: ';' */</v>
+        <v>    { 0x00, 0x6D, 0x6E, 0x00, 0x00 }, /* ASCII 59 (0x3B), character: ';' */</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="str">
+      <c r="A32" s="4" t="str">
         <f aca="false">Sheet1!V29</f>
-        <v>    0x00, 0x10, 0x28, 0x44, 0x82, /* ASCII 60 (0x3C), character: '&lt;' */</v>
+        <v>    { 0x00, 0x10, 0x28, 0x44, 0x82 }, /* ASCII 60 (0x3C), character: '&lt;' */</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3" t="str">
+      <c r="A33" s="4" t="str">
         <f aca="false">Sheet1!V30</f>
-        <v>    0x28, 0x28, 0x28, 0x28, 0x28, /* ASCII 61 (0x3D), character: '=' */</v>
+        <v>    { 0x28, 0x28, 0x28, 0x28, 0x28 }, /* ASCII 61 (0x3D), character: '=' */</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3" t="str">
+      <c r="A34" s="4" t="str">
         <f aca="false">Sheet1!V31</f>
-        <v>    0x82, 0x44, 0x28, 0x10, 0x00, /* ASCII 62 (0x3E), character: '&gt;' */</v>
+        <v>    { 0x82, 0x44, 0x28, 0x10, 0x00 }, /* ASCII 62 (0x3E), character: '&gt;' */</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3" t="str">
+      <c r="A35" s="4" t="str">
         <f aca="false">Sheet1!V32</f>
-        <v>    0x40, 0x80, 0x9A, 0xA0, 0x40, /* ASCII 63 (0x3F), character: '?' */</v>
+        <v>    { 0x40, 0x80, 0x9A, 0xA0, 0x40 }, /* ASCII 63 (0x3F), character: '?' */</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="3" t="str">
+      <c r="A36" s="4" t="str">
         <f aca="false">Sheet1!V33</f>
-        <v>    0x7C, 0x82, 0xBA, 0xAA, 0x7A, /* ASCII 64 (0x40), character: '@' */</v>
+        <v>    { 0x7C, 0x82, 0xBA, 0xAA, 0x7A }, /* ASCII 64 (0x40), character: '@' */</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3" t="str">
+      <c r="A37" s="4" t="str">
         <f aca="false">Sheet1!V34</f>
-        <v>    0x3E, 0x48, 0x88, 0x48, 0x3E, /* ASCII 65 (0x41), character: 'A' */</v>
+        <v>    { 0x3E, 0x48, 0x88, 0x48, 0x3E }, /* ASCII 65 (0x41), character: 'A' */</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="3" t="str">
+      <c r="A38" s="4" t="str">
         <f aca="false">Sheet1!V35</f>
-        <v>    0xFE, 0x92, 0x92, 0x92, 0x6C, /* ASCII 66 (0x42), character: 'B' */</v>
+        <v>    { 0xFE, 0x92, 0x92, 0x92, 0x6C }, /* ASCII 66 (0x42), character: 'B' */</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="3" t="str">
+      <c r="A39" s="4" t="str">
         <f aca="false">Sheet1!V36</f>
-        <v>    0x7C, 0x82, 0x82, 0x82, 0x44, /* ASCII 67 (0x43), character: 'C' */</v>
+        <v>    { 0x7C, 0x82, 0x82, 0x82, 0x44 }, /* ASCII 67 (0x43), character: 'C' */</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="3" t="str">
+      <c r="A40" s="4" t="str">
         <f aca="false">Sheet1!V37</f>
-        <v>    0xFE, 0x82, 0x82, 0x82, 0x7C, /* ASCII 68 (0x44), character: 'D' */</v>
+        <v>    { 0xFE, 0x82, 0x82, 0x82, 0x7C }, /* ASCII 68 (0x44), character: 'D' */</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="str">
+      <c r="A41" s="4" t="str">
         <f aca="false">Sheet1!V38</f>
-        <v>    0xFE, 0x92, 0x92, 0x92, 0x82, /* ASCII 69 (0x45), character: 'E' */</v>
+        <v>    { 0xFE, 0x92, 0x92, 0x92, 0x82 }, /* ASCII 69 (0x45), character: 'E' */</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="3" t="str">
+      <c r="A42" s="4" t="str">
         <f aca="false">Sheet1!V39</f>
-        <v>    0xFE, 0x90, 0x90, 0x90, 0x80, /* ASCII 70 (0x46), character: 'F' */</v>
+        <v>    { 0xFE, 0x90, 0x90, 0x90, 0x80 }, /* ASCII 70 (0x46), character: 'F' */</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="3" t="str">
+      <c r="A43" s="4" t="str">
         <f aca="false">Sheet1!V40</f>
-        <v>    0x7C, 0x82, 0x8A, 0x8A, 0x4C, /* ASCII 71 (0x47), character: 'G' */</v>
+        <v>    { 0x7C, 0x82, 0x8A, 0x8A, 0x4C }, /* ASCII 71 (0x47), character: 'G' */</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="3" t="str">
+      <c r="A44" s="4" t="str">
         <f aca="false">Sheet1!V41</f>
-        <v>    0xFE, 0x10, 0x10, 0x10, 0xFE, /* ASCII 72 (0x48), character: 'H' */</v>
+        <v>    { 0xFE, 0x10, 0x10, 0x10, 0xFE }, /* ASCII 72 (0x48), character: 'H' */</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="3" t="str">
+      <c r="A45" s="4" t="str">
         <f aca="false">Sheet1!V42</f>
-        <v>    0x00, 0x82, 0xFE, 0x82, 0x00, /* ASCII 73 (0x49), character: 'I' */</v>
+        <v>    { 0x00, 0x82, 0xFE, 0x82, 0x00 }, /* ASCII 73 (0x49), character: 'I' */</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="3" t="str">
+      <c r="A46" s="4" t="str">
         <f aca="false">Sheet1!V43</f>
-        <v>    0x0C, 0x02, 0x82, 0xFC, 0x80, /* ASCII 74 (0x4A), character: 'J' */</v>
+        <v>    { 0x0C, 0x02, 0x82, 0xFC, 0x80 }, /* ASCII 74 (0x4A), character: 'J' */</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="3" t="str">
+      <c r="A47" s="4" t="str">
         <f aca="false">Sheet1!V44</f>
-        <v>    0xFE, 0x10, 0x28, 0x44, 0x82, /* ASCII 75 (0x4B), character: 'K' */</v>
+        <v>    { 0xFE, 0x10, 0x28, 0x44, 0x82 }, /* ASCII 75 (0x4B), character: 'K' */</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="3" t="str">
+      <c r="A48" s="4" t="str">
         <f aca="false">Sheet1!V45</f>
-        <v>    0xFE, 0x02, 0x02, 0x02, 0x02, /* ASCII 76 (0x4C), character: 'L' */</v>
+        <v>    { 0xFE, 0x02, 0x02, 0x02, 0x02 }, /* ASCII 76 (0x4C), character: 'L' */</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="3" t="str">
+      <c r="A49" s="4" t="str">
         <f aca="false">Sheet1!V46</f>
-        <v>    0xFE, 0x40, 0x20, 0x40, 0xFE, /* ASCII 77 (0x4D), character: 'M' */</v>
+        <v>    { 0xFE, 0x40, 0x20, 0x40, 0xFE }, /* ASCII 77 (0x4D), character: 'M' */</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="3" t="str">
+      <c r="A50" s="4" t="str">
         <f aca="false">Sheet1!V47</f>
-        <v>    0xFE, 0x20, 0x10, 0x08, 0xFE, /* ASCII 78 (0x4E), character: 'N' */</v>
+        <v>    { 0xFE, 0x20, 0x10, 0x08, 0xFE }, /* ASCII 78 (0x4E), character: 'N' */</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="3" t="str">
+      <c r="A51" s="4" t="str">
         <f aca="false">Sheet1!V48</f>
-        <v>    0x7C, 0x82, 0x82, 0x82, 0x7C, /* ASCII 79 (0x4F), character: 'O' */</v>
+        <v>    { 0x7C, 0x82, 0x82, 0x82, 0x7C }, /* ASCII 79 (0x4F), character: 'O' */</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="3" t="str">
+      <c r="A52" s="4" t="str">
         <f aca="false">Sheet1!V49</f>
-        <v>    0xFE, 0x90, 0x90, 0x90, 0x60, /* ASCII 80 (0x50), character: 'P' */</v>
+        <v>    { 0xFE, 0x90, 0x90, 0x90, 0x60 }, /* ASCII 80 (0x50), character: 'P' */</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="3" t="str">
+      <c r="A53" s="4" t="str">
         <f aca="false">Sheet1!V50</f>
-        <v>    0x7C, 0x82, 0x86, 0x82, 0x7D, /* ASCII 81 (0x51), character: 'Q' */</v>
+        <v>    { 0x7C, 0x82, 0x86, 0x82, 0x7D }, /* ASCII 81 (0x51), character: 'Q' */</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="3" t="str">
+      <c r="A54" s="4" t="str">
         <f aca="false">Sheet1!V51</f>
-        <v>    0xFE, 0x90, 0x90, 0x90, 0x6E, /* ASCII 82 (0x52), character: 'R' */</v>
+        <v>    { 0xFE, 0x90, 0x90, 0x90, 0x6E }, /* ASCII 82 (0x52), character: 'R' */</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="3" t="str">
+      <c r="A55" s="4" t="str">
         <f aca="false">Sheet1!V52</f>
-        <v>    0x62, 0x92, 0x92, 0x92, 0x8C, /* ASCII 83 (0x53), character: 'S' */</v>
+        <v>    { 0x62, 0x92, 0x92, 0x92, 0x8C }, /* ASCII 83 (0x53), character: 'S' */</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="3" t="str">
+      <c r="A56" s="4" t="str">
         <f aca="false">Sheet1!V53</f>
-        <v>    0x80, 0x80, 0xFE, 0x80, 0x80, /* ASCII 84 (0x54), character: 'T' */</v>
+        <v>    { 0x80, 0x80, 0xFE, 0x80, 0x80 }, /* ASCII 84 (0x54), character: 'T' */</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="3" t="str">
+      <c r="A57" s="4" t="str">
         <f aca="false">Sheet1!V54</f>
-        <v>    0xFC, 0x02, 0x02, 0x02, 0xFC, /* ASCII 85 (0x55), character: 'U' */</v>
+        <v>    { 0xFC, 0x02, 0x02, 0x02, 0xFC }, /* ASCII 85 (0x55), character: 'U' */</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="3" t="str">
+      <c r="A58" s="4" t="str">
         <f aca="false">Sheet1!V55</f>
-        <v>    0xE0, 0x38, 0x0E, 0x38, 0xE0, /* ASCII 86 (0x56), character: 'V' */</v>
+        <v>    { 0xE0, 0x38, 0x0E, 0x38, 0xE0 }, /* ASCII 86 (0x56), character: 'V' */</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="3" t="str">
+      <c r="A59" s="4" t="str">
         <f aca="false">Sheet1!V56</f>
-        <v>    0xFC, 0x02, 0x0C, 0x02, 0xFC, /* ASCII 87 (0x57), character: 'W' */</v>
+        <v>    { 0xFC, 0x02, 0x0C, 0x02, 0xFC }, /* ASCII 87 (0x57), character: 'W' */</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="3" t="str">
+      <c r="A60" s="4" t="str">
         <f aca="false">Sheet1!V57</f>
-        <v>    0xC6, 0x28, 0x10, 0x28, 0xC6, /* ASCII 88 (0x58), character: 'X' */</v>
+        <v>    { 0xC6, 0x28, 0x10, 0x28, 0xC6 }, /* ASCII 88 (0x58), character: 'X' */</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="3" t="str">
+      <c r="A61" s="4" t="str">
         <f aca="false">Sheet1!V58</f>
-        <v>    0xE0, 0x10, 0x0E, 0x10, 0xE0, /* ASCII 89 (0x59), character: 'Y' */</v>
+        <v>    { 0xE0, 0x10, 0x0E, 0x10, 0xE0 }, /* ASCII 89 (0x59), character: 'Y' */</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="3" t="str">
+      <c r="A62" s="4" t="str">
         <f aca="false">Sheet1!V59</f>
-        <v>    0x86, 0x8A, 0x92, 0xA2, 0xC2, /* ASCII 90 (0x5A), character: 'Z' */</v>
+        <v>    { 0x86, 0x8A, 0x92, 0xA2, 0xC2 }, /* ASCII 90 (0x5A), character: 'Z' */</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="3" t="str">
+      <c r="A63" s="4" t="str">
         <f aca="false">Sheet1!V60</f>
-        <v>    0x00, 0xFE, 0x82, 0x82, 0x00, /* ASCII 91 (0x5B), character: '[' */</v>
+        <v>    { 0x00, 0xFE, 0x82, 0x82, 0x00 }, /* ASCII 91 (0x5B), character: '[' */</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="3" t="str">
+      <c r="A64" s="4" t="str">
         <f aca="false">Sheet1!V61</f>
-        <v>    0x00, 0xC0, 0x30, 0x0C, 0x03, /* ASCII 92 (0x5C), character: '\' */</v>
+        <v>    { 0x00, 0xC0, 0x30, 0x0C, 0x03 }, /* ASCII 92 (0x5C), character: '\' */</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="3" t="str">
+      <c r="A65" s="4" t="str">
         <f aca="false">Sheet1!V62</f>
-        <v>    0x00, 0x82, 0x82, 0xFE, 0x00, /* ASCII 93 (0x5D), character: ']' */</v>
+        <v>    { 0x00, 0x82, 0x82, 0xFE, 0x00 }, /* ASCII 93 (0x5D), character: ']' */</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="3" t="str">
+      <c r="A66" s="4" t="str">
         <f aca="false">Sheet1!V63</f>
-        <v>    0x10, 0x20, 0x40, 0x20, 0x10, /* ASCII 94 (0x5E), character: '^' */</v>
+        <v>    { 0x10, 0x20, 0x40, 0x20, 0x10 }, /* ASCII 94 (0x5E), character: '^' */</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="3" t="str">
+      <c r="A67" s="4" t="str">
         <f aca="false">Sheet1!V64</f>
-        <v>    0x02, 0x02, 0x02, 0x02, 0x02, /* ASCII 95 (0x5F), character: '_' */</v>
+        <v>    { 0x02, 0x02, 0x02, 0x02, 0x02 }, /* ASCII 95 (0x5F), character: '_' */</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="3" t="str">
+      <c r="A68" s="4" t="str">
         <f aca="false">Sheet1!V65</f>
-        <v>    0x00, 0x80, 0x60, 0x00, 0x00, /* ASCII 96 (0x60), character: '`' */</v>
+        <v>    { 0x00, 0x80, 0x60, 0x00, 0x00 }, /* ASCII 96 (0x60), character: '`' */</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="3" t="str">
+      <c r="A69" s="4" t="str">
         <f aca="false">Sheet1!V66</f>
-        <v>    0x24, 0x4A, 0x4A, 0x3E, 0x00, /* ASCII 97 (0x61), character: 'a' */</v>
+        <v>    { 0x24, 0x4A, 0x4A, 0x3E, 0x00 }, /* ASCII 97 (0x61), character: 'a' */</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="3" t="str">
+      <c r="A70" s="4" t="str">
         <f aca="false">Sheet1!V67</f>
-        <v>    0x00, 0xFE, 0x12, 0x12, 0x0C, /* ASCII 98 (0x62), character: 'b' */</v>
+        <v>    { 0x00, 0xFE, 0x12, 0x12, 0x0C }, /* ASCII 98 (0x62), character: 'b' */</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="3" t="str">
+      <c r="A71" s="4" t="str">
         <f aca="false">Sheet1!V68</f>
-        <v>    0x0C, 0x12, 0x12, 0x12, 0x00, /* ASCII 99 (0x63), character: 'c' */</v>
+        <v>    { 0x0C, 0x12, 0x12, 0x12, 0x00 }, /* ASCII 99 (0x63), character: 'c' */</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="3" t="str">
+      <c r="A72" s="4" t="str">
         <f aca="false">Sheet1!V69</f>
-        <v>    0x00, 0x0C, 0x12, 0x12, 0xFE, /* ASCII 100 (0x64), character: 'd' */</v>
+        <v>    { 0x00, 0x0C, 0x12, 0x12, 0xFE }, /* ASCII 100 (0x64), character: 'd' */</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="3" t="str">
+      <c r="A73" s="4" t="str">
         <f aca="false">Sheet1!V70</f>
-        <v>    0x1C, 0x2A, 0x2A, 0x10, 0x00, /* ASCII 101 (0x65), character: 'e' */</v>
+        <v>    { 0x1C, 0x2A, 0x2A, 0x10, 0x00 }, /* ASCII 101 (0x65), character: 'e' */</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="3" t="str">
+      <c r="A74" s="4" t="str">
         <f aca="false">Sheet1!V71</f>
-        <v>    0x3E, 0x48, 0x40, 0x20, 0x00, /* ASCII 102 (0x66), character: 'f' */</v>
+        <v>    { 0x3E, 0x48, 0x40, 0x20, 0x00 }, /* ASCII 102 (0x66), character: 'f' */</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="3" t="str">
+      <c r="A75" s="4" t="str">
         <f aca="false">Sheet1!V72</f>
-        <v>    0x12, 0x29, 0x29, 0x3E, 0x00, /* ASCII 103 (0x67), character: 'g' */</v>
+        <v>    { 0x12, 0x29, 0x29, 0x3E, 0x00 }, /* ASCII 103 (0x67), character: 'g' */</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="3" t="str">
+      <c r="A76" s="4" t="str">
         <f aca="false">Sheet1!V73</f>
-        <v>    0x7E, 0x08, 0x08, 0x06, 0x00, /* ASCII 104 (0x68), character: 'h' */</v>
+        <v>    { 0x7E, 0x08, 0x08, 0x06, 0x00 }, /* ASCII 104 (0x68), character: 'h' */</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="3" t="str">
+      <c r="A77" s="4" t="str">
         <f aca="false">Sheet1!V74</f>
-        <v>    0x00, 0x12, 0x5E, 0x02, 0x00, /* ASCII 105 (0x69), character: 'i' */</v>
+        <v>    { 0x00, 0x12, 0x5E, 0x02, 0x00 }, /* ASCII 105 (0x69), character: 'i' */</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="3" t="str">
+      <c r="A78" s="4" t="str">
         <f aca="false">Sheet1!V75</f>
-        <v>    0x00, 0x02, 0x11, 0x5E, 0x10, /* ASCII 106 (0x6A), character: 'j' */</v>
+        <v>    { 0x00, 0x02, 0x11, 0x5E, 0x10 }, /* ASCII 106 (0x6A), character: 'j' */</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="3" t="str">
+      <c r="A79" s="4" t="str">
         <f aca="false">Sheet1!V76</f>
-        <v>    0x00, 0xFE, 0x08, 0x16, 0x00, /* ASCII 107 (0x6B), character: 'k' */</v>
+        <v>    { 0x00, 0xFE, 0x08, 0x16, 0x00 }, /* ASCII 107 (0x6B), character: 'k' */</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="3" t="str">
+      <c r="A80" s="4" t="str">
         <f aca="false">Sheet1!V77</f>
-        <v>    0x00, 0x42, 0x7E, 0x02, 0x00, /* ASCII 108 (0x6C), character: 'l' */</v>
+        <v>    { 0x00, 0x42, 0x7E, 0x02, 0x00 }, /* ASCII 108 (0x6C), character: 'l' */</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="3" t="str">
+      <c r="A81" s="4" t="str">
         <f aca="false">Sheet1!V78</f>
-        <v>    0x1E, 0x10, 0x0E, 0x10, 0x0E, /* ASCII 109 (0x6D), character: 'm' */</v>
+        <v>    { 0x1E, 0x10, 0x0E, 0x10, 0x0E }, /* ASCII 109 (0x6D), character: 'm' */</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="3" t="str">
+      <c r="A82" s="4" t="str">
         <f aca="false">Sheet1!V79</f>
-        <v>    0x1E, 0x10, 0x10, 0x0E, 0x00, /* ASCII 110 (0x6E), character: 'n' */</v>
+        <v>    { 0x1E, 0x10, 0x10, 0x0E, 0x00 }, /* ASCII 110 (0x6E), character: 'n' */</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="3" t="str">
+      <c r="A83" s="4" t="str">
         <f aca="false">Sheet1!V80</f>
-        <v>    0x0C, 0x12, 0x12, 0x0C, 0x00, /* ASCII 111 (0x6F), character: 'o' */</v>
+        <v>    { 0x0C, 0x12, 0x12, 0x0C, 0x00 }, /* ASCII 111 (0x6F), character: 'o' */</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="3" t="str">
+      <c r="A84" s="4" t="str">
         <f aca="false">Sheet1!V81</f>
-        <v>    0x00, 0x3F, 0x24, 0x24, 0x18, /* ASCII 112 (0x70), character: 'p' */</v>
+        <v>    { 0x00, 0x3F, 0x24, 0x24, 0x18 }, /* ASCII 112 (0x70), character: 'p' */</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="3" t="str">
+      <c r="A85" s="4" t="str">
         <f aca="false">Sheet1!V82</f>
-        <v>    0x18, 0x24, 0x24, 0x3F, 0x00, /* ASCII 113 (0x71), character: 'q' */</v>
+        <v>    { 0x18, 0x24, 0x24, 0x3F, 0x00 }, /* ASCII 113 (0x71), character: 'q' */</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="3" t="str">
+      <c r="A86" s="4" t="str">
         <f aca="false">Sheet1!V83</f>
-        <v>    0x1E, 0x08, 0x10, 0x08, 0x00, /* ASCII 114 (0x72), character: 'r' */</v>
+        <v>    { 0x1E, 0x08, 0x10, 0x08, 0x00 }, /* ASCII 114 (0x72), character: 'r' */</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="3" t="str">
+      <c r="A87" s="4" t="str">
         <f aca="false">Sheet1!V84</f>
-        <v>    0x12, 0x2A, 0x2A, 0x24, 0x00, /* ASCII 115 (0x73), character: 's' */</v>
+        <v>    { 0x12, 0x2A, 0x2A, 0x24, 0x00 }, /* ASCII 115 (0x73), character: 's' */</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="3" t="str">
+      <c r="A88" s="4" t="str">
         <f aca="false">Sheet1!V85</f>
-        <v>    0x10, 0x3E, 0x11, 0x02, 0x00, /* ASCII 116 (0x74), character: 't' */</v>
+        <v>    { 0x10, 0x3E, 0x11, 0x02, 0x00 }, /* ASCII 116 (0x74), character: 't' */</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="3" t="str">
+      <c r="A89" s="4" t="str">
         <f aca="false">Sheet1!V86</f>
-        <v>    0x1C, 0x02, 0x02, 0x1C, 0x00, /* ASCII 117 (0x75), character: 'u' */</v>
+        <v>    { 0x1C, 0x02, 0x02, 0x1C, 0x00 }, /* ASCII 117 (0x75), character: 'u' */</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="3" t="str">
+      <c r="A90" s="4" t="str">
         <f aca="false">Sheet1!V87</f>
-        <v>    0x18, 0x04, 0x02, 0x04, 0x18, /* ASCII 118 (0x76), character: 'v' */</v>
+        <v>    { 0x18, 0x04, 0x02, 0x04, 0x18 }, /* ASCII 118 (0x76), character: 'v' */</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="3" t="str">
+      <c r="A91" s="4" t="str">
         <f aca="false">Sheet1!V88</f>
-        <v>    0x1C, 0x02, 0x1C, 0x02, 0x1C, /* ASCII 119 (0x77), character: 'w' */</v>
+        <v>    { 0x1C, 0x02, 0x1C, 0x02, 0x1C }, /* ASCII 119 (0x77), character: 'w' */</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="3" t="str">
+      <c r="A92" s="4" t="str">
         <f aca="false">Sheet1!V89</f>
-        <v>    0x22, 0x14, 0x08, 0x14, 0x22, /* ASCII 120 (0x78), character: 'x' */</v>
+        <v>    { 0x22, 0x14, 0x08, 0x14, 0x22 }, /* ASCII 120 (0x78), character: 'x' */</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="3" t="str">
+      <c r="A93" s="4" t="str">
         <f aca="false">Sheet1!V90</f>
-        <v>    0x39, 0x05, 0x05, 0x3E, 0x00, /* ASCII 121 (0x79), character: 'y' */</v>
+        <v>    { 0x39, 0x05, 0x05, 0x3E, 0x00 }, /* ASCII 121 (0x79), character: 'y' */</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="3" t="str">
+      <c r="A94" s="4" t="str">
         <f aca="false">Sheet1!V91</f>
-        <v>    0x00, 0x26, 0x2A, 0x32, 0x00, /* ASCII 122 (0x7A), character: 'z' */</v>
+        <v>    { 0x00, 0x26, 0x2A, 0x32, 0x00 }, /* ASCII 122 (0x7A), character: 'z' */</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="3" t="str">
+      <c r="A95" s="4" t="str">
         <f aca="false">Sheet1!V92</f>
-        <v>    0x00, 0x10, 0x7C, 0x82, 0x00, /* ASCII 123 (0x7B), character: '{' */</v>
+        <v>    { 0x00, 0x10, 0x7C, 0x82, 0x00 }, /* ASCII 123 (0x7B), character: '{' */</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="3" t="str">
+      <c r="A96" s="4" t="str">
         <f aca="false">Sheet1!V93</f>
-        <v>    0x00, 0x00, 0xFF, 0x00, 0x00, /* ASCII 124 (0x7C), character: '|' */</v>
+        <v>    { 0x00, 0x00, 0xFF, 0x00, 0x00 }, /* ASCII 124 (0x7C), character: '|' */</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="3" t="str">
+      <c r="A97" s="4" t="str">
         <f aca="false">Sheet1!V94</f>
-        <v>    0x00, 0x82, 0x7C, 0x10, 0x00, /* ASCII 125 (0x7D), character: '}' */</v>
+        <v>    { 0x00, 0x82, 0x7C, 0x10, 0x00 }, /* ASCII 125 (0x7D), character: '}' */</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="3" t="str">
+      <c r="A98" s="4" t="str">
         <f aca="false">Sheet1!V95</f>
-        <v>    0x10, 0x20, 0x10, 0x08, 0x10, /* ASCII 126 (0x7E), character: '~' */</v>
+        <v>    { 0x10, 0x20, 0x10, 0x08, 0x10 }, /* ASCII 126 (0x7E), character: '~' */</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="3" t="str">
+      <c r="A99" s="4" t="str">
         <f aca="false">Sheet1!V96</f>
-        <v>    0x00, 0xE0, 0xA0, 0xE0, 0x00, /* ASCII 127 (0x7F), character: '' */</v>
+        <v>    { 0x00, 0xE0, 0xA0, 0xE0, 0x00 }, /* ASCII 127 (0x7F), character: '' */</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="3" t="str">
+      <c r="A100" s="4" t="str">
         <f aca="false">Sheet1!V97</f>
-        <v>    0x28, 0x7C, 0xAA, 0x82, 0x44, /* ASCII 128 (0x80), character: '€' */</v>
+        <v>    { 0x28, 0x7C, 0xAA, 0x82, 0x44 }, /* ASCII 128 (0x80), character: '€' */</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="3" t="str">
+      <c r="A101" s="4" t="str">
         <f aca="false">CONCATENATE("};")</f>
         <v>};</v>
       </c>

</xml_diff>